<commit_message>
Item menu and cursor
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="128">
   <si>
     <t>N</t>
   </si>
@@ -175,6 +175,15 @@
     <t>false</t>
   </si>
   <si>
+    <t>PICKABLE_ITEM_CHOSEN</t>
+  </si>
+  <si>
+    <t>GamePickableItem</t>
+  </si>
+  <si>
+    <t>GamePickableItem.ITEM_PICK_NONE</t>
+  </si>
+  <si>
     <t>SERVICE_ID</t>
   </si>
   <si>
@@ -376,13 +385,22 @@
     <t>ItemMasterClass.TakeItemObjectService</t>
   </si>
   <si>
-    <t>GET_ITEM_LIST</t>
-  </si>
-  <si>
-    <t>GET_ITEM_LIST_DELEGATE</t>
-  </si>
-  <si>
-    <t>LevelMasterClass.GetItemListService</t>
+    <t>GET_SCENARIO_ITEM_LIST</t>
+  </si>
+  <si>
+    <t>GET_SCENARIO_ITEM_LIST_DELEGATE</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.GetScenarioItemListService</t>
+  </si>
+  <si>
+    <t>GET_PICKED_ITEM_LIST</t>
+  </si>
+  <si>
+    <t>GET_PICKED_ITEM_LIST_DELEGATE</t>
+  </si>
+  <si>
+    <t>ItemMasterClass.GetPickedItemListService</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1316,56 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1"/>
@@ -2281,13 +2348,13 @@
     <row r="991" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D13">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G13">
       <formula1>"N,Y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:Q12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:Q13">
       <formula1>"R,R E,W,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2309,8 +2376,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="22.86"/>
-    <col customWidth="1" min="3" max="3" width="32.57"/>
+    <col customWidth="1" min="1" max="1" width="22.86"/>
+    <col customWidth="1" min="2" max="2" width="24.14"/>
+    <col customWidth="1" min="3" max="3" width="33.71"/>
     <col customWidth="1" min="4" max="4" width="44.0"/>
     <col customWidth="1" min="5" max="5" width="4.86"/>
   </cols>
@@ -2320,13 +2388,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -2364,13 +2432,13 @@
         <v>0.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -2388,7 +2456,7 @@
         <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>24</v>
@@ -2408,13 +2476,13 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -2426,7 +2494,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>24</v>
@@ -2452,13 +2520,13 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -2476,7 +2544,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>24</v>
@@ -2496,13 +2564,13 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
@@ -2514,7 +2582,7 @@
         <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>24</v>
@@ -2540,13 +2608,13 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
@@ -2558,7 +2626,7 @@
         <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>24</v>
@@ -2584,13 +2652,13 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -2614,7 +2682,7 @@
         <v>24</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>24</v>
@@ -2628,13 +2696,13 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>24</v>
@@ -2658,7 +2726,7 @@
         <v>24</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>24</v>
@@ -2669,13 +2737,13 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>24</v>
@@ -2693,7 +2761,7 @@
         <v>24</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>24</v>
@@ -2710,13 +2778,13 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>24</v>
@@ -2751,13 +2819,13 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>24</v>
@@ -2766,7 +2834,7 @@
         <v>24</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>24</v>
@@ -2792,13 +2860,13 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>24</v>
@@ -2816,7 +2884,7 @@
         <v>24</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>24</v>
@@ -2833,13 +2901,13 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>24</v>
@@ -2857,13 +2925,13 @@
         <v>24</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>24</v>
@@ -2874,13 +2942,13 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>24</v>
@@ -2889,7 +2957,7 @@
         <v>24</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>24</v>
@@ -2898,13 +2966,13 @@
         <v>24</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>23</v>
@@ -2915,13 +2983,13 @@
         <v>13.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>24</v>
@@ -2930,7 +2998,7 @@
         <v>24</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>24</v>
@@ -2939,13 +3007,13 @@
         <v>24</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>23</v>
@@ -2956,13 +3024,13 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>24</v>
@@ -2986,7 +3054,7 @@
         <v>24</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>23</v>
@@ -2997,13 +3065,13 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>24</v>
@@ -3027,7 +3095,7 @@
         <v>24</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>23</v>
@@ -3038,13 +3106,13 @@
         <v>16.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>24</v>
@@ -3053,7 +3121,7 @@
         <v>24</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>24</v>
@@ -3068,7 +3136,7 @@
         <v>24</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>23</v>
@@ -3079,13 +3147,13 @@
         <v>17.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>24</v>
@@ -3109,7 +3177,7 @@
         <v>24</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>23</v>
@@ -3120,13 +3188,13 @@
         <v>18.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>24</v>
@@ -3135,7 +3203,7 @@
         <v>24</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>24</v>
@@ -3161,13 +3229,13 @@
         <v>19.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>24</v>
@@ -3185,7 +3253,7 @@
         <v>24</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>24</v>
@@ -3202,13 +3270,13 @@
         <v>20.0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>24</v>
@@ -3217,7 +3285,7 @@
         <v>24</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>24</v>
@@ -3226,7 +3294,7 @@
         <v>24</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>24</v>
@@ -3243,13 +3311,13 @@
         <v>21.0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>24</v>
@@ -3273,15 +3341,56 @@
         <v>24</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N23" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <v>22.0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N23">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N24">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Custom actions for every player-item or item-item interaction
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="A4IXCiYJIjW8BBdIXp/5Ur/q0ejgCDmXLTfyD1YJk2w="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="HG1rVsdSrIWZrSsHm7ZEAfLmsQLt9s4FHbTeOCBADTY="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="143">
   <si>
     <t>N</t>
   </si>
@@ -184,10 +184,10 @@
     <t>PICKABLE_ITEM_CHOSEN</t>
   </si>
   <si>
-    <t>GamePickableItem</t>
-  </si>
-  <si>
-    <t>GamePickableItem.ITEM_PICK_NONE</t>
+    <t>GameItem</t>
+  </si>
+  <si>
+    <t>GameItem.ITEM_NONE</t>
   </si>
   <si>
     <t>SERVICE_ID</t>
@@ -211,6 +211,24 @@
     <t>X</t>
   </si>
   <si>
+    <t>SAVE_GAME</t>
+  </si>
+  <si>
+    <t>SAVE_GAME_DELEGATE</t>
+  </si>
+  <si>
+    <t>GameMasterClass.SaveGameService</t>
+  </si>
+  <si>
+    <t>LOAD_GAME</t>
+  </si>
+  <si>
+    <t>LOAD_GAME_DELEGATE</t>
+  </si>
+  <si>
+    <t>GameMasterClass.LoadGameService</t>
+  </si>
+  <si>
     <t>LOAD_ROOM</t>
   </si>
   <si>
@@ -229,6 +247,15 @@
     <t>GameMasterClass.ExitGameService</t>
   </si>
   <si>
+    <t>LATE_START_SUBSCRIPTION</t>
+  </si>
+  <si>
+    <t>LATE_START_SUBSCRIPTION_DELEGATE</t>
+  </si>
+  <si>
+    <t>GameMasterClass.LateStartSubrsciptionService</t>
+  </si>
+  <si>
     <t>LOADING_COMPLETED</t>
   </si>
   <si>
@@ -265,6 +292,15 @@
     <t>LevelMasterClass.ItemRegisterService</t>
   </si>
   <si>
+    <t>ITEM_REMOVE_FROM_SCENE</t>
+  </si>
+  <si>
+    <t>ITEM_REMOVE_FROM_SCENE_DELEGATE</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.ItemRemoveFromSceneService</t>
+  </si>
+  <si>
     <t>MONO_REGISTER</t>
   </si>
   <si>
@@ -346,13 +382,13 @@
     <t>GameEventMasterClass.TakeItemFromSceneEventService</t>
   </si>
   <si>
-    <t>TAKE_ITEM</t>
-  </si>
-  <si>
-    <t>TAKE_ITEM_DELEGATE</t>
-  </si>
-  <si>
-    <t>ItemMasterClass.TakeItemService</t>
+    <t>USE_ITEM</t>
+  </si>
+  <si>
+    <t>USE_ITEM_DELEGATE</t>
+  </si>
+  <si>
+    <t>ItemMasterClass.UseItemService</t>
   </si>
   <si>
     <t>IS_ITEM_TAKEN_FROM_SCENE</t>
@@ -373,15 +409,6 @@
     <t>PlayerMasterClass.InteractPlayerItemService</t>
   </si>
   <si>
-    <t>GET_ITEM_INTERACTION</t>
-  </si>
-  <si>
-    <t>GET_ITEM_INTERACTION_DELEGATE</t>
-  </si>
-  <si>
-    <t>GameEventMasterClass.GetItemInteractionService</t>
-  </si>
-  <si>
     <t>GET_SCENARIO_ITEM_LIST</t>
   </si>
   <si>
@@ -409,13 +436,13 @@
     <t>ItemMasterClass.CancelPickableItemService</t>
   </si>
   <si>
-    <t>USE_ITEM</t>
-  </si>
-  <si>
-    <t>USE_ITEM_DELEGATE</t>
-  </si>
-  <si>
-    <t>ItemMasterClass.UseItemService</t>
+    <t>SET_PLAYER_ANIMATION</t>
+  </si>
+  <si>
+    <t>SET_PLAYER_ANIMATION_DELEGATE</t>
+  </si>
+  <si>
+    <t>PlayerMasterClass.SetPlayerAnimation</t>
   </si>
   <si>
     <t>LAST_SERVICE</t>
@@ -425,7 +452,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -440,6 +467,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -456,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -469,6 +501,15 @@
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,7 +1046,7 @@
         <v>24</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>21</v>
@@ -2491,32 +2532,30 @@
       <c r="A3" s="2">
         <v>1.0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>63</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>24</v>
@@ -2527,7 +2566,7 @@
       <c r="M3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2535,19 +2574,17 @@
       <c r="A4" s="2">
         <v>2.0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -2559,7 +2596,7 @@
       <c r="I4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>63</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -2571,7 +2608,7 @@
       <c r="M4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2641,14 +2678,14 @@
       <c r="G6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>63</v>
+      <c r="H6" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>24</v>
+      <c r="J6" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>24</v>
@@ -2676,58 +2713,59 @@
       <c r="D7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>23</v>
+        <v>63</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
         <v>6.0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>24</v>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>23</v>
+      <c r="H8" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>24</v>
@@ -2742,9 +2780,9 @@
         <v>24</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2755,29 +2793,32 @@
       <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>63</v>
+        <v>63</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>24</v>
@@ -2793,37 +2834,40 @@
       <c r="A10" s="2">
         <v>8.0</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" s="3" t="s">
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N10" s="3" t="s">
@@ -2834,40 +2878,40 @@
       <c r="A11" s="2">
         <v>9.0</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="3" t="s">
+      <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2875,40 +2919,40 @@
       <c r="A12" s="2">
         <v>10.0</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="3" t="s">
+      <c r="F12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2916,13 +2960,13 @@
       <c r="A13" s="2">
         <v>11.0</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -2931,7 +2975,7 @@
       <c r="G13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="3" t="s">
@@ -2940,13 +2984,13 @@
       <c r="J13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="3" t="s">
+      <c r="K13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N13" s="3" t="s">
@@ -2982,13 +3026,13 @@
         <v>24</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>24</v>
@@ -3023,16 +3067,16 @@
         <v>24</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
@@ -3064,16 +3108,16 @@
         <v>24</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
@@ -3096,7 +3140,7 @@
         <v>24</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>24</v>
@@ -3105,16 +3149,16 @@
         <v>24</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
@@ -3137,7 +3181,7 @@
         <v>24</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>24</v>
@@ -3149,10 +3193,10 @@
         <v>63</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>24</v>
@@ -3187,10 +3231,10 @@
         <v>24</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>63</v>
@@ -3228,16 +3272,16 @@
         <v>24</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21">
@@ -3269,58 +3313,69 @@
         <v>24</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>24</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
         <v>20.0</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
     </row>
     <row r="23">
       <c r="A23" s="2">
@@ -3342,13 +3397,13 @@
         <v>24</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>24</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>24</v>
@@ -3357,10 +3412,10 @@
         <v>24</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24">
@@ -3389,16 +3444,16 @@
         <v>24</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>24</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>24</v>
@@ -3411,10 +3466,10 @@
       <c r="B25" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -3424,7 +3479,7 @@
         <v>24</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>24</v>
@@ -3439,7 +3494,7 @@
         <v>24</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="N25" s="3" t="s">
         <v>24</v>
@@ -3452,14 +3507,14 @@
       <c r="B26" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>69</v>
+      <c r="C26" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>24</v>
@@ -3471,7 +3526,7 @@
         <v>24</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>24</v>
@@ -3480,15 +3535,138 @@
         <v>24</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N26" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2">
+        <v>26.0</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2">
+        <v>27.0</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" s="3" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N26">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N29">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Created Doors - Pending array of positions depending on door part of room leading
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -14,7 +14,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="pys1ZFKMdqV2P+/TUyBltpRCWTBWFC4aC7I6IERgBAE="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="zUxspj3X3zpemYfQ3XD6LlXCv5sLtVszcU2xktVXE7U="/>
     </ext>
   </extLst>
 </workbook>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="194">
   <si>
     <t>N</t>
   </si>
@@ -201,6 +201,9 @@
     <t>int</t>
   </si>
   <si>
+    <t>MAP_EXCHANGE_DOOR</t>
+  </si>
+  <si>
     <t>GAMESTATUS</t>
   </si>
   <si>
@@ -252,6 +255,9 @@
     <t>GameItem.ITEM_NONE</t>
   </si>
   <si>
+    <t>LAST_VARMAP_VAL</t>
+  </si>
+  <si>
     <t>SERVICE_ID</t>
   </si>
   <si>
@@ -381,6 +387,15 @@
     <t>LevelMasterClass.WPRegisterService</t>
   </si>
   <si>
+    <t>DOOR_REGISTER</t>
+  </si>
+  <si>
+    <t>DOOR_REGISTER_DELEGATE</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.DoorRegisterService</t>
+  </si>
+  <si>
     <t>MOVE_PLAYER</t>
   </si>
   <si>
@@ -390,6 +405,15 @@
     <t>PlayerMasterClass.MovePlayerService</t>
   </si>
   <si>
+    <t>PLAYER_WAYPOINT_UPDATE</t>
+  </si>
+  <si>
+    <t>PLAYER_WAYPOINT_UPDATE_DELEGATE</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.PlayerWaypointUpdateService</t>
+  </si>
+  <si>
     <t>SELECT_PLAYER</t>
   </si>
   <si>
@@ -505,6 +529,15 @@
   </si>
   <si>
     <t>GameEventMasterClass.EventSubscriptionService</t>
+  </si>
+  <si>
+    <t>CROSS_DOOR</t>
+  </si>
+  <si>
+    <t>CROSS_DOOR_DELEGATE</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.CrossDoorService</t>
   </si>
   <si>
     <t>LAST_SERVICE</t>
@@ -1423,7 +1456,7 @@
     <col customWidth="1" min="7" max="7" width="8.29"/>
     <col customWidth="1" min="8" max="8" width="3.71"/>
     <col customWidth="1" min="9" max="11" width="12.29"/>
-    <col customWidth="1" min="12" max="12" width="10.71"/>
+    <col customWidth="1" min="12" max="12" width="14.57"/>
     <col customWidth="1" min="13" max="14" width="14.71"/>
     <col customWidth="1" min="15" max="24" width="10.71"/>
   </cols>
@@ -1483,7 +1516,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <f t="shared" ref="A2:A13" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A15" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1781,7 +1814,7 @@
         <v>39</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>39</v>
@@ -1790,7 +1823,7 @@
         <v>39</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>39</v>
@@ -1807,53 +1840,50 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="1">
         <v>0.0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="1">
         <v>0.0</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>37</v>
+      <c r="L8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
@@ -1862,10 +1892,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" s="3">
         <v>0.0</v>
@@ -1874,7 +1904,7 @@
         <v>0.0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>0</v>
@@ -1883,31 +1913,31 @@
         <v>22</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>39</v>
+      <c r="J9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
@@ -1916,10 +1946,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" s="3">
         <v>0.0</v>
@@ -1928,7 +1958,7 @@
         <v>0.0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>0</v>
@@ -1936,23 +1966,23 @@
       <c r="H10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="4" t="s">
-        <v>39</v>
+      <c r="N10" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="O10" s="4" t="s">
         <v>39</v>
@@ -1969,62 +1999,65 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="G11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D12" s="1">
         <v>0.0</v>
@@ -2032,8 +2065,8 @@
       <c r="E12" s="1">
         <v>0.0</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>67</v>
+      <c r="F12" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>0</v>
@@ -2044,23 +2077,23 @@
       <c r="J12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>38</v>
+      <c r="K12" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N12" s="4" t="s">
-        <v>39</v>
+      <c r="N12" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>39</v>
@@ -2072,19 +2105,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E13" s="1">
         <v>0.0</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>70</v>
+      <c r="F13" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>0</v>
@@ -2096,38 +2129,138 @@
         <v>39</v>
       </c>
       <c r="K13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="N13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="L14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="N14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q13" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
+      <c r="Q14" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="I22" s="1"/>
+    </row>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
@@ -3097,15 +3230,16 @@
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D13">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D15">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G13">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G15">
       <formula1>"N,Y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:Q13">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:Q15">
       <formula1>"R,R E,W,W E,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3140,13 +3274,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>22</v>
@@ -3181,17 +3315,17 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <f t="shared" ref="A2:A29" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A32" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>22</v>
@@ -3209,7 +3343,7 @@
         <v>39</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>39</v>
@@ -3230,13 +3364,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
@@ -3246,13 +3380,13 @@
         <v>39</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>39</v>
@@ -3273,13 +3407,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
@@ -3295,7 +3429,7 @@
         <v>39</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -3316,13 +3450,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>22</v>
@@ -3334,7 +3468,7 @@
         <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>39</v>
@@ -3361,13 +3495,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>22</v>
@@ -3385,7 +3519,7 @@
         <v>39</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>39</v>
@@ -3406,41 +3540,41 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
@@ -3449,13 +3583,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>22</v>
@@ -3467,7 +3601,7 @@
         <v>39</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>39</v>
@@ -3494,13 +3628,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>22</v>
@@ -3512,7 +3646,7 @@
         <v>39</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>39</v>
@@ -3539,13 +3673,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>22</v>
@@ -3569,7 +3703,7 @@
         <v>39</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>39</v>
@@ -3584,13 +3718,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>39</v>
@@ -3614,7 +3748,7 @@
         <v>39</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>39</v>
@@ -3626,13 +3760,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>39</v>
@@ -3656,7 +3790,7 @@
         <v>39</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>39</v>
@@ -3668,13 +3802,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>39</v>
@@ -3692,7 +3826,7 @@
         <v>39</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>39</v>
@@ -3710,13 +3844,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>39</v>
@@ -3752,13 +3886,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>39</v>
@@ -3767,7 +3901,7 @@
         <v>39</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>39</v>
@@ -3776,7 +3910,7 @@
         <v>39</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>39</v>
@@ -3794,13 +3928,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>39</v>
@@ -3809,7 +3943,7 @@
         <v>39</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>39</v>
@@ -3836,13 +3970,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
@@ -3854,13 +3988,13 @@
         <v>38</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>39</v>
@@ -3878,13 +4012,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>39</v>
@@ -3893,22 +4027,22 @@
         <v>39</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="L18" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>39</v>
@@ -3920,13 +4054,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>39</v>
@@ -3935,25 +4069,25 @@
         <v>39</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
@@ -3962,13 +4096,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>39</v>
@@ -3977,7 +4111,7 @@
         <v>39</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>39</v>
@@ -3986,16 +4120,16 @@
         <v>39</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21">
@@ -4004,13 +4138,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>39</v>
@@ -4019,7 +4153,7 @@
         <v>39</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
@@ -4028,13 +4162,13 @@
         <v>39</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>38</v>
@@ -4045,53 +4179,42 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="B22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="7" t="s">
+      <c r="C22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="8"/>
-      <c r="X22" s="8"/>
     </row>
     <row r="23">
       <c r="A23" s="1">
@@ -4099,13 +4222,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>39</v>
@@ -4114,7 +4237,7 @@
         <v>39</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>39</v>
@@ -4129,7 +4252,7 @@
         <v>39</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>38</v>
@@ -4140,42 +4263,53 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="B24" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="1" t="s">
+      <c r="C24" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="N24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="1">
@@ -4183,13 +4317,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>39</v>
@@ -4198,25 +4332,25 @@
         <v>39</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="26">
@@ -4225,13 +4359,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>39</v>
@@ -4240,22 +4374,22 @@
         <v>39</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>39</v>
@@ -4267,13 +4401,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>39</v>
@@ -4282,22 +4416,22 @@
         <v>39</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>39</v>
@@ -4309,14 +4443,14 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D28" s="4" t="s">
         <v>155</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>39</v>
       </c>
@@ -4324,25 +4458,25 @@
         <v>39</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
@@ -4351,45 +4485,171 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>89</v>
+        <v>158</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="N29" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N29">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N32">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4443,40 +4703,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="P1" s="11" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(P1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(P1)-COLUMN($P1),3),0))</f>
@@ -4562,82 +4822,82 @@
         <v>1.0</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="U2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="X2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AA2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AD2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AF2" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
@@ -4646,7 +4906,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="C3" s="10">
         <v>1.0</v>
@@ -4655,82 +4915,82 @@
         <v>1.0</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="U3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="X3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AA3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AC3" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AD3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AF3" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4">
@@ -4748,82 +5008,82 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="R4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="U4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="X4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AC4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AD4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE4" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AF4" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5">
@@ -4832,7 +5092,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="C5" s="10">
         <v>0.0</v>
@@ -4841,82 +5101,82 @@
         <v>0.0</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="R5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="U5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="X5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="Z5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AA5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AC5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AD5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE5" s="10" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AF5" s="10" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4954,48 +5214,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="1" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created array of positions depending on door entrance index
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -14,7 +14,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="zUxspj3X3zpemYfQ3XD6LlXCv5sLtVszcU2xktVXE7U="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="WiPYe5nRpAud4gPJlUTZeQbfEbV4jtnb5YWzgQx2CkU="/>
     </ext>
   </extLst>
 </workbook>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="193">
   <si>
     <t>N</t>
   </si>
@@ -174,7 +174,7 @@
     <t>Room</t>
   </si>
   <si>
-    <t>Room.NONE</t>
+    <t>Room.ROOM_NONE</t>
   </si>
   <si>
     <t>EVENTS_OCCURRED</t>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>int</t>
-  </si>
-  <si>
-    <t>MAP_EXCHANGE_DOOR</t>
   </si>
   <si>
     <t>GAMESTATUS</t>
@@ -1516,7 +1513,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <f t="shared" ref="A2:A15" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A14" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1639,7 +1636,7 @@
       <c r="E4" s="3">
         <v>0.0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1840,50 +1837,53 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="3">
         <v>0.0</v>
       </c>
-      <c r="F8" s="1">
+      <c r="E8" s="3">
         <v>0.0</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>39</v>
+      <c r="H8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>39</v>
+      <c r="K8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
@@ -1892,10 +1892,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3">
         <v>0.0</v>
@@ -1904,7 +1904,7 @@
         <v>0.0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>0</v>
@@ -1913,31 +1913,31 @@
         <v>22</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>37</v>
+      <c r="K9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10">
@@ -1946,10 +1946,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D10" s="3">
         <v>0.0</v>
@@ -1958,7 +1958,7 @@
         <v>0.0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>0</v>
@@ -1966,23 +1966,23 @@
       <c r="H10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>36</v>
+      <c r="N10" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="O10" s="4" t="s">
         <v>39</v>
@@ -1999,65 +1999,62 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1">
         <v>0.0</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>0.0</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="I11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="N11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="Q11" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1">
         <v>0.0</v>
@@ -2065,8 +2062,8 @@
       <c r="E12" s="1">
         <v>0.0</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>51</v>
+      <c r="F12" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>0</v>
@@ -2077,23 +2074,23 @@
       <c r="J12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>65</v>
+      <c r="N12" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>39</v>
@@ -2105,19 +2102,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E13" s="1">
         <v>0.0</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>68</v>
+      <c r="F13" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>0</v>
@@ -2129,22 +2126,22 @@
         <v>39</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q13" s="4" t="s">
         <v>39</v>
@@ -2156,111 +2153,61 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E14" s="1">
         <v>0.0</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>71</v>
+      <c r="F14" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q14" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
+    <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="I22" s="1"/>
-    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
@@ -3230,16 +3177,15 @@
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D15">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D14">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G15">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G14">
       <formula1>"N,Y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:Q15">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:Q14">
       <formula1>"R,R E,W,W E,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3274,13 +3220,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>22</v>
@@ -3319,13 +3265,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>22</v>
@@ -3343,7 +3289,7 @@
         <v>39</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>39</v>
@@ -3364,13 +3310,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
@@ -3380,13 +3326,13 @@
         <v>39</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>39</v>
@@ -3407,13 +3353,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
@@ -3429,7 +3375,7 @@
         <v>39</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -3450,13 +3396,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>22</v>
@@ -3468,7 +3414,7 @@
         <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>39</v>
@@ -3495,13 +3441,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>22</v>
@@ -3519,7 +3465,7 @@
         <v>39</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>39</v>
@@ -3540,41 +3486,41 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
@@ -3583,13 +3529,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>22</v>
@@ -3601,7 +3547,7 @@
         <v>39</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>39</v>
@@ -3628,13 +3574,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>22</v>
@@ -3646,7 +3592,7 @@
         <v>39</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>39</v>
@@ -3673,13 +3619,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>22</v>
@@ -3703,7 +3649,7 @@
         <v>39</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>39</v>
@@ -3718,13 +3664,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>39</v>
@@ -3748,7 +3694,7 @@
         <v>39</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>39</v>
@@ -3760,13 +3706,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>39</v>
@@ -3790,7 +3736,7 @@
         <v>39</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>39</v>
@@ -3802,13 +3748,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>39</v>
@@ -3826,7 +3772,7 @@
         <v>39</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>39</v>
@@ -3844,13 +3790,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>39</v>
@@ -3886,13 +3832,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>39</v>
@@ -3928,14 +3874,14 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
@@ -3943,7 +3889,7 @@
         <v>39</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>39</v>
@@ -3970,13 +3916,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
@@ -3994,7 +3940,7 @@
         <v>39</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>39</v>
@@ -4012,14 +3958,14 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="F18" s="1" t="s">
         <v>39</v>
       </c>
@@ -4027,7 +3973,7 @@
         <v>39</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>39</v>
@@ -4054,13 +4000,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>39</v>
@@ -4072,13 +4018,13 @@
         <v>38</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>39</v>
@@ -4096,13 +4042,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>39</v>
@@ -4120,13 +4066,13 @@
         <v>39</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>39</v>
@@ -4138,14 +4084,14 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="F21" s="1" t="s">
         <v>39</v>
       </c>
@@ -4153,7 +4099,7 @@
         <v>39</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
@@ -4162,13 +4108,13 @@
         <v>39</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>38</v>
@@ -4180,14 +4126,14 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="F22" s="1" t="s">
         <v>39</v>
       </c>
@@ -4195,7 +4141,7 @@
         <v>39</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>39</v>
@@ -4204,13 +4150,13 @@
         <v>39</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>38</v>
@@ -4222,14 +4168,14 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="F23" s="1" t="s">
         <v>39</v>
       </c>
@@ -4252,7 +4198,7 @@
         <v>39</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>38</v>
@@ -4264,13 +4210,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="7" t="s">
@@ -4289,7 +4235,7 @@
         <v>39</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L24" s="7" t="s">
         <v>39</v>
@@ -4317,14 +4263,14 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="F25" s="1" t="s">
         <v>39</v>
       </c>
@@ -4332,7 +4278,7 @@
         <v>39</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>39</v>
@@ -4347,7 +4293,7 @@
         <v>39</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>38</v>
@@ -4359,14 +4305,14 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="F26" s="1" t="s">
         <v>39</v>
       </c>
@@ -4374,7 +4320,7 @@
         <v>39</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>39</v>
@@ -4401,13 +4347,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>39</v>
@@ -4431,7 +4377,7 @@
         <v>39</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>39</v>
@@ -4443,14 +4389,14 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="F28" s="1" t="s">
         <v>39</v>
       </c>
@@ -4464,7 +4410,7 @@
         <v>39</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>39</v>
@@ -4485,14 +4431,14 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="F29" s="1" t="s">
         <v>39</v>
       </c>
@@ -4500,16 +4446,16 @@
         <v>39</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>39</v>
@@ -4527,14 +4473,14 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="F30" s="1" t="s">
         <v>39</v>
       </c>
@@ -4542,7 +4488,7 @@
         <v>39</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>39</v>
@@ -4551,13 +4497,13 @@
         <v>39</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>38</v>
@@ -4569,13 +4515,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>39</v>
@@ -4593,7 +4539,7 @@
         <v>39</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>39</v>
@@ -4611,13 +4557,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>38</v>
@@ -4703,40 +4649,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>178</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>179</v>
       </c>
       <c r="P1" s="11" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(P1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(P1)-COLUMN($P1),3),0))</f>
@@ -4822,82 +4768,82 @@
         <v>1.0</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q2" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="T2" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="U2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V2" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="W2" s="10" t="s">
         <v>184</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>185</v>
       </c>
       <c r="X2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="Y2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z2" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="AA2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC2" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="AD2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF2" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="AF2" s="10" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="3">
@@ -4906,7 +4852,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C3" s="10">
         <v>1.0</v>
@@ -4915,82 +4861,82 @@
         <v>1.0</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q3" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="T3" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="U3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="W3" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="X3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z3" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="Z3" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="AA3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC3" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="AC3" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="AD3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF3" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="AF3" s="10" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="4">
@@ -5008,82 +4954,82 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="R4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="T4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="U4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="W4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="X4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="Z4" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="AC4" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="AD4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF4" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="AF4" s="10" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="5">
@@ -5092,7 +5038,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" s="10">
         <v>0.0</v>
@@ -5101,82 +5047,82 @@
         <v>0.0</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="R5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="T5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="U5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="W5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="X5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="Z5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="AA5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="AC5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="AD5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="AF5" s="10" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -5214,48 +5160,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgrade to Unity 6.0.53f1
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -8,14 +8,15 @@
     <sheet state="visible" name="VARMAP" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="SERVICES" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="ITEMS" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="_REF" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="_TODO" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="NPCs" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="_REF" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="_TODO" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="Su4/pITLzZu7AvNXDsCcP1uwZ86qxv+o6aOfiFShYIo="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="/oiLA4/njSRxtTiuIPiq1w4IpK5Lh5MgklcDArEVD4g="/>
     </ext>
   </extLst>
 </workbook>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="214">
   <si>
     <t>N</t>
   </si>
@@ -430,6 +431,15 @@
     <t>LevelMasterClass.GetPlayerListService</t>
   </si>
   <si>
+    <t>GET_NPC_LIST</t>
+  </si>
+  <si>
+    <t>GET_NPC_LIST_DELEGATE</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.GetNPCListService</t>
+  </si>
+  <si>
     <t>GET_NEAREST_WP</t>
   </si>
   <si>
@@ -538,6 +548,15 @@
     <t>LevelMasterClass.CrossDoorService</t>
   </si>
   <si>
+    <t>INTERACT_PLAYER_NPC</t>
+  </si>
+  <si>
+    <t>INTERACT_PLAYER_NPC_DELEGATE</t>
+  </si>
+  <si>
+    <t>NPCMasterClass.InteractPlayerNPCService</t>
+  </si>
+  <si>
     <t>LAST_SERVICE</t>
   </si>
   <si>
@@ -601,6 +620,15 @@
     <t>ITEM_LAST</t>
   </si>
   <si>
+    <t>NPC_ID</t>
+  </si>
+  <si>
+    <t>NPC_FIRST</t>
+  </si>
+  <si>
+    <t>NPC_LAST</t>
+  </si>
+  <si>
     <t>_USE</t>
   </si>
   <si>
@@ -619,19 +647,37 @@
     <t>INTERACTION_TAKE_AND_RECEIVE</t>
   </si>
   <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Prio</t>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>PRIO</t>
   </si>
   <si>
     <t>DONE</t>
   </si>
   <si>
+    <t>ONGOING</t>
+  </si>
+  <si>
     <t>Talk with characters</t>
   </si>
   <si>
+    <t>Plot (1st part)</t>
+  </si>
+  <si>
+    <t>Improve Waypoint Tool (naming)</t>
+  </si>
+  <si>
+    <t>Language files</t>
+  </si>
+  <si>
+    <t>Background objects layers</t>
+  </si>
+  <si>
     <t>Bug with menu of items (not selecting)</t>
+  </si>
+  <si>
+    <t>Loading screen between rooms</t>
   </si>
   <si>
     <t>Last</t>
@@ -780,6 +826,10 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -3297,7 +3347,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <f t="shared" ref="A2:A32" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A19" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -4074,8 +4124,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <v>18.0</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>130</v>
@@ -4102,13 +4151,13 @@
         <v>39</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>39</v>
@@ -4116,7 +4165,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A21:A34" si="2">ROW()-ROW($A$2)</f>
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -4135,7 +4184,7 @@
         <v>39</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
@@ -4153,12 +4202,12 @@
         <v>78</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -4200,7 +4249,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -4219,7 +4268,7 @@
         <v>39</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>39</v>
@@ -4228,10 +4277,10 @@
         <v>39</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>78</v>
@@ -4242,102 +4291,102 @@
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="9" t="s">
+      <c r="F24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M24" s="7" t="s">
+      <c r="N24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="E25" s="8"/>
+      <c r="F25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N25" s="1" t="s">
+      <c r="L25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M25" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="N25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -4365,21 +4414,21 @@
         <v>39</v>
       </c>
       <c r="K26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -4398,22 +4447,22 @@
         <v>39</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="L27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>39</v>
@@ -4421,7 +4470,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -4440,22 +4489,22 @@
         <v>39</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>39</v>
@@ -4463,7 +4512,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -4482,7 +4531,7 @@
         <v>39</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>39</v>
@@ -4491,7 +4540,7 @@
         <v>78</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>39</v>
@@ -4505,16 +4554,16 @@
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="1" t="s">
         <v>162</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -4530,24 +4579,24 @@
         <v>39</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>78</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -4566,7 +4615,7 @@
         <v>39</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>39</v>
@@ -4578,60 +4627,144 @@
         <v>78</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N32" s="1" t="s">
+      <c r="G34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N32">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N34">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4685,40 +4818,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="P1" s="11" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(P1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(P1)-COLUMN($P1),3),0))</f>
@@ -4804,82 +4937,82 @@
         <v>1.0</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="U2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="X2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AA2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AD2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AF2" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3">
@@ -4888,7 +5021,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C3" s="10">
         <v>1.0</v>
@@ -4897,82 +5030,82 @@
         <v>1.0</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="U3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="X3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AA3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AC3" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AD3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AF3" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4">
@@ -4990,82 +5123,82 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="R4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="U4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="X4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AC4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AD4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE4" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AF4" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5">
@@ -5074,7 +5207,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C5" s="10">
         <v>0.0</v>
@@ -5083,82 +5216,82 @@
         <v>0.0</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="R5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="U5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="X5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Y5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="Z5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AA5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AB5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AC5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AD5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="AE5" s="10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AF5" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -5183,6 +5316,48 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FF6AA84F"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10">
+        <f t="shared" ref="A2:A3" si="1">ROW()-ROW($A$2)</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
@@ -5196,48 +5371,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="1" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -5245,7 +5420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF783F04"/>
@@ -5257,24 +5432,27 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="34.0"/>
-    <col customWidth="1" min="2" max="2" width="4.57"/>
+    <col customWidth="1" min="2" max="2" width="5.29"/>
     <col customWidth="1" min="3" max="3" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>195</v>
+        <v>204</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B2" s="1">
         <v>1.0</v>
@@ -5282,31 +5460,110 @@
       <c r="C2" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="B3" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D3" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B4" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D4" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B4">
+  <conditionalFormatting sqref="B2:B9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="1"/>
@@ -5318,7 +5575,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A4">
+  <conditionalFormatting sqref="A2:A9">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$C2=TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
-Reorganization of Services -Pending a method to lock or check if player still there when using item with another player -Also pending review all game structs to put readonly in functions
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -16,7 +16,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="/oiLA4/njSRxtTiuIPiq1w4IpK5Lh5MgklcDArEVD4g="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="YuwGJ/xnf0TwDH/8VMhaZAvsN68002g6692b9FjB8z0="/>
     </ext>
   </extLst>
 </workbook>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="249">
   <si>
     <t>N</t>
   </si>
@@ -266,6 +266,12 @@
     <t>SERVICE_ROUTE</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Separator</t>
+  </si>
+  <si>
     <t>START_GAME</t>
   </si>
   <si>
@@ -275,6 +281,9 @@
     <t>GameMasterClass.StartGameService</t>
   </si>
   <si>
+    <t>Starts game from main menu</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
@@ -287,6 +296,9 @@
     <t>GameMasterClass.SaveGameService</t>
   </si>
   <si>
+    <t>Saves game at any moment</t>
+  </si>
+  <si>
     <t>LOAD_GAME</t>
   </si>
   <si>
@@ -296,6 +308,9 @@
     <t>GameMasterClass.LoadGameService</t>
   </si>
   <si>
+    <t>Loads game from any moment</t>
+  </si>
+  <si>
     <t>LOAD_ROOM</t>
   </si>
   <si>
@@ -305,6 +320,9 @@
     <t>GameMasterClass.LoadRoomService</t>
   </si>
   <si>
+    <t>Loads a room (for example when crossing a door)</t>
+  </si>
+  <si>
     <t>EXIT_GAME</t>
   </si>
   <si>
@@ -314,6 +332,9 @@
     <t>GameMasterClass.ExitGameService</t>
   </si>
   <si>
+    <t>Exits games to OS</t>
+  </si>
+  <si>
     <t>LATE_START_SUBSCRIPTION</t>
   </si>
   <si>
@@ -323,6 +344,9 @@
     <t>GameMasterClass.LateStartSubrsciptionService</t>
   </si>
   <si>
+    <t>This service subscribes for late start. This happens at some moment after Start event. when everything has been setup</t>
+  </si>
+  <si>
     <t>LOADING_COMPLETED</t>
   </si>
   <si>
@@ -332,6 +356,9 @@
     <t>GameMasterClass.LoadingCompletedService</t>
   </si>
   <si>
+    <t>This service is called when whole room has been loaded</t>
+  </si>
+  <si>
     <t>FREEZE_PLAY</t>
   </si>
   <si>
@@ -341,6 +368,9 @@
     <t>GameMasterClass.FreezePlayService</t>
   </si>
   <si>
+    <t>This service is called to pause game or enter cinematic</t>
+  </si>
+  <si>
     <t>NPC_REGISTER</t>
   </si>
   <si>
@@ -350,6 +380,9 @@
     <t>LevelMasterClass.NPCRegisterService</t>
   </si>
   <si>
+    <t>Registers an NPC in system</t>
+  </si>
+  <si>
     <t>ITEM_REGISTER</t>
   </si>
   <si>
@@ -359,13 +392,31 @@
     <t>LevelMasterClass.ItemRegisterService</t>
   </si>
   <si>
-    <t>ITEM_REMOVE_FROM_SCENE</t>
-  </si>
-  <si>
-    <t>ITEM_REMOVE_FROM_SCENE_DELEGATE</t>
-  </si>
-  <si>
-    <t>LevelMasterClass.ItemRemoveFromSceneService</t>
+    <t>Registers an item in system</t>
+  </si>
+  <si>
+    <t>ITEM_OBTAIN_PICKABLE</t>
+  </si>
+  <si>
+    <t>ITEM_OBTAIN_PICKABLE_DELEGATE</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.ItemObtainPickableService</t>
+  </si>
+  <si>
+    <t>Removes an item from level</t>
+  </si>
+  <si>
+    <t>ITEM_OBTAIN_PICKABLE_EVENT</t>
+  </si>
+  <si>
+    <t>ITEM_OBTAIN_PICKABLE_EVENT_DELEGATE</t>
+  </si>
+  <si>
+    <t>GameEventMasterClass.ItemObtainPickableEventService</t>
+  </si>
+  <si>
+    <t>Takes an item from scene (triggering event)</t>
   </si>
   <si>
     <t>MONO_REGISTER</t>
@@ -377,6 +428,9 @@
     <t>LevelMasterClass.MonoRegisterService</t>
   </si>
   <si>
+    <t>Registers a player in scene</t>
+  </si>
+  <si>
     <t>WP_REGISTER</t>
   </si>
   <si>
@@ -386,6 +440,9 @@
     <t>LevelMasterClass.WPRegisterService</t>
   </si>
   <si>
+    <t>Registers a Waypoint in level</t>
+  </si>
+  <si>
     <t>DOOR_REGISTER</t>
   </si>
   <si>
@@ -395,13 +452,7 @@
     <t>LevelMasterClass.DoorRegisterService</t>
   </si>
   <si>
-    <t>MOVE_PLAYER</t>
-  </si>
-  <si>
-    <t>MOVE_PLAYER_DELEGATE</t>
-  </si>
-  <si>
-    <t>PlayerMasterClass.MovePlayerService</t>
+    <t>Registers a door in level</t>
   </si>
   <si>
     <t>PLAYER_WAYPOINT_UPDATE</t>
@@ -413,6 +464,9 @@
     <t>LevelMasterClass.PlayerWaypointUpdateService</t>
   </si>
   <si>
+    <t>Updates actual player waypoint when crossing or stopping on it</t>
+  </si>
+  <si>
     <t>SELECT_PLAYER</t>
   </si>
   <si>
@@ -422,6 +476,9 @@
     <t>PlayerMasterClass.SelectPlayerService</t>
   </si>
   <si>
+    <t>Selects player</t>
+  </si>
+  <si>
     <t>GET_PLAYER_LIST</t>
   </si>
   <si>
@@ -431,6 +488,9 @@
     <t>LevelMasterClass.GetPlayerListService</t>
   </si>
   <si>
+    <t>Gets a list of actual players</t>
+  </si>
+  <si>
     <t>GET_NPC_LIST</t>
   </si>
   <si>
@@ -440,6 +500,9 @@
     <t>LevelMasterClass.GetNPCListService</t>
   </si>
   <si>
+    <t xml:space="preserve">Gets a list of actual NPCs </t>
+  </si>
+  <si>
     <t>GET_NEAREST_WP</t>
   </si>
   <si>
@@ -449,6 +512,9 @@
     <t>LevelMasterClass.GetNearestWPService</t>
   </si>
   <si>
+    <t>Gets nearest WP from a given coordinates of level</t>
+  </si>
+  <si>
     <t>IS_EVENT_OCCURRED</t>
   </si>
   <si>
@@ -458,6 +524,9 @@
     <t>GameEventMasterClass.IsEventOccurredService</t>
   </si>
   <si>
+    <t>Tells if an event is occurred</t>
+  </si>
+  <si>
     <t>COMMIT_EVENT</t>
   </si>
   <si>
@@ -467,13 +536,7 @@
     <t>GameEventMasterClass.CommitEventService</t>
   </si>
   <si>
-    <t>TAKE_ITEM_FROM_SCENE_EVENT</t>
-  </si>
-  <si>
-    <t>TAKE_ITEM_FROM_SCENE_EVENT_DELEGATE</t>
-  </si>
-  <si>
-    <t>GameEventMasterClass.TakeItemFromSceneEventService</t>
+    <t>Activates/Deactivates an event</t>
   </si>
   <si>
     <t>USE_ITEM</t>
@@ -485,6 +548,9 @@
     <t>ItemMasterClass.UseItemService</t>
   </si>
   <si>
+    <t>Uses an item with something</t>
+  </si>
+  <si>
     <t>IS_ITEM_TAKEN_FROM_SCENE</t>
   </si>
   <si>
@@ -494,13 +560,19 @@
     <t>GameEventMasterClass.IsItemTakenFromSceneService</t>
   </si>
   <si>
-    <t>INTERACT_PLAYER_ITEM</t>
-  </si>
-  <si>
-    <t>INTERACT_PLAYER_ITEM_DELEGATE</t>
-  </si>
-  <si>
-    <t>PlayerMasterClass.InteractPlayerItemService</t>
+    <t>Tells if item is taken from scene</t>
+  </si>
+  <si>
+    <t>INTERACT_PLAYER</t>
+  </si>
+  <si>
+    <t>INTERACT_PLAYER_DELEGATE</t>
+  </si>
+  <si>
+    <t>PlayerMasterClass.InteractPlayerService</t>
+  </si>
+  <si>
+    <t>Interacts player with an item</t>
   </si>
   <si>
     <t>GET_SCENARIO_ITEM_LIST</t>
@@ -512,6 +584,9 @@
     <t>LevelMasterClass.GetScenarioItemListService</t>
   </si>
   <si>
+    <t>Gets scenario item list</t>
+  </si>
+  <si>
     <t>SELECT_PICKABLE_ITEM</t>
   </si>
   <si>
@@ -521,6 +596,9 @@
     <t>ItemMasterClass.SelectPickableItemService</t>
   </si>
   <si>
+    <t>Selects some pickable from inventory</t>
+  </si>
+  <si>
     <t>CANCEL_PICKABLE_ITEM</t>
   </si>
   <si>
@@ -530,6 +608,9 @@
     <t>ItemMasterClass.CancelPickableItemService</t>
   </si>
   <si>
+    <t>Cancels selected item</t>
+  </si>
+  <si>
     <t>EVENT_SUBSCRIPTION</t>
   </si>
   <si>
@@ -539,6 +620,9 @@
     <t>GameEventMasterClass.EventSubscriptionService</t>
   </si>
   <si>
+    <t>Subscribe to an event. Invoke when event changes</t>
+  </si>
+  <si>
     <t>CROSS_DOOR</t>
   </si>
   <si>
@@ -548,6 +632,9 @@
     <t>LevelMasterClass.CrossDoorService</t>
   </si>
   <si>
+    <t>Trigger actions when crossing a door</t>
+  </si>
+  <si>
     <t>INTERACT_PLAYER_NPC</t>
   </si>
   <si>
@@ -557,7 +644,25 @@
     <t>NPCMasterClass.InteractPlayerNPCService</t>
   </si>
   <si>
+    <t>Interacts player with NPC</t>
+  </si>
+  <si>
+    <t>LOCK_PLAYER</t>
+  </si>
+  <si>
+    <t>LOCK_PLAYER_DELEGATE</t>
+  </si>
+  <si>
+    <t>PlayerMasterClass.LockPlayerService</t>
+  </si>
+  <si>
+    <t>Locks player so it cannot act until an action over it has been done (or removes lock)</t>
+  </si>
+  <si>
     <t>LAST_SERVICE</t>
+  </si>
+  <si>
+    <t>Last service</t>
   </si>
   <si>
     <t>ITEM_ID</t>
@@ -729,8 +834,176 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF356854"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF284E3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF356854"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF356854"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF284E3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF356854"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF284E3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF6F8F9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF6F8F9"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF6F8F9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF6F8F9"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF6F8F9"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -749,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -767,24 +1040,154 @@
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="13" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF356854"/>
+          <bgColor rgb="FF356854"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6F8F9"/>
+          <bgColor rgb="FFF6F8F9"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -798,6 +1201,13 @@
       <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="1">
+    <tableStyle count="3" pivot="0" name="SERVICES-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -831,6 +1241,29 @@
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O34" displayName="Table_Services" name="Table_Services" id="1">
+  <tableColumns count="15">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="SERVICE_ID" id="2"/>
+    <tableColumn name="SPECIAL_DELEGATE" id="3"/>
+    <tableColumn name="SERVICE_ROUTE" id="4"/>
+    <tableColumn name="Description" id="5"/>
+    <tableColumn name="Separator" id="6"/>
+    <tableColumn name="GameMaster" id="7"/>
+    <tableColumn name="InputMaster" id="8"/>
+    <tableColumn name="LevelMaster" id="9"/>
+    <tableColumn name="GraphicsMaster" id="10"/>
+    <tableColumn name="GameMenu" id="11"/>
+    <tableColumn name="PlayerMaster" id="12"/>
+    <tableColumn name="NPCMaster" id="13"/>
+    <tableColumn name="ItemMaster" id="14"/>
+    <tableColumn name="GameEventMaster" id="15"/>
+  </tableColumns>
+  <tableStyleInfo name="SERVICES-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3290,1485 +3723,1607 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
+    <col customWidth="1" min="1" max="1" width="11.29"/>
     <col customWidth="1" min="2" max="2" width="30.14"/>
-    <col customWidth="1" min="3" max="3" width="39.86"/>
+    <col customWidth="1" min="3" max="3" width="41.0"/>
     <col customWidth="1" min="4" max="4" width="49.57"/>
-    <col customWidth="1" min="5" max="5" width="4.86"/>
+    <col customWidth="1" min="5" max="5" width="8.86"/>
+    <col customWidth="1" min="6" max="6" width="5.29"/>
+    <col customWidth="1" min="7" max="7" width="21.14"/>
+    <col customWidth="1" min="8" max="8" width="20.57"/>
+    <col customWidth="1" min="9" max="9" width="20.43"/>
+    <col customWidth="1" min="10" max="10" width="23.43"/>
+    <col customWidth="1" min="11" max="11" width="20.14"/>
+    <col customWidth="1" min="12" max="12" width="21.29"/>
+    <col customWidth="1" min="13" max="13" width="19.57"/>
+    <col customWidth="1" min="14" max="14" width="20.0"/>
+    <col customWidth="1" min="15" max="15" width="25.86"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11">
+        <f t="shared" ref="A2:A34" si="1">ROW()-ROW($A$2)</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="17">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="17">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="17">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="17">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O13" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="17">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="O16" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="17">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="N20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="17">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M21" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="N21" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O21" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="M22" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="N22" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="17">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M23" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="N23" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O23" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="11">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24" s="31"/>
+      <c r="G24" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="N24" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="O24" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
+      <c r="X24" s="35"/>
+      <c r="Y24" s="35"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="17">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="B25" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="M25" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N25" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O25" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="11">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="B26" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M26" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="17">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="B27" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N27" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O27" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="11">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="B28" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="L28" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M28" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="O28" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="17">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="B29" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K29" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="L29" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="O29" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="11">
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="B30" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J30" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K30" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L30" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="N30" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="O30" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="17">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="B31" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M31" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N31" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="O31" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="11">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="B32" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L32" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="M32" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="N32" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="O32" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="17">
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <f t="shared" ref="A2:A19" si="1">ROW()-ROW($A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="B33" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="G33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
+      <c r="M33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="O33" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="36">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G34" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1">
-        <f t="shared" ref="A21:A34" si="2">ROW()-ROW($A$2)</f>
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="1">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N34" s="1" t="s">
+      <c r="H34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="M34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="O34" s="40" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:N34">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A34">
+      <formula1>AND(ISNUMBER(A2),(NOT(OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D")))))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:O34">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4814,484 +5369,484 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="P1" s="11" t="str">
+      <c r="B1" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="J1" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="K1" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="L1" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="M1" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="P1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(P1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(P1)-COLUMN($P1),3),0))</f>
         <v>ITEM_POTION_USE</v>
       </c>
-      <c r="Q1" s="11" t="str">
+      <c r="Q1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(Q1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(Q1)-COLUMN($P1),3),0))</f>
         <v>ITEM_POTION_ANIM</v>
       </c>
-      <c r="R1" s="11" t="str">
+      <c r="R1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(R1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(R1)-COLUMN($P1),3),0))</f>
         <v>ITEM_POTION_EVENT</v>
       </c>
-      <c r="S1" s="11" t="str">
+      <c r="S1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(S1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(S1)-COLUMN($P1),3),0))</f>
         <v>ITEM_POTION_BLUE_USE</v>
       </c>
-      <c r="T1" s="11" t="str">
+      <c r="T1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(T1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(T1)-COLUMN($P1),3),0))</f>
         <v>ITEM_POTION_BLUE_ANIM</v>
       </c>
-      <c r="U1" s="11" t="str">
+      <c r="U1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(U1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(U1)-COLUMN($P1),3),0))</f>
         <v>ITEM_POTION_BLUE_EVENT</v>
       </c>
-      <c r="V1" s="11" t="str">
+      <c r="V1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(V1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(V1)-COLUMN($P1),3),0))</f>
         <v>ITEM_FOUNTAIN_USE</v>
       </c>
-      <c r="W1" s="11" t="str">
+      <c r="W1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(W1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(W1)-COLUMN($P1),3),0))</f>
         <v>ITEM_FOUNTAIN_ANIM</v>
       </c>
-      <c r="X1" s="11" t="str">
+      <c r="X1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(X1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(X1)-COLUMN($P1),3),0))</f>
         <v>ITEM_FOUNTAIN_EVENT</v>
       </c>
-      <c r="Y1" s="11" t="str">
+      <c r="Y1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(Y1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(Y1)-COLUMN($P1),3),0))</f>
         <v>ITEM_LAST_USE</v>
       </c>
-      <c r="Z1" s="11" t="str">
+      <c r="Z1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(Z1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(Z1)-COLUMN($P1),3),0))</f>
         <v>ITEM_LAST_ANIM</v>
       </c>
-      <c r="AA1" s="11" t="str">
+      <c r="AA1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(AA1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(AA1)-COLUMN($P1),3),0))</f>
         <v>ITEM_LAST_EVENT</v>
       </c>
-      <c r="AB1" s="11" t="str">
+      <c r="AB1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(AB1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(AB1)-COLUMN($P1),3),0))</f>
         <v>_USE</v>
       </c>
-      <c r="AC1" s="11" t="str">
+      <c r="AC1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(AC1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(AC1)-COLUMN($P1),3),0))</f>
         <v>_ANIM</v>
       </c>
-      <c r="AD1" s="11" t="str">
+      <c r="AD1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(AD1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(AD1)-COLUMN($P1),3),0))</f>
         <v>_EVENT</v>
       </c>
-      <c r="AE1" s="11" t="str">
+      <c r="AE1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(AE1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(AE1)-COLUMN($P1),3),0))</f>
         <v>_USE</v>
       </c>
-      <c r="AF1" s="11" t="str">
+      <c r="AF1" s="42" t="str">
         <f>CONCAT(OFFSET($B$2,_xlfn.FLOOR.MATH((COLUMN(AF1)-COLUMN($P1))/3,1),0),OFFSET('_REF'!$A$1,MOD(COLUMN(AF1)-COLUMN($P1),3),0))</f>
         <v>_ANIM</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10">
+      <c r="A2" s="41">
         <f t="shared" ref="A2:A5" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="41">
         <v>1.0</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="41">
         <v>1.0</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="K2" s="10" t="s">
+      <c r="I2" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="K2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="N2" s="10" t="s">
+      <c r="L2" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="N2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="R2" s="10" t="s">
+      <c r="P2" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q2" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="R2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="U2" s="10" t="s">
+      <c r="S2" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="T2" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="U2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="X2" s="10" t="s">
+      <c r="V2" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="W2" s="41" t="s">
+        <v>225</v>
+      </c>
+      <c r="X2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA2" s="10" t="s">
+      <c r="Y2" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z2" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AD2" s="10" t="s">
+      <c r="AB2" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC2" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="AF2" s="10" t="s">
-        <v>188</v>
+      <c r="AE2" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF2" s="41" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10">
+      <c r="A3" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="B3" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="41">
         <v>1.0</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="41">
         <v>1.0</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="F3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="H3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="K3" s="10" t="s">
+      <c r="I3" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="K3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="N3" s="10" t="s">
+      <c r="L3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="M3" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="N3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="R3" s="10" t="s">
+      <c r="P3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q3" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="R3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="U3" s="10" t="s">
+      <c r="S3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="T3" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="U3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="X3" s="10" t="s">
+      <c r="V3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="W3" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="X3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="Z3" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA3" s="10" t="s">
+      <c r="Y3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z3" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AB3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="AC3" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AD3" s="10" t="s">
+      <c r="AB3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC3" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AE3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="AF3" s="10" t="s">
-        <v>188</v>
+      <c r="AE3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF3" s="41" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="41">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="41">
         <v>0.0</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="41">
         <v>0.0</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="H4" s="10" t="s">
+      <c r="F4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="K4" s="10" t="s">
+      <c r="I4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="K4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="N4" s="10" t="s">
+      <c r="L4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="M4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="N4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="R4" s="10" t="s">
+      <c r="P4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="R4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="U4" s="10" t="s">
+      <c r="S4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="T4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="U4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="X4" s="10" t="s">
+      <c r="V4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="W4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="X4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="Z4" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA4" s="10" t="s">
+      <c r="Y4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AB4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="AC4" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AD4" s="10" t="s">
+      <c r="AB4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AE4" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="AF4" s="10" t="s">
-        <v>188</v>
+      <c r="AE4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF4" s="41" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10">
+      <c r="A5" s="41">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="B5" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="41">
         <v>0.0</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="41">
         <v>0.0</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="H5" s="10" t="s">
+      <c r="F5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="K5" s="10" t="s">
+      <c r="I5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="K5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="N5" s="10" t="s">
+      <c r="L5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="M5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="N5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="R5" s="10" t="s">
+      <c r="P5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="R5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="U5" s="10" t="s">
+      <c r="S5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="T5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="U5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="V5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="X5" s="10" t="s">
+      <c r="V5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="W5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="X5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="Y5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="Z5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA5" s="10" t="s">
+      <c r="Y5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="AC5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AD5" s="10" t="s">
+      <c r="AB5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AE5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="AF5" s="10" t="s">
-        <v>188</v>
+      <c r="AE5" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF5" s="41" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -5325,29 +5880,29 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>193</v>
+      <c r="B1" s="41" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10">
+      <c r="A2" s="41">
         <f t="shared" ref="A2:A3" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>194</v>
+      <c r="B2" s="41" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10">
+      <c r="A3" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>195</v>
+      <c r="B3" s="41" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -5371,48 +5926,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>231</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>188</v>
+        <v>223</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>197</v>
+        <v>232</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>190</v>
+        <v>225</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>189</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>200</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="1" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -5438,21 +5993,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>238</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>239</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>241</v>
       </c>
       <c r="B2" s="1">
         <v>1.0</v>
@@ -5466,7 +6021,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>242</v>
       </c>
       <c r="B3" s="1">
         <v>1.0</v>
@@ -5480,7 +6035,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>208</v>
+        <v>243</v>
       </c>
       <c r="B4" s="1">
         <v>3.0</v>
@@ -5494,7 +6049,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="B5" s="1">
         <v>1.0</v>
@@ -5508,7 +6063,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="B6" s="1">
         <v>3.0</v>
@@ -5522,7 +6077,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
       <c r="B7" s="1">
         <v>3.0</v>
@@ -5536,7 +6091,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="B8" s="1">
         <v>4.0</v>
@@ -5550,7 +6105,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>248</v>
       </c>
       <c r="B9" s="1">
         <v>5.0</v>
@@ -5576,7 +6131,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A9">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$C2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[Partial] Direct info of services
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -6622,23 +6622,23 @@
     </row>
   </sheetData>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="I2:I6 O2:O6">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="J2:J6 P2:P6">
+      <formula1>#REF!</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H6">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="P2:P6">
-      <formula1>Table_Item_Conditions[ITEM_COND_ID]</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="O2:O6">
-      <formula1>Table_Items[ITEM_ID]</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="K2:K6 Q2:Q6">
+      <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M2:M6">
       <formula1>Table_Characters[Type]</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N2:N6">
       <formula1>'_REF'!$B$2:$B$6</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I2:K6 Q2:Q6">
-      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Usage of shadow values to let events increment and not overwrite events in same cycles
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -20,7 +20,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="y36D/GbfhgY+X7cfY1itUoQRr3DIByplvZef/Qhatf8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="zXWrutDY46wAzOxsLNDNzItt4A5Qr5fb78IlINitF5k="/>
     </ext>
   </extLst>
 </workbook>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="282">
   <si>
     <t>N</t>
   </si>
@@ -895,6 +895,9 @@
   </si>
   <si>
     <t>Seealso in services. Add owner in descr</t>
+  </si>
+  <si>
+    <t>Avoid services modifying VARMAP</t>
   </si>
   <si>
     <t>Last</t>
@@ -945,7 +948,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border/>
     <border>
       <left style="thin">
@@ -1299,6 +1302,20 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB7E1CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB7E1CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB7E1CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF57BB8A"/>
       </left>
       <right style="thin">
@@ -1367,9 +1384,6 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="10" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1579,6 +1593,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="26" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="27" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1779,7 +1796,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D13" displayName="Table_TODO" name="Table_TODO" id="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D14" displayName="Table_TODO" name="Table_TODO" id="11">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -2401,7 +2418,7 @@
       <c r="P5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2419,9 +2436,9 @@
       <c r="D6" s="8">
         <v>2.0</v>
       </c>
-      <c r="E6" s="18">
-        <f>COUNT(ITEMS!A:A)-COUNT(ITEMS!A1)</f>
-        <v>5</v>
+      <c r="E6" s="17">
+        <f>COUNT(Table_Items[N])-2</f>
+        <v>3</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>37</v>
@@ -2472,388 +2489,388 @@
       <c r="D7" s="13">
         <v>2.0</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
+        <f>COUNT(Table_Characters[N])</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="16">
+        <v>-1.0</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="10">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="17">
         <f>Table_Constants[NUM_PLAYERS]</f>
         <v>3</v>
       </c>
-      <c r="F7" s="16">
-        <v>-1.0</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="P7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="10">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q9" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="10">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="O11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="5">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="10">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="P13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q13" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="5">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E14" s="18">
-        <f>Table_Constants[NUM_PLAYERS]</f>
-        <v>3</v>
-      </c>
       <c r="F14" s="15" t="s">
         <v>28</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="21"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="8" t="s">
         <v>25</v>
       </c>
@@ -2883,54 +2900,54 @@
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="22">
+      <c r="A15" s="21">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <v>0.0</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="22">
         <v>0.0</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="24" t="s">
+      <c r="H15" s="25"/>
+      <c r="I15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="N15" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="O15" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q15" s="27" t="s">
+      <c r="J15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="26" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2941,7 +2958,7 @@
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="I22" s="28"/>
+      <c r="I22" s="27"/>
     </row>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -3954,55 +3971,55 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="78" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="78" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="79" t="s">
         <v>258</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="79" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="80" t="s">
         <v>259</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="80" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="79" t="s">
         <v>231</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="79" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="80" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="80" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="79" t="s">
         <v>235</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="81" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="82" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4030,364 +4047,364 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="28">
+      <c r="A2" s="27">
         <f t="shared" ref="A2:A32" si="1">ROW()-ROW($G$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="84" t="str">
+      <c r="B2" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A2,0)</f>
         <v>ITEM_POTION</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="28">
+      <c r="A3" s="27">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="str">
+      <c r="B3" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A3,0)</f>
         <v>ITEM_POTION_BLUE</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="28">
+      <c r="A4" s="27">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="84" t="str">
+      <c r="B4" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A4,0)</f>
         <v>ITEM_FOUNTAIN</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="28">
+      <c r="A5" s="27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="84" t="str">
+      <c r="B5" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A5,0)</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="28">
+      <c r="A6" s="27">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="84" t="str">
+      <c r="B6" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A6,0)</f>
         <v/>
       </c>
-      <c r="C6" s="84"/>
+      <c r="C6" s="83"/>
     </row>
     <row r="7">
-      <c r="A7" s="28">
+      <c r="A7" s="27">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="84" t="str">
+      <c r="B7" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A7,0)</f>
         <v/>
       </c>
-      <c r="C7" s="84"/>
+      <c r="C7" s="83"/>
     </row>
     <row r="8">
-      <c r="A8" s="28">
+      <c r="A8" s="27">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="84" t="str">
+      <c r="B8" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A8,0)</f>
         <v/>
       </c>
-      <c r="C8" s="84"/>
+      <c r="C8" s="83"/>
     </row>
     <row r="9">
-      <c r="A9" s="28">
+      <c r="A9" s="27">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="84" t="str">
+      <c r="B9" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A9,0)</f>
         <v/>
       </c>
-      <c r="C9" s="84"/>
+      <c r="C9" s="83"/>
     </row>
     <row r="10">
-      <c r="A10" s="28">
+      <c r="A10" s="27">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="84" t="str">
+      <c r="B10" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A10,0)</f>
         <v/>
       </c>
-      <c r="C10" s="84"/>
+      <c r="C10" s="83"/>
     </row>
     <row r="11">
-      <c r="A11" s="28">
+      <c r="A11" s="27">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="84" t="str">
+      <c r="B11" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A11,0)</f>
         <v/>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="83"/>
     </row>
     <row r="12">
-      <c r="A12" s="28">
+      <c r="A12" s="27">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="84" t="str">
+      <c r="B12" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A12,0)</f>
         <v/>
       </c>
-      <c r="C12" s="84"/>
+      <c r="C12" s="83"/>
     </row>
     <row r="13">
-      <c r="A13" s="28">
+      <c r="A13" s="27">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="84" t="str">
+      <c r="B13" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A13,0)</f>
         <v/>
       </c>
-      <c r="C13" s="84"/>
+      <c r="C13" s="83"/>
     </row>
     <row r="14">
-      <c r="A14" s="28">
+      <c r="A14" s="27">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="84" t="str">
+      <c r="B14" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A14,0)</f>
         <v/>
       </c>
-      <c r="C14" s="84"/>
+      <c r="C14" s="83"/>
     </row>
     <row r="15">
-      <c r="A15" s="28">
+      <c r="A15" s="27">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="84" t="str">
+      <c r="B15" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A15,0)</f>
         <v/>
       </c>
-      <c r="C15" s="84"/>
+      <c r="C15" s="83"/>
     </row>
     <row r="16">
-      <c r="A16" s="28">
+      <c r="A16" s="27">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="84" t="str">
+      <c r="B16" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A16,0)</f>
         <v/>
       </c>
-      <c r="C16" s="84"/>
+      <c r="C16" s="83"/>
     </row>
     <row r="17">
-      <c r="A17" s="28">
+      <c r="A17" s="27">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="84" t="str">
+      <c r="B17" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A17,0)</f>
         <v/>
       </c>
-      <c r="C17" s="84"/>
+      <c r="C17" s="83"/>
     </row>
     <row r="18">
-      <c r="A18" s="28">
+      <c r="A18" s="27">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="84" t="str">
+      <c r="B18" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A18,0)</f>
         <v/>
       </c>
-      <c r="C18" s="84"/>
+      <c r="C18" s="83"/>
     </row>
     <row r="19">
-      <c r="A19" s="28">
+      <c r="A19" s="27">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="84" t="str">
+      <c r="B19" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A19,0)</f>
         <v/>
       </c>
-      <c r="C19" s="84"/>
+      <c r="C19" s="83"/>
     </row>
     <row r="20">
-      <c r="A20" s="28">
+      <c r="A20" s="27">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="84" t="str">
+      <c r="B20" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A20,0)</f>
         <v/>
       </c>
-      <c r="C20" s="84"/>
+      <c r="C20" s="83"/>
     </row>
     <row r="21">
-      <c r="A21" s="28">
+      <c r="A21" s="27">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="84" t="str">
+      <c r="B21" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A21,0)</f>
         <v/>
       </c>
-      <c r="C21" s="84"/>
+      <c r="C21" s="83"/>
     </row>
     <row r="22">
-      <c r="A22" s="28">
+      <c r="A22" s="27">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="84" t="str">
+      <c r="B22" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A22,0)</f>
         <v/>
       </c>
-      <c r="C22" s="84"/>
+      <c r="C22" s="83"/>
     </row>
     <row r="23">
-      <c r="A23" s="28">
+      <c r="A23" s="27">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="84" t="str">
+      <c r="B23" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A23,0)</f>
         <v/>
       </c>
-      <c r="C23" s="84"/>
+      <c r="C23" s="83"/>
     </row>
     <row r="24">
-      <c r="A24" s="28">
+      <c r="A24" s="27">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="84" t="str">
+      <c r="B24" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A24,0)</f>
         <v/>
       </c>
-      <c r="C24" s="84"/>
+      <c r="C24" s="83"/>
     </row>
     <row r="25">
-      <c r="A25" s="28">
+      <c r="A25" s="27">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="84" t="str">
+      <c r="B25" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A25,0)</f>
         <v/>
       </c>
-      <c r="C25" s="84"/>
+      <c r="C25" s="83"/>
     </row>
     <row r="26">
-      <c r="A26" s="28">
+      <c r="A26" s="27">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="84" t="str">
+      <c r="B26" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A26,0)</f>
         <v/>
       </c>
-      <c r="C26" s="84"/>
+      <c r="C26" s="83"/>
     </row>
     <row r="27">
-      <c r="A27" s="28">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="B27" s="84" t="str">
+      <c r="A27" s="27">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A27,0)</f>
         <v/>
       </c>
-      <c r="C27" s="84"/>
+      <c r="C27" s="83"/>
     </row>
     <row r="28">
-      <c r="A28" s="28">
+      <c r="A28" s="27">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="84" t="str">
+      <c r="B28" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A28,0)</f>
         <v/>
       </c>
-      <c r="C28" s="84"/>
+      <c r="C28" s="83"/>
     </row>
     <row r="29">
-      <c r="A29" s="28">
+      <c r="A29" s="27">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="84" t="str">
+      <c r="B29" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A29,0)</f>
         <v/>
       </c>
-      <c r="C29" s="84"/>
+      <c r="C29" s="83"/>
     </row>
     <row r="30">
-      <c r="A30" s="28">
+      <c r="A30" s="27">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="84" t="str">
+      <c r="B30" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A30,0)</f>
         <v/>
       </c>
-      <c r="C30" s="84"/>
+      <c r="C30" s="83"/>
     </row>
     <row r="31">
-      <c r="A31" s="28">
+      <c r="A31" s="27">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="84" t="str">
+      <c r="B31" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A31,0)</f>
         <v/>
       </c>
-      <c r="C31" s="84"/>
+      <c r="C31" s="83"/>
     </row>
     <row r="32">
-      <c r="A32" s="28">
+      <c r="A32" s="27">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="84" t="str">
+      <c r="B32" s="83" t="str">
         <f>OFFSET(ITEMS!$B$3,A32,0)</f>
         <v/>
       </c>
-      <c r="C32" s="84"/>
+      <c r="C32" s="83"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -4413,195 +4430,209 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="38.57"/>
-    <col customWidth="1" min="2" max="2" width="5.29"/>
+    <col customWidth="1" min="2" max="2" width="9.43"/>
     <col customWidth="1" min="3" max="3" width="11.71"/>
     <col customWidth="1" min="4" max="4" width="15.57"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>265</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="52" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>269</v>
       </c>
-      <c r="B2" s="85">
+      <c r="B2" s="84">
         <v>1.0</v>
       </c>
-      <c r="C2" s="55" t="b">
+      <c r="C2" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="66" t="b">
+      <c r="D2" s="65" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>270</v>
       </c>
-      <c r="B3" s="85">
+      <c r="B3" s="84">
         <v>1.0</v>
       </c>
-      <c r="C3" s="59" t="b">
+      <c r="C3" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="69" t="b">
+      <c r="D3" s="68" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="B4" s="86">
+      <c r="B4" s="85">
         <v>3.0</v>
       </c>
-      <c r="C4" s="55" t="b">
+      <c r="C4" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="66" t="b">
+      <c r="D4" s="65" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="57" t="s">
         <v>272</v>
       </c>
-      <c r="B5" s="85">
+      <c r="B5" s="84">
         <v>1.0</v>
       </c>
-      <c r="C5" s="59" t="b">
+      <c r="C5" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="69" t="b">
+      <c r="D5" s="68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="53" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="86">
+      <c r="B6" s="85">
         <v>3.0</v>
       </c>
-      <c r="C6" s="55" t="b">
+      <c r="C6" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="66" t="b">
+      <c r="D6" s="65" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="86">
+      <c r="B7" s="85">
         <v>3.0</v>
       </c>
-      <c r="C7" s="59" t="b">
+      <c r="C7" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="69" t="b">
+      <c r="D7" s="68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="87">
+      <c r="B8" s="86">
         <v>4.0</v>
       </c>
-      <c r="C8" s="55" t="b">
+      <c r="C8" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="66" t="b">
+      <c r="D8" s="65" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="87">
+      <c r="B9" s="86">
         <v>4.0</v>
       </c>
-      <c r="C9" s="59" t="b">
+      <c r="C9" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="69" t="b">
+      <c r="D9" s="68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="53" t="s">
         <v>277</v>
       </c>
-      <c r="B10" s="87">
+      <c r="B10" s="86">
         <v>4.0</v>
       </c>
-      <c r="C10" s="55" t="b">
+      <c r="C10" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="66" t="b">
+      <c r="D10" s="65" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="57" t="s">
         <v>278</v>
       </c>
-      <c r="B11" s="85">
+      <c r="B11" s="84">
         <v>1.0</v>
       </c>
-      <c r="C11" s="59" t="b">
+      <c r="C11" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="69" t="b">
+      <c r="D11" s="68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="87" t="s">
         <v>279</v>
       </c>
-      <c r="B12" s="87">
+      <c r="B12" s="86">
         <v>4.0</v>
       </c>
-      <c r="C12" s="55" t="b">
+      <c r="C12" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="57" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" s="84">
+        <v>1.0</v>
+      </c>
+      <c r="C13" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D12" s="66" t="b">
+      <c r="D13" s="68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="69" t="s">
+        <v>281</v>
+      </c>
+      <c r="B14" s="88">
+        <v>5.0</v>
+      </c>
+      <c r="C14" s="75" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="62" t="s">
-        <v>280</v>
-      </c>
-      <c r="B13" s="88">
-        <v>5.0</v>
-      </c>
-      <c r="C13" s="63" t="b">
+      <c r="D14" s="70" t="b">
         <v>0</v>
       </c>
-      <c r="D13" s="67" t="b">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B13">
+  <conditionalFormatting sqref="B2:B14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="1"/>
@@ -4613,13 +4644,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A13">
+  <conditionalFormatting sqref="A2:A14">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>$C2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B13">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B14">
       <formula1>AND(ISNUMBER(B2),(NOT(OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -4662,7 +4693,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4709,7 +4740,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="30">
+      <c r="A2" s="29">
         <f t="shared" ref="A2:A34" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
@@ -4757,7 +4788,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="31">
+      <c r="A3" s="30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4803,7 +4834,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="30">
+      <c r="A4" s="29">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -4849,7 +4880,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="31">
+      <c r="A5" s="30">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -4897,7 +4928,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="30">
+      <c r="A6" s="29">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -4945,7 +4976,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="31">
+      <c r="A7" s="30">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -4991,7 +5022,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="30">
+      <c r="A8" s="29">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -5039,7 +5070,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="31">
+      <c r="A9" s="30">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -5087,7 +5118,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="30">
+      <c r="A10" s="29">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -5135,7 +5166,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="31">
+      <c r="A11" s="30">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -5151,7 +5182,7 @@
       <c r="E11" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="13" t="s">
         <v>25</v>
       </c>
@@ -5181,7 +5212,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="30">
+      <c r="A12" s="29">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -5197,7 +5228,7 @@
       <c r="E12" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="8" t="s">
         <v>25</v>
       </c>
@@ -5227,7 +5258,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="31">
+      <c r="A13" s="30">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -5243,7 +5274,7 @@
       <c r="E13" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="F13" s="19"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="13" t="s">
         <v>25</v>
       </c>
@@ -5273,7 +5304,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="30">
+      <c r="A14" s="29">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -5289,7 +5320,7 @@
       <c r="E14" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="8" t="s">
         <v>25</v>
       </c>
@@ -5319,7 +5350,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="31">
+      <c r="A15" s="30">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -5335,7 +5366,7 @@
       <c r="E15" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="19"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="13" t="s">
         <v>25</v>
       </c>
@@ -5365,7 +5396,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="30">
+      <c r="A16" s="29">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
@@ -5381,7 +5412,7 @@
       <c r="E16" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="21"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="8" t="s">
         <v>25</v>
       </c>
@@ -5411,7 +5442,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="31">
+      <c r="A17" s="30">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
@@ -5427,7 +5458,7 @@
       <c r="E17" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="13" t="s">
         <v>25</v>
       </c>
@@ -5457,7 +5488,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="30">
+      <c r="A18" s="29">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
@@ -5473,7 +5504,7 @@
       <c r="E18" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="F18" s="21"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="8" t="s">
         <v>25</v>
       </c>
@@ -5503,7 +5534,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="31">
+      <c r="A19" s="30">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
@@ -5519,7 +5550,7 @@
       <c r="E19" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="13" t="s">
         <v>25</v>
       </c>
@@ -5549,7 +5580,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="30">
+      <c r="A20" s="29">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
@@ -5565,7 +5596,7 @@
       <c r="E20" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="F20" s="21"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="8" t="s">
         <v>25</v>
       </c>
@@ -5595,7 +5626,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="31">
+      <c r="A21" s="30">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
@@ -5611,7 +5642,7 @@
       <c r="E21" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="13" t="s">
         <v>25</v>
       </c>
@@ -5641,7 +5672,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="30">
+      <c r="A22" s="29">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -5657,7 +5688,7 @@
       <c r="E22" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="F22" s="21"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="8" t="s">
         <v>25</v>
       </c>
@@ -5687,7 +5718,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="31">
+      <c r="A23" s="30">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
@@ -5703,7 +5734,7 @@
       <c r="E23" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="13" t="s">
         <v>25</v>
       </c>
@@ -5733,63 +5764,63 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="30">
+      <c r="A24" s="29">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24" s="36" t="s">
+      <c r="F24" s="33"/>
+      <c r="G24" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="M24" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="N24" s="35" t="s">
+      <c r="M24" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="O24" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="38"/>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38"/>
+      <c r="O24" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="37"/>
     </row>
     <row r="25">
-      <c r="A25" s="31">
+      <c r="A25" s="30">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
@@ -5805,7 +5836,7 @@
       <c r="E25" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="F25" s="19"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="13" t="s">
         <v>25</v>
       </c>
@@ -5835,7 +5866,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="30">
+      <c r="A26" s="29">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
@@ -5851,7 +5882,7 @@
       <c r="E26" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="21"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="8" t="s">
         <v>25</v>
       </c>
@@ -5881,7 +5912,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="31">
+      <c r="A27" s="30">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
@@ -5897,7 +5928,7 @@
       <c r="E27" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="F27" s="19"/>
+      <c r="F27" s="18"/>
       <c r="G27" s="13" t="s">
         <v>25</v>
       </c>
@@ -5927,7 +5958,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="30">
+      <c r="A28" s="29">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
@@ -5943,7 +5974,7 @@
       <c r="E28" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="F28" s="21"/>
+      <c r="F28" s="20"/>
       <c r="G28" s="8" t="s">
         <v>25</v>
       </c>
@@ -5973,7 +6004,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="31">
+      <c r="A29" s="30">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
@@ -5989,7 +6020,7 @@
       <c r="E29" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="F29" s="19"/>
+      <c r="F29" s="18"/>
       <c r="G29" s="13" t="s">
         <v>25</v>
       </c>
@@ -6019,7 +6050,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="30">
+      <c r="A30" s="29">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -6035,7 +6066,7 @@
       <c r="E30" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="F30" s="21"/>
+      <c r="F30" s="20"/>
       <c r="G30" s="8" t="s">
         <v>25</v>
       </c>
@@ -6065,7 +6096,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="31">
+      <c r="A31" s="30">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
@@ -6081,7 +6112,7 @@
       <c r="E31" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="F31" s="19"/>
+      <c r="F31" s="18"/>
       <c r="G31" s="13" t="s">
         <v>25</v>
       </c>
@@ -6111,7 +6142,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="30">
+      <c r="A32" s="29">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
@@ -6127,7 +6158,7 @@
       <c r="E32" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="8" t="s">
         <v>25</v>
       </c>
@@ -6157,7 +6188,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="31">
+      <c r="A33" s="30">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
@@ -6173,7 +6204,7 @@
       <c r="E33" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="F33" s="19"/>
+      <c r="F33" s="18"/>
       <c r="G33" s="13" t="s">
         <v>25</v>
       </c>
@@ -6203,48 +6234,48 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="39">
+      <c r="A34" s="38">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43" t="s">
+      <c r="F34" s="41"/>
+      <c r="G34" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="J34" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="K34" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="L34" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="M34" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="N34" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="O34" s="44" t="s">
+      <c r="H34" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="N34" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="O34" s="43" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6298,325 +6329,325 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="O1" s="47" t="s">
+      <c r="O1" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="47" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49">
+      <c r="A2" s="48">
         <v>0.0</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="50" t="b">
+      <c r="C2" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="50" t="b">
+      <c r="D2" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="51">
+      <c r="E2" s="50">
         <f t="shared" ref="E2:E6" si="1">COUNTIF($F2:$AC2,"=TRUE")</f>
         <v>0</v>
       </c>
-      <c r="F2" s="50" t="b">
+      <c r="F2" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="L2" s="49" t="b">
+      <c r="L2" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="O2" s="52" t="s">
+      <c r="O2" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="P2" s="52" t="s">
+      <c r="P2" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="Q2" s="52" t="s">
+      <c r="Q2" s="51" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="49">
+      <c r="A3" s="48">
         <v>1.0</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="50" t="b">
+      <c r="C3" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="50" t="b">
+      <c r="D3" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="50">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F3" s="50" t="b">
+      <c r="F3" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="L3" s="49" t="b">
+      <c r="L3" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M3" s="52" t="s">
+      <c r="M3" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="N3" s="52" t="s">
+      <c r="N3" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="O3" s="52" t="s">
+      <c r="O3" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="P3" s="52" t="s">
+      <c r="P3" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="51" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="49">
+      <c r="A4" s="48">
         <v>2.0</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="50" t="b">
+      <c r="C4" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="50" t="b">
+      <c r="D4" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="50">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F4" s="50" t="b">
+      <c r="F4" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="I4" s="52" t="s">
+      <c r="I4" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="J4" s="52" t="s">
+      <c r="J4" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="K4" s="52" t="s">
+      <c r="K4" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="L4" s="49" t="b">
+      <c r="L4" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="M4" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="O4" s="52" t="s">
+      <c r="O4" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="51" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="49">
+      <c r="A5" s="48">
         <v>3.0</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="50" t="b">
+      <c r="C5" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="50" t="b">
+      <c r="D5" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="50">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F5" s="50" t="b">
+      <c r="F5" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="52" t="s">
+      <c r="I5" s="51" t="s">
         <v>215</v>
       </c>
-      <c r="J5" s="52" t="s">
+      <c r="J5" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="L5" s="49" t="b">
+      <c r="L5" s="48" t="b">
         <v>1</v>
       </c>
-      <c r="M5" s="52" t="s">
+      <c r="M5" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="N5" s="52" t="s">
+      <c r="N5" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="O5" s="52" t="s">
+      <c r="O5" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="P5" s="52" t="s">
+      <c r="P5" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="Q5" s="52" t="s">
+      <c r="Q5" s="51" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="49">
+      <c r="A6" s="48">
         <v>4.0</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="C6" s="50" t="b">
+      <c r="C6" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="50" t="b">
+      <c r="D6" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F6" s="50" t="b">
+      <c r="F6" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="K6" s="52" t="s">
+      <c r="K6" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="L6" s="49" t="b">
+      <c r="L6" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M6" s="52" t="s">
+      <c r="M6" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="O6" s="52" t="s">
+      <c r="O6" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="P6" s="52" t="s">
+      <c r="P6" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="Q6" s="52" t="s">
+      <c r="Q6" s="51" t="s">
         <v>214</v>
       </c>
     </row>
@@ -6671,123 +6702,129 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="52" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="54">
+      <c r="A2" s="53">
         <v>0.0</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="55" t="s">
         <v>231</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="55" t="s">
         <v>232</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="55" t="s">
         <v>233</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="56" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="58">
+      <c r="A3" s="57">
         <v>1.0</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="59" t="s">
         <v>232</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="59" t="s">
         <v>233</v>
       </c>
-      <c r="G3" s="61" t="s">
+      <c r="G3" s="60" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="54">
+      <c r="A4" s="53">
         <v>2.0</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="54" t="s">
         <v>223</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="55" t="s">
         <v>235</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="55" t="s">
         <v>232</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="55" t="s">
         <v>236</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="56" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="62">
+      <c r="A5" s="61">
         <v>3.0</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="63" t="s">
         <v>214</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="63" t="s">
         <v>231</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="63" t="s">
         <v>232</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="63" t="s">
         <v>233</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="64" t="s">
         <v>233</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:G5">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:E5">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C5">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F2:G5">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -6817,41 +6854,41 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>238</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="52" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="54">
+      <c r="A2" s="53">
         <v>0.0</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>233</v>
       </c>
-      <c r="D2" s="66">
+      <c r="D2" s="65">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="62">
+      <c r="A3" s="61">
         <v>1.0</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="D3" s="67">
+      <c r="D3" s="66">
         <v>0.0</v>
       </c>
     </row>
@@ -6875,28 +6912,28 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="67" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="68">
+      <c r="A2" s="67">
         <f t="shared" ref="A2:A3" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="67" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="68">
+      <c r="A3" s="67">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="67" t="s">
         <v>244</v>
       </c>
     </row>
@@ -6923,34 +6960,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="52" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="54">
+      <c r="A2" s="53">
         <v>0.0</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="65" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="58">
+      <c r="A3" s="57">
         <v>1.0</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="68" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="70">
+      <c r="A4" s="69">
         <v>2.0</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="70" t="s">
         <v>246</v>
       </c>
     </row>
@@ -6980,12 +7017,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="71" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="73">
+      <c r="A2" s="72">
         <v>3.0</v>
       </c>
     </row>
@@ -7022,75 +7059,75 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="52" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="54">
+      <c r="A2" s="53">
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="G2" s="75"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3">
-      <c r="A3" s="58">
+      <c r="A3" s="57">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>254</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="F3" s="59"/>
-      <c r="G3" s="61" t="s">
+      <c r="F3" s="58"/>
+      <c r="G3" s="60" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="70">
+      <c r="A4" s="69">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="G4" s="78"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="G4" s="77"/>
     </row>
   </sheetData>
   <dataValidations>

</xml_diff>

<commit_message>
Added consume flag for interactions which only unchain dialogs or special animations
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -12,15 +12,14 @@
     <sheet state="visible" name="CHARACTERS" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="CONSTANTS" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="EVENTS" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="_REF" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="_ITEM_AVAIL" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="_TODO" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="_ITEM_AVAIL" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="_TODO" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="zXWrutDY46wAzOxsLNDNzItt4A5Qr5fb78IlINitF5k="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataChecksum="i4XDMNVZBdM1RBA7RxuzpUb691zyqDO4P6SPPOEJgLk="/>
     </ext>
   </extLst>
 </workbook>
@@ -54,8 +53,24 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="E2">
+      <text>
+        <t xml:space="preserve">Calculated
+======</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="285">
   <si>
     <t>N</t>
   </si>
@@ -669,6 +684,9 @@
     <t>Action1_UnchainEvent</t>
   </si>
   <si>
+    <t>Action1_Consume</t>
+  </si>
+  <si>
     <t>Action2</t>
   </si>
   <si>
@@ -687,6 +705,9 @@
     <t>Action2_UnchainEvent</t>
   </si>
   <si>
+    <t>Action2_Consume</t>
+  </si>
+  <si>
     <t>ITEM_NONE</t>
   </si>
   <si>
@@ -795,9 +816,30 @@
     <t>Type</t>
   </si>
   <si>
+    <t>CHARACTER_NONE</t>
+  </si>
+  <si>
     <t>CHARACTER_SNAKE</t>
   </si>
   <si>
+    <t>ANIMATION_ID</t>
+  </si>
+  <si>
+    <t>ITEM_USE_ANIMATION_NONE</t>
+  </si>
+  <si>
+    <t>ITEM_USE_ANIMATION_NORMAL</t>
+  </si>
+  <si>
+    <t>INTERACTION_ID</t>
+  </si>
+  <si>
+    <t>INTERACTION_RECEIVE</t>
+  </si>
+  <si>
+    <t>INTERACTION_TAKE_AND_RECEIVE</t>
+  </si>
+  <si>
     <t>NUM_PLAYERS</t>
   </si>
   <si>
@@ -823,24 +865,6 @@
   </si>
   <si>
     <t>EVENT_LAST</t>
-  </si>
-  <si>
-    <t>ANIMATION_ID</t>
-  </si>
-  <si>
-    <t>INTERACTION_ID</t>
-  </si>
-  <si>
-    <t>ITEM_USE_ANIMATION_NONE</t>
-  </si>
-  <si>
-    <t>ITEM_USE_ANIMATION_NORMAL</t>
-  </si>
-  <si>
-    <t>INTERACTION_RECEIVE</t>
-  </si>
-  <si>
-    <t>INTERACTION_TAKE_AND_RECEIVE</t>
   </si>
   <si>
     <t>ITEM_ID (Ref)</t>
@@ -948,7 +972,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="26">
     <border/>
     <border>
       <left style="thin">
@@ -1218,48 +1242,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF6F8F9"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFFF0000"/>
       </left>
       <right style="thin">
@@ -1284,6 +1266,20 @@
       </top>
       <bottom style="thin">
         <color rgb="FFFFFF00"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF57BB8A"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF57BB8A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF57BB8A"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF57BB8A"/>
       </bottom>
     </border>
     <border>
@@ -1332,7 +1328,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="85">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1483,7 +1479,7 @@
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1567,22 +1563,16 @@
     <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="22" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="23" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1590,12 +1580,6 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="25" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="26" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1684,22 +1668,22 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
+    <tableStyle count="3" pivot="0" name="CHARACTERS-style 2">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="CHARACTERS-style 3">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
     <tableStyle count="3" pivot="0" name="CONSTANTS-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="EVENTS-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="_REF-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="_REF-style 2">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1722,10 +1706,6 @@
 </file>
 
 <file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1787,11 +1767,17 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:B6" displayName="Table_Interaction" name="Table_Interaction" id="10">
-  <tableColumns count="1">
-    <tableColumn name="INTERACTION_ID" id="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Events" name="Table_Events" id="10">
+  <tableColumns count="7">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="EVENT_ID" id="2"/>
+    <tableColumn name="TRIGGERING_ACTION" id="3"/>
+    <tableColumn name="TRIGGERING_ITEM1" id="4"/>
+    <tableColumn name="TRIGGERING_ITEM2" id="5"/>
+    <tableColumn name="TRIGGERING_NPC" id="6"/>
+    <tableColumn name="TRIGGERED_EVENT (CONSEQUENCE)" id="7"/>
   </tableColumns>
-  <tableStyleInfo name="_REF-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="EVENTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -1831,8 +1817,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Q6" displayName="Table_Items" name="Table_Items" id="3">
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:S6" displayName="Table_Items" name="Table_Items" id="3">
+  <tableColumns count="19">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_ID" id="2"/>
     <tableColumn name="PICKABLE" id="3"/>
@@ -1844,12 +1830,14 @@
     <tableColumn name="Action1_ItemSrc" id="9"/>
     <tableColumn name="Action1_Condition" id="10"/>
     <tableColumn name="Action1_UnchainEvent" id="11"/>
-    <tableColumn name="Action2" id="12"/>
-    <tableColumn name="Action2_SourceChar" id="13"/>
-    <tableColumn name="Action2_Action" id="14"/>
-    <tableColumn name="Action2_ItemSrc" id="15"/>
-    <tableColumn name="Action2_Condition" id="16"/>
-    <tableColumn name="Action2_UnchainEvent" id="17"/>
+    <tableColumn name="Action1_Consume" id="12"/>
+    <tableColumn name="Action2" id="13"/>
+    <tableColumn name="Action2_SourceChar" id="14"/>
+    <tableColumn name="Action2_Action" id="15"/>
+    <tableColumn name="Action2_ItemSrc" id="16"/>
+    <tableColumn name="Action2_Condition" id="17"/>
+    <tableColumn name="Action2_UnchainEvent" id="18"/>
+    <tableColumn name="Action2_Consume" id="19"/>
   </tableColumns>
   <tableStyleInfo name="ITEMS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -1883,7 +1871,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B4" displayName="Table_Characters" name="Table_Characters" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="6">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="Type" id="2"/>
@@ -1893,35 +1881,31 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A2" displayName="Table_Constants" name="Table_Constants" id="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="7">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="ANIMATION_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="CHARACTERS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B20" displayName="Table_Interaction" name="Table_Interaction" id="8">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="INTERACTION_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="CHARACTERS-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A2" displayName="Table_Constants" name="Table_Constants" id="9">
   <tableColumns count="1">
     <tableColumn name="NUM_PLAYERS" id="1"/>
   </tableColumns>
   <tableStyleInfo name="CONSTANTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Events" name="Table_Events" id="8">
-  <tableColumns count="7">
-    <tableColumn name="N" id="1"/>
-    <tableColumn name="EVENT_ID" id="2"/>
-    <tableColumn name="TRIGGERING_ACTION" id="3"/>
-    <tableColumn name="TRIGGERING_ITEM1" id="4"/>
-    <tableColumn name="TRIGGERING_ITEM2" id="5"/>
-    <tableColumn name="TRIGGERING_NPC" id="6"/>
-    <tableColumn name="TRIGGERED_EVENT (CONSEQUENCE)" id="7"/>
-  </tableColumns>
-  <tableStyleInfo name="EVENTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A7" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="9">
-  <tableColumns count="1">
-    <tableColumn name="ANIMATION_ID" id="1"/>
-  </tableColumns>
-  <tableStyleInfo name="_REF-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -2490,7 +2474,7 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="17">
-        <f>COUNT(Table_Characters[N])</f>
+        <f>COUNT(Table_Characters[N])-1</f>
         <v>3</v>
       </c>
       <c r="F7" s="16">
@@ -2861,7 +2845,7 @@
         <v>0.0</v>
       </c>
       <c r="E14" s="17">
-        <f>Table_Constants[NUM_PLAYERS]</f>
+        <f>COUNT(Table_Characters[N])-1</f>
         <v>3</v>
       </c>
       <c r="F14" s="15" t="s">
@@ -3959,85 +3943,6 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="44.71"/>
-    <col customWidth="1" min="2" max="2" width="36.0"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="78" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="78" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="79" t="s">
-        <v>258</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="80" t="s">
-        <v>259</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="79" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" s="79" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="80" t="s">
-        <v>232</v>
-      </c>
-      <c r="B5" s="80" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="79" t="s">
-        <v>235</v>
-      </c>
-      <c r="B6" s="81" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="82" t="s">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
@@ -4051,10 +3956,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2">
@@ -4062,12 +3967,12 @@
         <f t="shared" ref="A2:A32" si="1">ROW()-ROW($G$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="83" t="str">
+      <c r="B2" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A2,0)</f>
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
@@ -4075,12 +3980,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="83" t="str">
+      <c r="B3" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A3,0)</f>
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
@@ -4088,12 +3993,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="83" t="str">
+      <c r="B4" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A4,0)</f>
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5">
@@ -4101,12 +4006,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="83" t="str">
+      <c r="B5" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A5,0)</f>
         <v>ITEM_LAST</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6">
@@ -4114,297 +4019,297 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="83" t="str">
+      <c r="B6" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A6,0)</f>
         <v/>
       </c>
-      <c r="C6" s="83"/>
+      <c r="C6" s="78"/>
     </row>
     <row r="7">
       <c r="A7" s="27">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="83" t="str">
+      <c r="B7" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A7,0)</f>
         <v/>
       </c>
-      <c r="C7" s="83"/>
+      <c r="C7" s="78"/>
     </row>
     <row r="8">
       <c r="A8" s="27">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="83" t="str">
+      <c r="B8" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A8,0)</f>
         <v/>
       </c>
-      <c r="C8" s="83"/>
+      <c r="C8" s="78"/>
     </row>
     <row r="9">
       <c r="A9" s="27">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="83" t="str">
+      <c r="B9" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A9,0)</f>
         <v/>
       </c>
-      <c r="C9" s="83"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10">
       <c r="A10" s="27">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="83" t="str">
+      <c r="B10" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A10,0)</f>
         <v/>
       </c>
-      <c r="C10" s="83"/>
+      <c r="C10" s="78"/>
     </row>
     <row r="11">
       <c r="A11" s="27">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="83" t="str">
+      <c r="B11" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A11,0)</f>
         <v/>
       </c>
-      <c r="C11" s="83"/>
+      <c r="C11" s="78"/>
     </row>
     <row r="12">
       <c r="A12" s="27">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="83" t="str">
+      <c r="B12" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A12,0)</f>
         <v/>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="78"/>
     </row>
     <row r="13">
       <c r="A13" s="27">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="83" t="str">
+      <c r="B13" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A13,0)</f>
         <v/>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="78"/>
     </row>
     <row r="14">
       <c r="A14" s="27">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="83" t="str">
+      <c r="B14" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A14,0)</f>
         <v/>
       </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="78"/>
     </row>
     <row r="15">
       <c r="A15" s="27">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="83" t="str">
+      <c r="B15" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A15,0)</f>
         <v/>
       </c>
-      <c r="C15" s="83"/>
+      <c r="C15" s="78"/>
     </row>
     <row r="16">
       <c r="A16" s="27">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="83" t="str">
+      <c r="B16" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A16,0)</f>
         <v/>
       </c>
-      <c r="C16" s="83"/>
+      <c r="C16" s="78"/>
     </row>
     <row r="17">
       <c r="A17" s="27">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="83" t="str">
+      <c r="B17" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A17,0)</f>
         <v/>
       </c>
-      <c r="C17" s="83"/>
+      <c r="C17" s="78"/>
     </row>
     <row r="18">
       <c r="A18" s="27">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="83" t="str">
+      <c r="B18" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A18,0)</f>
         <v/>
       </c>
-      <c r="C18" s="83"/>
+      <c r="C18" s="78"/>
     </row>
     <row r="19">
       <c r="A19" s="27">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="83" t="str">
+      <c r="B19" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A19,0)</f>
         <v/>
       </c>
-      <c r="C19" s="83"/>
+      <c r="C19" s="78"/>
     </row>
     <row r="20">
       <c r="A20" s="27">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="83" t="str">
+      <c r="B20" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A20,0)</f>
         <v/>
       </c>
-      <c r="C20" s="83"/>
+      <c r="C20" s="78"/>
     </row>
     <row r="21">
       <c r="A21" s="27">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="83" t="str">
+      <c r="B21" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A21,0)</f>
         <v/>
       </c>
-      <c r="C21" s="83"/>
+      <c r="C21" s="78"/>
     </row>
     <row r="22">
       <c r="A22" s="27">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="83" t="str">
+      <c r="B22" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A22,0)</f>
         <v/>
       </c>
-      <c r="C22" s="83"/>
+      <c r="C22" s="78"/>
     </row>
     <row r="23">
       <c r="A23" s="27">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="83" t="str">
+      <c r="B23" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A23,0)</f>
         <v/>
       </c>
-      <c r="C23" s="83"/>
+      <c r="C23" s="78"/>
     </row>
     <row r="24">
       <c r="A24" s="27">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="83" t="str">
+      <c r="B24" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A24,0)</f>
         <v/>
       </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="78"/>
     </row>
     <row r="25">
       <c r="A25" s="27">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="83" t="str">
+      <c r="B25" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A25,0)</f>
         <v/>
       </c>
-      <c r="C25" s="83"/>
+      <c r="C25" s="78"/>
     </row>
     <row r="26">
       <c r="A26" s="27">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="83" t="str">
+      <c r="B26" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A26,0)</f>
         <v/>
       </c>
-      <c r="C26" s="83"/>
+      <c r="C26" s="78"/>
     </row>
     <row r="27">
       <c r="A27" s="27">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="83" t="str">
+      <c r="B27" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A27,0)</f>
         <v/>
       </c>
-      <c r="C27" s="83"/>
+      <c r="C27" s="78"/>
     </row>
     <row r="28">
       <c r="A28" s="27">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="83" t="str">
+      <c r="B28" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A28,0)</f>
         <v/>
       </c>
-      <c r="C28" s="83"/>
+      <c r="C28" s="78"/>
     </row>
     <row r="29">
       <c r="A29" s="27">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="83" t="str">
+      <c r="B29" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A29,0)</f>
         <v/>
       </c>
-      <c r="C29" s="83"/>
+      <c r="C29" s="78"/>
     </row>
     <row r="30">
       <c r="A30" s="27">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="83" t="str">
+      <c r="B30" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A30,0)</f>
         <v/>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="78"/>
     </row>
     <row r="31">
       <c r="A31" s="27">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="83" t="str">
+      <c r="B31" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A31,0)</f>
         <v/>
       </c>
-      <c r="C31" s="83"/>
+      <c r="C31" s="78"/>
     </row>
     <row r="32">
       <c r="A32" s="27">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="83" t="str">
+      <c r="B32" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A32,0)</f>
         <v/>
       </c>
-      <c r="C32" s="83"/>
+      <c r="C32" s="78"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -4416,7 +4321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4437,23 +4342,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="44" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="53" t="s">
-        <v>269</v>
-      </c>
-      <c r="B2" s="84">
+        <v>272</v>
+      </c>
+      <c r="B2" s="79">
         <v>1.0</v>
       </c>
       <c r="C2" s="54" t="b">
@@ -4465,9 +4370,9 @@
     </row>
     <row r="3">
       <c r="A3" s="57" t="s">
-        <v>270</v>
-      </c>
-      <c r="B3" s="84">
+        <v>273</v>
+      </c>
+      <c r="B3" s="79">
         <v>1.0</v>
       </c>
       <c r="C3" s="58" t="b">
@@ -4479,9 +4384,9 @@
     </row>
     <row r="4">
       <c r="A4" s="53" t="s">
-        <v>271</v>
-      </c>
-      <c r="B4" s="85">
+        <v>274</v>
+      </c>
+      <c r="B4" s="80">
         <v>3.0</v>
       </c>
       <c r="C4" s="54" t="b">
@@ -4493,9 +4398,9 @@
     </row>
     <row r="5">
       <c r="A5" s="57" t="s">
-        <v>272</v>
-      </c>
-      <c r="B5" s="84">
+        <v>275</v>
+      </c>
+      <c r="B5" s="79">
         <v>1.0</v>
       </c>
       <c r="C5" s="58" t="b">
@@ -4507,9 +4412,9 @@
     </row>
     <row r="6">
       <c r="A6" s="53" t="s">
-        <v>273</v>
-      </c>
-      <c r="B6" s="85">
+        <v>276</v>
+      </c>
+      <c r="B6" s="80">
         <v>3.0</v>
       </c>
       <c r="C6" s="54" t="b">
@@ -4521,9 +4426,9 @@
     </row>
     <row r="7">
       <c r="A7" s="57" t="s">
-        <v>274</v>
-      </c>
-      <c r="B7" s="85">
+        <v>277</v>
+      </c>
+      <c r="B7" s="80">
         <v>3.0</v>
       </c>
       <c r="C7" s="58" t="b">
@@ -4535,10 +4440,10 @@
     </row>
     <row r="8">
       <c r="A8" s="53" t="s">
-        <v>275</v>
-      </c>
-      <c r="B8" s="86">
-        <v>4.0</v>
+        <v>278</v>
+      </c>
+      <c r="B8" s="81">
+        <v>5.0</v>
       </c>
       <c r="C8" s="54" t="b">
         <v>0</v>
@@ -4549,9 +4454,9 @@
     </row>
     <row r="9">
       <c r="A9" s="57" t="s">
-        <v>276</v>
-      </c>
-      <c r="B9" s="86">
+        <v>279</v>
+      </c>
+      <c r="B9" s="82">
         <v>4.0</v>
       </c>
       <c r="C9" s="58" t="b">
@@ -4563,9 +4468,9 @@
     </row>
     <row r="10">
       <c r="A10" s="53" t="s">
-        <v>277</v>
-      </c>
-      <c r="B10" s="86">
+        <v>280</v>
+      </c>
+      <c r="B10" s="82">
         <v>4.0</v>
       </c>
       <c r="C10" s="54" t="b">
@@ -4577,9 +4482,9 @@
     </row>
     <row r="11">
       <c r="A11" s="57" t="s">
-        <v>278</v>
-      </c>
-      <c r="B11" s="84">
+        <v>281</v>
+      </c>
+      <c r="B11" s="79">
         <v>1.0</v>
       </c>
       <c r="C11" s="58" t="b">
@@ -4590,10 +4495,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="87" t="s">
-        <v>279</v>
-      </c>
-      <c r="B12" s="86">
+      <c r="A12" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="B12" s="82">
         <v>4.0</v>
       </c>
       <c r="C12" s="54" t="b">
@@ -4604,14 +4509,14 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="57" t="s">
-        <v>280</v>
-      </c>
-      <c r="B13" s="84">
+      <c r="A13" s="83" t="s">
+        <v>283</v>
+      </c>
+      <c r="B13" s="79">
         <v>1.0</v>
       </c>
       <c r="C13" s="58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="68" t="b">
         <v>1</v>
@@ -4619,9 +4524,9 @@
     </row>
     <row r="14">
       <c r="A14" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="B14" s="88">
+        <v>284</v>
+      </c>
+      <c r="B14" s="84">
         <v>5.0</v>
       </c>
       <c r="C14" s="75" t="b">
@@ -6319,13 +6224,15 @@
     <col customWidth="1" min="8" max="8" width="26.57"/>
     <col customWidth="1" min="9" max="10" width="23.57"/>
     <col customWidth="1" min="11" max="11" width="30.0"/>
-    <col customWidth="1" min="12" max="12" width="12.0"/>
-    <col customWidth="1" min="13" max="13" width="27.57"/>
-    <col customWidth="1" min="14" max="14" width="26.57"/>
-    <col customWidth="1" min="15" max="15" width="26.0"/>
-    <col customWidth="1" min="16" max="16" width="24.71"/>
-    <col customWidth="1" min="17" max="17" width="30.0"/>
-    <col customWidth="1" min="18" max="29" width="12.43"/>
+    <col customWidth="1" min="12" max="12" width="21.86"/>
+    <col customWidth="1" min="13" max="13" width="12.0"/>
+    <col customWidth="1" min="14" max="14" width="27.57"/>
+    <col customWidth="1" min="15" max="15" width="26.57"/>
+    <col customWidth="1" min="16" max="16" width="26.0"/>
+    <col customWidth="1" min="17" max="17" width="24.71"/>
+    <col customWidth="1" min="18" max="18" width="30.0"/>
+    <col customWidth="1" min="19" max="19" width="21.86"/>
+    <col customWidth="1" min="20" max="30" width="12.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6362,7 +6269,7 @@
       <c r="K1" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="46" t="s">
         <v>204</v>
       </c>
       <c r="M1" s="45" t="s">
@@ -6371,14 +6278,20 @@
       <c r="N1" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="Q1" s="45" t="s">
         <v>209</v>
+      </c>
+      <c r="R1" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="S1" s="47" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="2">
@@ -6386,53 +6299,59 @@
         <v>0.0</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C2" s="49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="49" t="b">
         <v>0</v>
       </c>
       <c r="E2" s="50">
-        <f t="shared" ref="E2:E6" si="1">COUNTIF($F2:$AC2,"=TRUE")</f>
+        <f t="shared" ref="E2:E6" si="1">COUNTIF(F2,"=TRUE")+COUNTIF(M2,"=TRUE")</f>
         <v>0</v>
       </c>
       <c r="F2" s="49" t="b">
         <v>0</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H2" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="I2" s="51" t="s">
-        <v>210</v>
-      </c>
       <c r="J2" s="51" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K2" s="51" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="L2" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="51" t="s">
-        <v>211</v>
+      <c r="M2" s="48" t="b">
+        <v>0</v>
       </c>
       <c r="N2" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="O2" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="P2" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="O2" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="P2" s="51" t="s">
-        <v>213</v>
-      </c>
       <c r="Q2" s="51" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="R2" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="S2" s="48" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -6440,7 +6359,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C3" s="49" t="b">
         <v>1</v>
@@ -6456,37 +6375,43 @@
         <v>1</v>
       </c>
       <c r="G3" s="51" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H3" s="51" t="s">
+        <v>218</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="K3" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="I3" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="J3" s="51" t="s">
+      <c r="L3" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="O3" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="L3" s="48" t="b">
+      <c r="P3" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q3" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="R3" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="S3" s="48" t="b">
         <v>0</v>
-      </c>
-      <c r="M3" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="N3" s="51" t="s">
-        <v>212</v>
-      </c>
-      <c r="O3" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="P3" s="51" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q3" s="51" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4">
@@ -6494,7 +6419,7 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C4" s="49" t="b">
         <v>1</v>
@@ -6510,37 +6435,43 @@
         <v>1</v>
       </c>
       <c r="G4" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="H4" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="I4" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="I4" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="J4" s="51" t="s">
+      <c r="L4" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="K4" s="51" t="s">
+      <c r="O4" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="L4" s="48" t="b">
+      <c r="P4" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q4" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="R4" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="S4" s="48" t="b">
         <v>0</v>
-      </c>
-      <c r="M4" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="N4" s="51" t="s">
-        <v>212</v>
-      </c>
-      <c r="O4" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="P4" s="51" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q4" s="51" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="5">
@@ -6548,7 +6479,7 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C5" s="49" t="b">
         <v>0</v>
@@ -6564,37 +6495,43 @@
         <v>1</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="K5" s="51" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="L5" s="48" t="b">
         <v>1</v>
       </c>
-      <c r="M5" s="51" t="s">
-        <v>218</v>
+      <c r="M5" s="48" t="b">
+        <v>1</v>
       </c>
       <c r="N5" s="51" t="s">
         <v>220</v>
       </c>
       <c r="O5" s="51" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="P5" s="51" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="Q5" s="51" t="s">
-        <v>214</v>
+        <v>225</v>
+      </c>
+      <c r="R5" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="S5" s="48" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -6602,7 +6539,7 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C6" s="49" t="b">
         <v>0</v>
@@ -6618,63 +6555,70 @@
         <v>0</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H6" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="I6" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="I6" s="51" t="s">
-        <v>210</v>
-      </c>
       <c r="J6" s="51" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K6" s="51" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="L6" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M6" s="51" t="s">
-        <v>211</v>
+      <c r="M6" s="48" t="b">
+        <v>0</v>
       </c>
       <c r="N6" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="O6" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="P6" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="O6" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="P6" s="51" t="s">
-        <v>213</v>
-      </c>
       <c r="Q6" s="51" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="R6" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="S6" s="48" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I6 O2:O6">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I6 P2:P6">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J6 P2:P6">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J6 Q2:Q6">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H6">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G6">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K2:K6 Q2:Q6">
+    <dataValidation type="list" allowBlank="1" sqref="K2:K6 R2:R6">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M2:M6">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N2:N6">
       <formula1>Table_Characters[Type]</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N2:N6">
-      <formula1>'_REF'!$B$2:$B$6</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="H2:H6 O2:O6">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6706,22 +6650,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2">
@@ -6729,22 +6673,22 @@
         <v>0.0</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D2" s="55" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
@@ -6752,22 +6696,22 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D3" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="E3" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="E3" s="59" t="s">
-        <v>232</v>
-      </c>
       <c r="F3" s="59" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G3" s="60" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4">
@@ -6775,22 +6719,22 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D4" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>234</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" s="56" t="s">
         <v>235</v>
-      </c>
-      <c r="E4" s="55" t="s">
-        <v>232</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>236</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="5">
@@ -6798,33 +6742,33 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D5" s="63" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E5" s="63" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F5" s="63" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G5" s="64" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:E5">
-      <formula1>#REF!</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C5">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="F2:G5">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D2:E5">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -6858,13 +6802,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2">
@@ -6872,7 +6816,7 @@
         <v>0.0</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D2" s="65">
         <v>0.0</v>
@@ -6883,10 +6827,10 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="62" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D3" s="66">
         <v>0.0</v>
@@ -6916,7 +6860,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="67" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2">
@@ -6925,7 +6869,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
@@ -6934,7 +6878,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -6956,7 +6900,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="23.29"/>
+    <col customWidth="1" min="2" max="3" width="38.86"/>
+    <col customWidth="1" min="4" max="4" width="23.29"/>
+    <col customWidth="1" min="6" max="6" width="38.86"/>
+    <col customWidth="1" min="8" max="8" width="34.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6964,7 +6911,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
@@ -6972,7 +6919,7 @@
         <v>0.0</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3">
@@ -6980,21 +6927,135 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="68" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="53">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="61">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="53">
+        <v>0.0</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="57">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="53">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="57">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="53">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="61">
+        <v>5.0</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="53">
+        <v>0.0</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="57">
+        <v>1.0</v>
+      </c>
+      <c r="B17" s="68" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="69">
+    <row r="18">
+      <c r="A18" s="53">
         <v>2.0</v>
       </c>
-      <c r="B4" s="70" t="s">
-        <v>246</v>
+      <c r="B18" s="65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="57">
+        <v>3.0</v>
+      </c>
+      <c r="B19" s="68" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="B20" s="70" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7018,7 +7079,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="71" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2">
@@ -7063,22 +7124,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2">
@@ -7087,7 +7148,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C2" s="73"/>
       <c r="D2" s="73"/>
@@ -7100,20 +7161,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F3" s="58"/>
       <c r="G3" s="60" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4">
@@ -7122,7 +7183,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="76"/>

</xml_diff>

<commit_message>
[Partial] Adding dialogs -Reliable loading process
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -8,18 +8,19 @@
     <sheet state="visible" name="ITEMS" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="ITEMS_CONDS" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="DIALOGS" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="NPCs" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="CHARACTERS" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="CONSTANTS" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="ROOMS" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="NPCs" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="CHARACTERS" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="EVENTS" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="_ITEM_AVAIL" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="_TODO" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="CONSTANTS" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="_ITEM_AVAIL" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="_TODO" sheetId="12" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataChecksum="yWvJgkSV7a65VtGwoNU7vekdXM7sHn1smO4WgMYwNto="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="s4Gx29HYjtFA4VIdk44SgsA8ZMcTp6N/brQlDNGJdGY="/>
     </ext>
   </extLst>
 </workbook>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="300">
   <si>
     <t>N</t>
   </si>
@@ -174,7 +175,7 @@
     <t>MultiBitFieldStruct</t>
   </si>
   <si>
-    <t>default(MultiBitFieldStruct)</t>
+    <t>default</t>
   </si>
   <si>
     <t>PICKABLE_ITEM_OWNER</t>
@@ -336,7 +337,7 @@
     <t>This service subscribes for late start. This happens at some moment after Start event. when everything has been setup</t>
   </si>
   <si>
-    <t>LOADING_COMPLETED</t>
+    <t>MODULE_LOADING_COMPLETED</t>
   </si>
   <si>
     <t>LODING_COMPLETED_DELEGATE</t>
@@ -348,6 +349,18 @@
     <t>This service is called when whole room has been loaded</t>
   </si>
   <si>
+    <t>IS_MODULE_LOADED</t>
+  </si>
+  <si>
+    <t>IS_MODULE_LOADED_DELEGATE</t>
+  </si>
+  <si>
+    <t>GameMasterClass.IsModuleLoadedService</t>
+  </si>
+  <si>
+    <t>This service returns a bool which tells if given module has been loaded in Room Loading Process</t>
+  </si>
+  <si>
     <t>FREEZE_PLAY</t>
   </si>
   <si>
@@ -804,15 +817,39 @@
     <t>DIALOG_ID</t>
   </si>
   <si>
+    <t>Room_used</t>
+  </si>
+  <si>
+    <t>Room_Code</t>
+  </si>
+  <si>
     <t>Text_English</t>
   </si>
   <si>
+    <t>Text_Spanish</t>
+  </si>
+  <si>
     <t>Sound</t>
   </si>
   <si>
+    <t>ROOM_NONE</t>
+  </si>
+  <si>
     <t>That has no sense!</t>
   </si>
   <si>
+    <t>¡Eso no tiene sentido!</t>
+  </si>
+  <si>
+    <t>ROOM_ID</t>
+  </si>
+  <si>
+    <t>ROOM_FIRST</t>
+  </si>
+  <si>
+    <t>ROOM_LAST</t>
+  </si>
+  <si>
     <t>NPC_ID</t>
   </si>
   <si>
@@ -849,31 +886,31 @@
     <t>INTERACTION_TAKE_AND_RECEIVE</t>
   </si>
   <si>
+    <t>EVENT_ID</t>
+  </si>
+  <si>
+    <t>TRIGGERING_ACTION</t>
+  </si>
+  <si>
+    <t>TRIGGERING_ITEM1</t>
+  </si>
+  <si>
+    <t>TRIGGERING_ITEM2</t>
+  </si>
+  <si>
+    <t>TRIGGERING_NPC</t>
+  </si>
+  <si>
+    <t>TRIGGERED_EVENT (CONSEQUENCE)</t>
+  </si>
+  <si>
+    <t>ITEM_USE</t>
+  </si>
+  <si>
+    <t>EVENT_LAST</t>
+  </si>
+  <si>
     <t>NUM_PLAYERS</t>
-  </si>
-  <si>
-    <t>EVENT_ID</t>
-  </si>
-  <si>
-    <t>TRIGGERING_ACTION</t>
-  </si>
-  <si>
-    <t>TRIGGERING_ITEM1</t>
-  </si>
-  <si>
-    <t>TRIGGERING_ITEM2</t>
-  </si>
-  <si>
-    <t>TRIGGERING_NPC</t>
-  </si>
-  <si>
-    <t>TRIGGERED_EVENT (CONSEQUENCE)</t>
-  </si>
-  <si>
-    <t>ITEM_USE</t>
-  </si>
-  <si>
-    <t>EVENT_LAST</t>
   </si>
   <si>
     <t>ITEM_ID (Ref)</t>
@@ -1167,21 +1204,21 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF284E3F"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF284E3F"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
@@ -1209,6 +1246,20 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
@@ -1227,20 +1278,6 @@
       </left>
       <right style="thin">
         <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
         <color rgb="FFFFFFFF"/>
@@ -1337,7 +1374,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="85">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1431,32 +1468,44 @@
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1470,95 +1519,95 @@
     <xf borderId="3" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="19" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="19" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1634,7 +1683,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="11">
+  <tableStyles count="13">
     <tableStyle count="3" pivot="0" name="VARMAP-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1660,6 +1709,16 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
+    <tableStyle count="3" pivot="0" name="ROOMS-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="NPCs-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
     <tableStyle count="3" pivot="0" name="CHARACTERS-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1675,12 +1734,12 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="CONSTANTS-style">
+    <tableStyle count="3" pivot="0" name="EVENTS-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="EVENTS-style">
+    <tableStyle count="3" pivot="0" name="CONSTANTS-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1703,6 +1762,10 @@
 </file>
 
 <file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1764,7 +1827,17 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Events" name="Table_Events" id="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B20" displayName="Table_Interaction" name="Table_Interaction" id="10">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="INTERACTION_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="CHARACTERS-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Events" name="Table_Events" id="11">
   <tableColumns count="7">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_ID" id="2"/>
@@ -1778,8 +1851,17 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D14" displayName="Table_TODO" name="Table_TODO" id="11">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A2" displayName="Table_Constants" name="Table_Constants" id="12">
+  <tableColumns count="1">
+    <tableColumn name="NUM_PLAYERS" id="1"/>
+  </tableColumns>
+  <tableStyleInfo name="CONSTANTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D14" displayName="Table_TODO" name="Table_TODO" id="13">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -1791,7 +1873,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O35" displayName="Table_Services" name="Table_Services" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O36" displayName="Table_Services" name="Table_Services" id="2">
   <tableColumns count="15">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SERVICE_ID" id="2"/>
@@ -1855,19 +1937,42 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D3" displayName="Table_Dialogs" name="Table_Dialogs" id="5">
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G3" displayName="Table_Dialogs" name="Table_Dialogs" id="5">
+  <tableColumns count="7">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ID" id="2"/>
-    <tableColumn name="Text_English" id="3"/>
-    <tableColumn name="Sound" id="4"/>
+    <tableColumn name="Room_used" id="3"/>
+    <tableColumn name="Room_Code" id="4"/>
+    <tableColumn name="Text_English" id="5"/>
+    <tableColumn name="Text_Spanish" id="6"/>
+    <tableColumn name="Sound" id="7"/>
   </tableColumns>
   <tableStyleInfo name="DIALOGS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B4" displayName="Table_Rooms" name="Table_Rooms" id="6">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="ROOM_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="ROOMS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B3" displayName="Table_NPCs" name="Table_NPCs" id="7">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="NPC_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="NPCs-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="8">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="Type" id="2"/>
@@ -1876,32 +1981,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="7">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="9">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ANIMATION_ID" id="2"/>
   </tableColumns>
   <tableStyleInfo name="CHARACTERS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B20" displayName="Table_Interaction" name="Table_Interaction" id="8">
-  <tableColumns count="2">
-    <tableColumn name="N" id="1"/>
-    <tableColumn name="INTERACTION_ID" id="2"/>
-  </tableColumns>
-  <tableStyleInfo name="CHARACTERS-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A2" displayName="Table_Constants" name="Table_Constants" id="9">
-  <tableColumns count="1">
-    <tableColumn name="NUM_PLAYERS" id="1"/>
-  </tableColumns>
-  <tableStyleInfo name="CONSTANTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -3936,6 +4022,41 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FFB45F06"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="20.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="76" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="77">
+        <v>3.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
@@ -3952,10 +4073,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2">
@@ -3963,12 +4084,12 @@
         <f t="shared" ref="A2:A32" si="1">ROW()-ROW($G$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="74" t="str">
+      <c r="B2" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A2,0)</f>
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3">
@@ -3976,12 +4097,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="74" t="str">
+      <c r="B3" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A3,0)</f>
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4">
@@ -3989,12 +4110,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="74" t="str">
+      <c r="B4" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A4,0)</f>
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5">
@@ -4002,12 +4123,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="74" t="str">
+      <c r="B5" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A5,0)</f>
         <v>ITEM_LAST</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6">
@@ -4015,297 +4136,297 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="74" t="str">
+      <c r="B6" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A6,0)</f>
         <v/>
       </c>
-      <c r="C6" s="74"/>
+      <c r="C6" s="78"/>
     </row>
     <row r="7">
       <c r="A7" s="27">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="74" t="str">
+      <c r="B7" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A7,0)</f>
         <v/>
       </c>
-      <c r="C7" s="74"/>
+      <c r="C7" s="78"/>
     </row>
     <row r="8">
       <c r="A8" s="27">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="74" t="str">
+      <c r="B8" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A8,0)</f>
         <v/>
       </c>
-      <c r="C8" s="74"/>
+      <c r="C8" s="78"/>
     </row>
     <row r="9">
       <c r="A9" s="27">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="74" t="str">
+      <c r="B9" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A9,0)</f>
         <v/>
       </c>
-      <c r="C9" s="74"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10">
       <c r="A10" s="27">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="74" t="str">
+      <c r="B10" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A10,0)</f>
         <v/>
       </c>
-      <c r="C10" s="74"/>
+      <c r="C10" s="78"/>
     </row>
     <row r="11">
       <c r="A11" s="27">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="74" t="str">
+      <c r="B11" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A11,0)</f>
         <v/>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="78"/>
     </row>
     <row r="12">
       <c r="A12" s="27">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="74" t="str">
+      <c r="B12" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A12,0)</f>
         <v/>
       </c>
-      <c r="C12" s="74"/>
+      <c r="C12" s="78"/>
     </row>
     <row r="13">
       <c r="A13" s="27">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="74" t="str">
+      <c r="B13" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A13,0)</f>
         <v/>
       </c>
-      <c r="C13" s="74"/>
+      <c r="C13" s="78"/>
     </row>
     <row r="14">
       <c r="A14" s="27">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="74" t="str">
+      <c r="B14" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A14,0)</f>
         <v/>
       </c>
-      <c r="C14" s="74"/>
+      <c r="C14" s="78"/>
     </row>
     <row r="15">
       <c r="A15" s="27">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="74" t="str">
+      <c r="B15" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A15,0)</f>
         <v/>
       </c>
-      <c r="C15" s="74"/>
+      <c r="C15" s="78"/>
     </row>
     <row r="16">
       <c r="A16" s="27">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="74" t="str">
+      <c r="B16" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A16,0)</f>
         <v/>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="78"/>
     </row>
     <row r="17">
       <c r="A17" s="27">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="74" t="str">
+      <c r="B17" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A17,0)</f>
         <v/>
       </c>
-      <c r="C17" s="74"/>
+      <c r="C17" s="78"/>
     </row>
     <row r="18">
       <c r="A18" s="27">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="74" t="str">
+      <c r="B18" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A18,0)</f>
         <v/>
       </c>
-      <c r="C18" s="74"/>
+      <c r="C18" s="78"/>
     </row>
     <row r="19">
       <c r="A19" s="27">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="74" t="str">
+      <c r="B19" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A19,0)</f>
         <v/>
       </c>
-      <c r="C19" s="74"/>
+      <c r="C19" s="78"/>
     </row>
     <row r="20">
       <c r="A20" s="27">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="74" t="str">
+      <c r="B20" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A20,0)</f>
         <v/>
       </c>
-      <c r="C20" s="74"/>
+      <c r="C20" s="78"/>
     </row>
     <row r="21">
       <c r="A21" s="27">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="74" t="str">
+      <c r="B21" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A21,0)</f>
         <v/>
       </c>
-      <c r="C21" s="74"/>
+      <c r="C21" s="78"/>
     </row>
     <row r="22">
       <c r="A22" s="27">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="74" t="str">
+      <c r="B22" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A22,0)</f>
         <v/>
       </c>
-      <c r="C22" s="74"/>
+      <c r="C22" s="78"/>
     </row>
     <row r="23">
       <c r="A23" s="27">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="74" t="str">
+      <c r="B23" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A23,0)</f>
         <v/>
       </c>
-      <c r="C23" s="74"/>
+      <c r="C23" s="78"/>
     </row>
     <row r="24">
       <c r="A24" s="27">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="74" t="str">
+      <c r="B24" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A24,0)</f>
         <v/>
       </c>
-      <c r="C24" s="74"/>
+      <c r="C24" s="78"/>
     </row>
     <row r="25">
       <c r="A25" s="27">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="74" t="str">
+      <c r="B25" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A25,0)</f>
         <v/>
       </c>
-      <c r="C25" s="74"/>
+      <c r="C25" s="78"/>
     </row>
     <row r="26">
       <c r="A26" s="27">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="74" t="str">
+      <c r="B26" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A26,0)</f>
         <v/>
       </c>
-      <c r="C26" s="74"/>
+      <c r="C26" s="78"/>
     </row>
     <row r="27">
       <c r="A27" s="27">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="74" t="str">
+      <c r="B27" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A27,0)</f>
         <v/>
       </c>
-      <c r="C27" s="74"/>
+      <c r="C27" s="78"/>
     </row>
     <row r="28">
       <c r="A28" s="27">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="74" t="str">
+      <c r="B28" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A28,0)</f>
         <v/>
       </c>
-      <c r="C28" s="74"/>
+      <c r="C28" s="78"/>
     </row>
     <row r="29">
       <c r="A29" s="27">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="74" t="str">
+      <c r="B29" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A29,0)</f>
         <v/>
       </c>
-      <c r="C29" s="74"/>
+      <c r="C29" s="78"/>
     </row>
     <row r="30">
       <c r="A30" s="27">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="74" t="str">
+      <c r="B30" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A30,0)</f>
         <v/>
       </c>
-      <c r="C30" s="74"/>
+      <c r="C30" s="78"/>
     </row>
     <row r="31">
       <c r="A31" s="27">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="74" t="str">
+      <c r="B31" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A31,0)</f>
         <v/>
       </c>
-      <c r="C31" s="74"/>
+      <c r="C31" s="78"/>
     </row>
     <row r="32">
       <c r="A32" s="27">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="74" t="str">
+      <c r="B32" s="78" t="str">
         <f>OFFSET(ITEMS!$B$3,A32,0)</f>
         <v/>
       </c>
-      <c r="C32" s="74"/>
+      <c r="C32" s="78"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -4317,7 +4438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4337,198 +4458,198 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>273</v>
-      </c>
-      <c r="D1" s="48" t="s">
-        <v>274</v>
+      <c r="A1" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49" t="s">
-        <v>275</v>
-      </c>
-      <c r="B2" s="75">
+      <c r="A2" s="53" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" s="79">
         <v>1.0</v>
       </c>
-      <c r="C2" s="50" t="b">
+      <c r="C2" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="61" t="b">
+      <c r="D2" s="66" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="53" t="s">
-        <v>276</v>
-      </c>
-      <c r="B3" s="75">
+      <c r="A3" s="57" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" s="79">
         <v>1.0</v>
       </c>
-      <c r="C3" s="54" t="b">
+      <c r="C3" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="64" t="b">
+      <c r="D3" s="68" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="49" t="s">
-        <v>277</v>
-      </c>
-      <c r="B4" s="76">
+      <c r="A4" s="53" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="80">
         <v>3.0</v>
       </c>
-      <c r="C4" s="50" t="b">
+      <c r="C4" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="61" t="b">
+      <c r="D4" s="66" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="53" t="s">
-        <v>278</v>
-      </c>
-      <c r="B5" s="75">
+      <c r="A5" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="79">
         <v>1.0</v>
       </c>
-      <c r="C5" s="54" t="b">
+      <c r="C5" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="64" t="b">
+      <c r="D5" s="68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="49" t="s">
-        <v>279</v>
-      </c>
-      <c r="B6" s="76">
+      <c r="A6" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="80">
         <v>3.0</v>
       </c>
-      <c r="C6" s="50" t="b">
+      <c r="C6" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="61" t="b">
+      <c r="D6" s="66" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="53" t="s">
-        <v>280</v>
-      </c>
-      <c r="B7" s="76">
+      <c r="A7" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="80">
         <v>3.0</v>
       </c>
-      <c r="C7" s="54" t="b">
+      <c r="C7" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="64" t="b">
+      <c r="D7" s="68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="s">
-        <v>281</v>
-      </c>
-      <c r="B8" s="77">
+      <c r="A8" s="53" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" s="81">
         <v>5.0</v>
       </c>
-      <c r="C8" s="50" t="b">
+      <c r="C8" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="61" t="b">
+      <c r="D8" s="66" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="53" t="s">
-        <v>282</v>
-      </c>
-      <c r="B9" s="78">
+      <c r="A9" s="57" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" s="82">
         <v>4.0</v>
       </c>
-      <c r="C9" s="54" t="b">
+      <c r="C9" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="64" t="b">
+      <c r="D9" s="68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49" t="s">
-        <v>283</v>
-      </c>
-      <c r="B10" s="78">
+      <c r="A10" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="82">
         <v>4.0</v>
       </c>
-      <c r="C10" s="50" t="b">
+      <c r="C10" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="61" t="b">
+      <c r="D10" s="66" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="53" t="s">
-        <v>284</v>
-      </c>
-      <c r="B11" s="75">
+      <c r="A11" s="57" t="s">
+        <v>296</v>
+      </c>
+      <c r="B11" s="79">
         <v>1.0</v>
       </c>
-      <c r="C11" s="54" t="b">
+      <c r="C11" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="64" t="b">
+      <c r="D11" s="68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="79" t="s">
-        <v>285</v>
-      </c>
-      <c r="B12" s="78">
+      <c r="A12" s="83" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" s="82">
         <v>4.0</v>
       </c>
-      <c r="C12" s="50" t="b">
+      <c r="C12" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="61" t="b">
+      <c r="D12" s="66" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="79" t="s">
-        <v>286</v>
-      </c>
-      <c r="B13" s="75">
+      <c r="A13" s="83" t="s">
+        <v>298</v>
+      </c>
+      <c r="B13" s="79">
         <v>1.0</v>
       </c>
-      <c r="C13" s="54" t="b">
+      <c r="C13" s="58" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="64" t="b">
+      <c r="D13" s="68" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="65" t="s">
-        <v>287</v>
-      </c>
-      <c r="B14" s="80">
+      <c r="A14" s="69" t="s">
+        <v>299</v>
+      </c>
+      <c r="B14" s="84">
         <v>5.0</v>
       </c>
-      <c r="C14" s="71" t="b">
+      <c r="C14" s="73" t="b">
         <v>0</v>
       </c>
-      <c r="D14" s="66" t="b">
+      <c r="D14" s="70" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4642,7 +4763,7 @@
     </row>
     <row r="2">
       <c r="A2" s="29">
-        <f t="shared" ref="A2:A35" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A36" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -4927,7 +5048,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="15" t="s">
         <v>88</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -4946,28 +5067,28 @@
         <v>24</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>67</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
@@ -4975,47 +5096,45 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="16" t="s">
         <v>94</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="12" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="12" t="s">
         <v>67</v>
       </c>
+      <c r="I9" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="J9" s="13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
@@ -5023,13 +5142,13 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -5038,14 +5157,14 @@
       <c r="F10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>25</v>
+      <c r="G10" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>25</v>
@@ -5057,7 +5176,7 @@
         <v>25</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>25</v>
@@ -5083,14 +5202,16 @@
       <c r="E11" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="J11" s="13" t="s">
@@ -5103,10 +5224,10 @@
         <v>25</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="O11" s="14" t="s">
         <v>25</v>
@@ -5183,7 +5304,7 @@
         <v>25</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J13" s="13" t="s">
         <v>25</v>
@@ -5201,7 +5322,7 @@
         <v>67</v>
       </c>
       <c r="O13" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
@@ -5209,13 +5330,13 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="15" t="s">
         <v>112</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="15" t="s">
         <v>114</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -5228,26 +5349,26 @@
       <c r="H14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15">
@@ -5255,13 +5376,13 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="11" t="s">
         <v>116</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="11" t="s">
         <v>118</v>
       </c>
       <c r="E15" s="16" t="s">
@@ -5274,7 +5395,7 @@
       <c r="H15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="12" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="13" t="s">
@@ -5283,8 +5404,8 @@
       <c r="K15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="13" t="s">
-        <v>25</v>
+      <c r="L15" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>25</v>
@@ -5376,7 +5497,7 @@
         <v>25</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="M17" s="13" t="s">
         <v>25</v>
@@ -5413,16 +5534,16 @@
         <v>25</v>
       </c>
       <c r="I18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>25</v>
@@ -5459,16 +5580,16 @@
         <v>25</v>
       </c>
       <c r="I19" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="13" t="s">
         <v>24</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="M19" s="13" t="s">
         <v>25</v>
@@ -5508,16 +5629,16 @@
         <v>24</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>25</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="N20" s="8" t="s">
         <v>25</v>
@@ -5560,13 +5681,13 @@
         <v>25</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="M21" s="13" t="s">
         <v>67</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="O21" s="14" t="s">
         <v>25</v>
@@ -5597,7 +5718,7 @@
         <v>25</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>25</v>
@@ -5615,7 +5736,7 @@
         <v>67</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23">
@@ -5669,102 +5790,102 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24" s="35" t="s">
+      <c r="F24" s="20"/>
+      <c r="G24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="M24" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="N24" s="34" t="s">
+      <c r="J24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O24" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="37"/>
-      <c r="U24" s="37"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="37"/>
     </row>
     <row r="25">
       <c r="A25" s="30">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" s="13" t="s">
+      <c r="F25" s="33"/>
+      <c r="G25" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="J25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N25" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="O25" s="14" t="s">
+      <c r="M25" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="34" t="s">
         <v>24</v>
       </c>
+      <c r="O25" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="37"/>
     </row>
     <row r="26">
       <c r="A26" s="29">
@@ -5800,16 +5921,16 @@
         <v>25</v>
       </c>
       <c r="L26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O26" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O26" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="27">
@@ -5837,22 +5958,22 @@
         <v>25</v>
       </c>
       <c r="I27" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="M27" s="13" t="s">
         <v>25</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="O27" s="14" t="s">
         <v>25</v>
@@ -5883,22 +6004,22 @@
         <v>25</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="O28" s="9" t="s">
         <v>25</v>
@@ -5929,7 +6050,7 @@
         <v>25</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="J29" s="13" t="s">
         <v>25</v>
@@ -5938,7 +6059,7 @@
         <v>67</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="M29" s="13" t="s">
         <v>25</v>
@@ -5969,7 +6090,7 @@
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>25</v>
@@ -5981,19 +6102,19 @@
         <v>25</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31">
@@ -6021,7 +6142,7 @@
         <v>25</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>25</v>
@@ -6033,13 +6154,13 @@
         <v>67</v>
       </c>
       <c r="M31" s="13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="N31" s="13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="O31" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
@@ -6067,7 +6188,7 @@
         <v>25</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>25</v>
@@ -6079,7 +6200,7 @@
         <v>67</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N32" s="8" t="s">
         <v>25</v>
@@ -6113,19 +6234,19 @@
         <v>25</v>
       </c>
       <c r="I33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="J33" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L33" s="13" t="s">
+      <c r="M33" s="13" t="s">
         <v>24</v>
-      </c>
-      <c r="M33" s="13" t="s">
-        <v>25</v>
       </c>
       <c r="N33" s="13" t="s">
         <v>25</v>
@@ -6153,85 +6274,131 @@
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L34" s="8" t="s">
+      <c r="M34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O34" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="30">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F35" s="18"/>
+      <c r="G35" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="38">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" s="39" t="s">
+      <c r="M35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O35" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="38">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="C36" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D36" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="23" t="s">
+      <c r="E36" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="F36" s="41"/>
+      <c r="G36" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J35" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="K35" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L35" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="M35" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="N35" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="O35" s="26" t="s">
+      <c r="H36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="N36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="O36" s="43" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A35">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A36">
       <formula1>AND(ISNUMBER(A2),(NOT(OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D")))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:O35">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:O36">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6277,348 +6444,348 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>201</v>
-      </c>
-      <c r="F1" s="41" t="s">
+      <c r="B1" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="C1" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="D1" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="E1" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="F1" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="G1" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="H1" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="I1" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="J1" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="K1" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="L1" s="45" t="s">
         <v>212</v>
       </c>
-      <c r="Q1" s="42" t="s">
+      <c r="M1" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="R1" s="43" t="s">
+      <c r="N1" s="45" t="s">
         <v>214</v>
       </c>
+      <c r="O1" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q1" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="R1" s="47" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="44">
+      <c r="A2" s="48">
         <f t="shared" ref="A2:A6" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="C2" s="45" t="b">
+      <c r="B2" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="50">
         <f t="shared" ref="D2:D6" si="2">COUNTIF(E2,"=TRUE")+COUNTIF(L2,"=TRUE")</f>
         <v>0</v>
       </c>
-      <c r="E2" s="45" t="b">
+      <c r="E2" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="I2" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="J2" s="47" t="s">
+      <c r="F2" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="K2" s="44" t="b">
+      <c r="I2" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="K2" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="44" t="b">
+      <c r="L2" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="N2" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="O2" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="P2" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q2" s="47" t="s">
+      <c r="M2" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="N2" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="O2" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="R2" s="44" t="b">
+      <c r="P2" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q2" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="R2" s="48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="44">
+      <c r="A3" s="48">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="C3" s="45" t="b">
+      <c r="B3" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="50">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E3" s="45" t="b">
+      <c r="E3" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="G3" s="47" t="s">
+      <c r="F3" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="N3" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="H3" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="J3" s="47" t="s">
+      <c r="O3" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="K3" s="44" t="b">
+      <c r="P3" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q3" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="R3" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="48">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="L3" s="44" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="N3" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="O3" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="P3" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q3" s="47" t="s">
-        <v>219</v>
-      </c>
-      <c r="R3" s="44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="44">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>222</v>
-      </c>
-      <c r="C4" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="46">
+      <c r="D4" s="50">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E4" s="45" t="b">
+      <c r="E4" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="J4" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="K4" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="N4" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="H4" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="I4" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="J4" s="47" t="s">
+      <c r="O4" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="K4" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4" s="44" t="b">
+      <c r="P4" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q4" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="R4" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="N4" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="O4" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="P4" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q4" s="47" t="s">
-        <v>219</v>
-      </c>
-      <c r="R4" s="44" t="b">
+    </row>
+    <row r="5">
+      <c r="A5" s="48">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="44">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>224</v>
-      </c>
-      <c r="C5" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="46">
+      <c r="D5" s="50">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E5" s="45" t="b">
+      <c r="E5" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="G5" s="47" t="s">
-        <v>225</v>
-      </c>
-      <c r="H5" s="47" t="s">
+      <c r="F5" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="G5" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="K5" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="N5" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="O5" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="J5" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="K5" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="47" t="s">
+      <c r="P5" s="51" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q5" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="N5" s="47" t="s">
-        <v>225</v>
-      </c>
-      <c r="O5" s="47" t="s">
-        <v>222</v>
-      </c>
-      <c r="P5" s="47" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q5" s="47" t="s">
-        <v>219</v>
-      </c>
-      <c r="R5" s="44" t="b">
+      <c r="R5" s="48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="44">
+      <c r="A6" s="48">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="44" t="s">
-        <v>229</v>
-      </c>
-      <c r="C6" s="45" t="b">
+      <c r="B6" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E6" s="45" t="b">
+      <c r="E6" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="G6" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="J6" s="47" t="s">
+      <c r="F6" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="H6" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="K6" s="44" t="b">
+      <c r="I6" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="J6" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="K6" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="44" t="b">
+      <c r="L6" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="M6" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="N6" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="O6" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="P6" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q6" s="47" t="s">
+      <c r="M6" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="N6" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="O6" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="R6" s="44" t="b">
+      <c r="P6" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q6" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="R6" s="48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6674,118 +6841,118 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="53">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>241</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="57">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>231</v>
-      </c>
-      <c r="D1" s="41" t="s">
+      <c r="C3" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="53">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>234</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="49">
-        <v>0.0</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>236</v>
-      </c>
-      <c r="E2" s="51" t="s">
-        <v>237</v>
-      </c>
-      <c r="F2" s="51" t="s">
-        <v>238</v>
-      </c>
-      <c r="G2" s="52" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="53">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="54" t="s">
-        <v>226</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>239</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>237</v>
-      </c>
-      <c r="F3" s="55" t="s">
-        <v>238</v>
-      </c>
-      <c r="G3" s="56" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="49">
-        <v>2.0</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="D4" s="51" t="s">
+      <c r="C4" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>241</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="61">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="63" t="s">
         <v>240</v>
       </c>
-      <c r="E4" s="51" t="s">
-        <v>237</v>
-      </c>
-      <c r="F4" s="51" t="s">
+      <c r="E5" s="63" t="s">
         <v>241</v>
       </c>
-      <c r="G4" s="52" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="57">
-        <v>3.0</v>
-      </c>
-      <c r="B5" s="58" t="s">
+      <c r="F5" s="63" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>236</v>
-      </c>
-      <c r="E5" s="59" t="s">
-        <v>237</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>238</v>
-      </c>
-      <c r="G5" s="60" t="s">
-        <v>238</v>
+      <c r="G5" s="64" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -6822,49 +6989,83 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="21.57"/>
-    <col customWidth="1" min="3" max="3" width="59.14"/>
+    <col customWidth="1" min="3" max="3" width="22.43"/>
+    <col customWidth="1" min="4" max="5" width="32.14"/>
+    <col customWidth="1" min="6" max="6" width="21.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>243</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" s="48" t="s">
+      <c r="B1" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="53">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" s="65">
+        <f t="array" ref="D2">INDEX(Table_Rooms[N],MATCH(C2,Table_Rooms[ROOM_ID],0))</f>
+        <v>-1</v>
+      </c>
+      <c r="F2" s="54"/>
+      <c r="G2" s="66">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="49">
+      <c r="C3" s="63" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" s="62">
+        <f t="array" ref="D3">INDEX(Table_Rooms[N],MATCH(C3,Table_Rooms[ROOM_ID],0))</f>
+        <v>-1</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>255</v>
+      </c>
+      <c r="G3" s="67">
         <v>0.0</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>238</v>
-      </c>
-      <c r="D2" s="61">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="57">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="D3" s="62">
-        <v>0.0</v>
-      </c>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C3">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -6875,46 +7076,111 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="15.14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="53">
+        <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)-1</f>
+        <v>-1</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63" t="s">
-        <v>247</v>
+      <c r="B1" s="52" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="63">
+      <c r="A2" s="48">
         <f t="shared" ref="A2:A3" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="63" t="s">
-        <v>248</v>
+      <c r="B2" s="48" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="63">
+      <c r="A3" s="48">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="63" t="s">
-        <v>249</v>
+      <c r="B3" s="48" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF990000"/>
@@ -6935,147 +7201,147 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>250</v>
+      <c r="B1" s="52" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49">
+      <c r="A2" s="53">
         <v>0.0</v>
       </c>
-      <c r="B2" s="61" t="s">
-        <v>251</v>
+      <c r="B2" s="66" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="53">
+      <c r="A3" s="57">
         <v>1.0</v>
       </c>
-      <c r="B3" s="64" t="s">
-        <v>216</v>
+      <c r="B3" s="68" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="49">
+      <c r="A4" s="53">
         <v>2.0</v>
       </c>
-      <c r="B4" s="61" t="s">
-        <v>223</v>
+      <c r="B4" s="66" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="57">
+      <c r="A5" s="61">
         <v>3.0</v>
       </c>
-      <c r="B5" s="62" t="s">
-        <v>252</v>
+      <c r="B5" s="67" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>253</v>
+      <c r="B7" s="52" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="49">
+      <c r="A8" s="53">
         <v>0.0</v>
       </c>
-      <c r="B8" s="61" t="s">
-        <v>254</v>
+      <c r="B8" s="66" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="53">
+      <c r="A9" s="57">
         <v>1.0</v>
       </c>
-      <c r="B9" s="64" t="s">
-        <v>255</v>
+      <c r="B9" s="68" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49">
+      <c r="A10" s="53">
         <v>2.0</v>
       </c>
-      <c r="B10" s="61" t="s">
-        <v>236</v>
+      <c r="B10" s="66" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="53">
+      <c r="A11" s="57">
         <v>3.0</v>
       </c>
-      <c r="B11" s="64" t="s">
-        <v>237</v>
+      <c r="B11" s="68" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="49">
+      <c r="A12" s="53">
         <v>4.0</v>
       </c>
-      <c r="B12" s="61" t="s">
-        <v>240</v>
+      <c r="B12" s="66" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="57">
+      <c r="A13" s="61">
         <v>5.0</v>
       </c>
-      <c r="B13" s="62" t="s">
-        <v>239</v>
+      <c r="B13" s="67" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="48" t="s">
-        <v>256</v>
+      <c r="B15" s="52" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="49">
+      <c r="A16" s="53">
         <v>0.0</v>
       </c>
-      <c r="B16" s="61" t="s">
-        <v>217</v>
+      <c r="B16" s="66" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="53">
+      <c r="A17" s="57">
         <v>1.0</v>
       </c>
-      <c r="B17" s="64" t="s">
-        <v>221</v>
+      <c r="B17" s="68" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="49">
+      <c r="A18" s="53">
         <v>2.0</v>
       </c>
-      <c r="B18" s="61" t="s">
-        <v>225</v>
+      <c r="B18" s="66" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="53">
+      <c r="A19" s="57">
         <v>3.0</v>
       </c>
-      <c r="B19" s="64" t="s">
-        <v>257</v>
+      <c r="B19" s="68" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="65">
+      <c r="A20" s="69">
         <v>4.0</v>
       </c>
-      <c r="B20" s="66" t="s">
-        <v>258</v>
+      <c r="B20" s="70" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -7084,41 +7350,6 @@
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <tabColor rgb="FFB45F06"/>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="67" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="68">
-        <v>3.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7148,75 +7379,75 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>260</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>262</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>263</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>264</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>265</v>
+      <c r="B1" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49">
+      <c r="A2" s="53">
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="G2" s="70"/>
+      <c r="B2" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="G2" s="72"/>
     </row>
     <row r="3">
-      <c r="A3" s="53">
+      <c r="A3" s="57">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>227</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>266</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>220</v>
-      </c>
-      <c r="E3" s="55" t="s">
+      <c r="B3" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="56" t="s">
-        <v>227</v>
+      <c r="E3" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="58"/>
+      <c r="G3" s="60" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="65">
+      <c r="A4" s="69">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="71" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="G4" s="73"/>
+      <c r="B4" s="73" t="s">
+        <v>278</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="G4" s="75"/>
     </row>
   </sheetData>
   <dataValidations>

</xml_diff>

<commit_message>
[Partial] Adding dialogs -Basic dialog working -Refs for strings
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -20,7 +20,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="s4Gx29HYjtFA4VIdk44SgsA8ZMcTp6N/brQlDNGJdGY="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="NQY0q4nAuQW+tyNRdgL2oNSuG2ILqHEPgvkCiU5W2Lw="/>
     </ext>
   </extLst>
 </workbook>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="310">
   <si>
     <t>N</t>
   </si>
@@ -673,6 +673,18 @@
     <t>Starts a dialogue with given text and sound</t>
   </si>
   <si>
+    <t>SHOW_DIALOGUE</t>
+  </si>
+  <si>
+    <t>SHOW_DIALOGUE_DELEGATE</t>
+  </si>
+  <si>
+    <t>GraphicsMasterClass.ShowDialogueService</t>
+  </si>
+  <si>
+    <t>Tell Graphics Maste which dialogue to show</t>
+  </si>
+  <si>
     <t>LAST_SERVICE</t>
   </si>
   <si>
@@ -823,6 +835,9 @@
     <t>Room_Code</t>
   </si>
   <si>
+    <t>Sender</t>
+  </si>
+  <si>
     <t>Text_English</t>
   </si>
   <si>
@@ -835,6 +850,9 @@
     <t>ROOM_NONE</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
     <t>That has no sense!</t>
   </si>
   <si>
@@ -884,6 +902,18 @@
   </si>
   <si>
     <t>INTERACTION_TAKE_AND_RECEIVE</t>
+  </si>
+  <si>
+    <t>CharName</t>
+  </si>
+  <si>
+    <t>Main Character</t>
+  </si>
+  <si>
+    <t>Parrot Character</t>
+  </si>
+  <si>
+    <t>Snake Character</t>
   </si>
   <si>
     <t>EVENT_ID</t>
@@ -1204,21 +1234,21 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF284E3F"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF284E3F"/>
+        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
@@ -1246,16 +1276,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF284E3F"/>
       </bottom>
     </border>
     <border>
@@ -1374,7 +1404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="81">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1489,23 +1519,11 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1519,85 +1537,85 @@
     <xf borderId="3" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1683,7 +1701,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="13">
+  <tableStyles count="14">
     <tableStyle count="3" pivot="0" name="VARMAP-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1730,6 +1748,11 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="CHARACTERS-style 3">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="CHARACTERS-style 4">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1837,7 +1860,17 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Events" name="Table_Events" id="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A22:B25" displayName="Table_Characters_Name" name="Table_Characters_Name" id="11">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="CharName" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="CHARACTERS-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Events" name="Table_Events" id="12">
   <tableColumns count="7">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_ID" id="2"/>
@@ -1851,8 +1884,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A2" displayName="Table_Constants" name="Table_Constants" id="12">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A2" displayName="Table_Constants" name="Table_Constants" id="13">
   <tableColumns count="1">
     <tableColumn name="NUM_PLAYERS" id="1"/>
   </tableColumns>
@@ -1860,8 +1893,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D14" displayName="Table_TODO" name="Table_TODO" id="13">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D14" displayName="Table_TODO" name="Table_TODO" id="14">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -1873,7 +1906,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O36" displayName="Table_Services" name="Table_Services" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O37" displayName="Table_Services" name="Table_Services" id="2">
   <tableColumns count="15">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SERVICE_ID" id="2"/>
@@ -1937,15 +1970,16 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G3" displayName="Table_Dialogs" name="Table_Dialogs" id="5">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H3" displayName="Table_Dialogs" name="Table_Dialogs" id="5">
+  <tableColumns count="8">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ID" id="2"/>
     <tableColumn name="Room_used" id="3"/>
     <tableColumn name="Room_Code" id="4"/>
-    <tableColumn name="Text_English" id="5"/>
-    <tableColumn name="Text_Spanish" id="6"/>
-    <tableColumn name="Sound" id="7"/>
+    <tableColumn name="Sender" id="5"/>
+    <tableColumn name="Text_English" id="6"/>
+    <tableColumn name="Text_Spanish" id="7"/>
+    <tableColumn name="Sound" id="8"/>
   </tableColumns>
   <tableStyleInfo name="DIALOGS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -4037,12 +4071,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="76" t="s">
-        <v>279</v>
+      <c r="A1" s="72" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="77">
+      <c r="A2" s="73">
         <v>3.0</v>
       </c>
     </row>
@@ -4073,10 +4107,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2">
@@ -4084,12 +4118,12 @@
         <f t="shared" ref="A2:A32" si="1">ROW()-ROW($G$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="78" t="str">
+      <c r="B2" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A2,0)</f>
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3">
@@ -4097,12 +4131,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="78" t="str">
+      <c r="B3" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A3,0)</f>
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4">
@@ -4110,12 +4144,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="78" t="str">
+      <c r="B4" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A4,0)</f>
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5">
@@ -4123,12 +4157,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="78" t="str">
+      <c r="B5" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A5,0)</f>
         <v>ITEM_LAST</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6">
@@ -4136,297 +4170,297 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="78" t="str">
+      <c r="B6" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A6,0)</f>
         <v/>
       </c>
-      <c r="C6" s="78"/>
+      <c r="C6" s="74"/>
     </row>
     <row r="7">
       <c r="A7" s="27">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="78" t="str">
+      <c r="B7" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A7,0)</f>
         <v/>
       </c>
-      <c r="C7" s="78"/>
+      <c r="C7" s="74"/>
     </row>
     <row r="8">
       <c r="A8" s="27">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="78" t="str">
+      <c r="B8" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A8,0)</f>
         <v/>
       </c>
-      <c r="C8" s="78"/>
+      <c r="C8" s="74"/>
     </row>
     <row r="9">
       <c r="A9" s="27">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="78" t="str">
+      <c r="B9" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A9,0)</f>
         <v/>
       </c>
-      <c r="C9" s="78"/>
+      <c r="C9" s="74"/>
     </row>
     <row r="10">
       <c r="A10" s="27">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="78" t="str">
+      <c r="B10" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A10,0)</f>
         <v/>
       </c>
-      <c r="C10" s="78"/>
+      <c r="C10" s="74"/>
     </row>
     <row r="11">
       <c r="A11" s="27">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="78" t="str">
+      <c r="B11" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A11,0)</f>
         <v/>
       </c>
-      <c r="C11" s="78"/>
+      <c r="C11" s="74"/>
     </row>
     <row r="12">
       <c r="A12" s="27">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="78" t="str">
+      <c r="B12" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A12,0)</f>
         <v/>
       </c>
-      <c r="C12" s="78"/>
+      <c r="C12" s="74"/>
     </row>
     <row r="13">
       <c r="A13" s="27">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="78" t="str">
+      <c r="B13" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A13,0)</f>
         <v/>
       </c>
-      <c r="C13" s="78"/>
+      <c r="C13" s="74"/>
     </row>
     <row r="14">
       <c r="A14" s="27">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="78" t="str">
+      <c r="B14" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A14,0)</f>
         <v/>
       </c>
-      <c r="C14" s="78"/>
+      <c r="C14" s="74"/>
     </row>
     <row r="15">
       <c r="A15" s="27">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="78" t="str">
+      <c r="B15" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A15,0)</f>
         <v/>
       </c>
-      <c r="C15" s="78"/>
+      <c r="C15" s="74"/>
     </row>
     <row r="16">
       <c r="A16" s="27">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="78" t="str">
+      <c r="B16" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A16,0)</f>
         <v/>
       </c>
-      <c r="C16" s="78"/>
+      <c r="C16" s="74"/>
     </row>
     <row r="17">
       <c r="A17" s="27">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="78" t="str">
+      <c r="B17" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A17,0)</f>
         <v/>
       </c>
-      <c r="C17" s="78"/>
+      <c r="C17" s="74"/>
     </row>
     <row r="18">
       <c r="A18" s="27">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="78" t="str">
+      <c r="B18" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A18,0)</f>
         <v/>
       </c>
-      <c r="C18" s="78"/>
+      <c r="C18" s="74"/>
     </row>
     <row r="19">
       <c r="A19" s="27">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="78" t="str">
+      <c r="B19" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A19,0)</f>
         <v/>
       </c>
-      <c r="C19" s="78"/>
+      <c r="C19" s="74"/>
     </row>
     <row r="20">
       <c r="A20" s="27">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="78" t="str">
+      <c r="B20" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A20,0)</f>
         <v/>
       </c>
-      <c r="C20" s="78"/>
+      <c r="C20" s="74"/>
     </row>
     <row r="21">
       <c r="A21" s="27">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="78" t="str">
+      <c r="B21" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A21,0)</f>
         <v/>
       </c>
-      <c r="C21" s="78"/>
+      <c r="C21" s="74"/>
     </row>
     <row r="22">
       <c r="A22" s="27">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="78" t="str">
+      <c r="B22" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A22,0)</f>
         <v/>
       </c>
-      <c r="C22" s="78"/>
+      <c r="C22" s="74"/>
     </row>
     <row r="23">
       <c r="A23" s="27">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="78" t="str">
+      <c r="B23" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A23,0)</f>
         <v/>
       </c>
-      <c r="C23" s="78"/>
+      <c r="C23" s="74"/>
     </row>
     <row r="24">
       <c r="A24" s="27">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="78" t="str">
+      <c r="B24" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A24,0)</f>
         <v/>
       </c>
-      <c r="C24" s="78"/>
+      <c r="C24" s="74"/>
     </row>
     <row r="25">
       <c r="A25" s="27">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="78" t="str">
+      <c r="B25" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A25,0)</f>
         <v/>
       </c>
-      <c r="C25" s="78"/>
+      <c r="C25" s="74"/>
     </row>
     <row r="26">
       <c r="A26" s="27">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="78" t="str">
+      <c r="B26" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A26,0)</f>
         <v/>
       </c>
-      <c r="C26" s="78"/>
+      <c r="C26" s="74"/>
     </row>
     <row r="27">
       <c r="A27" s="27">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="78" t="str">
+      <c r="B27" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A27,0)</f>
         <v/>
       </c>
-      <c r="C27" s="78"/>
+      <c r="C27" s="74"/>
     </row>
     <row r="28">
       <c r="A28" s="27">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="78" t="str">
+      <c r="B28" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A28,0)</f>
         <v/>
       </c>
-      <c r="C28" s="78"/>
+      <c r="C28" s="74"/>
     </row>
     <row r="29">
       <c r="A29" s="27">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="78" t="str">
+      <c r="B29" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A29,0)</f>
         <v/>
       </c>
-      <c r="C29" s="78"/>
+      <c r="C29" s="74"/>
     </row>
     <row r="30">
       <c r="A30" s="27">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="78" t="str">
+      <c r="B30" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A30,0)</f>
         <v/>
       </c>
-      <c r="C30" s="78"/>
+      <c r="C30" s="74"/>
     </row>
     <row r="31">
       <c r="A31" s="27">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="78" t="str">
+      <c r="B31" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A31,0)</f>
         <v/>
       </c>
-      <c r="C31" s="78"/>
+      <c r="C31" s="74"/>
     </row>
     <row r="32">
       <c r="A32" s="27">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="78" t="str">
+      <c r="B32" s="74" t="str">
         <f>OFFSET(ITEMS!$B$3,A32,0)</f>
         <v/>
       </c>
-      <c r="C32" s="78"/>
+      <c r="C32" s="74"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -4458,198 +4492,198 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>284</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>285</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>286</v>
+      <c r="A1" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53" t="s">
-        <v>287</v>
-      </c>
-      <c r="B2" s="79">
+      <c r="A2" s="49" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="75">
         <v>1.0</v>
       </c>
-      <c r="C2" s="54" t="b">
+      <c r="C2" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="66" t="b">
+      <c r="D2" s="62" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="B3" s="79">
+      <c r="A3" s="53" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="75">
         <v>1.0</v>
       </c>
-      <c r="C3" s="58" t="b">
+      <c r="C3" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="68" t="b">
+      <c r="D3" s="64" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53" t="s">
-        <v>289</v>
-      </c>
-      <c r="B4" s="80">
+      <c r="A4" s="49" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="76">
         <v>3.0</v>
       </c>
-      <c r="C4" s="54" t="b">
+      <c r="C4" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="66" t="b">
+      <c r="D4" s="62" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="57" t="s">
-        <v>290</v>
-      </c>
-      <c r="B5" s="79">
+      <c r="A5" s="53" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" s="75">
         <v>1.0</v>
       </c>
-      <c r="C5" s="58" t="b">
+      <c r="C5" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="68" t="b">
+      <c r="D5" s="64" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="53" t="s">
-        <v>291</v>
-      </c>
-      <c r="B6" s="80">
+      <c r="A6" s="49" t="s">
+        <v>301</v>
+      </c>
+      <c r="B6" s="76">
         <v>3.0</v>
       </c>
-      <c r="C6" s="54" t="b">
+      <c r="C6" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="66" t="b">
+      <c r="D6" s="62" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="57" t="s">
-        <v>292</v>
-      </c>
-      <c r="B7" s="80">
+      <c r="A7" s="53" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7" s="76">
         <v>3.0</v>
       </c>
-      <c r="C7" s="58" t="b">
+      <c r="C7" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="68" t="b">
+      <c r="D7" s="64" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="53" t="s">
-        <v>293</v>
-      </c>
-      <c r="B8" s="81">
+      <c r="A8" s="49" t="s">
+        <v>303</v>
+      </c>
+      <c r="B8" s="77">
         <v>5.0</v>
       </c>
-      <c r="C8" s="54" t="b">
+      <c r="C8" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="66" t="b">
+      <c r="D8" s="62" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="57" t="s">
-        <v>294</v>
-      </c>
-      <c r="B9" s="82">
+      <c r="A9" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9" s="78">
         <v>4.0</v>
       </c>
-      <c r="C9" s="58" t="b">
+      <c r="C9" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="68" t="b">
+      <c r="D9" s="64" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="53" t="s">
-        <v>295</v>
-      </c>
-      <c r="B10" s="82">
+      <c r="A10" s="49" t="s">
+        <v>305</v>
+      </c>
+      <c r="B10" s="78">
         <v>4.0</v>
       </c>
-      <c r="C10" s="54" t="b">
+      <c r="C10" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="66" t="b">
+      <c r="D10" s="62" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="57" t="s">
-        <v>296</v>
-      </c>
-      <c r="B11" s="79">
+      <c r="A11" s="53" t="s">
+        <v>306</v>
+      </c>
+      <c r="B11" s="75">
         <v>1.0</v>
       </c>
-      <c r="C11" s="58" t="b">
+      <c r="C11" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="68" t="b">
+      <c r="D11" s="64" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="83" t="s">
-        <v>297</v>
-      </c>
-      <c r="B12" s="82">
+      <c r="A12" s="79" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" s="78">
         <v>4.0</v>
       </c>
-      <c r="C12" s="54" t="b">
+      <c r="C12" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="66" t="b">
+      <c r="D12" s="62" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="83" t="s">
-        <v>298</v>
-      </c>
-      <c r="B13" s="79">
+      <c r="A13" s="79" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" s="75">
         <v>1.0</v>
       </c>
-      <c r="C13" s="58" t="b">
+      <c r="C13" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="68" t="b">
+      <c r="D13" s="64" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="69" t="s">
-        <v>299</v>
-      </c>
-      <c r="B14" s="84">
+      <c r="A14" s="65" t="s">
+        <v>309</v>
+      </c>
+      <c r="B14" s="80">
         <v>5.0</v>
       </c>
-      <c r="C14" s="73" t="b">
+      <c r="C14" s="69" t="b">
         <v>0</v>
       </c>
-      <c r="D14" s="70" t="b">
+      <c r="D14" s="66" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4763,7 +4797,7 @@
     </row>
     <row r="2">
       <c r="A2" s="29">
-        <f t="shared" ref="A2:A36" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A37" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -6348,57 +6382,103 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="38">
+      <c r="A36" s="29">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O36" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="38">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="40" t="s">
+      <c r="D37" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="F36" s="41"/>
-      <c r="G36" s="42" t="s">
+      <c r="E37" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="F37" s="25"/>
+      <c r="G37" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="I36" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="J36" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="K36" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="L36" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="M36" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="N36" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="O36" s="43" t="s">
+      <c r="H37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="O37" s="26" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A36">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A37">
       <formula1>AND(ISNUMBER(A2),(NOT(OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D")))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:O36">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:O37">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6444,348 +6524,348 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>202</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>205</v>
-      </c>
-      <c r="F1" s="45" t="s">
+      <c r="B1" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="C1" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="D1" s="41" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="E1" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="F1" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="G1" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="H1" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="I1" s="41" t="s">
         <v>213</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="J1" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="K1" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="L1" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="M1" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="N1" s="41" t="s">
         <v>218</v>
       </c>
+      <c r="O1" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="P1" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q1" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="R1" s="43" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="48">
+      <c r="A2" s="44">
         <f t="shared" ref="A2:A6" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="48" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="49" t="b">
+      <c r="B2" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="50">
+      <c r="D2" s="46">
         <f t="shared" ref="D2:D6" si="2">COUNTIF(E2,"=TRUE")+COUNTIF(L2,"=TRUE")</f>
         <v>0</v>
       </c>
-      <c r="E2" s="49" t="b">
+      <c r="E2" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="H2" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="J2" s="51" t="s">
+      <c r="F2" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="H2" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="K2" s="48" t="b">
+      <c r="I2" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="K2" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="48" t="b">
+      <c r="L2" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="N2" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="O2" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="P2" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q2" s="51" t="s">
+      <c r="M2" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="N2" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="O2" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="R2" s="48" t="b">
+      <c r="P2" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q2" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="R2" s="44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="48">
+      <c r="A3" s="44">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" s="49" t="b">
+      <c r="B3" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="50">
+      <c r="D3" s="46">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E3" s="49" t="b">
+      <c r="E3" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="G3" s="51" t="s">
+      <c r="F3" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="K3" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="N3" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="H3" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="I3" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="J3" s="51" t="s">
+      <c r="O3" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="48" t="b">
+      <c r="P3" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q3" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="R3" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="44">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="C4" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="L3" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="N3" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="O3" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="P3" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q3" s="51" t="s">
-        <v>223</v>
-      </c>
-      <c r="R3" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="48">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="50">
+      <c r="D4" s="46">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E4" s="49" t="b">
+      <c r="E4" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="J4" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="K4" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="N4" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="H4" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="I4" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="J4" s="51" t="s">
+      <c r="O4" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="K4" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4" s="48" t="b">
+      <c r="P4" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q4" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="R4" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="N4" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="O4" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="P4" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q4" s="51" t="s">
-        <v>223</v>
-      </c>
-      <c r="R4" s="48" t="b">
+    </row>
+    <row r="5">
+      <c r="A5" s="44">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="48">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>228</v>
-      </c>
-      <c r="C5" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="50">
+      <c r="D5" s="46">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E5" s="49" t="b">
+      <c r="E5" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="G5" s="51" t="s">
-        <v>229</v>
-      </c>
-      <c r="H5" s="51" t="s">
+      <c r="F5" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="G5" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="I5" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="J5" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="K5" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="N5" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="O5" s="47" t="s">
         <v>230</v>
       </c>
-      <c r="J5" s="51" t="s">
-        <v>231</v>
-      </c>
-      <c r="K5" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="51" t="s">
+      <c r="P5" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q5" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="N5" s="51" t="s">
-        <v>229</v>
-      </c>
-      <c r="O5" s="51" t="s">
-        <v>226</v>
-      </c>
-      <c r="P5" s="51" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q5" s="51" t="s">
-        <v>223</v>
-      </c>
-      <c r="R5" s="48" t="b">
+      <c r="R5" s="44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="48">
+      <c r="A6" s="44">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="48" t="s">
-        <v>233</v>
-      </c>
-      <c r="C6" s="49" t="b">
+      <c r="B6" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="50">
+      <c r="D6" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E6" s="49" t="b">
+      <c r="E6" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="H6" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="I6" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="J6" s="51" t="s">
+      <c r="F6" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="H6" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="K6" s="48" t="b">
+      <c r="I6" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="J6" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="K6" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="48" t="b">
+      <c r="L6" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="M6" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="N6" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="O6" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="P6" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q6" s="51" t="s">
+      <c r="M6" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="N6" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="O6" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="R6" s="48" t="b">
+      <c r="P6" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q6" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="R6" s="44" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6841,118 +6921,118 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="49">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="53">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="45" t="s">
-        <v>235</v>
-      </c>
-      <c r="D1" s="45" t="s">
+      <c r="C3" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" s="55" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="49">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="50" t="s">
         <v>236</v>
       </c>
-      <c r="E1" s="45" t="s">
-        <v>237</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>238</v>
-      </c>
-      <c r="G1" s="52" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>222</v>
-      </c>
-      <c r="C2" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>240</v>
-      </c>
-      <c r="E2" s="55" t="s">
-        <v>241</v>
-      </c>
-      <c r="F2" s="55" t="s">
-        <v>242</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="57">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="59" t="s">
-        <v>243</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>241</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>242</v>
-      </c>
-      <c r="G3" s="60" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="53">
-        <v>2.0</v>
-      </c>
-      <c r="B4" s="54" t="s">
-        <v>232</v>
-      </c>
-      <c r="C4" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="D4" s="55" t="s">
+      <c r="C4" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="57">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="55" t="s">
-        <v>241</v>
-      </c>
-      <c r="F4" s="55" t="s">
+      <c r="E5" s="59" t="s">
         <v>245</v>
       </c>
-      <c r="G4" s="56" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="61">
-        <v>3.0</v>
-      </c>
-      <c r="B5" s="62" t="s">
+      <c r="F5" s="59" t="s">
         <v>246</v>
       </c>
-      <c r="C5" s="63" t="s">
-        <v>223</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>240</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" s="63" t="s">
-        <v>242</v>
-      </c>
-      <c r="G5" s="64" t="s">
-        <v>242</v>
+      <c r="G5" s="60" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -6990,73 +7070,79 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="21.57"/>
     <col customWidth="1" min="3" max="3" width="22.43"/>
-    <col customWidth="1" min="4" max="5" width="32.14"/>
-    <col customWidth="1" min="6" max="6" width="21.0"/>
+    <col customWidth="1" min="4" max="6" width="32.14"/>
+    <col customWidth="1" min="7" max="7" width="21.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>247</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>248</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>249</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="F1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="C1" s="42" t="s">
         <v>252</v>
       </c>
+      <c r="D1" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <v>0.0</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="C2" s="55" t="s">
-        <v>253</v>
-      </c>
-      <c r="D2" s="65">
+      <c r="B2" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="61">
         <f t="array" ref="D2">INDEX(Table_Rooms[N],MATCH(C2,Table_Rooms[ROOM_ID],0))</f>
         <v>-1</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="66">
+      <c r="G2" s="50"/>
+      <c r="H2" s="62">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="61">
+      <c r="A3" s="57">
         <v>1.0</v>
       </c>
-      <c r="B3" s="62" t="s">
-        <v>245</v>
-      </c>
-      <c r="C3" s="63" t="s">
-        <v>253</v>
-      </c>
-      <c r="D3" s="62">
+      <c r="B3" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="58">
         <f t="array" ref="D3">INDEX(Table_Rooms[N],MATCH(C3,Table_Rooms[ROOM_ID],0))</f>
         <v>-1</v>
       </c>
-      <c r="E3" s="62" t="s">
-        <v>254</v>
-      </c>
-      <c r="F3" s="62" t="s">
-        <v>255</v>
-      </c>
-      <c r="G3" s="67">
+      <c r="E3" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>260</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>261</v>
+      </c>
+      <c r="H3" s="63">
         <v>0.0</v>
       </c>
     </row>
@@ -7090,38 +7176,38 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>256</v>
+      <c r="B1" s="48" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
-      <c r="B2" s="66" t="s">
-        <v>253</v>
+      <c r="B2" s="62" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="57">
+      <c r="A3" s="53">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="B3" s="68" t="s">
-        <v>257</v>
+      <c r="B3" s="64" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="69">
+      <c r="A4" s="65">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B4" s="70" t="s">
-        <v>258</v>
+      <c r="B4" s="66" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -7147,29 +7233,29 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>259</v>
+      <c r="B1" s="48" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="48">
+      <c r="A2" s="44">
         <f t="shared" ref="A2:A3" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="48" t="s">
-        <v>260</v>
+      <c r="B2" s="44" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="48">
+      <c r="A3" s="44">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
-        <v>261</v>
+      <c r="B3" s="44" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -7201,155 +7287,188 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>262</v>
+      <c r="B1" s="48" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <v>0.0</v>
       </c>
-      <c r="B2" s="66" t="s">
-        <v>263</v>
+      <c r="B2" s="62" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="57">
+      <c r="A3" s="53">
         <v>1.0</v>
       </c>
-      <c r="B3" s="68" t="s">
-        <v>220</v>
+      <c r="B3" s="64" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53">
+      <c r="A4" s="49">
         <v>2.0</v>
       </c>
-      <c r="B4" s="66" t="s">
-        <v>227</v>
+      <c r="B4" s="62" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="61">
+      <c r="A5" s="57">
         <v>3.0</v>
       </c>
-      <c r="B5" s="67" t="s">
-        <v>264</v>
+      <c r="B5" s="63" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>265</v>
+      <c r="B7" s="48" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="53">
+      <c r="A8" s="49">
         <v>0.0</v>
       </c>
-      <c r="B8" s="66" t="s">
-        <v>266</v>
+      <c r="B8" s="62" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="57">
+      <c r="A9" s="53">
         <v>1.0</v>
       </c>
-      <c r="B9" s="68" t="s">
-        <v>267</v>
+      <c r="B9" s="64" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="53">
+      <c r="A10" s="49">
         <v>2.0</v>
       </c>
-      <c r="B10" s="66" t="s">
-        <v>240</v>
+      <c r="B10" s="62" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="57">
+      <c r="A11" s="53">
         <v>3.0</v>
       </c>
-      <c r="B11" s="68" t="s">
-        <v>241</v>
+      <c r="B11" s="64" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="53">
+      <c r="A12" s="49">
         <v>4.0</v>
       </c>
-      <c r="B12" s="66" t="s">
-        <v>244</v>
+      <c r="B12" s="62" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="61">
+      <c r="A13" s="57">
         <v>5.0</v>
       </c>
-      <c r="B13" s="67" t="s">
-        <v>243</v>
+      <c r="B13" s="63" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="52" t="s">
-        <v>268</v>
+      <c r="B15" s="48" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="53">
+      <c r="A16" s="49">
         <v>0.0</v>
       </c>
-      <c r="B16" s="66" t="s">
-        <v>221</v>
+      <c r="B16" s="62" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="57">
+      <c r="A17" s="53">
         <v>1.0</v>
       </c>
-      <c r="B17" s="68" t="s">
-        <v>225</v>
+      <c r="B17" s="64" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="53">
+      <c r="A18" s="49">
         <v>2.0</v>
       </c>
-      <c r="B18" s="66" t="s">
-        <v>229</v>
+      <c r="B18" s="62" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="57">
+      <c r="A19" s="53">
         <v>3.0</v>
       </c>
-      <c r="B19" s="68" t="s">
-        <v>269</v>
+      <c r="B19" s="64" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="69">
+      <c r="A20" s="65">
         <v>4.0</v>
       </c>
-      <c r="B20" s="70" t="s">
-        <v>270</v>
+      <c r="B20" s="66" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="49">
+        <v>0.0</v>
+      </c>
+      <c r="B23" s="62" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="53">
+        <v>1.0</v>
+      </c>
+      <c r="B24" s="64" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="65">
+        <v>2.0</v>
+      </c>
+      <c r="B25" s="66" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
-  <tableParts count="3">
-    <tablePart r:id="rId5"/>
+  <tableParts count="4">
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7379,75 +7498,75 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>271</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>272</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>273</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>274</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="G1" s="52" t="s">
-        <v>276</v>
+      <c r="B1" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="G2" s="72"/>
+      <c r="B2" s="50" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="G2" s="68"/>
     </row>
     <row r="3">
-      <c r="A3" s="57">
+      <c r="A3" s="53">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>231</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>277</v>
-      </c>
-      <c r="D3" s="59" t="s">
-        <v>224</v>
-      </c>
-      <c r="E3" s="59" t="s">
+      <c r="B3" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="55" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="60" t="s">
-        <v>231</v>
+      <c r="E3" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="F3" s="54"/>
+      <c r="G3" s="56" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="69">
+      <c r="A4" s="65">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="73" t="s">
-        <v>278</v>
-      </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="G4" s="75"/>
+      <c r="B4" s="69" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="G4" s="71"/>
     </row>
   </sheetData>
   <dataValidations>

</xml_diff>

<commit_message>
[Partial] Adding dialogs -Distinction between dialog, option and phrase
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -20,7 +20,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="NQY0q4nAuQW+tyNRdgL2oNSuG2ILqHEPgvkCiU5W2Lw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="WtgYArt80jdk3iwt6u2KNbEVbrbmYhjnqhBUXFxjKn4="/>
     </ext>
   </extLst>
 </workbook>
@@ -70,8 +70,30 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="D7">
+      <text>
+        <t xml:space="preserve">Event triggered after all phrases
+======</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E7">
+      <text>
+        <t xml:space="preserve">New dialog shown after all phrases have been said
+======</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="348">
   <si>
     <t>N</t>
   </si>
@@ -802,9 +824,15 @@
     <t>Dialog_OK</t>
   </si>
   <si>
+    <t>Phrase_OK</t>
+  </si>
+  <si>
     <t>Dialog_NOK_Event</t>
   </si>
   <si>
+    <t>Phrase_NOK_Event</t>
+  </si>
+  <si>
     <t>ITEM_USE_ANIMATION_TAKE</t>
   </si>
   <si>
@@ -814,13 +842,19 @@
     <t>DIALOG_NONE</t>
   </si>
   <si>
+    <t>PHRASE_NONE</t>
+  </si>
+  <si>
     <t>ITEM_USE_ANIMATION_POUR</t>
   </si>
   <si>
     <t>ITEM_USE_ANIMATION_STARE_SCREEN</t>
   </si>
   <si>
-    <t>DIALOG_NONSENSE</t>
+    <t>DIALOG_SIMPLE</t>
+  </si>
+  <si>
+    <t>PHRASE_NONSENSE</t>
   </si>
   <si>
     <t>COND_LAST</t>
@@ -832,7 +866,97 @@
     <t>Room_used</t>
   </si>
   <si>
-    <t>Room_Code</t>
+    <t>Options_Count</t>
+  </si>
+  <si>
+    <t>Option1</t>
+  </si>
+  <si>
+    <t>Option2</t>
+  </si>
+  <si>
+    <t>Option3</t>
+  </si>
+  <si>
+    <t>Option4</t>
+  </si>
+  <si>
+    <t>Option5</t>
+  </si>
+  <si>
+    <t>Option6</t>
+  </si>
+  <si>
+    <t>Option7</t>
+  </si>
+  <si>
+    <t>Option8</t>
+  </si>
+  <si>
+    <t>ROOM_NONE</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_NONE</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_SIMPLE</t>
+  </si>
+  <si>
+    <t>DIALOG_FOUNTAIN</t>
+  </si>
+  <si>
+    <t>ROOM_FIRST</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_ASK_FOUNTAIN_1</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_ASK_FOUNTAIN_2</t>
+  </si>
+  <si>
+    <t>DIALOG_LAST</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_ID</t>
+  </si>
+  <si>
+    <t>EventCondition</t>
+  </si>
+  <si>
+    <t>EventTriggered</t>
+  </si>
+  <si>
+    <t>DialogTriggered</t>
+  </si>
+  <si>
+    <t>PhraseCount</t>
+  </si>
+  <si>
+    <t>Phrase1</t>
+  </si>
+  <si>
+    <t>Phrase2</t>
+  </si>
+  <si>
+    <t>Phrase3</t>
+  </si>
+  <si>
+    <t>Phrase4</t>
+  </si>
+  <si>
+    <t>PHRASE_ASK_FOUNTAIN1_1</t>
+  </si>
+  <si>
+    <t>PHRASE_ASK_FOUNTAIN1_2</t>
+  </si>
+  <si>
+    <t>PHRASE_ASK_FOUNTAIN2_1</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_LAST</t>
+  </si>
+  <si>
+    <t>PHRASE_ID</t>
   </si>
   <si>
     <t>Sender</t>
@@ -847,9 +971,6 @@
     <t>Sound</t>
   </si>
   <si>
-    <t>ROOM_NONE</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -859,10 +980,25 @@
     <t>¡Eso no tiene sentido!</t>
   </si>
   <si>
+    <t>Are you the fountain?</t>
+  </si>
+  <si>
+    <t>¿Eres tú la fuente?</t>
+  </si>
+  <si>
+    <t>Sure?</t>
+  </si>
+  <si>
+    <t>¿De verdad?</t>
+  </si>
+  <si>
+    <t>Why are you red?</t>
+  </si>
+  <si>
+    <t>¿Por qué estás roja?</t>
+  </si>
+  <si>
     <t>ROOM_ID</t>
-  </si>
-  <si>
-    <t>ROOM_FIRST</t>
   </si>
   <si>
     <t>ROOM_LAST</t>
@@ -1265,7 +1401,7 @@
         <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FF284E3F"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
         <color rgb="FFFFFFFF"/>
@@ -1279,7 +1415,7 @@
         <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF284E3F"/>
       </right>
       <top style="thin">
         <color rgb="FFFFFFFF"/>
@@ -1346,6 +1482,20 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB7E1CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB7E1CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB7E1CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF57BB8A"/>
       </left>
       <right style="thin">
@@ -1374,20 +1524,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB7E1CD"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB7E1CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB7E1CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF57BB8A"/>
       </left>
       <right style="thin">
@@ -1404,7 +1540,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="97">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1588,37 +1724,85 @@
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1701,7 +1885,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="14">
+  <tableStyles count="16">
     <tableStyle count="3" pivot="0" name="VARMAP-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1723,6 +1907,16 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="DIALOGS-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="DIALOGS-style 2">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="DIALOGS-style 3">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1850,7 +2044,27 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B20" displayName="Table_Interaction" name="Table_Interaction" id="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="10">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="Type" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="CHARACTERS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="11">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="ANIMATION_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="CHARACTERS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B20" displayName="Table_Interaction" name="Table_Interaction" id="12">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="INTERACTION_ID" id="2"/>
@@ -1859,8 +2073,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A22:B25" displayName="Table_Characters_Name" name="Table_Characters_Name" id="11">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A22:B25" displayName="Table_Characters_Name" name="Table_Characters_Name" id="13">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="CharName" id="2"/>
@@ -1869,8 +2083,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Events" name="Table_Events" id="12">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Events" name="Table_Events" id="14">
   <tableColumns count="7">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_ID" id="2"/>
@@ -1884,8 +2098,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A2" displayName="Table_Constants" name="Table_Constants" id="13">
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A2" displayName="Table_Constants" name="Table_Constants" id="15">
   <tableColumns count="1">
     <tableColumn name="NUM_PLAYERS" id="1"/>
   </tableColumns>
@@ -1893,8 +2107,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D14" displayName="Table_TODO" name="Table_TODO" id="14">
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D14" displayName="Table_TODO" name="Table_TODO" id="16">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -1955,38 +2169,77 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G5" displayName="Table_Item_Conditions" name="Table_Item_Conditions" id="4">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I5" displayName="Table_Item_Conditions" name="Table_Item_Conditions" id="4">
+  <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_COND_ID" id="2"/>
     <tableColumn name="Event" id="3"/>
     <tableColumn name="Animation_OK" id="4"/>
     <tableColumn name="Animation_NOK_Event" id="5"/>
     <tableColumn name="Dialog_OK" id="6"/>
-    <tableColumn name="Dialog_NOK_Event" id="7"/>
+    <tableColumn name="Phrase_OK" id="7"/>
+    <tableColumn name="Dialog_NOK_Event" id="8"/>
+    <tableColumn name="Phrase_NOK_Event" id="9"/>
   </tableColumns>
   <tableStyleInfo name="ITEMS_CONDS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H3" displayName="Table_Dialogs" name="Table_Dialogs" id="5">
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L5" displayName="Table_Dialogs" name="Table_Dialogs" id="5">
+  <tableColumns count="12">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ID" id="2"/>
     <tableColumn name="Room_used" id="3"/>
-    <tableColumn name="Room_Code" id="4"/>
-    <tableColumn name="Sender" id="5"/>
-    <tableColumn name="Text_English" id="6"/>
-    <tableColumn name="Text_Spanish" id="7"/>
-    <tableColumn name="Sound" id="8"/>
+    <tableColumn name="Options_Count" id="4"/>
+    <tableColumn name="Option1" id="5"/>
+    <tableColumn name="Option2" id="6"/>
+    <tableColumn name="Option3" id="7"/>
+    <tableColumn name="Option4" id="8"/>
+    <tableColumn name="Option5" id="9"/>
+    <tableColumn name="Option6" id="10"/>
+    <tableColumn name="Option7" id="11"/>
+    <tableColumn name="Option8" id="12"/>
   </tableColumns>
   <tableStyleInfo name="DIALOGS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B4" displayName="Table_Rooms" name="Table_Rooms" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:J12" displayName="Table_Dialog_Options" name="Table_Dialog_Options" id="6">
+  <tableColumns count="10">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="DIALOG_OPTION_ID" id="2"/>
+    <tableColumn name="EventCondition" id="3"/>
+    <tableColumn name="EventTriggered" id="4"/>
+    <tableColumn name="DialogTriggered" id="5"/>
+    <tableColumn name="PhraseCount" id="6"/>
+    <tableColumn name="Phrase1" id="7"/>
+    <tableColumn name="Phrase2" id="8"/>
+    <tableColumn name="Phrase3" id="9"/>
+    <tableColumn name="Phrase4" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="DIALOGS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A14:G19" displayName="Table_Phrases" name="Table_Phrases" id="7">
+  <tableColumns count="7">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="PHRASE_ID" id="2"/>
+    <tableColumn name="Room_used" id="3"/>
+    <tableColumn name="Sender" id="4"/>
+    <tableColumn name="Text_English" id="5"/>
+    <tableColumn name="Text_Spanish" id="6"/>
+    <tableColumn name="Sound" id="7"/>
+  </tableColumns>
+  <tableStyleInfo name="DIALOGS-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B4" displayName="Table_Rooms" name="Table_Rooms" id="8">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
@@ -1995,33 +2248,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B3" displayName="Table_NPCs" name="Table_NPCs" id="7">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B3" displayName="Table_NPCs" name="Table_NPCs" id="9">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="NPC_ID" id="2"/>
   </tableColumns>
   <tableStyleInfo name="NPCs-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="8">
-  <tableColumns count="2">
-    <tableColumn name="N" id="1"/>
-    <tableColumn name="Type" id="2"/>
-  </tableColumns>
-  <tableStyleInfo name="CHARACTERS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="9">
-  <tableColumns count="2">
-    <tableColumn name="N" id="1"/>
-    <tableColumn name="ANIMATION_ID" id="2"/>
-  </tableColumns>
-  <tableStyleInfo name="CHARACTERS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -4071,12 +4304,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="72" t="s">
-        <v>289</v>
+      <c r="A1" s="88" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="73">
+      <c r="A2" s="89">
         <v>3.0</v>
       </c>
     </row>
@@ -4107,10 +4340,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>290</v>
+        <v>328</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>291</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2">
@@ -4118,12 +4351,12 @@
         <f t="shared" ref="A2:A32" si="1">ROW()-ROW($G$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="74" t="str">
+      <c r="B2" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A2,0)</f>
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>292</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3">
@@ -4131,12 +4364,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="74" t="str">
+      <c r="B3" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A3,0)</f>
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>292</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4">
@@ -4144,12 +4377,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="74" t="str">
+      <c r="B4" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A4,0)</f>
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>292</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5">
@@ -4157,12 +4390,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="74" t="str">
+      <c r="B5" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A5,0)</f>
         <v>ITEM_LAST</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>292</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6">
@@ -4170,297 +4403,297 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="74" t="str">
+      <c r="B6" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A6,0)</f>
         <v/>
       </c>
-      <c r="C6" s="74"/>
+      <c r="C6" s="90"/>
     </row>
     <row r="7">
       <c r="A7" s="27">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="74" t="str">
+      <c r="B7" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A7,0)</f>
         <v/>
       </c>
-      <c r="C7" s="74"/>
+      <c r="C7" s="90"/>
     </row>
     <row r="8">
       <c r="A8" s="27">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="74" t="str">
+      <c r="B8" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A8,0)</f>
         <v/>
       </c>
-      <c r="C8" s="74"/>
+      <c r="C8" s="90"/>
     </row>
     <row r="9">
       <c r="A9" s="27">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="74" t="str">
+      <c r="B9" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A9,0)</f>
         <v/>
       </c>
-      <c r="C9" s="74"/>
+      <c r="C9" s="90"/>
     </row>
     <row r="10">
       <c r="A10" s="27">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="74" t="str">
+      <c r="B10" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A10,0)</f>
         <v/>
       </c>
-      <c r="C10" s="74"/>
+      <c r="C10" s="90"/>
     </row>
     <row r="11">
       <c r="A11" s="27">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="74" t="str">
+      <c r="B11" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A11,0)</f>
         <v/>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="90"/>
     </row>
     <row r="12">
       <c r="A12" s="27">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="74" t="str">
+      <c r="B12" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A12,0)</f>
         <v/>
       </c>
-      <c r="C12" s="74"/>
+      <c r="C12" s="90"/>
     </row>
     <row r="13">
       <c r="A13" s="27">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="74" t="str">
+      <c r="B13" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A13,0)</f>
         <v/>
       </c>
-      <c r="C13" s="74"/>
+      <c r="C13" s="90"/>
     </row>
     <row r="14">
       <c r="A14" s="27">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="74" t="str">
+      <c r="B14" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A14,0)</f>
         <v/>
       </c>
-      <c r="C14" s="74"/>
+      <c r="C14" s="90"/>
     </row>
     <row r="15">
       <c r="A15" s="27">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="74" t="str">
+      <c r="B15" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A15,0)</f>
         <v/>
       </c>
-      <c r="C15" s="74"/>
+      <c r="C15" s="90"/>
     </row>
     <row r="16">
       <c r="A16" s="27">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="74" t="str">
+      <c r="B16" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A16,0)</f>
         <v/>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="90"/>
     </row>
     <row r="17">
       <c r="A17" s="27">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="74" t="str">
+      <c r="B17" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A17,0)</f>
         <v/>
       </c>
-      <c r="C17" s="74"/>
+      <c r="C17" s="90"/>
     </row>
     <row r="18">
       <c r="A18" s="27">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="74" t="str">
+      <c r="B18" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A18,0)</f>
         <v/>
       </c>
-      <c r="C18" s="74"/>
+      <c r="C18" s="90"/>
     </row>
     <row r="19">
       <c r="A19" s="27">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="74" t="str">
+      <c r="B19" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A19,0)</f>
         <v/>
       </c>
-      <c r="C19" s="74"/>
+      <c r="C19" s="90"/>
     </row>
     <row r="20">
       <c r="A20" s="27">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="74" t="str">
+      <c r="B20" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A20,0)</f>
         <v/>
       </c>
-      <c r="C20" s="74"/>
+      <c r="C20" s="90"/>
     </row>
     <row r="21">
       <c r="A21" s="27">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="74" t="str">
+      <c r="B21" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A21,0)</f>
         <v/>
       </c>
-      <c r="C21" s="74"/>
+      <c r="C21" s="90"/>
     </row>
     <row r="22">
       <c r="A22" s="27">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="74" t="str">
+      <c r="B22" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A22,0)</f>
         <v/>
       </c>
-      <c r="C22" s="74"/>
+      <c r="C22" s="90"/>
     </row>
     <row r="23">
       <c r="A23" s="27">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="74" t="str">
+      <c r="B23" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A23,0)</f>
         <v/>
       </c>
-      <c r="C23" s="74"/>
+      <c r="C23" s="90"/>
     </row>
     <row r="24">
       <c r="A24" s="27">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="74" t="str">
+      <c r="B24" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A24,0)</f>
         <v/>
       </c>
-      <c r="C24" s="74"/>
+      <c r="C24" s="90"/>
     </row>
     <row r="25">
       <c r="A25" s="27">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="74" t="str">
+      <c r="B25" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A25,0)</f>
         <v/>
       </c>
-      <c r="C25" s="74"/>
+      <c r="C25" s="90"/>
     </row>
     <row r="26">
       <c r="A26" s="27">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="74" t="str">
+      <c r="B26" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A26,0)</f>
         <v/>
       </c>
-      <c r="C26" s="74"/>
+      <c r="C26" s="90"/>
     </row>
     <row r="27">
       <c r="A27" s="27">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="74" t="str">
+      <c r="B27" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A27,0)</f>
         <v/>
       </c>
-      <c r="C27" s="74"/>
+      <c r="C27" s="90"/>
     </row>
     <row r="28">
       <c r="A28" s="27">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="74" t="str">
+      <c r="B28" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A28,0)</f>
         <v/>
       </c>
-      <c r="C28" s="74"/>
+      <c r="C28" s="90"/>
     </row>
     <row r="29">
       <c r="A29" s="27">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="74" t="str">
+      <c r="B29" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A29,0)</f>
         <v/>
       </c>
-      <c r="C29" s="74"/>
+      <c r="C29" s="90"/>
     </row>
     <row r="30">
       <c r="A30" s="27">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="74" t="str">
+      <c r="B30" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A30,0)</f>
         <v/>
       </c>
-      <c r="C30" s="74"/>
+      <c r="C30" s="90"/>
     </row>
     <row r="31">
       <c r="A31" s="27">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="74" t="str">
+      <c r="B31" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A31,0)</f>
         <v/>
       </c>
-      <c r="C31" s="74"/>
+      <c r="C31" s="90"/>
     </row>
     <row r="32">
       <c r="A32" s="27">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="74" t="str">
+      <c r="B32" s="90" t="str">
         <f>OFFSET(ITEMS!$B$3,A32,0)</f>
         <v/>
       </c>
-      <c r="C32" s="74"/>
+      <c r="C32" s="90"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -4493,197 +4726,197 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="40" t="s">
-        <v>293</v>
+        <v>331</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>294</v>
+        <v>332</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>295</v>
-      </c>
-      <c r="D1" s="48" t="s">
-        <v>296</v>
+        <v>333</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="49" t="s">
-        <v>297</v>
-      </c>
-      <c r="B2" s="75">
+        <v>335</v>
+      </c>
+      <c r="B2" s="91">
         <v>1.0</v>
       </c>
       <c r="C2" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="62" t="b">
+      <c r="D2" s="80" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="53" t="s">
-        <v>298</v>
-      </c>
-      <c r="B3" s="75">
+        <v>336</v>
+      </c>
+      <c r="B3" s="91">
         <v>1.0</v>
       </c>
       <c r="C3" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="64" t="b">
+      <c r="D3" s="81" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="49" t="s">
-        <v>299</v>
-      </c>
-      <c r="B4" s="76">
+        <v>337</v>
+      </c>
+      <c r="B4" s="92">
         <v>3.0</v>
       </c>
       <c r="C4" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="62" t="b">
+      <c r="D4" s="80" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="53" t="s">
-        <v>300</v>
-      </c>
-      <c r="B5" s="75">
+      <c r="A5" s="93" t="s">
+        <v>338</v>
+      </c>
+      <c r="B5" s="91">
         <v>1.0</v>
       </c>
       <c r="C5" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="64" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D5" s="81" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="49" t="s">
-        <v>301</v>
-      </c>
-      <c r="B6" s="76">
+        <v>339</v>
+      </c>
+      <c r="B6" s="92">
         <v>3.0</v>
       </c>
       <c r="C6" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="62" t="b">
+      <c r="D6" s="80" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="53" t="s">
-        <v>302</v>
-      </c>
-      <c r="B7" s="76">
+        <v>340</v>
+      </c>
+      <c r="B7" s="92">
         <v>3.0</v>
       </c>
       <c r="C7" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="64" t="b">
+      <c r="D7" s="81" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="s">
-        <v>303</v>
-      </c>
-      <c r="B8" s="77">
+      <c r="A8" s="93" t="s">
+        <v>341</v>
+      </c>
+      <c r="B8" s="94">
         <v>5.0</v>
       </c>
       <c r="C8" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="62" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D8" s="80" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="53" t="s">
-        <v>304</v>
-      </c>
-      <c r="B9" s="78">
+        <v>342</v>
+      </c>
+      <c r="B9" s="95">
         <v>4.0</v>
       </c>
       <c r="C9" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="64" t="b">
+      <c r="D9" s="81" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="49" t="s">
-        <v>305</v>
-      </c>
-      <c r="B10" s="78">
+        <v>343</v>
+      </c>
+      <c r="B10" s="95">
         <v>4.0</v>
       </c>
       <c r="C10" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="62" t="b">
+      <c r="D10" s="80" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="53" t="s">
-        <v>306</v>
-      </c>
-      <c r="B11" s="75">
+        <v>344</v>
+      </c>
+      <c r="B11" s="91">
         <v>1.0</v>
       </c>
       <c r="C11" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="64" t="b">
+      <c r="D11" s="81" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="79" t="s">
-        <v>307</v>
-      </c>
-      <c r="B12" s="78">
+      <c r="A12" s="93" t="s">
+        <v>345</v>
+      </c>
+      <c r="B12" s="95">
         <v>4.0</v>
       </c>
       <c r="C12" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="62" t="b">
+      <c r="D12" s="80" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="79" t="s">
-        <v>308</v>
-      </c>
-      <c r="B13" s="75">
+      <c r="A13" s="93" t="s">
+        <v>346</v>
+      </c>
+      <c r="B13" s="91">
         <v>1.0</v>
       </c>
       <c r="C13" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="64" t="b">
+      <c r="D13" s="81" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="65" t="s">
-        <v>309</v>
-      </c>
-      <c r="B14" s="80">
+      <c r="A14" s="74" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14" s="96">
         <v>5.0</v>
       </c>
-      <c r="C14" s="69" t="b">
+      <c r="C14" s="75" t="b">
         <v>0</v>
       </c>
-      <c r="D14" s="66" t="b">
+      <c r="D14" s="82" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6917,7 +7150,8 @@
     <col customWidth="1" min="4" max="4" width="44.57"/>
     <col customWidth="1" min="5" max="5" width="38.86"/>
     <col customWidth="1" min="6" max="6" width="25.86"/>
-    <col customWidth="1" min="7" max="7" width="27.14"/>
+    <col customWidth="1" min="7" max="8" width="27.14"/>
+    <col customWidth="1" min="9" max="9" width="22.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6939,8 +7173,14 @@
       <c r="F1" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="42" t="s">
         <v>243</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="2">
@@ -6954,16 +7194,22 @@
         <v>227</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>246</v>
-      </c>
-      <c r="G2" s="52" t="s">
-        <v>246</v>
+        <v>248</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="3">
@@ -6977,16 +7223,22 @@
         <v>227</v>
       </c>
       <c r="D3" s="55" t="s">
+        <v>250</v>
+      </c>
+      <c r="E3" s="55" t="s">
         <v>247</v>
       </c>
-      <c r="E3" s="55" t="s">
-        <v>245</v>
-      </c>
       <c r="F3" s="55" t="s">
-        <v>246</v>
-      </c>
-      <c r="G3" s="56" t="s">
-        <v>246</v>
+        <v>248</v>
+      </c>
+      <c r="G3" s="55" t="s">
+        <v>249</v>
+      </c>
+      <c r="H3" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="I3" s="56" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="4">
@@ -7000,16 +7252,22 @@
         <v>227</v>
       </c>
       <c r="D4" s="51" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>247</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="H4" s="51" t="s">
         <v>248</v>
       </c>
-      <c r="E4" s="51" t="s">
-        <v>245</v>
-      </c>
-      <c r="F4" s="51" t="s">
+      <c r="I4" s="52" t="s">
         <v>249</v>
-      </c>
-      <c r="G4" s="52" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="5">
@@ -7017,30 +7275,45 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C5" s="59" t="s">
         <v>227</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F5" s="59" t="s">
-        <v>246</v>
-      </c>
-      <c r="G5" s="60" t="s">
-        <v>246</v>
+        <v>248</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="I5" s="60" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="G2:G5">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="I2:I5">
+      <formula1>Table_Phrases[PHRASE_ID]</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F2:F5">
+      <formula1>#REF!</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C5">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:G5">
+    <dataValidation type="list" allowBlank="1" sqref="H2:H5">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D2:E5">
@@ -7068,10 +7341,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="21.57"/>
-    <col customWidth="1" min="3" max="3" width="22.43"/>
-    <col customWidth="1" min="4" max="6" width="32.14"/>
-    <col customWidth="1" min="7" max="7" width="21.0"/>
+    <col customWidth="1" min="2" max="2" width="34.86"/>
+    <col customWidth="1" min="3" max="3" width="30.0"/>
+    <col customWidth="1" min="4" max="4" width="32.14"/>
+    <col customWidth="1" min="5" max="6" width="40.57"/>
+    <col customWidth="1" min="7" max="8" width="33.86"/>
+    <col customWidth="1" min="9" max="13" width="32.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7079,82 +7354,572 @@
         <v>0</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>254</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="G1" s="42" t="s">
         <v>256</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="D1" s="61" t="s">
         <v>257</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>258</v>
+      </c>
+      <c r="F1" s="61" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" s="61" t="s">
+        <v>260</v>
+      </c>
+      <c r="H1" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="I1" s="61" t="s">
+        <v>262</v>
+      </c>
+      <c r="J1" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="K1" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="49">
+        <f>ROW()-ROW(Table_Dialogs[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="62">
+        <f t="shared" ref="D2:D5" si="1">COUNTIFS(E2:L2,"&lt;&gt;DIALOG_OPTION_NONE",E2:L2,"&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="F2" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="G2" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="H2" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="I2" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="J2" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="K2" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="L2" s="64" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="53">
+        <f>ROW()-ROW(Table_Dialogs[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="65">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="G3" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="H3" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="I3" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="J3" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="K3" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="L3" s="67" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="49">
+        <f>ROW()-ROW(Table_Dialogs[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" s="68">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>271</v>
+      </c>
+      <c r="F4" s="63" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="H4" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="I4" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="J4" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="K4" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="L4" s="64" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="57">
+        <f>ROW()-ROW(Table_Dialogs[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="H5" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="I5" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="J5" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="K5" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="L5" s="71" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="H7" s="61" t="s">
+        <v>280</v>
+      </c>
+      <c r="I7" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="J7" s="48" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="49">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" s="68">
+        <f t="shared" ref="F8:F12" si="2">COUNTIFS(G8:J8,"&lt;&gt;PHRASE_NONE",G8:J8,"&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="J8" s="52" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="53">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" s="55" t="s">
+        <v>249</v>
+      </c>
+      <c r="I9" s="55" t="s">
+        <v>249</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="49">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="F10" s="73">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>283</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>284</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="53">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" s="72">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>285</v>
+      </c>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="74">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>4</v>
+      </c>
+      <c r="B12" s="75" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" s="76" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="F12" s="77">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="76" t="s">
+        <v>249</v>
+      </c>
+      <c r="H12" s="76" t="s">
+        <v>249</v>
+      </c>
+      <c r="I12" s="76" t="s">
+        <v>249</v>
+      </c>
+      <c r="J12" s="78" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>288</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="G14" s="79" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="49">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>266</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>292</v>
+      </c>
+      <c r="F15" s="50"/>
+      <c r="G15" s="80">
         <v>0.0</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>246</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="61">
-        <f t="array" ref="D2">INDEX(Table_Rooms[N],MATCH(C2,Table_Rooms[ROOM_ID],0))</f>
-        <v>-1</v>
-      </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="62">
+    </row>
+    <row r="16">
+      <c r="A16" s="53">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>253</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>266</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>292</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>293</v>
+      </c>
+      <c r="F16" s="54" t="s">
+        <v>294</v>
+      </c>
+      <c r="G16" s="81">
         <v>0.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="57">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="58">
-        <f t="array" ref="D3">INDEX(Table_Rooms[N],MATCH(C3,Table_Rooms[ROOM_ID],0))</f>
-        <v>-1</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>259</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>260</v>
-      </c>
-      <c r="G3" s="58" t="s">
-        <v>261</v>
-      </c>
-      <c r="H3" s="63">
+    <row r="17">
+      <c r="A17" s="49">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>270</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>292</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>295</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>296</v>
+      </c>
+      <c r="G17" s="80">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="53">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>284</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>270</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>292</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>297</v>
+      </c>
+      <c r="F18" s="54" t="s">
+        <v>298</v>
+      </c>
+      <c r="G18" s="81">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="74">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>4</v>
+      </c>
+      <c r="B19" s="75" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="76" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="75" t="s">
+        <v>292</v>
+      </c>
+      <c r="E19" s="75" t="s">
+        <v>299</v>
+      </c>
+      <c r="F19" s="75" t="s">
+        <v>300</v>
+      </c>
+      <c r="G19" s="82">
         <v>0.0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C3">
+    <dataValidation type="list" allowBlank="1" sqref="G8:G12">
       <formula1>#REF!</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="H8:J12">
+      <formula1>Table_Phrases[PHRASE_ID]</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="E2:E5">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D8:D12">
+      <formula1>Table_Events[EVENT_ID]</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C8:C12">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="D2:D5 F8:F12">
+      <formula1>AND(ISNUMBER(D2),(NOT(OR(NOT(ISERROR(DATEVALUE(D2))), AND(ISNUMBER(D2), LEFT(CELL("format", D2))="D")))))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C15:C19">
+      <formula1>Table_Rooms[ROOM_ID]</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F2:L5">
+      <formula1>Table_Dialog_Options[DIALOG_OPTION_ID]</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C5">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="E8:E12">
+      <formula1>Table_Dialogs[DIALOG_ID]</formula1>
+    </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7179,8 +7944,8 @@
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>262</v>
+      <c r="B1" s="79" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="2">
@@ -7188,8 +7953,8 @@
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
-      <c r="B2" s="62" t="s">
-        <v>258</v>
+      <c r="B2" s="80" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="3">
@@ -7197,17 +7962,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="B3" s="64" t="s">
-        <v>263</v>
+      <c r="B3" s="81" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="65">
+      <c r="A4" s="74">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B4" s="66" t="s">
-        <v>264</v>
+      <c r="B4" s="82" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -7236,8 +8001,8 @@
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>265</v>
+      <c r="B1" s="79" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="2">
@@ -7246,7 +8011,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>266</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3">
@@ -7255,7 +8020,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>267</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -7290,23 +8055,23 @@
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>268</v>
+      <c r="B1" s="79" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="49">
         <v>0.0</v>
       </c>
-      <c r="B2" s="62" t="s">
-        <v>269</v>
+      <c r="B2" s="80" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="53">
         <v>1.0</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="81" t="s">
         <v>224</v>
       </c>
     </row>
@@ -7314,7 +8079,7 @@
       <c r="A4" s="49">
         <v>2.0</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="80" t="s">
         <v>231</v>
       </c>
     </row>
@@ -7322,79 +8087,79 @@
       <c r="A5" s="57">
         <v>3.0</v>
       </c>
-      <c r="B5" s="63" t="s">
-        <v>270</v>
+      <c r="B5" s="83" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>271</v>
+      <c r="B7" s="79" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="49">
         <v>0.0</v>
       </c>
-      <c r="B8" s="62" t="s">
-        <v>272</v>
+      <c r="B8" s="80" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="53">
         <v>1.0</v>
       </c>
-      <c r="B9" s="64" t="s">
-        <v>273</v>
+      <c r="B9" s="81" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="49">
         <v>2.0</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>244</v>
+      <c r="B10" s="80" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="53">
         <v>3.0</v>
       </c>
-      <c r="B11" s="64" t="s">
-        <v>245</v>
+      <c r="B11" s="81" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="49">
         <v>4.0</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>248</v>
+      <c r="B12" s="80" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="57">
         <v>5.0</v>
       </c>
-      <c r="B13" s="63" t="s">
-        <v>247</v>
+      <c r="B13" s="83" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="48" t="s">
-        <v>274</v>
+      <c r="B15" s="79" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="49">
         <v>0.0</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="80" t="s">
         <v>225</v>
       </c>
     </row>
@@ -7402,7 +8167,7 @@
       <c r="A17" s="53">
         <v>1.0</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="81" t="s">
         <v>229</v>
       </c>
     </row>
@@ -7410,7 +8175,7 @@
       <c r="A18" s="49">
         <v>2.0</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="80" t="s">
         <v>233</v>
       </c>
     </row>
@@ -7418,48 +8183,48 @@
       <c r="A19" s="53">
         <v>3.0</v>
       </c>
-      <c r="B19" s="64" t="s">
-        <v>275</v>
+      <c r="B19" s="81" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="65">
+      <c r="A20" s="74">
         <v>4.0</v>
       </c>
-      <c r="B20" s="66" t="s">
-        <v>276</v>
+      <c r="B20" s="82" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="48" t="s">
-        <v>277</v>
+      <c r="B22" s="79" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="49">
         <v>0.0</v>
       </c>
-      <c r="B23" s="62" t="s">
-        <v>278</v>
+      <c r="B23" s="80" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="53">
         <v>1.0</v>
       </c>
-      <c r="B24" s="64" t="s">
-        <v>279</v>
+      <c r="B24" s="81" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="65">
+      <c r="A25" s="74">
         <v>2.0</v>
       </c>
-      <c r="B25" s="66" t="s">
-        <v>280</v>
+      <c r="B25" s="82" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -7502,22 +8267,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>281</v>
+        <v>319</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>283</v>
+        <v>321</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>284</v>
+        <v>322</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>286</v>
+        <v>323</v>
+      </c>
+      <c r="G1" s="79" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="2">
@@ -7528,10 +8293,10 @@
       <c r="B2" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="G2" s="68"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="G2" s="85"/>
     </row>
     <row r="3">
       <c r="A3" s="53">
@@ -7542,7 +8307,7 @@
         <v>235</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>287</v>
+        <v>325</v>
       </c>
       <c r="D3" s="55" t="s">
         <v>228</v>
@@ -7556,17 +8321,17 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="65">
+      <c r="A4" s="74">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="69" t="s">
-        <v>288</v>
-      </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="G4" s="71"/>
+      <c r="B4" s="75" t="s">
+        <v>326</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="G4" s="87"/>
     </row>
   </sheetData>
   <dataValidations>

</xml_diff>

<commit_message>
[Partial] Fixed mouse over bug
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="zemEGP61/Qsn62AreRdmMzAc5WTt+jRs8AR9io3o91g="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="Aax0f1fmZiGbGskZ2MsUEVCwLOdnAGfn+GhbmUsxFws="/>
     </ext>
   </extLst>
 </workbook>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="394">
   <si>
     <t>N</t>
   </si>
@@ -538,18 +538,6 @@
     <t>Activates/Deactivates an event</t>
   </si>
   <si>
-    <t>IS_ITEM_AVAILABLE</t>
-  </si>
-  <si>
-    <t>IS_ITEM_AVAILABLE_DELEGATE</t>
-  </si>
-  <si>
-    <t>LevelMasterClass.IsItemAvailableService</t>
-  </si>
-  <si>
-    <t>Gets if an item is available to interact with</t>
-  </si>
-  <si>
     <t>INTERACT_PLAYER</t>
   </si>
   <si>
@@ -562,6 +550,15 @@
     <t>Makes player interact with usage data</t>
   </si>
   <si>
+    <t>PLAYER_REACHED_WAYPOINT</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.PlayerReachedWaypointService</t>
+  </si>
+  <si>
+    <t>Tells LevelMaster that player reached Waypoint to start action in case</t>
+  </si>
+  <si>
     <t>USE_ITEM</t>
   </si>
   <si>
@@ -634,18 +631,6 @@
     <t>Subscribe to an event. Invoke when event changes</t>
   </si>
   <si>
-    <t>CROSS_DOOR</t>
-  </si>
-  <si>
-    <t>CROSS_DOOR_DELEGATE</t>
-  </si>
-  <si>
-    <t>LevelMasterClass.CrossDoorService</t>
-  </si>
-  <si>
-    <t>Trigger actions when crossing a door</t>
-  </si>
-  <si>
     <t>LOCK_PLAYER</t>
   </si>
   <si>
@@ -1141,7 +1126,7 @@
     <t>ROOM_FIRST</t>
   </si>
   <si>
-    <t>ITEM_PLAYER_MAIN, ITEM_PLAYER_PARROT, ITEM_POTION, ITEM_POTION_BLUE, ITEM_FOUNTAIN, ITEM_NPC_MILITO</t>
+    <t>ITEM_PLAYER_MAIN, ITEM_PLAYER_PARROT, ITEM_POTION, ITEM_POTION_BLUE, ITEM_FOUNTAIN</t>
   </si>
   <si>
     <t>PHRASE_NONSENSE, PHRASE_ASK_FOUNTAIN1_1, PHRASE_ASK_FOUNTAIN1_2, PHRASE_ASK_FOUNTAIN2_1, PHRASE_ASK_FOUNTAIN3_1, PHRASE_ASK_FOUNTAIN4_1</t>
@@ -1277,6 +1262,12 @@
   </si>
   <si>
     <t>Use Dictionaries for LevelManager</t>
+  </si>
+  <si>
+    <t>State change deactivation/activation</t>
+  </si>
+  <si>
+    <t>Adressables instead of Resources</t>
   </si>
   <si>
     <t>Re-think usage of ITEM_TAKE, USE_TALK</t>
@@ -1541,6 +1532,20 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
@@ -1551,20 +1556,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
@@ -1669,7 +1660,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="128">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1796,23 +1787,11 @@
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1904,91 +1883,91 @@
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -2001,7 +1980,7 @@
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2412,7 +2391,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N36" displayName="Table_Services" name="Table_Services" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N35" displayName="Table_Services" name="Table_Services" id="2">
   <tableColumns count="14">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SERVICE_ID" id="2"/>
@@ -2434,7 +2413,7 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D17" displayName="Table_TODO" name="Table_TODO" id="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D19" displayName="Table_TODO" name="Table_TODO" id="20">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -3258,7 +3237,7 @@
         <v>20</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>23</v>
@@ -4452,47 +4431,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
-        <v>353</v>
+      <c r="B1" s="69" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <f>ROW()-ROW(Table_Characters[N])</f>
         <v>0</v>
       </c>
-      <c r="B2" s="75" t="s">
-        <v>214</v>
+      <c r="B2" s="71" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="59">
+      <c r="A3" s="55">
         <f>ROW()-ROW(Table_Characters[N])</f>
         <v>1</v>
       </c>
-      <c r="B3" s="74" t="s">
-        <v>222</v>
+      <c r="B3" s="70" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53">
+      <c r="A4" s="49">
         <f>ROW()-ROW(Table_Characters[N])</f>
         <v>2</v>
       </c>
-      <c r="B4" s="75" t="s">
-        <v>226</v>
+      <c r="B4" s="71" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="67">
+      <c r="A5" s="63">
         <f>ROW()-ROW(Table_Characters[N])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="103" t="s">
-        <v>354</v>
+      <c r="B5" s="99" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="6">
@@ -4500,192 +4479,192 @@
       <c r="B6" s="25"/>
     </row>
     <row r="7">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="69" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="49">
+        <v>0.0</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="55">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="70" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="49">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="71" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="55">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="49">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="71" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="63">
+        <v>5.0</v>
+      </c>
+      <c r="B13" s="99" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="49">
+        <v>0.0</v>
+      </c>
+      <c r="B16" s="71" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="55">
+        <v>1.0</v>
+      </c>
+      <c r="B17" s="70" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="49">
+        <v>2.0</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="55">
+        <v>3.0</v>
+      </c>
+      <c r="B19" s="70" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="49">
+        <v>4.0</v>
+      </c>
+      <c r="B20" s="71" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="63">
+        <v>5.0</v>
+      </c>
+      <c r="B21" s="99" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="53">
+    <row r="23">
+      <c r="A23" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="69" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="49">
         <v>0.0</v>
       </c>
-      <c r="B8" s="75" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="59">
+      <c r="B24" s="71" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="63">
         <v>1.0</v>
       </c>
-      <c r="B9" s="74" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="53">
-        <v>2.0</v>
-      </c>
-      <c r="B10" s="75" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="59">
-        <v>3.0</v>
-      </c>
-      <c r="B11" s="74" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="53">
-        <v>4.0</v>
-      </c>
-      <c r="B12" s="75" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="67">
-        <v>5.0</v>
-      </c>
-      <c r="B13" s="103" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="48" t="s">
+      <c r="B25" s="99" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B27" s="69" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="B16" s="75" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="59">
-        <v>1.0</v>
-      </c>
-      <c r="B17" s="74" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="53">
-        <v>2.0</v>
-      </c>
-      <c r="B18" s="75" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="59">
-        <v>3.0</v>
-      </c>
-      <c r="B19" s="74" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="53">
-        <v>4.0</v>
-      </c>
-      <c r="B20" s="75" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="67">
-        <v>5.0</v>
-      </c>
-      <c r="B21" s="103" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="73" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="B24" s="75" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="67">
-        <v>1.0</v>
-      </c>
-      <c r="B25" s="103" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="73" t="s">
-        <v>362</v>
-      </c>
-    </row>
     <row r="28">
-      <c r="A28" s="53">
+      <c r="A28" s="49">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>0</v>
       </c>
-      <c r="B28" s="75" t="s">
-        <v>259</v>
+      <c r="B28" s="71" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="59">
+      <c r="A29" s="55">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>1</v>
       </c>
-      <c r="B29" s="104" t="s">
-        <v>363</v>
+      <c r="B29" s="100" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="53">
+      <c r="A30" s="49">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>2</v>
       </c>
-      <c r="B30" s="105" t="s">
-        <v>268</v>
+      <c r="B30" s="101" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="59">
+      <c r="A31" s="55">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>3</v>
       </c>
-      <c r="B31" s="104" t="s">
-        <v>276</v>
+      <c r="B31" s="100" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="76">
+      <c r="A32" s="72">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>4</v>
       </c>
-      <c r="B32" s="106" t="s">
-        <v>262</v>
+      <c r="B32" s="102" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -4725,136 +4704,136 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
-        <v>364</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>365</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>366</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>367</v>
-      </c>
-      <c r="F1" s="73" t="s">
-        <v>368</v>
+      <c r="B1" s="45" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>362</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>213</v>
-      </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="108"/>
+      <c r="B2" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="104"/>
     </row>
     <row r="3">
-      <c r="A3" s="59">
+      <c r="A3" s="55">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>232</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>369</v>
-      </c>
-      <c r="D3" s="62" t="s">
-        <v>229</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>270</v>
-      </c>
-      <c r="F3" s="109" t="s">
-        <v>232</v>
+      <c r="B3" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>364</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>265</v>
+      </c>
+      <c r="F3" s="105" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="76">
+      <c r="A4" s="72">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>370</v>
-      </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="111"/>
+      <c r="B4" s="73" t="s">
+        <v>365</v>
+      </c>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="107"/>
     </row>
     <row r="6">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="73" t="s">
-        <v>371</v>
+      <c r="B6" s="69" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="112">
+      <c r="A7" s="108">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>0</v>
       </c>
-      <c r="B7" s="113" t="str">
+      <c r="B7" s="109" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(FLATTEN(Table_Events[EVENT_ID],""(NOT)""&amp;Table_Events[EVENT_ID]))"),"EVENT_NONE")</f>
         <v>EVENT_NONE</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="114">
+      <c r="A8" s="110">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>1</v>
       </c>
-      <c r="B8" s="115" t="str">
+      <c r="B8" s="111" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_FOUNTAIN_FULL")</f>
         <v>EVENT_FOUNTAIN_FULL</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="112">
+      <c r="A9" s="108">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>2</v>
       </c>
-      <c r="B9" s="113" t="str">
+      <c r="B9" s="109" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAST")</f>
         <v>EVENT_LAST</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="114">
+      <c r="A10" s="110">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>3</v>
       </c>
-      <c r="B10" s="115" t="str">
+      <c r="B10" s="111" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_NONE")</f>
         <v>(NOT)EVENT_NONE</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="112">
+      <c r="A11" s="108">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>4</v>
       </c>
-      <c r="B11" s="113" t="str">
+      <c r="B11" s="109" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_FOUNTAIN_FULL")</f>
         <v>(NOT)EVENT_FOUNTAIN_FULL</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="116">
+      <c r="A12" s="112">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>5</v>
       </c>
-      <c r="B12" s="117" t="str">
+      <c r="B12" s="113" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAST")</f>
         <v>(NOT)EVENT_LAST</v>
       </c>
@@ -4896,106 +4875,106 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="118" t="s">
-        <v>372</v>
-      </c>
-      <c r="B1" s="119" t="s">
-        <v>373</v>
-      </c>
-      <c r="D1" s="118" t="s">
-        <v>374</v>
-      </c>
-      <c r="E1" s="119" t="s">
-        <v>373</v>
+      <c r="A1" s="114" t="s">
+        <v>367</v>
+      </c>
+      <c r="B1" s="115" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="114" t="s">
+        <v>369</v>
+      </c>
+      <c r="E1" s="115" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="120" t="str">
+      <c r="A2" s="116" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"SPRITE_POTION_RED")</f>
         <v>SPRITE_POTION_RED</v>
       </c>
-      <c r="B2" s="121" t="str">
+      <c r="B2" s="117" t="str">
         <f t="array" ref="B2:B10">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
         <v/>
       </c>
-      <c r="D2" s="120" t="str">
+      <c r="D2" s="116" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"NAME_ITEM_POTION")</f>
         <v>NAME_ITEM_POTION</v>
       </c>
-      <c r="E2" s="121" t="str">
+      <c r="E2" s="117" t="str">
         <f t="array" ref="E2:E10">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
         <v/>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="122" t="str">
+      <c r="A3" s="118" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_POTION_BLUE")</f>
         <v>SPRITE_POTION_BLUE</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="122" t="str">
+      <c r="D3" s="118" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_BLUE_POTION")</f>
         <v>NAME_ITEM_BLUE_POTION</v>
       </c>
-      <c r="E3" s="123" t="s">
+      <c r="E3" s="119" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="121" t="s">
+      <c r="E4" s="117" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="119" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="121" t="s">
-        <v>240</v>
-      </c>
-      <c r="E6" s="121" t="s">
-        <v>267</v>
+      <c r="B6" s="117" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" s="117" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="123" t="s">
-        <v>242</v>
-      </c>
-      <c r="E7" s="123" t="s">
-        <v>269</v>
+      <c r="B7" s="119" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="119" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="121" t="s">
+      <c r="E8" s="117" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="123" t="s">
+      <c r="E9" s="119" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="121" t="s">
+      <c r="E10" s="117" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5027,10 +5006,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2">
@@ -5038,12 +5017,12 @@
         <f t="shared" ref="A2:A32" si="1">ROW()-ROW($G$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="124" t="str">
+      <c r="B2" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A2,0)</f>
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3">
@@ -5051,12 +5030,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="124" t="str">
+      <c r="B3" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A3,0)</f>
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4">
@@ -5064,12 +5043,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="124" t="str">
+      <c r="B4" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A4,0)</f>
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5">
@@ -5077,12 +5056,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="124" t="str">
+      <c r="B5" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A5,0)</f>
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6">
@@ -5090,297 +5069,297 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="124" t="str">
+      <c r="B6" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A6,0)</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="C6" s="124"/>
+      <c r="C6" s="120"/>
     </row>
     <row r="7">
       <c r="A7" s="25">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="124" t="str">
+      <c r="B7" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A7,0)</f>
         <v/>
       </c>
-      <c r="C7" s="124"/>
+      <c r="C7" s="120"/>
     </row>
     <row r="8">
       <c r="A8" s="25">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="124" t="str">
+      <c r="B8" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A8,0)</f>
         <v/>
       </c>
-      <c r="C8" s="124"/>
+      <c r="C8" s="120"/>
     </row>
     <row r="9">
       <c r="A9" s="25">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="124" t="str">
+      <c r="B9" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A9,0)</f>
         <v/>
       </c>
-      <c r="C9" s="124"/>
+      <c r="C9" s="120"/>
     </row>
     <row r="10">
       <c r="A10" s="25">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="124" t="str">
+      <c r="B10" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A10,0)</f>
         <v/>
       </c>
-      <c r="C10" s="124"/>
+      <c r="C10" s="120"/>
     </row>
     <row r="11">
       <c r="A11" s="25">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="124" t="str">
+      <c r="B11" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A11,0)</f>
         <v/>
       </c>
-      <c r="C11" s="124"/>
+      <c r="C11" s="120"/>
     </row>
     <row r="12">
       <c r="A12" s="25">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="124" t="str">
+      <c r="B12" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A12,0)</f>
         <v/>
       </c>
-      <c r="C12" s="124"/>
+      <c r="C12" s="120"/>
     </row>
     <row r="13">
       <c r="A13" s="25">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="124" t="str">
+      <c r="B13" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A13,0)</f>
         <v/>
       </c>
-      <c r="C13" s="124"/>
+      <c r="C13" s="120"/>
     </row>
     <row r="14">
       <c r="A14" s="25">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="124" t="str">
+      <c r="B14" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A14,0)</f>
         <v/>
       </c>
-      <c r="C14" s="124"/>
+      <c r="C14" s="120"/>
     </row>
     <row r="15">
       <c r="A15" s="25">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="124" t="str">
+      <c r="B15" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A15,0)</f>
         <v/>
       </c>
-      <c r="C15" s="124"/>
+      <c r="C15" s="120"/>
     </row>
     <row r="16">
       <c r="A16" s="25">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="124" t="str">
+      <c r="B16" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A16,0)</f>
         <v/>
       </c>
-      <c r="C16" s="124"/>
+      <c r="C16" s="120"/>
     </row>
     <row r="17">
       <c r="A17" s="25">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="124" t="str">
+      <c r="B17" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A17,0)</f>
         <v/>
       </c>
-      <c r="C17" s="124"/>
+      <c r="C17" s="120"/>
     </row>
     <row r="18">
       <c r="A18" s="25">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="124" t="str">
+      <c r="B18" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A18,0)</f>
         <v/>
       </c>
-      <c r="C18" s="124"/>
+      <c r="C18" s="120"/>
     </row>
     <row r="19">
       <c r="A19" s="25">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="124" t="str">
+      <c r="B19" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A19,0)</f>
         <v/>
       </c>
-      <c r="C19" s="124"/>
+      <c r="C19" s="120"/>
     </row>
     <row r="20">
       <c r="A20" s="25">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="124" t="str">
+      <c r="B20" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A20,0)</f>
         <v/>
       </c>
-      <c r="C20" s="124"/>
+      <c r="C20" s="120"/>
     </row>
     <row r="21">
       <c r="A21" s="25">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="124" t="str">
+      <c r="B21" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A21,0)</f>
         <v/>
       </c>
-      <c r="C21" s="124"/>
+      <c r="C21" s="120"/>
     </row>
     <row r="22">
       <c r="A22" s="25">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="124" t="str">
+      <c r="B22" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A22,0)</f>
         <v/>
       </c>
-      <c r="C22" s="124"/>
+      <c r="C22" s="120"/>
     </row>
     <row r="23">
       <c r="A23" s="25">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="124" t="str">
+      <c r="B23" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A23,0)</f>
         <v/>
       </c>
-      <c r="C23" s="124"/>
+      <c r="C23" s="120"/>
     </row>
     <row r="24">
       <c r="A24" s="25">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="124" t="str">
+      <c r="B24" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A24,0)</f>
         <v/>
       </c>
-      <c r="C24" s="124"/>
+      <c r="C24" s="120"/>
     </row>
     <row r="25">
       <c r="A25" s="25">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="124" t="str">
+      <c r="B25" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A25,0)</f>
         <v/>
       </c>
-      <c r="C25" s="124"/>
+      <c r="C25" s="120"/>
     </row>
     <row r="26">
       <c r="A26" s="25">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="124" t="str">
+      <c r="B26" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A26,0)</f>
         <v/>
       </c>
-      <c r="C26" s="124"/>
+      <c r="C26" s="120"/>
     </row>
     <row r="27">
       <c r="A27" s="25">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="124" t="str">
+      <c r="B27" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A27,0)</f>
         <v/>
       </c>
-      <c r="C27" s="124"/>
+      <c r="C27" s="120"/>
     </row>
     <row r="28">
       <c r="A28" s="25">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="124" t="str">
+      <c r="B28" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A28,0)</f>
         <v/>
       </c>
-      <c r="C28" s="124"/>
+      <c r="C28" s="120"/>
     </row>
     <row r="29">
       <c r="A29" s="25">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="124" t="str">
+      <c r="B29" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A29,0)</f>
         <v/>
       </c>
-      <c r="C29" s="124"/>
+      <c r="C29" s="120"/>
     </row>
     <row r="30">
       <c r="A30" s="25">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="124" t="str">
+      <c r="B30" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A30,0)</f>
         <v/>
       </c>
-      <c r="C30" s="124"/>
+      <c r="C30" s="120"/>
     </row>
     <row r="31">
       <c r="A31" s="25">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="124" t="str">
+      <c r="B31" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A31,0)</f>
         <v/>
       </c>
-      <c r="C31" s="124"/>
+      <c r="C31" s="120"/>
     </row>
     <row r="32">
       <c r="A32" s="25">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="124" t="str">
+      <c r="B32" s="120" t="str">
         <f>OFFSET(ITEMS!$B$6,A32,0)</f>
         <v/>
       </c>
-      <c r="C32" s="124"/>
+      <c r="C32" s="120"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -5412,245 +5391,273 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="121" t="s">
+        <v>377</v>
+      </c>
+      <c r="B2" s="122">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="55" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B3" s="122">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="49" t="s">
         <v>379</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="B4" s="123">
+        <v>3.0</v>
+      </c>
+      <c r="C4" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="121" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="B5" s="122">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="49" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="125" t="s">
+      <c r="B6" s="123">
+        <v>3.0</v>
+      </c>
+      <c r="C6" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="121" t="s">
         <v>382</v>
       </c>
-      <c r="B2" s="126">
+      <c r="B7" s="123">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="121" t="s">
+        <v>383</v>
+      </c>
+      <c r="B8" s="124">
+        <v>5.0</v>
+      </c>
+      <c r="C8" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="55" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="125">
+        <v>4.0</v>
+      </c>
+      <c r="C9" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="49" t="s">
+        <v>385</v>
+      </c>
+      <c r="B10" s="125">
+        <v>4.0</v>
+      </c>
+      <c r="C10" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="55" t="s">
+        <v>386</v>
+      </c>
+      <c r="B11" s="122">
         <v>1.0</v>
       </c>
-      <c r="C2" s="54" t="b">
+      <c r="C11" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="121" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" s="125">
+        <v>4.0</v>
+      </c>
+      <c r="C12" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="75" t="b">
+      <c r="D12" s="71" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="59" t="s">
-        <v>383</v>
-      </c>
-      <c r="B3" s="126">
+    <row r="13">
+      <c r="A13" s="121" t="s">
+        <v>388</v>
+      </c>
+      <c r="B13" s="122">
         <v>1.0</v>
       </c>
-      <c r="C3" s="60" t="b">
+      <c r="C13" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="121" t="s">
+        <v>389</v>
+      </c>
+      <c r="B14" s="126">
+        <v>2.0</v>
+      </c>
+      <c r="C14" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="121" t="s">
+        <v>390</v>
+      </c>
+      <c r="B15" s="123">
+        <v>3.0</v>
+      </c>
+      <c r="C15" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="49" t="s">
+        <v>391</v>
+      </c>
+      <c r="B16" s="126">
+        <v>2.0</v>
+      </c>
+      <c r="C16" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="53" t="s">
-        <v>384</v>
-      </c>
-      <c r="B4" s="127">
+      <c r="D16" s="71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="55" t="s">
+        <v>392</v>
+      </c>
+      <c r="B17" s="126">
+        <v>2.0</v>
+      </c>
+      <c r="C17" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="49" t="s">
+        <v>393</v>
+      </c>
+      <c r="B18" s="123">
         <v>3.0</v>
       </c>
-      <c r="C4" s="54" t="b">
+      <c r="C18" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="75" t="b">
+      <c r="D18" s="71" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="125" t="s">
-        <v>385</v>
-      </c>
-      <c r="B5" s="126">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="60" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="53" t="s">
-        <v>386</v>
-      </c>
-      <c r="B6" s="127">
-        <v>3.0</v>
-      </c>
-      <c r="C6" s="54" t="b">
+    <row r="19">
+      <c r="A19" s="63" t="s">
+        <v>312</v>
+      </c>
+      <c r="B19" s="127">
+        <v>5.0</v>
+      </c>
+      <c r="C19" s="64" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="75" t="b">
+      <c r="D19" s="99" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="125" t="s">
-        <v>387</v>
-      </c>
-      <c r="B7" s="127">
-        <v>3.0</v>
-      </c>
-      <c r="C7" s="60" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="125" t="s">
-        <v>388</v>
-      </c>
-      <c r="B8" s="128">
-        <v>5.0</v>
-      </c>
-      <c r="C8" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="75" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="59" t="s">
-        <v>389</v>
-      </c>
-      <c r="B9" s="129">
-        <v>4.0</v>
-      </c>
-      <c r="C9" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="74" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="53" t="s">
-        <v>390</v>
-      </c>
-      <c r="B10" s="129">
-        <v>4.0</v>
-      </c>
-      <c r="C10" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="75" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="59" t="s">
-        <v>391</v>
-      </c>
-      <c r="B11" s="126">
-        <v>1.0</v>
-      </c>
-      <c r="C11" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="74" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="125" t="s">
-        <v>392</v>
-      </c>
-      <c r="B12" s="129">
-        <v>4.0</v>
-      </c>
-      <c r="C12" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="75" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="125" t="s">
-        <v>393</v>
-      </c>
-      <c r="B13" s="126">
-        <v>1.0</v>
-      </c>
-      <c r="C13" s="60" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="125" t="s">
-        <v>394</v>
-      </c>
-      <c r="B14" s="130">
-        <v>2.0</v>
-      </c>
-      <c r="C14" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="75" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="59" t="s">
-        <v>395</v>
-      </c>
-      <c r="B15" s="127">
-        <v>3.0</v>
-      </c>
-      <c r="C15" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="74" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="53" t="s">
-        <v>396</v>
-      </c>
-      <c r="B16" s="127">
-        <v>3.0</v>
-      </c>
-      <c r="C16" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="75" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="67" t="s">
-        <v>317</v>
-      </c>
-      <c r="B17" s="131">
-        <v>5.0</v>
-      </c>
-      <c r="C17" s="68" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="103" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B17">
+  <conditionalFormatting sqref="B2:B19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="1"/>
@@ -5662,13 +5669,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A17">
+  <conditionalFormatting sqref="A2:A19">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>$C2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B17">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B19">
       <formula1>AND(ISNUMBER(B2),(NOT(OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -5756,7 +5763,7 @@
     </row>
     <row r="2">
       <c r="A2" s="28">
-        <f t="shared" ref="A2:A36" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A35" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -6142,7 +6149,7 @@
         <v>24</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>64</v>
@@ -6745,16 +6752,16 @@
         <v>24</v>
       </c>
       <c r="I24" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="32" t="s">
         <v>23</v>
-      </c>
-      <c r="J24" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" s="32" t="s">
-        <v>64</v>
       </c>
       <c r="M24" s="32" t="s">
         <v>24</v>
@@ -6782,13 +6789,13 @@
         <v>153</v>
       </c>
       <c r="C25" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="E25" s="35" t="s">
         <v>155</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>156</v>
       </c>
       <c r="F25" s="36"/>
       <c r="G25" s="37" t="s">
@@ -6798,16 +6805,16 @@
         <v>24</v>
       </c>
       <c r="I25" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="J25" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="K25" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="L25" s="37" t="s">
-        <v>23</v>
       </c>
       <c r="M25" s="37" t="s">
         <v>24</v>
@@ -6832,16 +6839,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="D26" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="E26" s="30" t="s">
         <v>159</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>160</v>
       </c>
       <c r="F26" s="31"/>
       <c r="G26" s="40" t="s">
@@ -6851,7 +6858,7 @@
         <v>24</v>
       </c>
       <c r="I26" s="32" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="J26" s="40" t="s">
         <v>24</v>
@@ -6860,7 +6867,7 @@
         <v>24</v>
       </c>
       <c r="L26" s="32" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="M26" s="40" t="s">
         <v>23</v>
@@ -6885,16 +6892,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="E27" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>164</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="12" t="s">
@@ -6928,16 +6935,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="D28" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="E28" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>168</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="7" t="s">
@@ -6971,16 +6978,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="D29" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="E29" s="15" t="s">
         <v>171</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>172</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="12" t="s">
@@ -7014,16 +7021,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="D30" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="E30" s="14" t="s">
         <v>175</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>176</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="7" t="s">
@@ -7057,16 +7064,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="D31" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="E31" s="15" t="s">
         <v>179</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>180</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
@@ -7100,16 +7107,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>184</v>
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="7" t="s">
@@ -7119,16 +7126,16 @@
         <v>24</v>
       </c>
       <c r="I32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L32" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="M32" s="7" t="s">
         <v>24</v>
@@ -7143,20 +7150,20 @@
         <v>31</v>
       </c>
       <c r="B33" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="D33" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="E33" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>188</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>24</v>
@@ -7168,10 +7175,10 @@
         <v>24</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>24</v>
@@ -7186,35 +7193,35 @@
         <v>32</v>
       </c>
       <c r="B34" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="D34" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="E34" s="14" t="s">
         <v>191</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>192</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K34" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="L34" s="7" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="M34" s="7" t="s">
         <v>24</v>
@@ -7224,97 +7231,54 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="29">
+      <c r="A35" s="42">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K35" s="12" t="s">
+      <c r="F35" s="23"/>
+      <c r="G35" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="L35" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="N35" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="42">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>197</v>
-      </c>
-      <c r="C36" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="43" t="s">
-        <v>198</v>
-      </c>
-      <c r="F36" s="45"/>
-      <c r="G36" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="I36" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="L36" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="N36" s="47" t="s">
+      <c r="H35" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M35" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" s="24" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A36">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A35">
       <formula1>AND(ISNUMBER(A2),(NOT(OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D")))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:N36">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:N35">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7355,316 +7319,316 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="H1" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="I1" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="J1" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="K1" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="L1" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="M1" s="47" t="s">
         <v>205</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="N1" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="J1" s="50" t="s">
-        <v>207</v>
-      </c>
-      <c r="K1" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" s="51" t="s">
-        <v>209</v>
-      </c>
-      <c r="M1" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="N1" s="52" t="s">
-        <v>211</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <f>ROW()-ROW(Table_Action_Conditions[N])</f>
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="G2" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="H2" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="I2" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="J2" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>217</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>218</v>
-      </c>
-      <c r="I2" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="J2" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="K2" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="L2" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="M2" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="N2" s="58" t="b">
+      <c r="K2" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="L2" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="M2" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="N2" s="54" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="59">
+      <c r="A3" s="55">
         <f>ROW()-ROW(Table_Action_Conditions[N])</f>
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" s="61" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" s="62" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" s="62" t="s">
+      <c r="B3" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>212</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="I3" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="J3" s="58" t="s">
         <v>215</v>
       </c>
-      <c r="F3" s="62" t="s">
-        <v>223</v>
-      </c>
-      <c r="G3" s="62" t="s">
-        <v>217</v>
-      </c>
-      <c r="H3" s="62" t="s">
-        <v>224</v>
-      </c>
-      <c r="I3" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="J3" s="62" t="s">
-        <v>220</v>
-      </c>
-      <c r="K3" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="L3" s="62" t="s">
-        <v>220</v>
-      </c>
-      <c r="M3" s="63" t="s">
-        <v>213</v>
-      </c>
-      <c r="N3" s="64" t="b">
+      <c r="K3" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="L3" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="M3" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="N3" s="60" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53">
+      <c r="A4" s="49">
         <f>ROW()-ROW(Table_Action_Conditions[N])</f>
         <v>2</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="65" t="s">
-        <v>213</v>
-      </c>
-      <c r="D4" s="56" t="s">
-        <v>226</v>
-      </c>
-      <c r="E4" s="56" t="s">
-        <v>227</v>
-      </c>
-      <c r="F4" s="56" t="s">
-        <v>223</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>217</v>
-      </c>
-      <c r="H4" s="56" t="s">
-        <v>224</v>
-      </c>
-      <c r="I4" s="56" t="s">
+      <c r="B4" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="H4" s="52" t="s">
         <v>219</v>
       </c>
-      <c r="J4" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="K4" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="L4" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="M4" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="N4" s="58" t="b">
+      <c r="I4" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="J4" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="L4" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="M4" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="N4" s="54" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="59">
+      <c r="A5" s="55">
         <f>ROW()-ROW(Table_Action_Conditions[N])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>228</v>
-      </c>
-      <c r="C5" s="66" t="s">
+      <c r="B5" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="D5" s="62" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" s="62" t="s">
-        <v>230</v>
-      </c>
-      <c r="G5" s="62" t="s">
-        <v>231</v>
-      </c>
-      <c r="H5" s="62" t="s">
-        <v>218</v>
-      </c>
-      <c r="I5" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="J5" s="62" t="s">
-        <v>220</v>
-      </c>
-      <c r="K5" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="L5" s="62" t="s">
-        <v>220</v>
-      </c>
-      <c r="M5" s="63" t="s">
-        <v>232</v>
-      </c>
-      <c r="N5" s="64" t="b">
+      <c r="I5" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="J5" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="K5" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="L5" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="M5" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="N5" s="60" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="53">
+      <c r="A6" s="49">
         <f>ROW()-ROW(Table_Action_Conditions[N])</f>
         <v>4</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>233</v>
-      </c>
-      <c r="C6" s="55" t="s">
+      <c r="B6" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>222</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="G6" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="H6" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="D6" s="56" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>227</v>
-      </c>
-      <c r="F6" s="56" t="s">
+      <c r="I6" s="52" t="s">
         <v>230</v>
       </c>
-      <c r="G6" s="56" t="s">
-        <v>234</v>
-      </c>
-      <c r="H6" s="56" t="s">
-        <v>218</v>
-      </c>
-      <c r="I6" s="56" t="s">
-        <v>235</v>
-      </c>
-      <c r="J6" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="K6" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="L6" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="M6" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="N6" s="58" t="b">
+      <c r="J6" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="K6" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="L6" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="M6" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="N6" s="54" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="67">
+      <c r="A7" s="63">
         <f>ROW()-ROW(Table_Action_Conditions[N])</f>
         <v>5</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>236</v>
-      </c>
-      <c r="C7" s="69" t="s">
+      <c r="B7" s="64" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="66" t="s">
+        <v>212</v>
+      </c>
+      <c r="H7" s="66" t="s">
         <v>213</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="I7" s="66" t="s">
         <v>214</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="J7" s="66" t="s">
         <v>215</v>
       </c>
-      <c r="F7" s="70" t="s">
-        <v>216</v>
-      </c>
-      <c r="G7" s="70" t="s">
-        <v>217</v>
-      </c>
-      <c r="H7" s="70" t="s">
-        <v>218</v>
-      </c>
-      <c r="I7" s="70" t="s">
-        <v>219</v>
-      </c>
-      <c r="J7" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="K7" s="70" t="s">
-        <v>219</v>
-      </c>
-      <c r="L7" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="M7" s="71" t="s">
-        <v>213</v>
-      </c>
-      <c r="N7" s="72" t="b">
+      <c r="K7" s="66" t="s">
+        <v>214</v>
+      </c>
+      <c r="L7" s="66" t="s">
+        <v>215</v>
+      </c>
+      <c r="M7" s="67" t="s">
+        <v>208</v>
+      </c>
+      <c r="N7" s="68" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7713,92 +7677,92 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
-        <v>237</v>
-      </c>
-      <c r="C1" s="73" t="s">
-        <v>238</v>
+      <c r="B1" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <f>ROW()-ROW(Table_sprites[N])</f>
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>239</v>
+      <c r="B2" s="50" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="59">
+      <c r="A3" s="55">
         <f>ROW()-ROW(Table_sprites[N])</f>
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="74" t="s">
-        <v>241</v>
+      <c r="B3" s="56" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53">
+      <c r="A4" s="49">
         <f>ROW()-ROW(Table_sprites[N])</f>
         <v>2</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>243</v>
+      <c r="B4" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="59">
+      <c r="A5" s="55">
         <f>ROW()-ROW(Table_sprites[N])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>244</v>
-      </c>
-      <c r="C5" s="74" t="s">
-        <v>245</v>
+      <c r="B5" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="53">
+      <c r="A6" s="49">
         <f>ROW()-ROW(Table_sprites[N])</f>
         <v>4</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>246</v>
-      </c>
-      <c r="C6" s="75" t="s">
-        <v>247</v>
+      <c r="B6" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="59">
+      <c r="A7" s="55">
         <f>ROW()-ROW(Table_sprites[N])</f>
         <v>5</v>
       </c>
-      <c r="B7" s="60" t="s">
-        <v>248</v>
-      </c>
-      <c r="C7" s="74" t="s">
-        <v>249</v>
+      <c r="B7" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="76">
+      <c r="A8" s="72">
         <f>ROW()-ROW(Table_sprites[N])</f>
         <v>6</v>
       </c>
-      <c r="B8" s="77" t="s">
-        <v>250</v>
+      <c r="B8" s="73" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -7835,272 +7799,272 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="G1" s="46" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="H1" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1" s="50" t="s">
-        <v>254</v>
-      </c>
-      <c r="F1" s="49" t="s">
-        <v>255</v>
-      </c>
-      <c r="G1" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="H1" s="52" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="78">
+      <c r="A2" s="74">
         <f t="shared" ref="A2:A10" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="78" t="s">
-        <v>215</v>
-      </c>
-      <c r="C2" s="79" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="80" t="s">
-        <v>259</v>
-      </c>
-      <c r="E2" s="81" t="s">
-        <v>239</v>
-      </c>
-      <c r="F2" s="82" t="b">
+      <c r="B2" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>234</v>
+      </c>
+      <c r="F2" s="78" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="79" t="s">
-        <v>239</v>
-      </c>
-      <c r="H2" s="83" t="s">
-        <v>212</v>
+      <c r="G2" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="H2" s="79" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="78">
+      <c r="A3" s="74">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="78" t="s">
-        <v>260</v>
-      </c>
-      <c r="C3" s="79" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>262</v>
-      </c>
-      <c r="E3" s="81" t="s">
-        <v>240</v>
-      </c>
-      <c r="F3" s="82" t="b">
+      <c r="B3" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="75" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>257</v>
+      </c>
+      <c r="E3" s="77" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="78" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="79" t="s">
-        <v>239</v>
-      </c>
-      <c r="H3" s="83" t="s">
-        <v>212</v>
+      <c r="G3" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="H3" s="79" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="78">
+      <c r="A4" s="74">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="78" t="s">
-        <v>263</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>264</v>
-      </c>
-      <c r="D4" s="80" t="s">
-        <v>262</v>
-      </c>
-      <c r="E4" s="81" t="s">
-        <v>240</v>
-      </c>
-      <c r="F4" s="82" t="b">
+      <c r="B4" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>257</v>
+      </c>
+      <c r="E4" s="77" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="78" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="79" t="s">
-        <v>239</v>
-      </c>
-      <c r="H4" s="83" t="s">
-        <v>212</v>
+      <c r="G4" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="H4" s="79" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="78">
+      <c r="A5" s="74">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="78" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" s="80" t="s">
-        <v>262</v>
-      </c>
-      <c r="E5" s="81" t="s">
-        <v>239</v>
-      </c>
-      <c r="F5" s="82" t="b">
+      <c r="B5" s="74" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>257</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>235</v>
+      </c>
+      <c r="F5" s="78" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="79" t="s">
-        <v>239</v>
-      </c>
-      <c r="H5" s="83" t="s">
-        <v>212</v>
+      <c r="G5" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="H5" s="79" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="78">
+      <c r="A6" s="74">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="78" t="s">
-        <v>229</v>
-      </c>
-      <c r="C6" s="79" t="s">
-        <v>267</v>
-      </c>
-      <c r="D6" s="80" t="s">
-        <v>268</v>
-      </c>
-      <c r="E6" s="81" t="s">
-        <v>240</v>
-      </c>
-      <c r="F6" s="82" t="b">
+      <c r="B6" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="75" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" s="77" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" s="78" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="79" t="s">
-        <v>240</v>
-      </c>
-      <c r="H6" s="83" t="s">
-        <v>221</v>
+      <c r="G6" s="75" t="s">
+        <v>235</v>
+      </c>
+      <c r="H6" s="79" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="78">
+      <c r="A7" s="74">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="C7" s="79" t="s">
-        <v>269</v>
-      </c>
-      <c r="D7" s="80" t="s">
-        <v>268</v>
-      </c>
-      <c r="E7" s="81" t="s">
-        <v>242</v>
-      </c>
-      <c r="F7" s="82" t="b">
+      <c r="B7" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>264</v>
+      </c>
+      <c r="D7" s="76" t="s">
+        <v>263</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="F7" s="78" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="79" t="s">
-        <v>242</v>
-      </c>
-      <c r="H7" s="83" t="s">
-        <v>225</v>
+      <c r="G7" s="75" t="s">
+        <v>237</v>
+      </c>
+      <c r="H7" s="79" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="78">
+      <c r="A8" s="74">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="78" t="s">
-        <v>270</v>
-      </c>
-      <c r="C8" s="79" t="s">
-        <v>271</v>
-      </c>
-      <c r="D8" s="80" t="s">
+      <c r="B8" s="74" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" s="77" t="s">
+        <v>267</v>
+      </c>
+      <c r="F8" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="H8" s="79" t="s">
         <v>268</v>
       </c>
-      <c r="E8" s="81" t="s">
-        <v>272</v>
-      </c>
-      <c r="F8" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="79" t="s">
-        <v>239</v>
-      </c>
-      <c r="H8" s="83" t="s">
-        <v>273</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="78">
+      <c r="A9" s="74">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="78" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" s="79" t="s">
-        <v>275</v>
-      </c>
-      <c r="D9" s="80" t="s">
-        <v>276</v>
-      </c>
-      <c r="E9" s="81" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" s="82" t="b">
+      <c r="B9" s="74" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" s="76" t="s">
+        <v>271</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>243</v>
+      </c>
+      <c r="F9" s="78" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="79" t="s">
-        <v>239</v>
-      </c>
-      <c r="H9" s="83" t="s">
-        <v>212</v>
+      <c r="G9" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="H9" s="79" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="78">
+      <c r="A10" s="74">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="78" t="s">
-        <v>277</v>
-      </c>
-      <c r="C10" s="79" t="s">
-        <v>278</v>
-      </c>
-      <c r="D10" s="80" t="s">
-        <v>259</v>
-      </c>
-      <c r="E10" s="81" t="s">
-        <v>250</v>
-      </c>
-      <c r="F10" s="82" t="b">
+      <c r="B10" s="74" t="s">
+        <v>272</v>
+      </c>
+      <c r="C10" s="75" t="s">
+        <v>273</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="78" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="79" t="s">
-        <v>239</v>
-      </c>
-      <c r="H10" s="83" t="s">
-        <v>212</v>
+      <c r="G10" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="H10" s="79" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -8143,293 +8107,293 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
-        <v>279</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>280</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>281</v>
+      <c r="B1" s="45" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <f>ROW()-ROW(Table_Dialogs[N])</f>
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="84" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="85" t="s">
-        <v>282</v>
+      <c r="B2" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="59">
+      <c r="A3" s="55">
         <f>ROW()-ROW(Table_Dialogs[N])</f>
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>283</v>
-      </c>
-      <c r="C3" s="86" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" s="87" t="s">
-        <v>284</v>
+      <c r="B3" s="56" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53">
+      <c r="A4" s="49">
         <f>ROW()-ROW(Table_Dialogs[N])</f>
         <v>2</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>235</v>
-      </c>
-      <c r="C4" s="84" t="s">
-        <v>215</v>
-      </c>
-      <c r="D4" s="85" t="s">
-        <v>285</v>
+      <c r="B4" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="C4" s="80" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="81" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="67">
+      <c r="A5" s="63">
         <f>ROW()-ROW(Table_Dialogs[N])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="C5" s="88" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" s="89" t="s">
+      <c r="B5" s="64" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="84" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="85" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="45" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>287</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>200</v>
-      </c>
-      <c r="D7" s="51" t="s">
-        <v>288</v>
-      </c>
-      <c r="E7" s="51" t="s">
-        <v>289</v>
-      </c>
-      <c r="F7" s="52" t="s">
-        <v>290</v>
+      <c r="C7" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="53">
+      <c r="A8" s="49">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>0</v>
       </c>
-      <c r="B8" s="54" t="s">
-        <v>282</v>
-      </c>
-      <c r="C8" s="55" t="s">
-        <v>213</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="F8" s="90" t="s">
-        <v>220</v>
+      <c r="B8" s="50" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" s="86" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="59">
+      <c r="A9" s="55">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>1</v>
       </c>
-      <c r="B9" s="60" t="s">
-        <v>284</v>
-      </c>
-      <c r="C9" s="66" t="s">
-        <v>213</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>213</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="F9" s="91" t="s">
-        <v>220</v>
+      <c r="B9" s="56" t="s">
+        <v>279</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" s="87" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="53">
+      <c r="A10" s="49">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>2</v>
       </c>
-      <c r="B10" s="54" t="s">
-        <v>291</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>213</v>
-      </c>
-      <c r="D10" s="56" t="s">
-        <v>213</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="F10" s="90" t="s">
-        <v>292</v>
+      <c r="B10" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="F10" s="86" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="59">
+      <c r="A11" s="55">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>3</v>
       </c>
-      <c r="B11" s="60" t="s">
-        <v>293</v>
-      </c>
-      <c r="C11" s="66" t="s">
-        <v>213</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>213</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="F11" s="91" t="s">
-        <v>294</v>
+      <c r="B11" s="56" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="87" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="53">
+      <c r="A12" s="49">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>4</v>
       </c>
-      <c r="B12" s="54" t="s">
-        <v>295</v>
-      </c>
-      <c r="C12" s="55" t="s">
-        <v>232</v>
-      </c>
-      <c r="D12" s="56" t="s">
-        <v>213</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="F12" s="90" t="s">
-        <v>296</v>
+      <c r="B12" s="50" t="s">
+        <v>290</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="F12" s="86" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="59">
+      <c r="A13" s="55">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>5</v>
       </c>
-      <c r="B13" s="60" t="s">
-        <v>297</v>
-      </c>
-      <c r="C13" s="66" t="s">
-        <v>298</v>
-      </c>
-      <c r="D13" s="62" t="s">
-        <v>213</v>
-      </c>
-      <c r="E13" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="F13" s="91" t="s">
-        <v>299</v>
+      <c r="B13" s="56" t="s">
+        <v>292</v>
+      </c>
+      <c r="C13" s="62" t="s">
+        <v>293</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="F13" s="87" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="76">
+      <c r="A14" s="72">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>6</v>
       </c>
-      <c r="B14" s="77" t="s">
-        <v>300</v>
-      </c>
-      <c r="C14" s="92" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" s="93" t="s">
-        <v>213</v>
-      </c>
-      <c r="E14" s="93" t="s">
-        <v>219</v>
-      </c>
-      <c r="F14" s="94" t="s">
-        <v>220</v>
+      <c r="B14" s="73" t="s">
+        <v>295</v>
+      </c>
+      <c r="C14" s="88" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" s="89" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" s="89" t="s">
+        <v>214</v>
+      </c>
+      <c r="F14" s="90" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="95"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
     </row>
     <row r="17">
-      <c r="A17" s="95"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
     </row>
     <row r="18">
-      <c r="A18" s="95"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="95"/>
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
     </row>
     <row r="19">
-      <c r="A19" s="95"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="95"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
     </row>
     <row r="20">
-      <c r="A20" s="95"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95"/>
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
     </row>
     <row r="21">
-      <c r="A21" s="95"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -8478,148 +8442,148 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97" t="s">
-        <v>301</v>
-      </c>
-      <c r="C1" s="96" t="s">
-        <v>302</v>
-      </c>
-      <c r="D1" s="96" t="s">
-        <v>303</v>
+      <c r="B1" s="93" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" s="92" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="78">
+      <c r="A2" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>0</v>
       </c>
-      <c r="B2" s="78" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
+      <c r="B2" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
     </row>
     <row r="3">
-      <c r="A3" s="78">
+      <c r="A3" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>1</v>
       </c>
-      <c r="B3" s="78" t="s">
-        <v>261</v>
-      </c>
-      <c r="C3" s="78" t="s">
-        <v>304</v>
-      </c>
-      <c r="D3" s="78" t="s">
-        <v>304</v>
+      <c r="B3" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="78">
+      <c r="A4" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>2</v>
       </c>
-      <c r="B4" s="78" t="s">
-        <v>264</v>
-      </c>
-      <c r="C4" s="78" t="s">
-        <v>305</v>
-      </c>
-      <c r="D4" s="78" t="s">
-        <v>306</v>
+      <c r="B4" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="78">
+      <c r="A5" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="78" t="s">
-        <v>266</v>
-      </c>
-      <c r="C5" s="78" t="s">
-        <v>307</v>
-      </c>
-      <c r="D5" s="78" t="s">
-        <v>308</v>
+      <c r="B5" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>302</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="78">
+      <c r="A6" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>4</v>
       </c>
-      <c r="B6" s="78" t="s">
-        <v>267</v>
-      </c>
-      <c r="C6" s="78" t="s">
-        <v>309</v>
-      </c>
-      <c r="D6" s="78" t="s">
-        <v>310</v>
+      <c r="B6" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>304</v>
+      </c>
+      <c r="D6" s="74" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="78">
+      <c r="A7" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>5</v>
       </c>
-      <c r="B7" s="78" t="s">
-        <v>269</v>
-      </c>
-      <c r="C7" s="78" t="s">
-        <v>311</v>
-      </c>
-      <c r="D7" s="78" t="s">
-        <v>312</v>
+      <c r="B7" s="74" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>306</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="78">
+      <c r="A8" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>6</v>
       </c>
-      <c r="B8" s="78" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="78" t="s">
-        <v>313</v>
-      </c>
-      <c r="D8" s="78" t="s">
-        <v>314</v>
+      <c r="B8" s="74" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>308</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="78">
+      <c r="A9" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>7</v>
       </c>
-      <c r="B9" s="78" t="s">
-        <v>275</v>
-      </c>
-      <c r="C9" s="78" t="s">
-        <v>315</v>
-      </c>
-      <c r="D9" s="78" t="s">
-        <v>316</v>
+      <c r="B9" s="74" t="s">
+        <v>270</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>310</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="78">
+      <c r="A10" s="74">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>8</v>
       </c>
-      <c r="B10" s="78" t="s">
-        <v>278</v>
-      </c>
-      <c r="C10" s="78" t="s">
-        <v>317</v>
-      </c>
-      <c r="D10" s="78" t="s">
-        <v>318</v>
+      <c r="B10" s="74" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="74" t="s">
+        <v>312</v>
+      </c>
+      <c r="D10" s="74" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -8651,189 +8615,189 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>318</v>
+      </c>
+      <c r="G1" s="95" t="s">
         <v>319</v>
       </c>
-      <c r="C1" s="50" t="s">
-        <v>320</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>321</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>322</v>
-      </c>
-      <c r="F1" s="49" t="s">
-        <v>323</v>
-      </c>
-      <c r="G1" s="99" t="s">
-        <v>324</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="53">
+      <c r="A2" s="49">
         <f>ROW()-ROW(Table_Phrases[N])</f>
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" s="54">
+      <c r="B2" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="50">
         <v>0.0</v>
       </c>
-      <c r="D2" s="54">
+      <c r="D2" s="50">
         <v>0.0</v>
       </c>
-      <c r="E2" s="57" t="s">
-        <v>325</v>
-      </c>
-      <c r="G2" s="75"/>
+      <c r="E2" s="53" t="s">
+        <v>320</v>
+      </c>
+      <c r="G2" s="71"/>
     </row>
     <row r="3">
-      <c r="A3" s="59">
+      <c r="A3" s="55">
         <f>ROW()-ROW(Table_Phrases[N])</f>
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>326</v>
-      </c>
-      <c r="C3" s="60">
+      <c r="B3" s="56" t="s">
+        <v>321</v>
+      </c>
+      <c r="C3" s="56">
         <v>0.0</v>
       </c>
-      <c r="D3" s="60">
+      <c r="D3" s="56">
         <v>0.0</v>
       </c>
-      <c r="E3" s="63" t="s">
-        <v>327</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>328</v>
-      </c>
-      <c r="G3" s="74" t="s">
-        <v>329</v>
+      <c r="E3" s="59" t="s">
+        <v>322</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>323</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53">
+      <c r="A4" s="49">
         <f>ROW()-ROW(Table_Phrases[N])</f>
         <v>2</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" s="54">
+      <c r="B4" s="50" t="s">
+        <v>325</v>
+      </c>
+      <c r="C4" s="50">
         <v>0.0</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="50">
         <v>0.0</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="53" t="s">
+        <v>322</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>326</v>
+      </c>
+      <c r="G4" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="F4" s="54" t="s">
-        <v>331</v>
-      </c>
-      <c r="G4" s="75" t="s">
-        <v>332</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" s="59">
+      <c r="A5" s="55">
         <f>ROW()-ROW(Table_Phrases[N])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>333</v>
-      </c>
-      <c r="C5" s="60">
+      <c r="B5" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" s="56">
         <v>0.0</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="56">
         <v>0.0</v>
       </c>
-      <c r="E5" s="63" t="s">
-        <v>327</v>
-      </c>
-      <c r="F5" s="60" t="s">
-        <v>334</v>
-      </c>
-      <c r="G5" s="74" t="s">
-        <v>335</v>
+      <c r="E5" s="59" t="s">
+        <v>322</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="53">
+      <c r="A6" s="49">
         <f>ROW()-ROW(Table_Phrases[N])</f>
         <v>4</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>294</v>
-      </c>
-      <c r="C6" s="54">
+      <c r="B6" s="50" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" s="50">
         <v>0.0</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="50">
         <v>0.0</v>
       </c>
-      <c r="E6" s="57" t="s">
-        <v>327</v>
-      </c>
-      <c r="F6" s="54" t="s">
-        <v>336</v>
-      </c>
-      <c r="G6" s="75" t="s">
-        <v>337</v>
+      <c r="E6" s="53" t="s">
+        <v>322</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>331</v>
+      </c>
+      <c r="G6" s="71" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="59">
+      <c r="A7" s="55">
         <f>ROW()-ROW(Table_Phrases[N])</f>
         <v>5</v>
       </c>
-      <c r="B7" s="60" t="s">
-        <v>296</v>
-      </c>
-      <c r="C7" s="60">
+      <c r="B7" s="56" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" s="56">
         <v>0.0</v>
       </c>
-      <c r="D7" s="60">
+      <c r="D7" s="56">
         <v>0.0</v>
       </c>
-      <c r="E7" s="63" t="s">
-        <v>327</v>
-      </c>
-      <c r="F7" s="60" t="s">
-        <v>338</v>
-      </c>
-      <c r="G7" s="74" t="s">
-        <v>339</v>
+      <c r="E7" s="59" t="s">
+        <v>322</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="76">
+      <c r="A8" s="72">
         <f>ROW()-ROW(Table_Phrases[N])</f>
         <v>6</v>
       </c>
-      <c r="B8" s="77" t="s">
-        <v>299</v>
-      </c>
-      <c r="C8" s="77">
+      <c r="B8" s="73" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8" s="73">
         <v>0.0</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="73">
         <v>0.0</v>
       </c>
-      <c r="E8" s="100" t="s">
-        <v>327</v>
-      </c>
-      <c r="F8" s="77" t="s">
-        <v>340</v>
-      </c>
-      <c r="G8" s="101" t="s">
-        <v>341</v>
+      <c r="E8" s="96" t="s">
+        <v>322</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>335</v>
+      </c>
+      <c r="G8" s="97" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -8873,37 +8837,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>339</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>340</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>341</v>
+      </c>
+      <c r="G1" s="48" t="s">
         <v>342</v>
       </c>
-      <c r="C1" s="51" t="s">
-        <v>343</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>344</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>345</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>346</v>
-      </c>
-      <c r="G1" s="52" t="s">
-        <v>347</v>
-      </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
-      <c r="A2" s="78">
+      <c r="A2" s="74">
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
-      <c r="B2" s="78" t="s">
-        <v>348</v>
-      </c>
-      <c r="C2" s="102" t="str">
+      <c r="B2" s="74" t="s">
+        <v>343</v>
+      </c>
+      <c r="C2" s="98" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8916,11 +8880,11 @@
 )"),"SPRITE_NONE|SPRITE_POTION_RED|SPRITE_POTION_BLUE")</f>
         <v>SPRITE_NONE|SPRITE_POTION_RED|SPRITE_POTION_BLUE</v>
       </c>
-      <c r="D2" s="102" t="str">
+      <c r="D2" s="98" t="str">
         <f t="shared" ref="D2:D4" si="2">SUBSTITUTE(G2,", ","|")</f>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="E2" s="102" t="str">
+      <c r="E2" s="98" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8933,22 +8897,22 @@
 )"),"NAME_NONE|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION")</f>
         <v>NAME_NONE|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION</v>
       </c>
-      <c r="F2" s="83" t="s">
-        <v>215</v>
-      </c>
-      <c r="G2" s="83" t="s">
-        <v>326</v>
+      <c r="F2" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="79" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
-      <c r="A3" s="78">
+      <c r="A3" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="B3" s="78" t="s">
-        <v>349</v>
-      </c>
-      <c r="C3" s="102" t="str">
+      <c r="B3" s="74" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" s="98" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8958,14 +8922,14 @@
 ),"", "")
 ))
 )
-)"),"SPRITE_POTION_RED|SPRITE_POTION_BLUE|SPRITE_FOUNTAIN|SPRITE_FOUNTAIN_FULL|SPRITE_NPC_MILITO")</f>
-        <v>SPRITE_POTION_RED|SPRITE_POTION_BLUE|SPRITE_FOUNTAIN|SPRITE_FOUNTAIN_FULL|SPRITE_NPC_MILITO</v>
-      </c>
-      <c r="D3" s="102" t="str">
+)"),"SPRITE_POTION_RED|SPRITE_POTION_BLUE|SPRITE_FOUNTAIN|SPRITE_FOUNTAIN_FULL")</f>
+        <v>SPRITE_POTION_RED|SPRITE_POTION_BLUE|SPRITE_FOUNTAIN|SPRITE_FOUNTAIN_FULL</v>
+      </c>
+      <c r="D3" s="98" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE|PHRASE_ASK_FOUNTAIN1_1|PHRASE_ASK_FOUNTAIN1_2|PHRASE_ASK_FOUNTAIN2_1|PHRASE_ASK_FOUNTAIN3_1|PHRASE_ASK_FOUNTAIN4_1</v>
       </c>
-      <c r="E3" s="102" t="str">
+      <c r="E3" s="98" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8975,25 +8939,25 @@
 ),"", "")
 ))
 )
-)"),"NAME_CHAR_MAIN|NAME_CHAR_PARROT|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION|NAME_ITEM_FOUNTAIN|NAME_NPC_MILITO")</f>
-        <v>NAME_CHAR_MAIN|NAME_CHAR_PARROT|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION|NAME_ITEM_FOUNTAIN|NAME_NPC_MILITO</v>
-      </c>
-      <c r="F3" s="83" t="s">
-        <v>350</v>
-      </c>
-      <c r="G3" s="83" t="s">
-        <v>351</v>
+)"),"NAME_CHAR_MAIN|NAME_CHAR_PARROT|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION|NAME_ITEM_FOUNTAIN")</f>
+        <v>NAME_CHAR_MAIN|NAME_CHAR_PARROT|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION|NAME_ITEM_FOUNTAIN</v>
+      </c>
+      <c r="F3" s="79" t="s">
+        <v>345</v>
+      </c>
+      <c r="G3" s="79" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="78">
+      <c r="A4" s="74">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B4" s="78" t="s">
-        <v>352</v>
-      </c>
-      <c r="C4" s="102" t="str">
+      <c r="B4" s="74" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="98" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -9006,11 +8970,11 @@
 )"),"SPRITE_LAST|SPRITE_POTION_RED|SPRITE_POTION_BLUE")</f>
         <v>SPRITE_LAST|SPRITE_POTION_RED|SPRITE_POTION_BLUE</v>
       </c>
-      <c r="D4" s="102" t="str">
+      <c r="D4" s="98" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="E4" s="102" t="str">
+      <c r="E4" s="98" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -9023,11 +8987,11 @@
 )"),"NAME_NPC_LAST|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION")</f>
         <v>NAME_NPC_LAST|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION</v>
       </c>
-      <c r="F4" s="83" t="s">
-        <v>277</v>
-      </c>
-      <c r="G4" s="83" t="s">
-        <v>326</v>
+      <c r="F4" s="79" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="79" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Added Background and cursor management -Avoid duplicates -Material for sprites must be default and not lit
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="Aax0f1fmZiGbGskZ2MsUEVCwLOdnAGfn+GhbmUsxFws="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="7HpSjmvl9/MN+qdlBOXR8fMZIVdPnazd/N6YkLe4oks="/>
     </ext>
   </extLst>
 </workbook>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="397">
   <si>
     <t>N</t>
   </si>
@@ -796,34 +796,40 @@
     <t>SPRITE_NONE</t>
   </si>
   <si>
+    <t>SPRITE_CURSOR_NORMAL</t>
+  </si>
+  <si>
+    <t>SPRITE_INVENTORY</t>
+  </si>
+  <si>
     <t>SPRITE_POTION_RED</t>
   </si>
   <si>
-    <t>Sprites/potion_64</t>
+    <t>SPRITE_ITEM_POTION</t>
   </si>
   <si>
     <t>SPRITE_POTION_BLUE</t>
   </si>
   <si>
-    <t>Sprites/potionblue_64</t>
+    <t>SPRITE_ITEM_POTION_BLUE</t>
   </si>
   <si>
     <t>SPRITE_FOUNTAIN</t>
   </si>
   <si>
-    <t>Sprites/spr_fountain_256</t>
+    <t>SPRITE_ITEM_FOUNTAIN</t>
   </si>
   <si>
     <t>SPRITE_FOUNTAIN_FULL</t>
   </si>
   <si>
-    <t>Sprites/spr_fountain_full_256</t>
+    <t>SPRITE_ITEM_FOUNTAIN_FULL</t>
   </si>
   <si>
     <t>SPRITE_NPC_MILITO</t>
   </si>
   <si>
-    <t>Sprites/spr_milito_1</t>
+    <t>BACKGROUND_ROOM_FIRST</t>
   </si>
   <si>
     <t>SPRITE_LAST</t>
@@ -1112,6 +1118,9 @@
   </si>
   <si>
     <t>CompoundNamesText</t>
+  </si>
+  <si>
+    <t>NeededBackgrounds_Sprites</t>
   </si>
   <si>
     <t>NeededItems</t>
@@ -1504,6 +1513,20 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
@@ -1528,20 +1551,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
@@ -1877,9 +1886,51 @@
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1887,77 +1938,35 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="16" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1977,7 +1986,7 @@
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2282,15 +2291,16 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G4" displayName="Table_Rooms" name="Table_Rooms" id="10">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H4" displayName="Table_Rooms" name="Table_Rooms" id="10">
+  <tableColumns count="8">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
     <tableColumn name="CompoundSpritesText" id="3"/>
     <tableColumn name="CompoundPhrasesText" id="4"/>
     <tableColumn name="CompoundNamesText" id="5"/>
-    <tableColumn name="NeededItems" id="6"/>
-    <tableColumn name="NeededPhrases" id="7"/>
+    <tableColumn name="NeededBackgrounds_Sprites" id="6"/>
+    <tableColumn name="NeededItems" id="7"/>
+    <tableColumn name="NeededPhrases" id="8"/>
   </tableColumns>
   <tableStyleInfo name="ROOMS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -2447,7 +2457,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C8" displayName="Table_sprites" name="Table_sprites" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C11" displayName="Table_sprites" name="Table_sprites" id="4">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SPRITE_ID" id="2"/>
@@ -4435,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2">
@@ -4470,8 +4480,8 @@
         <f>ROW()-ROW(Table_Characters[N])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="99" t="s">
-        <v>349</v>
+      <c r="B5" s="72" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="6">
@@ -4483,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="69" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8">
@@ -4499,7 +4509,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10">
@@ -4530,7 +4540,7 @@
       <c r="A13" s="63">
         <v>5.0</v>
       </c>
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="72" t="s">
         <v>226</v>
       </c>
     </row>
@@ -4539,7 +4549,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16">
@@ -4571,7 +4581,7 @@
         <v>3.0</v>
       </c>
       <c r="B19" s="70" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20">
@@ -4579,15 +4589,15 @@
         <v>4.0</v>
       </c>
       <c r="B20" s="71" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="63">
         <v>5.0</v>
       </c>
-      <c r="B21" s="99" t="s">
-        <v>355</v>
+      <c r="B21" s="72" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="23">
@@ -4595,7 +4605,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24">
@@ -4603,15 +4613,15 @@
         <v>0.0</v>
       </c>
       <c r="B24" s="71" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="63">
         <v>1.0</v>
       </c>
-      <c r="B25" s="99" t="s">
-        <v>322</v>
+      <c r="B25" s="72" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="27">
@@ -4619,7 +4629,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28">
@@ -4628,7 +4638,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="71" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29">
@@ -4637,7 +4647,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="100" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="30">
@@ -4646,7 +4656,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="101" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31">
@@ -4655,16 +4665,16 @@
         <v>3</v>
       </c>
       <c r="B31" s="100" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="72">
+      <c r="A32" s="87">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>4</v>
       </c>
       <c r="B32" s="102" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -4708,19 +4718,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="F1" s="69" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2">
@@ -4745,25 +4755,25 @@
         <v>227</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D3" s="58" t="s">
         <v>224</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F3" s="105" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="72">
+      <c r="A4" s="87">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="73" t="s">
-        <v>365</v>
+      <c r="B4" s="88" t="s">
+        <v>368</v>
       </c>
       <c r="C4" s="106"/>
       <c r="D4" s="106"/>
@@ -4775,7 +4785,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7">
@@ -4876,16 +4886,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="114" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B1" s="115" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="D1" s="114" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="E1" s="115" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2">
@@ -4940,18 +4950,18 @@
     </row>
     <row r="6">
       <c r="B6" s="117" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E6" s="117" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="119" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E7" s="119" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8">
@@ -5006,10 +5016,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2">
@@ -5022,7 +5032,7 @@
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3">
@@ -5035,7 +5045,7 @@
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4">
@@ -5048,7 +5058,7 @@
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5">
@@ -5061,7 +5071,7 @@
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6">
@@ -5392,21 +5402,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="44" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="121" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B2" s="122">
         <v>1.0</v>
@@ -5420,7 +5430,7 @@
     </row>
     <row r="3">
       <c r="A3" s="55" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B3" s="122">
         <v>1.0</v>
@@ -5434,7 +5444,7 @@
     </row>
     <row r="4">
       <c r="A4" s="49" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B4" s="123">
         <v>3.0</v>
@@ -5448,7 +5458,7 @@
     </row>
     <row r="5">
       <c r="A5" s="121" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B5" s="122">
         <v>1.0</v>
@@ -5462,7 +5472,7 @@
     </row>
     <row r="6">
       <c r="A6" s="49" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B6" s="123">
         <v>3.0</v>
@@ -5476,7 +5486,7 @@
     </row>
     <row r="7">
       <c r="A7" s="121" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B7" s="123">
         <v>3.0</v>
@@ -5490,7 +5500,7 @@
     </row>
     <row r="8">
       <c r="A8" s="121" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B8" s="124">
         <v>5.0</v>
@@ -5504,7 +5514,7 @@
     </row>
     <row r="9">
       <c r="A9" s="55" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B9" s="125">
         <v>4.0</v>
@@ -5518,7 +5528,7 @@
     </row>
     <row r="10">
       <c r="A10" s="49" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B10" s="125">
         <v>4.0</v>
@@ -5532,7 +5542,7 @@
     </row>
     <row r="11">
       <c r="A11" s="55" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B11" s="122">
         <v>1.0</v>
@@ -5546,7 +5556,7 @@
     </row>
     <row r="12">
       <c r="A12" s="121" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B12" s="125">
         <v>4.0</v>
@@ -5560,7 +5570,7 @@
     </row>
     <row r="13">
       <c r="A13" s="121" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B13" s="122">
         <v>1.0</v>
@@ -5574,7 +5584,7 @@
     </row>
     <row r="14">
       <c r="A14" s="121" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B14" s="126">
         <v>2.0</v>
@@ -5588,7 +5598,7 @@
     </row>
     <row r="15">
       <c r="A15" s="121" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B15" s="123">
         <v>3.0</v>
@@ -5601,36 +5611,36 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="49" t="s">
-        <v>391</v>
+      <c r="A16" s="121" t="s">
+        <v>394</v>
       </c>
       <c r="B16" s="126">
         <v>2.0</v>
       </c>
       <c r="C16" s="50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="55" t="s">
-        <v>392</v>
+      <c r="A17" s="121" t="s">
+        <v>395</v>
       </c>
       <c r="B17" s="126">
         <v>2.0</v>
       </c>
       <c r="C17" s="56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="49" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B18" s="123">
         <v>3.0</v>
@@ -5644,7 +5654,7 @@
     </row>
     <row r="19">
       <c r="A19" s="63" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B19" s="127">
         <v>5.0</v>
@@ -5652,7 +5662,7 @@
       <c r="C19" s="64" t="b">
         <v>0</v>
       </c>
-      <c r="D19" s="99" t="b">
+      <c r="D19" s="72" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7671,8 +7681,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="24.71"/>
-    <col customWidth="1" min="3" max="3" width="28.43"/>
+    <col customWidth="1" min="2" max="2" width="28.29"/>
+    <col customWidth="1" min="3" max="3" width="30.43"/>
     <col customWidth="1" min="4" max="4" width="26.0"/>
   </cols>
   <sheetData>
@@ -7705,7 +7715,7 @@
         <v>235</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4">
@@ -7714,10 +7724,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C4" s="71" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5">
@@ -7726,10 +7736,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6">
@@ -7738,10 +7748,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C6" s="71" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7">
@@ -7750,19 +7760,58 @@
         <v>5</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="72">
+      <c r="A8" s="49">
         <f>ROW()-ROW(Table_sprites[N])</f>
         <v>6</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="55">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="56" t="s">
         <v>245</v>
+      </c>
+      <c r="C9" s="70" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="49">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="63">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="64" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -7803,267 +7852,267 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="74">
+      <c r="A2" s="73">
         <f t="shared" ref="A2:A10" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="73" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="75" t="s">
-        <v>253</v>
-      </c>
-      <c r="D2" s="76" t="s">
-        <v>254</v>
-      </c>
-      <c r="E2" s="77" t="s">
+      <c r="C2" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" s="76" t="s">
         <v>234</v>
       </c>
-      <c r="F2" s="78" t="b">
+      <c r="F2" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="75" t="s">
+      <c r="G2" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="H2" s="79" t="s">
+      <c r="H2" s="78" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="74">
+      <c r="A3" s="73">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="74" t="s">
-        <v>255</v>
-      </c>
-      <c r="C3" s="75" t="s">
-        <v>256</v>
-      </c>
-      <c r="D3" s="76" t="s">
+      <c r="B3" s="73" t="s">
         <v>257</v>
       </c>
-      <c r="E3" s="77" t="s">
-        <v>235</v>
-      </c>
-      <c r="F3" s="78" t="b">
+      <c r="C3" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="G3" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="78" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="74">
+      <c r="A4" s="73">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="74" t="s">
-        <v>258</v>
-      </c>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="75" t="s">
         <v>259</v>
       </c>
-      <c r="D4" s="76" t="s">
-        <v>257</v>
-      </c>
-      <c r="E4" s="77" t="s">
-        <v>235</v>
-      </c>
-      <c r="F4" s="78" t="b">
+      <c r="E4" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="G4" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="H4" s="79" t="s">
+      <c r="H4" s="78" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="74" t="s">
-        <v>260</v>
-      </c>
-      <c r="C5" s="75" t="s">
-        <v>261</v>
-      </c>
-      <c r="D5" s="76" t="s">
-        <v>257</v>
-      </c>
-      <c r="E5" s="77" t="s">
-        <v>235</v>
-      </c>
-      <c r="F5" s="78" t="b">
+      <c r="B5" s="73" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>263</v>
+      </c>
+      <c r="D5" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="H5" s="78" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="74">
+      <c r="A6" s="73">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="C6" s="75" t="s">
-        <v>262</v>
-      </c>
-      <c r="D6" s="76" t="s">
-        <v>263</v>
-      </c>
-      <c r="E6" s="77" t="s">
-        <v>235</v>
-      </c>
-      <c r="F6" s="78" t="b">
+      <c r="C6" s="74" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="F6" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="75" t="s">
-        <v>235</v>
-      </c>
-      <c r="H6" s="79" t="s">
+      <c r="G6" s="74" t="s">
+        <v>237</v>
+      </c>
+      <c r="H6" s="78" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="75" t="s">
-        <v>264</v>
-      </c>
-      <c r="D7" s="76" t="s">
-        <v>263</v>
-      </c>
-      <c r="E7" s="77" t="s">
-        <v>237</v>
-      </c>
-      <c r="F7" s="78" t="b">
+      <c r="C7" s="74" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="E7" s="76" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="75" t="s">
-        <v>237</v>
-      </c>
-      <c r="H7" s="79" t="s">
+      <c r="G7" s="74" t="s">
+        <v>239</v>
+      </c>
+      <c r="H7" s="78" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="74">
+      <c r="A8" s="73">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="73" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="75" t="s">
         <v>265</v>
       </c>
-      <c r="C8" s="75" t="s">
-        <v>266</v>
-      </c>
-      <c r="D8" s="76" t="s">
-        <v>263</v>
-      </c>
-      <c r="E8" s="77" t="s">
-        <v>267</v>
-      </c>
-      <c r="F8" s="78" t="b">
+      <c r="E8" s="76" t="s">
+        <v>269</v>
+      </c>
+      <c r="F8" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="G8" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="H8" s="79" t="s">
-        <v>268</v>
+      <c r="H8" s="78" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="74" t="s">
-        <v>269</v>
-      </c>
-      <c r="C9" s="75" t="s">
-        <v>270</v>
-      </c>
-      <c r="D9" s="76" t="s">
+      <c r="B9" s="73" t="s">
         <v>271</v>
       </c>
-      <c r="E9" s="77" t="s">
-        <v>243</v>
-      </c>
-      <c r="F9" s="78" t="b">
+      <c r="C9" s="74" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" s="75" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="75" t="s">
+      <c r="G9" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="H9" s="79" t="s">
+      <c r="H9" s="78" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="74">
+      <c r="A10" s="73">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="74" t="s">
-        <v>272</v>
-      </c>
-      <c r="C10" s="75" t="s">
-        <v>273</v>
-      </c>
-      <c r="D10" s="76" t="s">
-        <v>254</v>
-      </c>
-      <c r="E10" s="77" t="s">
-        <v>245</v>
-      </c>
-      <c r="F10" s="78" t="b">
+      <c r="B10" s="73" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" s="74" t="s">
+        <v>275</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>256</v>
+      </c>
+      <c r="E10" s="76" t="s">
+        <v>247</v>
+      </c>
+      <c r="F10" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="75" t="s">
+      <c r="G10" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="H10" s="79" t="s">
+      <c r="H10" s="78" t="s">
         <v>207</v>
       </c>
     </row>
@@ -8111,13 +8160,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2">
@@ -8128,11 +8177,11 @@
       <c r="B2" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="79" t="s">
         <v>210</v>
       </c>
-      <c r="D2" s="81" t="s">
-        <v>277</v>
+      <c r="D2" s="80" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="3">
@@ -8141,13 +8190,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>278</v>
-      </c>
-      <c r="C3" s="82" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="81" t="s">
         <v>210</v>
       </c>
-      <c r="D3" s="83" t="s">
-        <v>279</v>
+      <c r="D3" s="82" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="4">
@@ -8158,11 +8207,11 @@
       <c r="B4" s="50" t="s">
         <v>230</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="79" t="s">
         <v>210</v>
       </c>
-      <c r="D4" s="81" t="s">
-        <v>280</v>
+      <c r="D4" s="80" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="5">
@@ -8171,13 +8220,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="64" t="s">
-        <v>281</v>
-      </c>
-      <c r="C5" s="84" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="83" t="s">
         <v>210</v>
       </c>
-      <c r="D5" s="85" t="s">
-        <v>277</v>
+      <c r="D5" s="84" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="7">
@@ -8185,19 +8234,19 @@
         <v>0</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C7" s="45" t="s">
         <v>195</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F7" s="48" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8">
@@ -8206,7 +8255,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C8" s="51" t="s">
         <v>208</v>
@@ -8217,7 +8266,7 @@
       <c r="E8" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="85" t="s">
         <v>215</v>
       </c>
     </row>
@@ -8227,7 +8276,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C9" s="62" t="s">
         <v>208</v>
@@ -8238,7 +8287,7 @@
       <c r="E9" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="F9" s="87" t="s">
+      <c r="F9" s="86" t="s">
         <v>215</v>
       </c>
     </row>
@@ -8248,7 +8297,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C10" s="51" t="s">
         <v>208</v>
@@ -8259,8 +8308,8 @@
       <c r="E10" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="F10" s="86" t="s">
-        <v>287</v>
+      <c r="F10" s="85" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="11">
@@ -8269,7 +8318,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C11" s="62" t="s">
         <v>208</v>
@@ -8280,8 +8329,8 @@
       <c r="E11" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="F11" s="87" t="s">
-        <v>289</v>
+      <c r="F11" s="86" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="12">
@@ -8290,7 +8339,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>227</v>
@@ -8301,8 +8350,8 @@
       <c r="E12" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="F12" s="86" t="s">
-        <v>291</v>
+      <c r="F12" s="85" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="13">
@@ -8311,10 +8360,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D13" s="58" t="s">
         <v>208</v>
@@ -8322,78 +8371,78 @@
       <c r="E13" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="F13" s="87" t="s">
-        <v>294</v>
+      <c r="F13" s="86" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="72">
+      <c r="A14" s="87">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>6</v>
       </c>
-      <c r="B14" s="73" t="s">
-        <v>295</v>
-      </c>
-      <c r="C14" s="88" t="s">
+      <c r="B14" s="88" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" s="89" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="89" t="s">
+      <c r="D14" s="90" t="s">
         <v>208</v>
       </c>
-      <c r="E14" s="89" t="s">
+      <c r="E14" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="F14" s="90" t="s">
+      <c r="F14" s="91" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="91"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
     </row>
     <row r="17">
-      <c r="A17" s="91"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
     </row>
     <row r="18">
-      <c r="A18" s="91"/>
-      <c r="B18" s="91"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
     </row>
     <row r="19">
-      <c r="A19" s="91"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
     </row>
     <row r="20">
-      <c r="A20" s="91"/>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
     </row>
     <row r="21">
-      <c r="A21" s="91"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91"/>
+      <c r="A21" s="92"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="92"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -8442,148 +8491,148 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="93" t="s">
-        <v>296</v>
-      </c>
-      <c r="C1" s="92" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" s="92" t="s">
+      <c r="B1" s="94" t="s">
         <v>298</v>
       </c>
+      <c r="C1" s="93" t="s">
+        <v>299</v>
+      </c>
+      <c r="D1" s="93" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="74">
+      <c r="A2" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>0</v>
       </c>
-      <c r="B2" s="74" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
+      <c r="B2" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
     </row>
     <row r="3">
-      <c r="A3" s="74">
+      <c r="A3" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>1</v>
       </c>
-      <c r="B3" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="C3" s="74" t="s">
-        <v>299</v>
-      </c>
-      <c r="D3" s="74" t="s">
-        <v>299</v>
+      <c r="B3" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="74">
+      <c r="A4" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>2</v>
       </c>
-      <c r="B4" s="74" t="s">
-        <v>259</v>
-      </c>
-      <c r="C4" s="74" t="s">
-        <v>300</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>301</v>
+      <c r="B4" s="73" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="74" t="s">
-        <v>261</v>
-      </c>
-      <c r="C5" s="74" t="s">
-        <v>302</v>
-      </c>
-      <c r="D5" s="74" t="s">
-        <v>303</v>
+      <c r="B5" s="73" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>304</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="74">
+      <c r="A6" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>4</v>
       </c>
-      <c r="B6" s="74" t="s">
-        <v>262</v>
-      </c>
-      <c r="C6" s="74" t="s">
-        <v>304</v>
-      </c>
-      <c r="D6" s="74" t="s">
-        <v>305</v>
+      <c r="B6" s="73" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>306</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>5</v>
       </c>
-      <c r="B7" s="74" t="s">
-        <v>264</v>
-      </c>
-      <c r="C7" s="74" t="s">
-        <v>306</v>
-      </c>
-      <c r="D7" s="74" t="s">
-        <v>307</v>
+      <c r="B7" s="73" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>308</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="74">
+      <c r="A8" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>6</v>
       </c>
-      <c r="B8" s="74" t="s">
-        <v>266</v>
-      </c>
-      <c r="C8" s="74" t="s">
-        <v>308</v>
-      </c>
-      <c r="D8" s="74" t="s">
-        <v>309</v>
+      <c r="B8" s="73" t="s">
+        <v>268</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>310</v>
+      </c>
+      <c r="D8" s="73" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>7</v>
       </c>
-      <c r="B9" s="74" t="s">
-        <v>270</v>
-      </c>
-      <c r="C9" s="74" t="s">
-        <v>310</v>
-      </c>
-      <c r="D9" s="74" t="s">
-        <v>311</v>
+      <c r="B9" s="73" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>312</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="74">
+      <c r="A10" s="73">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>8</v>
       </c>
-      <c r="B10" s="74" t="s">
-        <v>273</v>
-      </c>
-      <c r="C10" s="74" t="s">
-        <v>312</v>
-      </c>
-      <c r="D10" s="74" t="s">
-        <v>313</v>
+      <c r="B10" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -8619,22 +8668,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>318</v>
-      </c>
-      <c r="G1" s="95" t="s">
-        <v>319</v>
+        <v>320</v>
+      </c>
+      <c r="G1" s="96" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="2">
@@ -8652,7 +8701,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="G2" s="71"/>
     </row>
@@ -8662,7 +8711,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C3" s="56">
         <v>0.0</v>
@@ -8671,13 +8720,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4">
@@ -8686,7 +8735,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C4" s="50">
         <v>0.0</v>
@@ -8695,13 +8744,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G4" s="71" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5">
@@ -8710,7 +8759,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C5" s="56">
         <v>0.0</v>
@@ -8719,13 +8768,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G5" s="70" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6">
@@ -8734,7 +8783,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C6" s="50">
         <v>0.0</v>
@@ -8743,13 +8792,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G6" s="71" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7">
@@ -8758,7 +8807,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C7" s="56">
         <v>0.0</v>
@@ -8767,37 +8816,37 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="G7" s="70" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="72">
+      <c r="A8" s="87">
         <f>ROW()-ROW(Table_Phrases[N])</f>
         <v>6</v>
       </c>
-      <c r="B8" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="C8" s="73">
+      <c r="B8" s="88" t="s">
+        <v>296</v>
+      </c>
+      <c r="C8" s="88">
         <v>0.0</v>
       </c>
-      <c r="D8" s="73">
+      <c r="D8" s="88">
         <v>0.0</v>
       </c>
-      <c r="E8" s="96" t="s">
-        <v>322</v>
-      </c>
-      <c r="F8" s="73" t="s">
-        <v>335</v>
-      </c>
-      <c r="G8" s="97" t="s">
-        <v>336</v>
+      <c r="E8" s="97" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" s="88" t="s">
+        <v>337</v>
+      </c>
+      <c r="G8" s="98" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -8830,9 +8879,9 @@
     <col customWidth="1" min="2" max="2" width="15.14"/>
     <col customWidth="1" min="3" max="3" width="25.57"/>
     <col customWidth="1" min="4" max="5" width="29.86"/>
-    <col customWidth="1" min="6" max="6" width="31.57"/>
+    <col customWidth="1" min="6" max="6" width="34.57"/>
     <col customWidth="1" min="7" max="7" width="35.71"/>
-    <col customWidth="1" min="8" max="8" width="24.29"/>
+    <col customWidth="1" min="8" max="8" width="42.86"/>
     <col customWidth="1" min="9" max="9" width="31.71"/>
   </cols>
   <sheetData>
@@ -8841,55 +8890,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>341</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>342</v>
+        <v>343</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
-      <c r="A2" s="74">
+      <c r="A2" s="73">
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
-      <c r="B2" s="74" t="s">
-        <v>343</v>
-      </c>
-      <c r="C2" s="98" t="str">
+      <c r="B2" s="73" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="99" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
 SPLIT(TEXTJOIN("", "",TRUE,
-VLOOKUP(TRANSPOSE(SPLIT(F2,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Sprites]),2,FALSE),
-Table_PickableSprites[SPRITES]
+VLOOKUP(TRANSPOSE(SPLIT(G2,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Sprites]),2,FALSE),
+F2
 ),"", "")
 ))
 )
-)"),"SPRITE_NONE|SPRITE_POTION_RED|SPRITE_POTION_BLUE")</f>
-        <v>SPRITE_NONE|SPRITE_POTION_RED|SPRITE_POTION_BLUE</v>
-      </c>
-      <c r="D2" s="98" t="str">
-        <f t="shared" ref="D2:D4" si="2">SUBSTITUTE(G2,", ","|")</f>
+)"),"SPRITE_NONE")</f>
+        <v>SPRITE_NONE</v>
+      </c>
+      <c r="D2" s="99" t="str">
+        <f t="shared" ref="D2:D4" si="2">SUBSTITUTE(H2,", ","|")</f>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="E2" s="98" t="str">
+      <c r="E2" s="99" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
 SPLIT(TEXTJOIN("", "",TRUE,
-VLOOKUP(TRANSPOSE(SPLIT(F2,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Name]),2,FALSE),
+VLOOKUP(TRANSPOSE(SPLIT(G2,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Name]),2,FALSE),
 Table_PickableNames[NAMES]
 ),"", "")
 ))
@@ -8897,44 +8949,47 @@
 )"),"NAME_NONE|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION")</f>
         <v>NAME_NONE|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="78" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2" s="78" t="s">
         <v>210</v>
       </c>
-      <c r="G2" s="79" t="s">
-        <v>321</v>
+      <c r="H2" s="78" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
-      <c r="A3" s="74">
+      <c r="A3" s="73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="B3" s="74" t="s">
-        <v>344</v>
-      </c>
-      <c r="C3" s="98" t="str">
+      <c r="B3" s="73" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" s="99" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
 SPLIT(TEXTJOIN("", "",TRUE,
-VLOOKUP(TRANSPOSE(SPLIT(F3,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Sprites]),2,FALSE),
-Table_PickableSprites[SPRITES]
+VLOOKUP(TRANSPOSE(SPLIT(G3,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Sprites]),2,FALSE),
+F3
 ),"", "")
 ))
 )
-)"),"SPRITE_POTION_RED|SPRITE_POTION_BLUE|SPRITE_FOUNTAIN|SPRITE_FOUNTAIN_FULL")</f>
-        <v>SPRITE_POTION_RED|SPRITE_POTION_BLUE|SPRITE_FOUNTAIN|SPRITE_FOUNTAIN_FULL</v>
-      </c>
-      <c r="D3" s="98" t="str">
+)"),"SPRITE_POTION_RED|SPRITE_POTION_BLUE|SPRITE_FOUNTAIN|SPRITE_FOUNTAIN_FULL|BACKGROUND_ROOM_FIRST")</f>
+        <v>SPRITE_POTION_RED|SPRITE_POTION_BLUE|SPRITE_FOUNTAIN|SPRITE_FOUNTAIN_FULL|BACKGROUND_ROOM_FIRST</v>
+      </c>
+      <c r="D3" s="99" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE|PHRASE_ASK_FOUNTAIN1_1|PHRASE_ASK_FOUNTAIN1_2|PHRASE_ASK_FOUNTAIN2_1|PHRASE_ASK_FOUNTAIN3_1|PHRASE_ASK_FOUNTAIN4_1</v>
       </c>
-      <c r="E3" s="98" t="str">
+      <c r="E3" s="99" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
 SPLIT(TEXTJOIN("", "",TRUE,
-VLOOKUP(TRANSPOSE(SPLIT(F3,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Name]),2,FALSE),
+VLOOKUP(TRANSPOSE(SPLIT(G3,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Name]),2,FALSE),
 Table_PickableNames[NAMES]
 ),"", "")
 ))
@@ -8942,44 +8997,47 @@
 )"),"NAME_CHAR_MAIN|NAME_CHAR_PARROT|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION|NAME_ITEM_FOUNTAIN")</f>
         <v>NAME_CHAR_MAIN|NAME_CHAR_PARROT|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION|NAME_ITEM_FOUNTAIN</v>
       </c>
-      <c r="F3" s="79" t="s">
-        <v>345</v>
-      </c>
-      <c r="G3" s="79" t="s">
-        <v>346</v>
+      <c r="F3" s="78" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" s="78" t="s">
+        <v>348</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="74">
+      <c r="A4" s="73">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B4" s="74" t="s">
-        <v>347</v>
-      </c>
-      <c r="C4" s="98" t="str">
+      <c r="B4" s="73" t="s">
+        <v>350</v>
+      </c>
+      <c r="C4" s="99" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
 SPLIT(TEXTJOIN("", "",TRUE,
-VLOOKUP(TRANSPOSE(SPLIT(F4,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Sprites]),2,FALSE),
-Table_PickableSprites[SPRITES]
+VLOOKUP(TRANSPOSE(SPLIT(G4,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Sprites]),2,FALSE),
+F4
 ),"", "")
 ))
 )
-)"),"SPRITE_LAST|SPRITE_POTION_RED|SPRITE_POTION_BLUE")</f>
-        <v>SPRITE_LAST|SPRITE_POTION_RED|SPRITE_POTION_BLUE</v>
-      </c>
-      <c r="D4" s="98" t="str">
+)"),"SPRITE_LAST")</f>
+        <v>SPRITE_LAST</v>
+      </c>
+      <c r="D4" s="99" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="E4" s="98" t="str">
+      <c r="E4" s="99" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
 SPLIT(TEXTJOIN("", "",TRUE,
-VLOOKUP(TRANSPOSE(SPLIT(F4,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Name]),2,FALSE),
+VLOOKUP(TRANSPOSE(SPLIT(G4,"", "")),HSTACK(Table_Items[ITEM_ID],Table_Items[Name]),2,FALSE),
 Table_PickableNames[NAMES]
 ),"", "")
 ))
@@ -8987,16 +9045,19 @@
 )"),"NAME_NPC_LAST|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION")</f>
         <v>NAME_NPC_LAST|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION</v>
       </c>
-      <c r="F4" s="79" t="s">
-        <v>272</v>
-      </c>
-      <c r="G4" s="79" t="s">
-        <v>321</v>
+      <c r="F4" s="78" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="H4" s="78" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="F2:G4">
+    <dataValidation type="list" allowBlank="1" sqref="F2:H4">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[Partial] Using same WaitForNextFrame to avoid alloc -Fixed bug of glow not showing on first hover -Reduced stack call length when player arrived at final Waypoint -Pending move hover variable to Input and change its clas to Info structure
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="UgyXJt29kLu+k3nozhlHQ2DEoei1UgSSSS0y/CN1dQU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="ZuD4iZtiL1kKF/8saKb5AizWFVBp94LOfLe3NP5G1j8="/>
     </ext>
   </extLst>
 </workbook>
@@ -88,8 +88,32 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A19">
+      <text>
+        <t xml:space="preserve">NullReferenceException: Object reference not set to an instance of an object
+Gob3AQ.GameMenu.Dialog.DialogOptionButtonClass.SetOptionText (System.String&amp; text) (at Assets/Scripts/Menu/DialogOptionButtonClass.cs:27)
+Gob3AQ.GameMenu.GameMenuClass.ShowDialogueService (System.ReadOnlySpan`1[T] defaultTalkers, Gob3AQ.VARMAP.Types.DialogType dialog, Gob3AQ.VARMAP.Types.DialogPhrase phrase) (at Assets/Scripts/Master/GameMenuClass.cs:93)
+Gob3AQ.GameMaster.GameMasterClass.EnableDialogueService (System.Boolean enable, System.ReadOnlySpan`1[T] talkers, Gob3AQ.VARMAP.Types.DialogType dialog, Gob3AQ.VARMAP.Types.DialogPhrase phrase) (at Assets/Scripts/Master/GameMasterClass.cs:232)
+Gob3AQ.LevelMaster.LevelMasterClass.PlayerReachedWaypointService (Gob3AQ.VARMAP.Types.CharacterType character) (at Assets/Scripts/Master/LevelMasterClass.cs:183)
+Gob3AQ.GameElement.PlayableChar.PlayableCharScript.StartBufferedInteraction () (at Assets/Scripts/GameElement/PlayableCharScript.cs:351)
+Gob3AQ.GameElement.PlayableChar.PlayableCharScript.Execute_Walk () (at Assets/Scripts/GameElement/PlayableCharScript.cs:279)
+Gob3AQ.GameElement.PlayableChar.PlayableCharScript.Execute_Play () (at Assets/Scripts/GameElement/PlayableCharScript.cs:234)
+Gob3AQ.GameElement.PlayableChar.PlayableCharScript.Update () (at Assets/Scripts/GameElement/PlayableCharScript.cs:164)
+======</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="406">
   <si>
     <t>N</t>
   </si>
@@ -802,42 +826,57 @@
     <t>SPRITE_CURSOR_NORMAL</t>
   </si>
   <si>
+    <t>SPRITE_ATLAS_UI_0[SPRITE_CURSOR_NORMAL]</t>
+  </si>
+  <si>
     <t>SPRITE_CURSOR_USING</t>
   </si>
   <si>
+    <t>SPRITE_ATLAS_UI_0[SPRITE_CURSOR_USING]</t>
+  </si>
+  <si>
     <t>SPRITE_INVENTORY</t>
   </si>
   <si>
+    <t>SPRITE_ATLAS_UI_0[SPRITE_INVENTORY]</t>
+  </si>
+  <si>
     <t>SPRITE_POTION_RED</t>
   </si>
   <si>
-    <t>SPRITE_ITEM_POTION</t>
+    <t>SPRITE_ATLAS_PICKABLES_0[SPRITE_ITEM_POTION]</t>
   </si>
   <si>
     <t>SPRITE_POTION_BLUE</t>
   </si>
   <si>
-    <t>SPRITE_ITEM_POTION_BLUE</t>
+    <t>SPRITE_ATLAS_PICKABLES_0[SPRITE_ITEM_POTION_BLUE]</t>
   </si>
   <si>
     <t>SPRITE_FOUNTAIN</t>
   </si>
   <si>
-    <t>SPRITE_ITEM_FOUNTAIN</t>
+    <t>SPRITE_ATLAS_ROOM_FIRST_0[SPRITE_ITEM_FOUNTAIN]</t>
   </si>
   <si>
     <t>SPRITE_FOUNTAIN_FULL</t>
   </si>
   <si>
-    <t>SPRITE_ITEM_FOUNTAIN_FULL</t>
+    <t>SPRITE_ATLAS_ROOM_FIRST_0[SPRITE_ITEM_FOUNTAIN_FULL]</t>
   </si>
   <si>
     <t>SPRITE_NPC_MILITO</t>
   </si>
   <si>
+    <t>SPRITE_ATLAS_ROOM_FIRST_0[SPRITE_NPC_MILITO]</t>
+  </si>
+  <si>
     <t>BACKGROUND_ROOM_FIRST</t>
   </si>
   <si>
+    <t>SPRITE_ATLAS_ROOM_FIRST_0[SPRITE_BACKGROUND_ROOM_FIRST]</t>
+  </si>
+  <si>
     <t>SPRITE_LAST</t>
   </si>
   <si>
@@ -1286,6 +1325,9 @@
   </si>
   <si>
     <t>Sprite Atlas addressable</t>
+  </si>
+  <si>
+    <t>Enshorten stack</t>
   </si>
   <si>
     <t>Re-think usage of ITEM_TAKE, USE_TALK</t>
@@ -2444,7 +2486,7 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D20" displayName="Table_TODO" name="Table_TODO" id="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D21" displayName="Table_TODO" name="Table_TODO" id="20">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -4515,7 +4557,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
@@ -4551,7 +4593,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="103" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6">
@@ -4563,7 +4605,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="73" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8">
@@ -4579,7 +4621,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10">
@@ -4619,7 +4661,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="73" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16">
@@ -4651,7 +4693,7 @@
         <v>3.0</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20">
@@ -4659,7 +4701,7 @@
         <v>4.0</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21">
@@ -4667,7 +4709,7 @@
         <v>5.0</v>
       </c>
       <c r="B21" s="103" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23">
@@ -4675,7 +4717,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24">
@@ -4683,7 +4725,7 @@
         <v>0.0</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25">
@@ -4691,7 +4733,7 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="103" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27">
@@ -4699,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="28">
@@ -4708,7 +4750,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="75" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29">
@@ -4717,7 +4759,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="104" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30">
@@ -4726,7 +4768,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="105" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31">
@@ -4735,7 +4777,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="104" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32">
@@ -4744,7 +4786,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="106" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -4788,19 +4830,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="E1" s="49" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="F1" s="73" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2">
@@ -4825,13 +4867,13 @@
         <v>228</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="D3" s="62" t="s">
         <v>225</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="F3" s="109" t="s">
         <v>228</v>
@@ -4843,7 +4885,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="77" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="C4" s="110"/>
       <c r="D4" s="110"/>
@@ -4855,7 +4897,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7">
@@ -4956,16 +4998,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="118" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="B1" s="119" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="D1" s="118" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="E1" s="119" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
@@ -5020,18 +5062,18 @@
     </row>
     <row r="6">
       <c r="B6" s="121" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E6" s="121" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="123" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E7" s="123" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8">
@@ -5086,10 +5128,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2">
@@ -5102,7 +5144,7 @@
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3">
@@ -5115,7 +5157,7 @@
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4">
@@ -5128,7 +5170,7 @@
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5">
@@ -5141,7 +5183,7 @@
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6">
@@ -5472,21 +5514,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="48" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="125" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="B2" s="126">
         <v>1.0</v>
@@ -5500,7 +5542,7 @@
     </row>
     <row r="3">
       <c r="A3" s="59" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="B3" s="126">
         <v>1.0</v>
@@ -5514,7 +5556,7 @@
     </row>
     <row r="4">
       <c r="A4" s="53" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="B4" s="127">
         <v>3.0</v>
@@ -5528,7 +5570,7 @@
     </row>
     <row r="5">
       <c r="A5" s="125" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="B5" s="126">
         <v>1.0</v>
@@ -5542,7 +5584,7 @@
     </row>
     <row r="6">
       <c r="A6" s="53" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="B6" s="127">
         <v>3.0</v>
@@ -5556,7 +5598,7 @@
     </row>
     <row r="7">
       <c r="A7" s="125" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="B7" s="127">
         <v>3.0</v>
@@ -5570,7 +5612,7 @@
     </row>
     <row r="8">
       <c r="A8" s="125" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="B8" s="128">
         <v>5.0</v>
@@ -5584,7 +5626,7 @@
     </row>
     <row r="9">
       <c r="A9" s="59" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="B9" s="129">
         <v>4.0</v>
@@ -5598,7 +5640,7 @@
     </row>
     <row r="10">
       <c r="A10" s="53" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="B10" s="129">
         <v>4.0</v>
@@ -5612,7 +5654,7 @@
     </row>
     <row r="11">
       <c r="A11" s="59" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="B11" s="126">
         <v>1.0</v>
@@ -5626,7 +5668,7 @@
     </row>
     <row r="12">
       <c r="A12" s="125" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B12" s="129">
         <v>4.0</v>
@@ -5640,7 +5682,7 @@
     </row>
     <row r="13">
       <c r="A13" s="125" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="B13" s="126">
         <v>1.0</v>
@@ -5654,7 +5696,7 @@
     </row>
     <row r="14">
       <c r="A14" s="125" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="B14" s="130">
         <v>2.0</v>
@@ -5668,7 +5710,7 @@
     </row>
     <row r="15">
       <c r="A15" s="125" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="B15" s="127">
         <v>3.0</v>
@@ -5682,7 +5724,7 @@
     </row>
     <row r="16">
       <c r="A16" s="125" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="B16" s="130">
         <v>2.0</v>
@@ -5696,7 +5738,7 @@
     </row>
     <row r="17">
       <c r="A17" s="125" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="B17" s="130">
         <v>2.0</v>
@@ -5709,49 +5751,63 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="53" t="s">
-        <v>398</v>
+      <c r="A18" s="125" t="s">
+        <v>403</v>
       </c>
       <c r="B18" s="130">
         <v>2.0</v>
       </c>
       <c r="C18" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="125" t="s">
+        <v>404</v>
+      </c>
+      <c r="B19" s="130">
+        <v>2.0</v>
+      </c>
+      <c r="C19" s="60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="53" t="s">
+        <v>405</v>
+      </c>
+      <c r="B20" s="127">
+        <v>3.0</v>
+      </c>
+      <c r="C20" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="D18" s="75" t="b">
+      <c r="D20" s="75" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="59" t="s">
-        <v>399</v>
-      </c>
-      <c r="B19" s="127">
-        <v>3.0</v>
-      </c>
-      <c r="C19" s="60" t="b">
+    <row r="21">
+      <c r="A21" s="67" t="s">
+        <v>321</v>
+      </c>
+      <c r="B21" s="131">
+        <v>5.0</v>
+      </c>
+      <c r="C21" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="D19" s="74" t="b">
+      <c r="D21" s="103" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="76" t="s">
-        <v>316</v>
-      </c>
-      <c r="B20" s="131">
-        <v>5.0</v>
-      </c>
-      <c r="C20" s="77" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="78" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B20">
+  <conditionalFormatting sqref="B2:B21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="1"/>
@@ -5763,19 +5819,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A20">
+  <conditionalFormatting sqref="A2:A21">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>$C2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B20">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B21">
       <formula1>AND(ISNUMBER(B2),(NOT(OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7766,7 +7823,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="28.29"/>
-    <col customWidth="1" min="3" max="3" width="30.43"/>
+    <col customWidth="1" min="3" max="3" width="73.0"/>
     <col customWidth="1" min="4" max="4" width="26.0"/>
   </cols>
   <sheetData>
@@ -7799,7 +7856,7 @@
         <v>236</v>
       </c>
       <c r="C3" s="74" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4">
@@ -7808,10 +7865,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5">
@@ -7820,10 +7877,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6">
@@ -7832,10 +7889,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7">
@@ -7844,10 +7901,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8">
@@ -7856,10 +7913,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9">
@@ -7868,10 +7925,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10">
@@ -7880,10 +7937,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11">
@@ -7892,10 +7949,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C11" s="74" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12">
@@ -7904,10 +7961,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="77" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C12" s="78" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -7948,25 +8005,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="G1" s="50" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2">
@@ -7978,10 +8035,10 @@
         <v>211</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D2" s="81" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="E2" s="82" t="s">
         <v>235</v>
@@ -8002,16 +8059,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="79" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C3" s="80" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="E3" s="82" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F3" s="83" t="b">
         <v>0</v>
@@ -8029,16 +8086,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="E4" s="82" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F4" s="83" t="b">
         <v>0</v>
@@ -8056,16 +8113,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="79" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C5" s="80" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="D5" s="81" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="E5" s="82" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F5" s="83" t="b">
         <v>0</v>
@@ -8086,19 +8143,19 @@
         <v>225</v>
       </c>
       <c r="C6" s="80" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="E6" s="82" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F6" s="83" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="80" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H6" s="84" t="s">
         <v>217</v>
@@ -8113,19 +8170,19 @@
         <v>223</v>
       </c>
       <c r="C7" s="80" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="E7" s="82" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F7" s="83" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="80" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H7" s="84" t="s">
         <v>221</v>
@@ -8137,16 +8194,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C8" s="80" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="E8" s="82" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="F8" s="83" t="b">
         <v>0</v>
@@ -8155,7 +8212,7 @@
         <v>235</v>
       </c>
       <c r="H8" s="84" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9">
@@ -8164,16 +8221,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C9" s="80" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="E9" s="82" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="F9" s="83" t="b">
         <v>0</v>
@@ -8191,16 +8248,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C10" s="80" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="E10" s="82" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="F10" s="83" t="b">
         <v>0</v>
@@ -8256,13 +8313,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2">
@@ -8277,7 +8334,7 @@
         <v>211</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3">
@@ -8286,13 +8343,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="C3" s="87" t="s">
         <v>211</v>
       </c>
       <c r="D3" s="88" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4">
@@ -8307,7 +8364,7 @@
         <v>211</v>
       </c>
       <c r="D4" s="86" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5">
@@ -8316,13 +8373,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C5" s="89" t="s">
         <v>211</v>
       </c>
       <c r="D5" s="90" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7">
@@ -8330,19 +8387,19 @@
         <v>0</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="C7" s="49" t="s">
         <v>196</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8">
@@ -8351,7 +8408,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C8" s="55" t="s">
         <v>209</v>
@@ -8372,7 +8429,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C9" s="66" t="s">
         <v>209</v>
@@ -8393,7 +8450,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C10" s="55" t="s">
         <v>209</v>
@@ -8405,7 +8462,7 @@
         <v>215</v>
       </c>
       <c r="F10" s="91" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11">
@@ -8414,7 +8471,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="C11" s="66" t="s">
         <v>209</v>
@@ -8426,7 +8483,7 @@
         <v>215</v>
       </c>
       <c r="F11" s="92" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12">
@@ -8435,7 +8492,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="54" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="C12" s="55" t="s">
         <v>228</v>
@@ -8447,7 +8504,7 @@
         <v>215</v>
       </c>
       <c r="F12" s="91" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13">
@@ -8456,10 +8513,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="60" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="D13" s="62" t="s">
         <v>209</v>
@@ -8468,7 +8525,7 @@
         <v>215</v>
       </c>
       <c r="F13" s="92" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14">
@@ -8477,7 +8534,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="77" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="C14" s="93" t="s">
         <v>209</v>
@@ -8591,13 +8648,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="98" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C1" s="97" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="D1" s="97" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2">
@@ -8606,7 +8663,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C2" s="99"/>
       <c r="D2" s="99"/>
@@ -8617,13 +8674,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="79" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4">
@@ -8632,13 +8689,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="D4" s="79" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5">
@@ -8647,13 +8704,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="79" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6">
@@ -8662,13 +8719,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7">
@@ -8677,13 +8734,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="79" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D7" s="79" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8">
@@ -8692,13 +8749,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9">
@@ -8707,13 +8764,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="C9" s="79" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10">
@@ -8722,13 +8779,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -8764,22 +8821,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="G1" s="100" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2">
@@ -8797,7 +8854,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="57" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="G2" s="75"/>
     </row>
@@ -8807,7 +8864,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C3" s="60">
         <v>0.0</v>
@@ -8816,13 +8873,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F3" s="60" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="G3" s="74" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4">
@@ -8831,7 +8888,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="C4" s="54">
         <v>0.0</v>
@@ -8840,13 +8897,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="57" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="G4" s="75" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5">
@@ -8855,7 +8912,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C5" s="60">
         <v>0.0</v>
@@ -8864,13 +8921,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="63" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6">
@@ -8879,7 +8936,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="C6" s="54">
         <v>0.0</v>
@@ -8888,13 +8945,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="57" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7">
@@ -8903,7 +8960,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C7" s="60">
         <v>0.0</v>
@@ -8912,13 +8969,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="63" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="G7" s="74" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8">
@@ -8927,7 +8984,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="77" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C8" s="77">
         <v>0.0</v>
@@ -8936,13 +8993,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="101" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F8" s="77" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="G8" s="78" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -8986,25 +9043,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="F1" s="51" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
@@ -9013,7 +9070,7 @@
         <v>-1</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="C2" s="102" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9052,7 +9109,7 @@
         <v>211</v>
       </c>
       <c r="H2" s="84" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -9061,7 +9118,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="79" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="C3" s="102" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9094,13 +9151,13 @@
         <v>NAME_CHAR_MAIN|NAME_CHAR_PARROT|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION|NAME_ITEM_FOUNTAIN</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="G3" s="84" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="H3" s="84" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4">
@@ -9109,7 +9166,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="C4" s="102" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9142,13 +9199,13 @@
         <v>NAME_NPC_LAST|NAME_ITEM_POTION|NAME_ITEM_BLUE_POTION</v>
       </c>
       <c r="F4" s="84" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="H4" s="84" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Zoom in / Zoom Out Action selection with tab
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -14,15 +14,15 @@
     <sheet state="visible" name="ROOMS" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="TYPES" sheetId="10" r:id="rId13"/>
     <sheet state="visible" name="EVENTS" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="CONSTANTS" sheetId="12" r:id="rId15"/>
-    <sheet state="visible" name="_ITEM_AVAIL" sheetId="13" r:id="rId16"/>
-    <sheet state="visible" name="_TODO" sheetId="14" r:id="rId17"/>
+    <sheet state="visible" name="_ITEM_AVAIL" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="_TODO" sheetId="13" r:id="rId16"/>
+    <sheet state="visible" name="_CONSTANTS" sheetId="14" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="C3mO2XERvw6N5NJ5wmfKRzUiztfN2sTlFiFoFkj6Tuk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="tek0Ywa62/n4ybLRJ5+4rDe3Y6cdrV6T6+++l56J0Ig="/>
     </ext>
   </extLst>
 </workbook>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="438">
   <si>
     <t>N</t>
   </si>
@@ -592,7 +592,7 @@
     <t>GameEventMasterClass.IsItemTakenFromSceneService</t>
   </si>
   <si>
-    <t>Tells if item is taken from scene</t>
+    <t>Tells if a pickable item has already been picked in game</t>
   </si>
   <si>
     <t>CANCEL_PICKABLE_ITEM</t>
@@ -784,6 +784,33 @@
     <t>COND_LAST</t>
   </si>
   <si>
+    <t>SPAWN_COND_ID</t>
+  </si>
+  <si>
+    <t>Spawn</t>
+  </si>
+  <si>
+    <t>Despawn</t>
+  </si>
+  <si>
+    <t>ChangeSprite</t>
+  </si>
+  <si>
+    <t>TargetSprite</t>
+  </si>
+  <si>
+    <t>SPAWN_COND_NONE</t>
+  </si>
+  <si>
+    <t>SPRITE_NONE</t>
+  </si>
+  <si>
+    <t>SPAWN_COND_FOUNTAIN</t>
+  </si>
+  <si>
+    <t>SPRITE_FOUNTAIN_FULL</t>
+  </si>
+  <si>
     <t>ITEM_ID</t>
   </si>
   <si>
@@ -805,15 +832,15 @@
     <t>ActionConditions</t>
   </si>
   <si>
+    <t>SpawnConditions</t>
+  </si>
+  <si>
     <t>NAME_NONE</t>
   </si>
   <si>
     <t>ITEM_FAMILY_TYPE_NONE</t>
   </si>
   <si>
-    <t>SPRITE_NONE</t>
-  </si>
-  <si>
     <t>ITEM_PLAYER_MAIN</t>
   </si>
   <si>
@@ -946,9 +973,6 @@
     <t>SPRITE_ATLAS_ROOM_FIRST_0[SPRITE_ITEM_FOUNTAIN]</t>
   </si>
   <si>
-    <t>SPRITE_FOUNTAIN_FULL</t>
-  </si>
-  <si>
     <t>SPRITE_ATLAS_ROOM_FIRST_0[SPRITE_ITEM_FOUNTAIN_FULL]</t>
   </si>
   <si>
@@ -1312,6 +1336,90 @@
     <t>EVENT_COMBI_ID</t>
   </si>
   <si>
+    <t>ITEM_ID (Ref)</t>
+  </si>
+  <si>
+    <t>USABLE_AFTER_ACTION</t>
+  </si>
+  <si>
+    <t>ALWAYS</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>PRIO</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>ONGOING</t>
+  </si>
+  <si>
+    <t>Talk with characters</t>
+  </si>
+  <si>
+    <t>Plot (1st part)</t>
+  </si>
+  <si>
+    <t>Improve Waypoint Tool (naming)</t>
+  </si>
+  <si>
+    <t>Language files</t>
+  </si>
+  <si>
+    <t>Background objects layers</t>
+  </si>
+  <si>
+    <t>Bug with menu of items (not selecting)</t>
+  </si>
+  <si>
+    <t>Loading screen between rooms</t>
+  </si>
+  <si>
+    <t>Main event list (Tomba style)</t>
+  </si>
+  <si>
+    <t>Trophies</t>
+  </si>
+  <si>
+    <t>Observe items, NPCs, trigger events</t>
+  </si>
+  <si>
+    <t>Seealso in services. Add owner in descr</t>
+  </si>
+  <si>
+    <t>Avoid services modifying VARMAP</t>
+  </si>
+  <si>
+    <t>Normalize menu items with dialog opts</t>
+  </si>
+  <si>
+    <t>Use Dictionaries for LevelManager</t>
+  </si>
+  <si>
+    <t>State change deactivation/activation</t>
+  </si>
+  <si>
+    <t>Adressables instead of Resources</t>
+  </si>
+  <si>
+    <t>Sprite Atlas addressable</t>
+  </si>
+  <si>
+    <t>Enshorten stack</t>
+  </si>
+  <si>
+    <t>Re-think usage of ITEM_TAKE, USE_TALK</t>
+  </si>
+  <si>
+    <t>Spawn/Despawn conditions</t>
+  </si>
+  <si>
+    <t>Waypoint numeration in Editor</t>
+  </si>
+  <si>
     <t>SPRITES</t>
   </si>
   <si>
@@ -1319,84 +1427,6 @@
   </si>
   <si>
     <t>NAMES</t>
-  </si>
-  <si>
-    <t>ITEM_ID (Ref)</t>
-  </si>
-  <si>
-    <t>USABLE_AFTER_ACTION</t>
-  </si>
-  <si>
-    <t>ALWAYS</t>
-  </si>
-  <si>
-    <t>TASK</t>
-  </si>
-  <si>
-    <t>PRIO</t>
-  </si>
-  <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>ONGOING</t>
-  </si>
-  <si>
-    <t>Talk with characters</t>
-  </si>
-  <si>
-    <t>Plot (1st part)</t>
-  </si>
-  <si>
-    <t>Improve Waypoint Tool (naming)</t>
-  </si>
-  <si>
-    <t>Language files</t>
-  </si>
-  <si>
-    <t>Background objects layers</t>
-  </si>
-  <si>
-    <t>Bug with menu of items (not selecting)</t>
-  </si>
-  <si>
-    <t>Loading screen between rooms</t>
-  </si>
-  <si>
-    <t>Main event list (Tomba style)</t>
-  </si>
-  <si>
-    <t>Trophies</t>
-  </si>
-  <si>
-    <t>Observe items, NPCs, trigger events</t>
-  </si>
-  <si>
-    <t>Seealso in services. Add owner in descr</t>
-  </si>
-  <si>
-    <t>Avoid services modifying VARMAP</t>
-  </si>
-  <si>
-    <t>Normalize menu items with dialog opts</t>
-  </si>
-  <si>
-    <t>Use Dictionaries for LevelManager</t>
-  </si>
-  <si>
-    <t>State change deactivation/activation</t>
-  </si>
-  <si>
-    <t>Adressables instead of Resources</t>
-  </si>
-  <si>
-    <t>Sprite Atlas addressable</t>
-  </si>
-  <si>
-    <t>Enshorten stack</t>
-  </si>
-  <si>
-    <t>Re-think usage of ITEM_TAKE, USE_TALK</t>
   </si>
 </sst>
 </file>
@@ -1464,7 +1494,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1546,6 +1576,15 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1562,9 +1601,6 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1592,15 +1628,15 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1673,7 +1709,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="20">
+  <tableStyles count="21">
     <tableStyle count="4" pivot="0" name="VARMAP-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1687,6 +1723,12 @@
       <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
     <tableStyle count="4" pivot="0" name="ACTION_CONDS-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
+    <tableStyle count="4" pivot="0" name="ACTION_CONDS-style 2">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1776,19 +1818,19 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
       <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
-    <tableStyle count="4" pivot="0" name="CONSTANTS-style">
+    <tableStyle count="4" pivot="0" name="_TODO-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
       <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
-    <tableStyle count="4" pivot="0" name="CONSTANTS-style 2">
+    <tableStyle count="4" pivot="0" name="_CONSTANTS-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
       <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
-    <tableStyle count="4" pivot="0" name="_TODO-style">
+    <tableStyle count="4" pivot="0" name="_CONSTANTS-style 2">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1879,7 +1921,22 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H4" displayName="Table_Rooms" name="Table_Rooms" id="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G13" displayName="Table_Phrases" name="Table_Phrases" id="10">
+  <tableColumns count="7">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="PHRASE_ID" id="2"/>
+    <tableColumn name="TalkerIndex" id="3"/>
+    <tableColumn name="Sound" id="4"/>
+    <tableColumn name="CharAnimation" id="5"/>
+    <tableColumn name="Text_English" id="6"/>
+    <tableColumn name="Text_Spanish" id="7"/>
+  </tableColumns>
+  <tableStyleInfo name="PHRASES-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H4" displayName="Table_Rooms" name="Table_Rooms" id="11">
   <tableColumns count="8">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
@@ -1894,8 +1951,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="11">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="12">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="CHARACTER_TYPE_ID" id="2"/>
@@ -1904,8 +1961,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="12">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="13">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ANIMATION_ID" id="2"/>
@@ -1914,8 +1971,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B21" displayName="Table_Interaction" name="Table_Interaction" id="13">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B21" displayName="Table_Interaction" name="Table_Interaction" id="14">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="INTERACTION_ID" id="2"/>
@@ -1924,8 +1981,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A23:B25" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="14">
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A23:B25" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="15">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ANIMATION_ID" id="2"/>
@@ -1934,8 +1991,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A27:B32" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="15">
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A27:B32" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="16">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_FAMILY_TYPE_ID" id="2"/>
@@ -1944,8 +2001,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F4" displayName="Table_Events" name="Table_Events" id="16">
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F4" displayName="Table_Events" name="Table_Events" id="17">
   <tableColumns count="6">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_ID" id="2"/>
@@ -1958,8 +2015,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A6:B12" displayName="Table_EventsCombi" name="Table_EventsCombi" id="17">
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A6:B12" displayName="Table_EventsCombi" name="Table_EventsCombi" id="18">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_COMBI_ID" id="2"/>
@@ -1968,23 +2025,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B128" displayName="Table_PickableSprites" name="Table_PickableSprites" id="18">
-  <tableColumns count="2">
-    <tableColumn name="SPRITES" id="1"/>
-    <tableColumn name="WORK" id="2"/>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D23" displayName="Table_TODO" name="Table_TODO" id="19">
+  <tableColumns count="4">
+    <tableColumn name="TASK" id="1"/>
+    <tableColumn name="PRIO" id="2"/>
+    <tableColumn name="DONE" id="3"/>
+    <tableColumn name="ONGOING" id="4"/>
   </tableColumns>
-  <tableStyleInfo name="CONSTANTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="D1:E128" displayName="Table_PickableNames" name="Table_PickableNames" id="19">
-  <tableColumns count="2">
-    <tableColumn name="NAMES" id="1"/>
-    <tableColumn name="WORK" id="2"/>
-  </tableColumns>
-  <tableStyleInfo name="CONSTANTS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="_TODO-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -2011,14 +2060,22 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D21" displayName="Table_TODO" name="Table_TODO" id="20">
-  <tableColumns count="4">
-    <tableColumn name="TASK" id="1"/>
-    <tableColumn name="PRIO" id="2"/>
-    <tableColumn name="DONE" id="3"/>
-    <tableColumn name="ONGOING" id="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B128" displayName="Table_PickableSprites" name="Table_PickableSprites" id="20">
+  <tableColumns count="2">
+    <tableColumn name="SPRITES" id="1"/>
+    <tableColumn name="WORK" id="2"/>
   </tableColumns>
-  <tableStyleInfo name="_TODO-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="_CONSTANTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="D1:E128" displayName="Table_PickableNames" name="Table_PickableNames" id="21">
+  <tableColumns count="2">
+    <tableColumn name="NAMES" id="1"/>
+    <tableColumn name="WORK" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="_CONSTANTS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -2042,8 +2099,23 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H10" displayName="Table_Items" name="Table_Items" id="4">
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A11:G13" displayName="Table_Spawn_Conditions" name="Table_Spawn_Conditions" id="4">
+  <tableColumns count="7">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="SPAWN_COND_ID" id="2"/>
+    <tableColumn name="Spawn" id="3"/>
+    <tableColumn name="Despawn" id="4"/>
+    <tableColumn name="ChangeSprite" id="5"/>
+    <tableColumn name="NeededEvents" id="6"/>
+    <tableColumn name="TargetSprite" id="7"/>
+  </tableColumns>
+  <tableStyleInfo name="ACTION_CONDS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I10" displayName="Table_Items" name="Table_Items" id="5">
+  <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_ID" id="2"/>
     <tableColumn name="Name" id="3"/>
@@ -2052,13 +2124,14 @@
     <tableColumn name="PICKABLE" id="6"/>
     <tableColumn name="SpritePickable" id="7"/>
     <tableColumn name="ActionConditions" id="8"/>
+    <tableColumn name="SpawnConditions" id="9"/>
   </tableColumns>
   <tableStyleInfo name="ITEMS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C16" displayName="Table_sprites" name="Table_sprites" id="5">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C16" displayName="Table_sprites" name="Table_sprites" id="6">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SPRITE_ID" id="2"/>
@@ -2068,8 +2141,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D6" displayName="Table_Dialogs" name="Table_Dialogs" id="6">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D6" displayName="Table_Dialogs" name="Table_Dialogs" id="7">
   <tableColumns count="4">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ID" id="2"/>
@@ -2080,8 +2153,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A8:F17" displayName="Table_Dialog_Options" name="Table_Dialog_Options" id="7">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A8:F17" displayName="Table_Dialog_Options" name="Table_Dialog_Options" id="8">
   <tableColumns count="6">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_OPTION_ID" id="2"/>
@@ -2094,8 +2167,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D13" displayName="Table_Name" name="Table_Name" id="8">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D13" displayName="Table_Name" name="Table_Name" id="9">
   <tableColumns count="4">
     <tableColumn name="N" id="1"/>
     <tableColumn name="NAME_ID" id="2"/>
@@ -2103,21 +2176,6 @@
     <tableColumn name="Name_Spanish" id="4"/>
   </tableColumns>
   <tableStyleInfo name="NAMES-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G13" displayName="Table_Phrases" name="Table_Phrases" id="9">
-  <tableColumns count="7">
-    <tableColumn name="N" id="1"/>
-    <tableColumn name="PHRASE_ID" id="2"/>
-    <tableColumn name="TalkerIndex" id="3"/>
-    <tableColumn name="Sound" id="4"/>
-    <tableColumn name="CharAnimation" id="5"/>
-    <tableColumn name="Text_English" id="6"/>
-    <tableColumn name="Text_Spanish" id="7"/>
-  </tableColumns>
-  <tableStyleInfo name="PHRASES-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -4128,7 +4186,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2">
@@ -4164,7 +4222,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6">
@@ -4176,7 +4234,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8">
@@ -4192,7 +4250,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10">
@@ -4208,7 +4266,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12">
@@ -4232,7 +4290,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16">
@@ -4250,7 +4308,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18">
@@ -4294,7 +4352,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="24">
@@ -4302,7 +4360,7 @@
         <v>0.0</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
     </row>
     <row r="25">
@@ -4310,7 +4368,7 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27">
@@ -4318,7 +4376,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28">
@@ -4327,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="29">
@@ -4336,7 +4394,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
     </row>
     <row r="30">
@@ -4345,7 +4403,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31">
@@ -4354,7 +4412,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32">
@@ -4363,7 +4421,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4407,19 +4465,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2">
@@ -4430,10 +4488,10 @@
       <c r="B2" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3">
       <c r="A3" s="21">
@@ -4444,13 +4502,13 @@
         <v>215</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>212</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>215</v>
@@ -4462,77 +4520,77 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+        <v>405</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="41">
+      <c r="A7" s="43">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>0</v>
       </c>
-      <c r="B7" s="42" t="str">
+      <c r="B7" s="44" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(FLATTEN(Table_Events[EVENT_ID],""(NOT)""&amp;Table_Events[EVENT_ID]))"),"EVENT_NONE")</f>
         <v>EVENT_NONE</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="41">
+      <c r="A8" s="43">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="str">
+      <c r="B8" s="44" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_FOUNTAIN_FULL")</f>
         <v>EVENT_FOUNTAIN_FULL</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="41">
+      <c r="A9" s="43">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>2</v>
       </c>
-      <c r="B9" s="42" t="str">
+      <c r="B9" s="44" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAST")</f>
         <v>EVENT_LAST</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="41">
+      <c r="A10" s="43">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>3</v>
       </c>
-      <c r="B10" s="42" t="str">
+      <c r="B10" s="44" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_NONE")</f>
         <v>(NOT)EVENT_NONE</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="41">
+      <c r="A11" s="43">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>4</v>
       </c>
-      <c r="B11" s="42" t="str">
+      <c r="B11" s="44" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_FOUNTAIN_FULL")</f>
         <v>(NOT)EVENT_FOUNTAIN_FULL</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="41">
+      <c r="A12" s="43">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>5</v>
       </c>
-      <c r="B12" s="42" t="str">
+      <c r="B12" s="44" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAST")</f>
         <v>(NOT)EVENT_LAST</v>
       </c>
@@ -4558,137 +4616,6 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <tabColor rgb="FFB45F06"/>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="2" width="34.0"/>
-    <col customWidth="1" min="4" max="5" width="23.71"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="43" t="s">
-        <v>399</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>400</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>401</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="44" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"SPRITE_POTION_RED")</f>
-        <v>SPRITE_POTION_RED</v>
-      </c>
-      <c r="B2" s="44" t="str">
-        <f t="array" ref="B2:B10">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
-        <v/>
-      </c>
-      <c r="D2" s="44" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"NAME_ITEM_POTION")</f>
-        <v>NAME_ITEM_POTION</v>
-      </c>
-      <c r="E2" s="44" t="str">
-        <f t="array" ref="E2:E10">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="44" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_POTION_BLUE")</f>
-        <v>SPRITE_POTION_BLUE</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="44" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_BLUE_POTION")</f>
-        <v>NAME_ITEM_BLUE_POTION</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="44" t="s">
-        <v>236</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="44" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
@@ -4705,10 +4632,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2">
@@ -4721,7 +4648,7 @@
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3">
@@ -4734,7 +4661,7 @@
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4">
@@ -4747,7 +4674,7 @@
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5">
@@ -4760,7 +4687,7 @@
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6">
@@ -5070,7 +4997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5091,21 +5018,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="B2" s="46">
         <v>1.0</v>
@@ -5119,7 +5046,7 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="B3" s="46">
         <v>1.0</v>
@@ -5133,7 +5060,7 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="B4" s="46">
         <v>3.0</v>
@@ -5147,7 +5074,7 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="B5" s="46">
         <v>1.0</v>
@@ -5161,21 +5088,21 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="B6" s="46">
         <v>3.0</v>
       </c>
       <c r="C6" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B7" s="46">
         <v>3.0</v>
@@ -5189,7 +5116,7 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="B8" s="46">
         <v>5.0</v>
@@ -5203,7 +5130,7 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B9" s="46">
         <v>4.0</v>
@@ -5217,7 +5144,7 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="B10" s="46">
         <v>4.0</v>
@@ -5231,7 +5158,7 @@
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B11" s="46">
         <v>1.0</v>
@@ -5245,7 +5172,7 @@
     </row>
     <row r="12">
       <c r="A12" s="21" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="B12" s="46">
         <v>4.0</v>
@@ -5259,7 +5186,7 @@
     </row>
     <row r="13">
       <c r="A13" s="21" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="B13" s="46">
         <v>1.0</v>
@@ -5273,7 +5200,7 @@
     </row>
     <row r="14">
       <c r="A14" s="21" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="B14" s="46">
         <v>2.0</v>
@@ -5287,7 +5214,7 @@
     </row>
     <row r="15">
       <c r="A15" s="21" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="B15" s="46">
         <v>3.0</v>
@@ -5301,7 +5228,7 @@
     </row>
     <row r="16">
       <c r="A16" s="21" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="B16" s="46">
         <v>2.0</v>
@@ -5315,7 +5242,7 @@
     </row>
     <row r="17">
       <c r="A17" s="21" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="B17" s="46">
         <v>2.0</v>
@@ -5329,7 +5256,7 @@
     </row>
     <row r="18">
       <c r="A18" s="21" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="B18" s="46">
         <v>2.0</v>
@@ -5343,7 +5270,7 @@
     </row>
     <row r="19">
       <c r="A19" s="21" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="B19" s="46">
         <v>2.0</v>
@@ -5357,7 +5284,7 @@
     </row>
     <row r="20">
       <c r="A20" s="21" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="B20" s="46">
         <v>3.0</v>
@@ -5371,20 +5298,48 @@
     </row>
     <row r="21">
       <c r="A21" s="21" t="s">
-        <v>333</v>
+        <v>433</v>
       </c>
       <c r="B21" s="46">
+        <v>2.0</v>
+      </c>
+      <c r="C21" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="B22" s="46">
+        <v>2.0</v>
+      </c>
+      <c r="C22" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="B23" s="46">
         <v>5.0</v>
       </c>
-      <c r="C21" s="21" t="b">
+      <c r="C23" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D21" s="21" t="b">
+      <c r="D23" s="21" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B21">
+  <conditionalFormatting sqref="B2:B23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="1"/>
@@ -5396,19 +5351,150 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A21">
+  <conditionalFormatting sqref="A2:A23">
     <cfRule type="expression" dxfId="5" priority="2">
       <formula>$C2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B21">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B23">
       <formula1>AND(ISNUMBER(B2),(NOT(OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFB45F06"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="2" width="34.0"/>
+    <col customWidth="1" min="4" max="5" width="23.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>436</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>437</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="48" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"SPRITE_POTION_RED")</f>
+        <v>SPRITE_POTION_RED</v>
+      </c>
+      <c r="B2" s="48" t="str">
+        <f t="array" ref="B2:B10">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
+        <v/>
+      </c>
+      <c r="D2" s="48" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"NAME_ITEM_POTION")</f>
+        <v>NAME_ITEM_POTION</v>
+      </c>
+      <c r="E2" s="48" t="str">
+        <f t="array" ref="E2:E10">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="48" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_POTION_BLUE")</f>
+        <v>SPRITE_POTION_BLUE</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="48" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_BLUE_POTION")</f>
+        <v>NAME_ITEM_BLUE_POTION</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
@@ -6862,7 +6948,7 @@
     <col customWidth="1" min="3" max="3" width="20.43"/>
     <col customWidth="1" min="4" max="4" width="27.57"/>
     <col customWidth="1" min="5" max="5" width="26.0"/>
-    <col customWidth="1" min="6" max="6" width="30.0"/>
+    <col customWidth="1" min="6" max="6" width="33.57"/>
     <col customWidth="1" min="7" max="7" width="44.57"/>
     <col customWidth="1" min="8" max="8" width="38.86"/>
     <col customWidth="1" min="9" max="9" width="37.86"/>
@@ -7195,15 +7281,89 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="21">
+        <f>ROW()-ROW(Table_Spawn_Conditions[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="21">
+        <f>ROW()-ROW(Table_Spawn_Conditions[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>231</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="F12:F13">
+      <formula1>#REF!</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C9">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="H2:H9">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:G9 J2:J9">
+    <dataValidation type="list" allowBlank="1" sqref="D2:G9 J2:J9 G12:G13">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="I2:I9">
@@ -7211,8 +7371,9 @@
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7239,7 +7400,8 @@
     <col customWidth="1" min="6" max="6" width="14.43"/>
     <col customWidth="1" min="7" max="7" width="28.0"/>
     <col customWidth="1" min="8" max="8" width="38.0"/>
-    <col customWidth="1" min="9" max="15" width="12.43"/>
+    <col customWidth="1" min="9" max="9" width="33.14"/>
+    <col customWidth="1" min="10" max="15" width="12.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7247,273 +7409,303 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>229</v>
+        <v>238</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="27">
+      <c r="A2" s="30">
         <f t="shared" ref="A2:A10" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>232</v>
-      </c>
-      <c r="F2" s="31" t="b">
+      <c r="C2" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="H2" s="32" t="s">
+      <c r="G2" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H2" s="35" t="s">
         <v>192</v>
       </c>
+      <c r="I2" s="35" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="27">
+      <c r="A3" s="30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="F3" s="31" t="b">
+      <c r="B3" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" s="35" t="s">
         <v>192</v>
       </c>
+      <c r="I3" s="35" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="27">
+      <c r="A4" s="30">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="F4" s="31" t="b">
+      <c r="B4" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="H4" s="32" t="s">
+      <c r="G4" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H4" s="35" t="s">
         <v>192</v>
       </c>
+      <c r="I4" s="35" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="27">
+      <c r="A5" s="30">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>239</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="F5" s="31" t="b">
+      <c r="B5" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="F5" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="H5" s="32" t="s">
+      <c r="G5" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H5" s="35" t="s">
         <v>192</v>
       </c>
+      <c r="I5" s="35" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="27">
+      <c r="A6" s="30">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="F6" s="31" t="b">
+      <c r="C6" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>243</v>
+      <c r="G6" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="27">
+      <c r="A7" s="30">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="F7" s="31" t="b">
+      <c r="C7" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="F7" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="H7" s="32" t="s">
+      <c r="G7" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="H7" s="35" t="s">
         <v>208</v>
       </c>
+      <c r="I7" s="35" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="27">
+      <c r="A8" s="30">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="F8" s="31" t="b">
+      <c r="B8" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="F8" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>249</v>
+      <c r="G8" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="27">
+      <c r="A9" s="30">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="F9" s="31" t="b">
+      <c r="B9" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="F9" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="H9" s="32" t="s">
+      <c r="G9" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H9" s="35" t="s">
         <v>219</v>
       </c>
+      <c r="I9" s="35" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="27">
+      <c r="A10" s="30">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>256</v>
-      </c>
-      <c r="F10" s="31" t="b">
+      <c r="B10" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="F10" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="H10" s="32" t="s">
+      <c r="G10" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H10" s="35" t="s">
         <v>192</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E10 H2:H10">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E10 H2:I10">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:D10 G2:G10">
@@ -7551,10 +7743,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2">
@@ -7563,7 +7755,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
@@ -7572,10 +7764,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4">
@@ -7584,10 +7776,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5">
@@ -7596,10 +7788,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6">
@@ -7608,10 +7800,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7">
@@ -7620,10 +7812,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8">
@@ -7632,10 +7824,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9">
@@ -7644,10 +7836,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10">
@@ -7656,10 +7848,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11">
@@ -7668,10 +7860,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12">
@@ -7680,10 +7872,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13">
@@ -7692,10 +7884,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>277</v>
+        <v>231</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14">
@@ -7704,10 +7896,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15">
@@ -7716,10 +7908,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16">
@@ -7728,10 +7920,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -7770,13 +7962,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2">
@@ -7787,11 +7979,11 @@
       <c r="B2" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="D2" s="34" t="s">
-        <v>285</v>
+      <c r="D2" s="36" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="3">
@@ -7802,11 +7994,11 @@
       <c r="B3" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>286</v>
+      <c r="D3" s="36" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="4">
@@ -7817,11 +8009,11 @@
       <c r="B4" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>287</v>
+      <c r="D4" s="36" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="5">
@@ -7832,11 +8024,11 @@
       <c r="B5" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>288</v>
+      <c r="D5" s="29" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="6">
@@ -7845,13 +8037,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="C6" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="D6" s="34" t="s">
-        <v>285</v>
+      <c r="D6" s="36" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="8">
@@ -7859,19 +8051,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>183</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9">
@@ -7880,7 +8072,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>193</v>
@@ -7901,7 +8093,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>193</v>
@@ -7922,7 +8114,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>193</v>
@@ -7934,7 +8126,7 @@
         <v>198</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12">
@@ -7943,7 +8135,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>193</v>
@@ -7955,7 +8147,7 @@
         <v>198</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13">
@@ -7964,7 +8156,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>215</v>
@@ -7976,7 +8168,7 @@
         <v>198</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14">
@@ -7985,10 +8177,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>193</v>
@@ -7997,7 +8189,7 @@
         <v>198</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15">
@@ -8006,7 +8198,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>193</v>
@@ -8018,7 +8210,7 @@
         <v>198</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16">
@@ -8027,7 +8219,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>193</v>
@@ -8039,7 +8231,7 @@
         <v>198</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17">
@@ -8048,7 +8240,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>193</v>
@@ -8064,52 +8256,52 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -8158,193 +8350,193 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>308</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>309</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>310</v>
+      <c r="B1" s="39" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="27">
+      <c r="A2" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>0</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+      <c r="B2" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3">
-      <c r="A3" s="27">
+      <c r="A3" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>311</v>
+      <c r="B3" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="27">
+      <c r="A4" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>312</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>313</v>
+      <c r="B4" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>320</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="27">
+      <c r="A5" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>315</v>
+      <c r="B5" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="27">
+      <c r="A6" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>317</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>318</v>
+      <c r="B6" s="30" t="s">
+        <v>324</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="27">
+      <c r="A7" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>5</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>319</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>320</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>321</v>
+      <c r="B7" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="27">
+      <c r="A8" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>6</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>322</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>323</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>324</v>
+      <c r="B8" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="27">
+      <c r="A9" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>7</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>325</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>326</v>
+      <c r="B9" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="27">
+      <c r="A10" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>8</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>327</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>328</v>
+      <c r="B10" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="27">
+      <c r="A11" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>9</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>329</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>330</v>
+      <c r="B11" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>337</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="27">
+      <c r="A12" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>10</v>
       </c>
-      <c r="B12" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>332</v>
+      <c r="B12" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="27">
+      <c r="A13" s="30">
         <f>ROW()-ROW(Table_Name[NAME_ID])</f>
         <v>11</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>255</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>333</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>334</v>
+      <c r="B13" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>341</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -8381,22 +8573,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2">
@@ -8414,7 +8606,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="G2" s="21"/>
     </row>
@@ -8424,7 +8616,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C3" s="21">
         <v>0.0</v>
@@ -8433,13 +8625,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4">
@@ -8448,7 +8640,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="C4" s="21">
         <v>0.0</v>
@@ -8457,13 +8649,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5">
@@ -8472,7 +8664,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="C5" s="21">
         <v>0.0</v>
@@ -8481,13 +8673,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6">
@@ -8496,7 +8688,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C6" s="21">
         <v>0.0</v>
@@ -8505,13 +8697,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7">
@@ -8520,7 +8712,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="C7" s="21">
         <v>0.0</v>
@@ -8529,13 +8721,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8">
@@ -8544,7 +8736,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C8" s="21">
         <v>0.0</v>
@@ -8553,13 +8745,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9">
@@ -8568,7 +8760,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C9" s="21">
         <v>0.0</v>
@@ -8577,13 +8769,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10">
@@ -8592,7 +8784,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C10" s="21">
         <v>0.0</v>
@@ -8601,13 +8793,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11">
@@ -8625,13 +8817,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12">
@@ -8640,7 +8832,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="C12" s="21">
         <v>0.0</v>
@@ -8649,13 +8841,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13">
@@ -8664,7 +8856,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="C13" s="21">
         <v>0.0</v>
@@ -8673,13 +8865,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -8723,36 +8915,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
-      <c r="A2" s="27">
+      <c r="A2" s="30">
         <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>377</v>
-      </c>
-      <c r="C2" s="39" t="str">
+      <c r="B2" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="C2" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8764,11 +8956,11 @@
 )"),"SPRITE_NONE")</f>
         <v>SPRITE_NONE</v>
       </c>
-      <c r="D2" s="39" t="str">
+      <c r="D2" s="41" t="str">
         <f t="shared" ref="D2:D4" si="2">SUBSTITUTE(H2,", ","|")</f>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="E2" s="39" t="str">
+      <c r="E2" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8780,25 +8972,25 @@
 )"),"ITEM_NONE")</f>
         <v>ITEM_NONE</v>
       </c>
-      <c r="F2" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="G2" s="32" t="s">
+      <c r="F2" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="H2" s="32" t="s">
-        <v>342</v>
+      <c r="H2" s="35" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
-      <c r="A3" s="27">
+      <c r="A3" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>378</v>
-      </c>
-      <c r="C3" s="39" t="str">
+      <c r="B3" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="C3" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8810,11 +9002,11 @@
 )"),"BACKGROUND_ROOM_FIRST")</f>
         <v>BACKGROUND_ROOM_FIRST</v>
       </c>
-      <c r="D3" s="39" t="str">
+      <c r="D3" s="41" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="E3" s="39" t="str">
+      <c r="E3" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8826,25 +9018,25 @@
 )"),"ITEM_POTION|ITEM_POTION_BLUE|ITEM_FOUNTAIN|ITEM_NPC_MILITO")</f>
         <v>ITEM_POTION|ITEM_POTION_BLUE|ITEM_FOUNTAIN|ITEM_NPC_MILITO</v>
       </c>
-      <c r="F3" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>379</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>342</v>
+      <c r="F3" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>387</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="27">
+      <c r="A4" s="30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="C4" s="39" t="str">
+      <c r="B4" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="C4" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8856,11 +9048,11 @@
 )"),"SPRITE_LAST")</f>
         <v>SPRITE_LAST</v>
       </c>
-      <c r="D4" s="39" t="str">
+      <c r="D4" s="41" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="E4" s="39" t="str">
+      <c r="E4" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -8872,14 +9064,14 @@
 )"),"ITEM_LAST")</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>256</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>254</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>342</v>
+      <c r="F4" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Smoother zoom and removed accumulated Keys from previous engine -Cursor label also in Inventory Menu
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="tek0Ywa62/n4ybLRJ5+4rDe3Y6cdrV6T6+++l56J0Ig="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="OeKWLJkIQEg0CCenqfu1QqxB9aKFGVmg9n3u43+QQUA="/>
     </ext>
   </extLst>
 </workbook>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="443">
   <si>
     <t>N</t>
   </si>
@@ -931,6 +931,12 @@
     <t>SPRITE_ATLAS_UI_0[SPRITE_CURSOR_USING]</t>
   </si>
   <si>
+    <t>SPRITE_CURSOR_DRAG</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_UI_0[SPRITE_CURSOR_DRAG]</t>
+  </si>
+  <si>
     <t>SPRITE_INVENTORY</t>
   </si>
   <si>
@@ -1415,6 +1421,15 @@
   </si>
   <si>
     <t>Spawn/Despawn conditions</t>
+  </si>
+  <si>
+    <t>Drag with mouse</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>More upper button commands</t>
   </si>
   <si>
     <t>Waypoint numeration in Editor</t>
@@ -2026,7 +2041,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D23" displayName="Table_TODO" name="Table_TODO" id="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D26" displayName="Table_TODO" name="Table_TODO" id="19">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -2131,7 +2146,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C16" displayName="Table_sprites" name="Table_sprites" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C17" displayName="Table_sprites" name="Table_sprites" id="6">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SPRITE_ID" id="2"/>
@@ -2845,10 +2860,10 @@
         <v>23</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>21</v>
@@ -4186,7 +4201,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2">
@@ -4222,7 +4237,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6">
@@ -4234,7 +4249,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8">
@@ -4250,7 +4265,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10">
@@ -4266,7 +4281,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12">
@@ -4290,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16">
@@ -4308,7 +4323,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="18">
@@ -4352,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="24">
@@ -4360,7 +4375,7 @@
         <v>0.0</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="25">
@@ -4368,7 +4383,7 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27">
@@ -4376,7 +4391,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="28">
@@ -4394,7 +4409,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="30">
@@ -4465,19 +4480,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2">
@@ -4502,7 +4517,7 @@
         <v>215</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>212</v>
@@ -4520,7 +4535,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
@@ -4532,7 +4547,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7">
@@ -4632,10 +4647,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2">
@@ -4648,7 +4663,7 @@
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3">
@@ -4661,7 +4676,7 @@
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4">
@@ -4674,7 +4689,7 @@
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5">
@@ -4687,7 +4702,7 @@
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6">
@@ -5018,21 +5033,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B2" s="46">
         <v>1.0</v>
@@ -5046,7 +5061,7 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B3" s="46">
         <v>1.0</v>
@@ -5060,7 +5075,7 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B4" s="46">
         <v>3.0</v>
@@ -5074,7 +5089,7 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B5" s="46">
         <v>1.0</v>
@@ -5088,7 +5103,7 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B6" s="46">
         <v>3.0</v>
@@ -5102,7 +5117,7 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B7" s="46">
         <v>3.0</v>
@@ -5116,7 +5131,7 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B8" s="46">
         <v>5.0</v>
@@ -5130,7 +5145,7 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B9" s="46">
         <v>4.0</v>
@@ -5144,7 +5159,7 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B10" s="46">
         <v>4.0</v>
@@ -5158,7 +5173,7 @@
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B11" s="46">
         <v>1.0</v>
@@ -5172,7 +5187,7 @@
     </row>
     <row r="12">
       <c r="A12" s="21" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B12" s="46">
         <v>4.0</v>
@@ -5186,7 +5201,7 @@
     </row>
     <row r="13">
       <c r="A13" s="21" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B13" s="46">
         <v>1.0</v>
@@ -5200,7 +5215,7 @@
     </row>
     <row r="14">
       <c r="A14" s="21" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B14" s="46">
         <v>2.0</v>
@@ -5214,7 +5229,7 @@
     </row>
     <row r="15">
       <c r="A15" s="21" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B15" s="46">
         <v>3.0</v>
@@ -5228,7 +5243,7 @@
     </row>
     <row r="16">
       <c r="A16" s="21" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B16" s="46">
         <v>2.0</v>
@@ -5242,7 +5257,7 @@
     </row>
     <row r="17">
       <c r="A17" s="21" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B17" s="46">
         <v>2.0</v>
@@ -5256,7 +5271,7 @@
     </row>
     <row r="18">
       <c r="A18" s="21" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B18" s="46">
         <v>2.0</v>
@@ -5270,7 +5285,7 @@
     </row>
     <row r="19">
       <c r="A19" s="21" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B19" s="46">
         <v>2.0</v>
@@ -5284,7 +5299,7 @@
     </row>
     <row r="20">
       <c r="A20" s="21" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B20" s="46">
         <v>3.0</v>
@@ -5298,7 +5313,7 @@
     </row>
     <row r="21">
       <c r="A21" s="21" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B21" s="46">
         <v>2.0</v>
@@ -5312,34 +5327,76 @@
     </row>
     <row r="22">
       <c r="A22" s="21" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B22" s="46">
         <v>2.0</v>
       </c>
       <c r="C22" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="21" t="s">
-        <v>341</v>
+        <v>437</v>
       </c>
       <c r="B23" s="46">
+        <v>2.0</v>
+      </c>
+      <c r="C23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="21" t="s">
+        <v>438</v>
+      </c>
+      <c r="B24" s="46">
+        <v>2.0</v>
+      </c>
+      <c r="C24" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="21" t="s">
+        <v>439</v>
+      </c>
+      <c r="B25" s="46">
+        <v>2.0</v>
+      </c>
+      <c r="C25" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="B26" s="46">
         <v>5.0</v>
       </c>
-      <c r="C23" s="21" t="b">
+      <c r="C26" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D23" s="21" t="b">
+      <c r="D26" s="21" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B23">
+  <conditionalFormatting sqref="B2:B26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="1"/>
@@ -5351,13 +5408,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A23">
+  <conditionalFormatting sqref="A2:A26">
     <cfRule type="expression" dxfId="5" priority="2">
       <formula>$C2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B23">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B26">
       <formula1>AND(ISNUMBER(B2),(NOT(OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -5389,16 +5446,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="47" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2">
@@ -7848,10 +7905,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>245</v>
+        <v>282</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11">
@@ -7860,10 +7917,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12">
@@ -7872,7 +7929,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>285</v>
@@ -7884,10 +7941,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>231</v>
+        <v>286</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14">
@@ -7896,10 +7953,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15">
@@ -7908,7 +7965,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>289</v>
@@ -7920,9 +7977,21 @@
         <v>14</v>
       </c>
       <c r="B16" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="21">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C17" s="21" t="s">
         <v>265</v>
       </c>
     </row>
@@ -7962,13 +8031,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2">
@@ -7983,7 +8052,7 @@
         <v>195</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3">
@@ -7998,7 +8067,7 @@
         <v>195</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4">
@@ -8013,7 +8082,7 @@
         <v>195</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5">
@@ -8028,7 +8097,7 @@
         <v>195</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6">
@@ -8037,13 +8106,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>195</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8">
@@ -8051,19 +8120,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>183</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9">
@@ -8072,7 +8141,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>193</v>
@@ -8093,7 +8162,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>193</v>
@@ -8114,7 +8183,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>193</v>
@@ -8126,7 +8195,7 @@
         <v>198</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12">
@@ -8135,7 +8204,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>193</v>
@@ -8147,7 +8216,7 @@
         <v>198</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13">
@@ -8156,7 +8225,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>215</v>
@@ -8168,7 +8237,7 @@
         <v>198</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14">
@@ -8177,10 +8246,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>193</v>
@@ -8189,7 +8258,7 @@
         <v>198</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15">
@@ -8198,7 +8267,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>193</v>
@@ -8210,7 +8279,7 @@
         <v>198</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16">
@@ -8219,7 +8288,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>193</v>
@@ -8231,7 +8300,7 @@
         <v>198</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17">
@@ -8240,7 +8309,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>193</v>
@@ -8354,13 +8423,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2">
@@ -8383,10 +8452,10 @@
         <v>243</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4">
@@ -8398,10 +8467,10 @@
         <v>247</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5">
@@ -8413,10 +8482,10 @@
         <v>249</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6">
@@ -8425,13 +8494,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7">
@@ -8440,13 +8509,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8">
@@ -8455,13 +8524,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9">
@@ -8473,10 +8542,10 @@
         <v>250</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10">
@@ -8488,10 +8557,10 @@
         <v>253</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11">
@@ -8503,10 +8572,10 @@
         <v>256</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12">
@@ -8518,10 +8587,10 @@
         <v>260</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13">
@@ -8533,10 +8602,10 @@
         <v>264</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -8573,22 +8642,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2">
@@ -8606,7 +8675,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="G2" s="21"/>
     </row>
@@ -8616,7 +8685,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C3" s="21">
         <v>0.0</v>
@@ -8625,13 +8694,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4">
@@ -8640,7 +8709,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C4" s="21">
         <v>0.0</v>
@@ -8649,13 +8718,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5">
@@ -8664,7 +8733,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C5" s="21">
         <v>0.0</v>
@@ -8673,13 +8742,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6">
@@ -8688,7 +8757,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C6" s="21">
         <v>0.0</v>
@@ -8697,13 +8766,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7">
@@ -8712,7 +8781,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C7" s="21">
         <v>0.0</v>
@@ -8721,13 +8790,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8">
@@ -8736,7 +8805,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C8" s="21">
         <v>0.0</v>
@@ -8745,13 +8814,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9">
@@ -8760,7 +8829,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C9" s="21">
         <v>0.0</v>
@@ -8769,13 +8838,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10">
@@ -8784,7 +8853,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C10" s="21">
         <v>0.0</v>
@@ -8793,13 +8862,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11">
@@ -8817,13 +8886,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12">
@@ -8832,7 +8901,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C12" s="21">
         <v>0.0</v>
@@ -8841,13 +8910,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13">
@@ -8856,7 +8925,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C13" s="21">
         <v>0.0</v>
@@ -8865,13 +8934,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -8915,25 +8984,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
@@ -8942,7 +9011,7 @@
         <v>-1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C2" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -8979,7 +9048,7 @@
         <v>195</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -8988,7 +9057,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C3" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9019,13 +9088,13 @@
         <v>ITEM_POTION|ITEM_POTION_BLUE|ITEM_FOUNTAIN|ITEM_NPC_MILITO</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4">
@@ -9034,7 +9103,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C4" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9071,7 +9140,7 @@
         <v>263</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Improvement in UI -Pending think to insert KeyListener (such as GameEvent listeners) -Pending to implement action to Menu Buttons
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="OeKWLJkIQEg0CCenqfu1QqxB9aKFGVmg9n3u43+QQUA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="wvV+1sb9+CTKF7wq7n1rEJPi5BdTqcZaFvlKkj0mPhg="/>
     </ext>
   </extLst>
 </workbook>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="440">
   <si>
     <t>N</t>
   </si>
@@ -478,10 +478,10 @@
     <t>Updates actual player waypoint when crossing or stopping on it</t>
   </si>
   <si>
-    <t>GAME_ELEMENT_OVER</t>
-  </si>
-  <si>
-    <t>GAME_ELEMENT_OVER_DELEGATE</t>
+    <t>GAME_ELEMENT_HOVER</t>
+  </si>
+  <si>
+    <t>GAME_ELEMENT_HOVER_DELEGATE</t>
   </si>
   <si>
     <t>LevelMasterClass.GameElementOverService</t>
@@ -514,18 +514,6 @@
     <t>Gets nearest WP from a given coordinates of level</t>
   </si>
   <si>
-    <t>IS_EVENT_OCCURRED</t>
-  </si>
-  <si>
-    <t>IS_EVENT_OCCURRED_DELEGATE</t>
-  </si>
-  <si>
-    <t>GameEventMasterClass.IsEventOccurredService</t>
-  </si>
-  <si>
-    <t>Tells if an event is occurred</t>
-  </si>
-  <si>
     <t>IS_EVENT_COMBI_OCCURRED</t>
   </si>
   <si>
@@ -535,7 +523,7 @@
     <t>GameEventMasterClass.IsEventCombiOccurredService</t>
   </si>
   <si>
-    <t>Same as IsEventOccurredService but for array of combos with possible negation</t>
+    <t>Checks if a combination of events is totally complied (event absence can also be requested)</t>
   </si>
   <si>
     <t>COMMIT_EVENT</t>
@@ -563,6 +551,9 @@
   </si>
   <si>
     <t>PLAYER_REACHED_WAYPOINT</t>
+  </si>
+  <si>
+    <t>PLAYER_REACHED_WAYPOINT_DELEGATE</t>
   </si>
   <si>
     <t>LevelMasterClass.PlayerReachedWaypointService</t>
@@ -2053,7 +2044,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N31" displayName="Table_Services" name="Table_Services" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N30" displayName="Table_Services" name="Table_Services" id="2">
   <tableColumns count="14">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SERVICE_ID" id="2"/>
@@ -3107,13 +3098,13 @@
         <v>24</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>22</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>24</v>
@@ -4201,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2">
@@ -4210,7 +4201,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3">
@@ -4219,7 +4210,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4">
@@ -4228,7 +4219,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5">
@@ -4237,7 +4228,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6">
@@ -4249,7 +4240,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8">
@@ -4257,7 +4248,7 @@
         <v>0.0</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9">
@@ -4265,7 +4256,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="10">
@@ -4273,7 +4264,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11">
@@ -4281,7 +4272,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12">
@@ -4289,7 +4280,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13">
@@ -4297,7 +4288,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15">
@@ -4305,7 +4296,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16">
@@ -4314,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17">
@@ -4323,7 +4314,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18">
@@ -4332,7 +4323,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19">
@@ -4341,7 +4332,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20">
@@ -4350,7 +4341,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21">
@@ -4359,7 +4350,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23">
@@ -4367,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="24">
@@ -4375,7 +4366,7 @@
         <v>0.0</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25">
@@ -4383,7 +4374,7 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27">
@@ -4391,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28">
@@ -4400,7 +4391,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29">
@@ -4409,7 +4400,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="30">
@@ -4418,7 +4409,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31">
@@ -4427,7 +4418,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32">
@@ -4436,7 +4427,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4480,19 +4471,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>402</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>403</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>404</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="2">
@@ -4501,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
@@ -4514,19 +4505,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D3" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>212</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>255</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4">
@@ -4535,7 +4526,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
@@ -4547,7 +4538,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7">
@@ -4647,10 +4638,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="2">
@@ -4663,7 +4654,7 @@
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3">
@@ -4676,7 +4667,7 @@
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4">
@@ -4689,7 +4680,7 @@
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5">
@@ -4702,7 +4693,7 @@
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6">
@@ -5033,21 +5024,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>412</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B2" s="46">
         <v>1.0</v>
@@ -5061,7 +5052,7 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B3" s="46">
         <v>1.0</v>
@@ -5075,7 +5066,7 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B4" s="46">
         <v>3.0</v>
@@ -5089,7 +5080,7 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B5" s="46">
         <v>1.0</v>
@@ -5103,7 +5094,7 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B6" s="46">
         <v>3.0</v>
@@ -5117,7 +5108,7 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B7" s="46">
         <v>3.0</v>
@@ -5131,7 +5122,7 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B8" s="46">
         <v>5.0</v>
@@ -5145,7 +5136,7 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B9" s="46">
         <v>4.0</v>
@@ -5159,7 +5150,7 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B10" s="46">
         <v>4.0</v>
@@ -5173,7 +5164,7 @@
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B11" s="46">
         <v>1.0</v>
@@ -5187,7 +5178,7 @@
     </row>
     <row r="12">
       <c r="A12" s="21" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B12" s="46">
         <v>4.0</v>
@@ -5201,7 +5192,7 @@
     </row>
     <row r="13">
       <c r="A13" s="21" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B13" s="46">
         <v>1.0</v>
@@ -5215,7 +5206,7 @@
     </row>
     <row r="14">
       <c r="A14" s="21" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B14" s="46">
         <v>2.0</v>
@@ -5229,7 +5220,7 @@
     </row>
     <row r="15">
       <c r="A15" s="21" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B15" s="46">
         <v>3.0</v>
@@ -5243,7 +5234,7 @@
     </row>
     <row r="16">
       <c r="A16" s="21" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B16" s="46">
         <v>2.0</v>
@@ -5257,7 +5248,7 @@
     </row>
     <row r="17">
       <c r="A17" s="21" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B17" s="46">
         <v>2.0</v>
@@ -5271,7 +5262,7 @@
     </row>
     <row r="18">
       <c r="A18" s="21" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B18" s="46">
         <v>2.0</v>
@@ -5285,7 +5276,7 @@
     </row>
     <row r="19">
       <c r="A19" s="21" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B19" s="46">
         <v>2.0</v>
@@ -5299,7 +5290,7 @@
     </row>
     <row r="20">
       <c r="A20" s="21" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B20" s="46">
         <v>3.0</v>
@@ -5313,7 +5304,7 @@
     </row>
     <row r="21">
       <c r="A21" s="21" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B21" s="46">
         <v>2.0</v>
@@ -5327,7 +5318,7 @@
     </row>
     <row r="22">
       <c r="A22" s="21" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B22" s="46">
         <v>2.0</v>
@@ -5341,7 +5332,7 @@
     </row>
     <row r="23">
       <c r="A23" s="21" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B23" s="46">
         <v>2.0</v>
@@ -5355,7 +5346,7 @@
     </row>
     <row r="24">
       <c r="A24" s="21" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B24" s="46">
         <v>2.0</v>
@@ -5369,7 +5360,7 @@
     </row>
     <row r="25">
       <c r="A25" s="21" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B25" s="46">
         <v>2.0</v>
@@ -5383,7 +5374,7 @@
     </row>
     <row r="26">
       <c r="A26" s="21" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B26" s="46">
         <v>5.0</v>
@@ -5446,16 +5437,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="47" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2">
@@ -5510,18 +5501,18 @@
     </row>
     <row r="6">
       <c r="B6" s="48" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="48" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8">
@@ -5634,7 +5625,7 @@
     </row>
     <row r="2">
       <c r="A2" s="11">
-        <f t="shared" ref="A2:A31" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A30" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -6273,7 +6264,7 @@
         <v>24</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>24</v>
@@ -6376,139 +6367,149 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="5" t="s">
+      <c r="F19" s="13"/>
+      <c r="G19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="5" t="s">
+      <c r="J19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="M19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
     </row>
     <row r="20">
       <c r="A20" s="11">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="14" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" s="14" t="s">
+      <c r="J20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
     </row>
     <row r="21">
       <c r="A21" s="11">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="5" t="s">
+      <c r="F21" s="13"/>
+      <c r="G21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="N21" s="5" t="s">
+      <c r="J21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="M21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
     </row>
     <row r="22">
       <c r="A22" s="11">
@@ -6535,16 +6536,16 @@
         <v>24</v>
       </c>
       <c r="I22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="14" t="s">
         <v>68</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="M22" s="14" t="s">
         <v>24</v>
@@ -6568,41 +6569,41 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="16" t="s">
         <v>150</v>
       </c>
+      <c r="D23" s="16" t="s">
+        <v>151</v>
+      </c>
       <c r="E23" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F23" s="13"/>
-      <c r="G23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H23" s="14" t="s">
+      <c r="G23" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="17" t="s">
         <v>24</v>
       </c>
       <c r="I23" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="M23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="N23" s="14" t="s">
+      <c r="N23" s="17" t="s">
         <v>24</v>
       </c>
       <c r="O23" s="15"/>
@@ -6621,53 +6622,43 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="16" t="s">
+      <c r="B24" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="C24" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="D24" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="I24" s="14" t="s">
+      <c r="E24" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J24" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" s="17" t="s">
+      <c r="J24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="15"/>
     </row>
     <row r="25">
       <c r="A25" s="11">
@@ -6675,16 +6666,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="5" t="s">
@@ -6700,7 +6691,7 @@
         <v>24</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>24</v>
@@ -6709,7 +6700,7 @@
         <v>68</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
@@ -6718,16 +6709,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="5" t="s">
@@ -6743,16 +6734,16 @@
         <v>24</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>68</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
@@ -6761,16 +6752,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="5" t="s">
@@ -6789,13 +6780,13 @@
         <v>24</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
@@ -6804,20 +6795,20 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>24</v>
@@ -6829,10 +6820,10 @@
         <v>24</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M28" s="5" t="s">
         <v>24</v>
@@ -6847,20 +6838,20 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>24</v>
@@ -6872,7 +6863,7 @@
         <v>24</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>24</v>
@@ -6890,32 +6881,32 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C30" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="C30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>24</v>
@@ -6924,58 +6915,15 @@
         <v>24</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="11">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N31" s="5" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A31">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A30">
       <formula1>AND(ISNUMBER(A2),(NOT(OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D")))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:N31">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:N30">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7020,34 +6968,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="J1" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="K1" s="20" t="s">
         <v>188</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2">
@@ -7056,31 +7004,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="G2" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="H2" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="I2" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>199</v>
-      </c>
       <c r="J2" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K2" s="25" t="b">
         <v>0</v>
@@ -7092,31 +7040,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E3" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>198</v>
-      </c>
       <c r="I3" s="23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K3" s="25" t="b">
         <v>0</v>
@@ -7128,31 +7076,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="F4" s="23" t="s">
+      <c r="I4" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>207</v>
-      </c>
       <c r="J4" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K4" s="25" t="b">
         <v>0</v>
@@ -7164,31 +7112,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K5" s="25" t="b">
         <v>0</v>
@@ -7200,31 +7148,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="23" t="s">
+      <c r="H6" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="J6" s="24" t="s">
         <v>212</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>215</v>
       </c>
       <c r="K6" s="25" t="b">
         <v>1</v>
@@ -7236,31 +7184,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E7" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>213</v>
-      </c>
       <c r="G7" s="23" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K7" s="25" t="b">
         <v>0</v>
@@ -7272,31 +7220,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K8" s="25" t="b">
         <v>0</v>
@@ -7308,31 +7256,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C9" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="G9" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="I9" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>199</v>
-      </c>
       <c r="J9" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K9" s="25" t="b">
         <v>0</v>
@@ -7343,22 +7291,22 @@
         <v>0</v>
       </c>
       <c r="B11" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="F11" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>224</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="12">
@@ -7367,7 +7315,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C12" s="27" t="b">
         <v>0</v>
@@ -7379,10 +7327,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13">
@@ -7391,7 +7339,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C13" s="27" t="b">
         <v>0</v>
@@ -7403,10 +7351,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -7466,28 +7414,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="H1" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="I1" s="20" t="s">
         <v>236</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2">
@@ -7496,28 +7444,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F2" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
@@ -7526,28 +7474,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" s="33" t="s">
         <v>242</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>245</v>
       </c>
       <c r="F3" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4">
@@ -7556,28 +7504,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F4" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5">
@@ -7586,28 +7534,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F5" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6">
@@ -7616,28 +7564,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F6" s="34" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7">
@@ -7646,28 +7594,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D7" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="33" t="s">
         <v>251</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>254</v>
       </c>
       <c r="F7" s="34" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8">
@@ -7676,28 +7624,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F8" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9">
@@ -7706,28 +7654,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E9" s="33" t="s">
         <v>259</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>262</v>
       </c>
       <c r="F9" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I9" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10">
@@ -7736,28 +7684,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F10" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -7800,10 +7748,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2">
@@ -7812,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3">
@@ -7821,10 +7769,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4">
@@ -7833,10 +7781,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5">
@@ -7845,10 +7793,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6">
@@ -7857,10 +7805,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7">
@@ -7869,10 +7817,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8">
@@ -7881,10 +7829,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9">
@@ -7893,10 +7841,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10">
@@ -7905,10 +7853,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11">
@@ -7917,10 +7865,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12">
@@ -7929,10 +7877,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13">
@@ -7941,10 +7889,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14">
@@ -7953,10 +7901,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15">
@@ -7965,10 +7913,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16">
@@ -7977,10 +7925,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17">
@@ -7989,10 +7937,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -8031,13 +7979,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2">
@@ -8046,13 +7994,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3">
@@ -8061,13 +8009,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4">
@@ -8076,13 +8024,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5">
@@ -8091,13 +8039,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6">
@@ -8106,13 +8054,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8">
@@ -8120,19 +8068,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>300</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="9">
@@ -8141,19 +8089,19 @@
         <v>0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10">
@@ -8162,19 +8110,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11">
@@ -8183,19 +8131,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12">
@@ -8204,19 +8152,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13">
@@ -8225,19 +8173,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14">
@@ -8246,19 +8194,19 @@
         <v>5</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15">
@@ -8267,19 +8215,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16">
@@ -8288,19 +8236,19 @@
         <v>7</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17">
@@ -8309,19 +8257,19 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19">
@@ -8423,13 +8371,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2">
@@ -8438,7 +8386,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
@@ -8449,13 +8397,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4">
@@ -8464,13 +8412,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5">
@@ -8479,13 +8427,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6">
@@ -8494,13 +8442,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7">
@@ -8509,13 +8457,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8">
@@ -8524,13 +8472,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9">
@@ -8539,13 +8487,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10">
@@ -8554,13 +8502,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11">
@@ -8569,13 +8517,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12">
@@ -8584,13 +8532,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13">
@@ -8599,13 +8547,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -8642,22 +8590,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>347</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>348</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="2">
@@ -8666,7 +8614,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C2" s="21">
         <v>0.0</v>
@@ -8675,7 +8623,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G2" s="21"/>
     </row>
@@ -8685,7 +8633,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C3" s="21">
         <v>0.0</v>
@@ -8694,13 +8642,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4">
@@ -8709,7 +8657,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C4" s="21">
         <v>0.0</v>
@@ -8718,13 +8666,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5">
@@ -8733,7 +8681,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C5" s="21">
         <v>0.0</v>
@@ -8742,13 +8690,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6">
@@ -8757,7 +8705,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C6" s="21">
         <v>0.0</v>
@@ -8766,13 +8714,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7">
@@ -8781,7 +8729,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C7" s="21">
         <v>0.0</v>
@@ -8790,13 +8738,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8">
@@ -8805,7 +8753,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C8" s="21">
         <v>0.0</v>
@@ -8814,13 +8762,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9">
@@ -8829,7 +8777,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C9" s="21">
         <v>0.0</v>
@@ -8838,13 +8786,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10">
@@ -8853,7 +8801,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C10" s="21">
         <v>0.0</v>
@@ -8862,13 +8810,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11">
@@ -8877,7 +8825,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C11" s="21">
         <v>0.0</v>
@@ -8886,13 +8834,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12">
@@ -8901,7 +8849,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C12" s="21">
         <v>0.0</v>
@@ -8910,13 +8858,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13">
@@ -8925,7 +8873,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C13" s="21">
         <v>0.0</v>
@@ -8934,13 +8882,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -8984,25 +8932,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>380</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>383</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>384</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>385</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
@@ -9011,7 +8959,7 @@
         <v>-1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C2" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9042,13 +8990,13 @@
         <v>ITEM_NONE</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -9057,7 +9005,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C3" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9088,13 +9036,13 @@
         <v>ITEM_POTION|ITEM_POTION_BLUE|ITEM_FOUNTAIN|ITEM_NPC_MILITO</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4">
@@ -9103,7 +9051,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C4" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9134,13 +9082,13 @@
         <v>ITEM_LAST</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Saved camera last position and zoom and restored when loading game
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="OeKWLJkIQEg0CCenqfu1QqxB9aKFGVmg9n3u43+QQUA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="MXgFLQn1d5Hz97pPCSjQAIXwX+jrM00f1uW0l/CuIUs="/>
     </ext>
   </extLst>
 </workbook>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="446">
   <si>
     <t>N</t>
   </si>
@@ -181,33 +181,33 @@
     <t>-</t>
   </si>
   <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>ELAPSED_TIME_MS</t>
+  </si>
+  <si>
+    <t>ulong</t>
+  </si>
+  <si>
+    <t>0UL</t>
+  </si>
+  <si>
+    <t>ACTUAL_ROOM</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Room.ROOM_NONE</t>
+  </si>
+  <si>
     <t>R E</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>ELAPSED_TIME_MS</t>
-  </si>
-  <si>
-    <t>ulong</t>
-  </si>
-  <si>
-    <t>0UL</t>
-  </si>
-  <si>
-    <t>ACTUAL_ROOM</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Room.ROOM_NONE</t>
-  </si>
-  <si>
     <t>EVENTS_OCCURRED</t>
   </si>
   <si>
@@ -230,6 +230,15 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>CAMERA_DISPOSITION</t>
+  </si>
+  <si>
+    <t>CameraDispositionStruct</t>
+  </si>
+  <si>
+    <t>CameraDispositionStruct_Default</t>
   </si>
   <si>
     <t>GAMESTATUS</t>
@@ -1912,7 +1921,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:P15" displayName="Table_Varmap" name="Table_Varmap" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:P16" displayName="Table_Varmap" name="Table_Varmap" id="1">
   <tableColumns count="16">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ENUM_ID" id="2"/>
@@ -2404,7 +2413,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="10.71"/>
     <col customWidth="1" min="2" max="2" width="34.29"/>
-    <col customWidth="1" min="3" max="3" width="22.29"/>
+    <col customWidth="1" min="3" max="3" width="23.57"/>
     <col customWidth="1" min="4" max="4" width="14.14"/>
     <col customWidth="1" min="5" max="5" width="11.86"/>
     <col customWidth="1" min="6" max="6" width="42.71"/>
@@ -2474,7 +2483,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <f t="shared" ref="A2:A15" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A16" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2501,17 +2510,17 @@
       <c r="I2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>21</v>
@@ -2529,10 +2538,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D3" s="4">
         <v>2.0</v>
@@ -2541,7 +2550,7 @@
         <v>0.0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>19</v>
@@ -2550,19 +2559,19 @@
         <v>20</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>21</v>
@@ -2580,10 +2589,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D4" s="4">
         <v>2.0</v>
@@ -2592,7 +2601,7 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>19</v>
@@ -2601,19 +2610,19 @@
         <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>21</v>
@@ -2673,7 +2682,7 @@
         <v>21</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -2708,19 +2717,19 @@
         <v>21</v>
       </c>
       <c r="K6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>21</v>
@@ -2758,7 +2767,7 @@
         <v>21</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>21</v>
@@ -2767,7 +2776,7 @@
         <v>21</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>21</v>
@@ -2781,47 +2790,45 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>0.0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>0.0</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>24</v>
+      <c r="G8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>22</v>
+      <c r="K8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>21</v>
@@ -2857,22 +2864,22 @@
         <v>23</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>21</v>
@@ -2904,20 +2911,20 @@
       <c r="H10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>24</v>
+      <c r="I10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N10" s="5" t="s">
         <v>21</v>
@@ -2934,69 +2941,71 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="4">
         <v>0.0</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>0.0</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>21</v>
+      <c r="J11" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D12" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E12" s="2">
         <v>0.0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>0</v>
@@ -3012,16 +3021,16 @@
         <v>23</v>
       </c>
       <c r="L12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="N12" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>21</v>
@@ -3036,16 +3045,16 @@
         <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D13" s="5">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E13" s="2">
         <v>0.0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>0</v>
@@ -3058,19 +3067,19 @@
         <v>21</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>21</v>
@@ -3082,10 +3091,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D14" s="5">
         <v>0.0</v>
@@ -3094,7 +3103,7 @@
         <v>0.0</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>0</v>
@@ -3110,10 +3119,10 @@
         <v>23</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>21</v>
@@ -3142,7 +3151,7 @@
       <c r="E15" s="2">
         <v>0.0</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="2" t="s">
         <v>58</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -3150,19 +3159,19 @@
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N15" s="5" t="s">
         <v>21</v>
@@ -3174,16 +3183,64 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="I23" s="9"/>
+    </row>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
@@ -4153,15 +4210,16 @@
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G15">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G16">
       <formula1>"N,Y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D15">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D16">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:P15">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:P16">
       <formula1>"R,R E,W,W E,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4201,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2">
@@ -4210,7 +4268,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3">
@@ -4219,7 +4277,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4">
@@ -4228,7 +4286,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5">
@@ -4237,7 +4295,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6">
@@ -4249,7 +4307,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8">
@@ -4257,7 +4315,7 @@
         <v>0.0</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9">
@@ -4265,7 +4323,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10">
@@ -4273,7 +4331,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11">
@@ -4281,7 +4339,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12">
@@ -4289,7 +4347,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13">
@@ -4297,7 +4355,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15">
@@ -4305,7 +4363,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="16">
@@ -4314,7 +4372,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17">
@@ -4323,7 +4381,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18">
@@ -4332,7 +4390,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19">
@@ -4341,7 +4399,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20">
@@ -4350,7 +4408,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21">
@@ -4359,7 +4417,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23">
@@ -4367,7 +4425,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24">
@@ -4375,7 +4433,7 @@
         <v>0.0</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="25">
@@ -4383,7 +4441,7 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="27">
@@ -4391,7 +4449,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="28">
@@ -4400,7 +4458,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29">
@@ -4409,7 +4467,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="30">
@@ -4418,7 +4476,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31">
@@ -4427,7 +4485,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32">
@@ -4436,7 +4494,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -4480,19 +4538,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2">
@@ -4501,7 +4559,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
@@ -4514,19 +4572,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>406</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>212</v>
-      </c>
       <c r="E3" s="23" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4">
@@ -4535,7 +4593,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
@@ -4547,7 +4605,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7">
@@ -4647,10 +4705,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2">
@@ -4663,7 +4721,7 @@
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3">
@@ -4676,7 +4734,7 @@
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4">
@@ -4689,7 +4747,7 @@
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5">
@@ -4702,7 +4760,7 @@
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6">
@@ -5033,21 +5091,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B2" s="46">
         <v>1.0</v>
@@ -5061,7 +5119,7 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B3" s="46">
         <v>1.0</v>
@@ -5075,7 +5133,7 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B4" s="46">
         <v>3.0</v>
@@ -5089,7 +5147,7 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B5" s="46">
         <v>1.0</v>
@@ -5103,7 +5161,7 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B6" s="46">
         <v>3.0</v>
@@ -5117,7 +5175,7 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B7" s="46">
         <v>3.0</v>
@@ -5131,7 +5189,7 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B8" s="46">
         <v>5.0</v>
@@ -5145,7 +5203,7 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B9" s="46">
         <v>4.0</v>
@@ -5159,7 +5217,7 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B10" s="46">
         <v>4.0</v>
@@ -5173,7 +5231,7 @@
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="B11" s="46">
         <v>1.0</v>
@@ -5187,7 +5245,7 @@
     </row>
     <row r="12">
       <c r="A12" s="21" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B12" s="46">
         <v>4.0</v>
@@ -5201,7 +5259,7 @@
     </row>
     <row r="13">
       <c r="A13" s="21" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B13" s="46">
         <v>1.0</v>
@@ -5215,7 +5273,7 @@
     </row>
     <row r="14">
       <c r="A14" s="21" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="B14" s="46">
         <v>2.0</v>
@@ -5229,7 +5287,7 @@
     </row>
     <row r="15">
       <c r="A15" s="21" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B15" s="46">
         <v>3.0</v>
@@ -5243,7 +5301,7 @@
     </row>
     <row r="16">
       <c r="A16" s="21" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B16" s="46">
         <v>2.0</v>
@@ -5257,7 +5315,7 @@
     </row>
     <row r="17">
       <c r="A17" s="21" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B17" s="46">
         <v>2.0</v>
@@ -5271,7 +5329,7 @@
     </row>
     <row r="18">
       <c r="A18" s="21" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B18" s="46">
         <v>2.0</v>
@@ -5285,7 +5343,7 @@
     </row>
     <row r="19">
       <c r="A19" s="21" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="B19" s="46">
         <v>2.0</v>
@@ -5299,7 +5357,7 @@
     </row>
     <row r="20">
       <c r="A20" s="21" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B20" s="46">
         <v>3.0</v>
@@ -5313,7 +5371,7 @@
     </row>
     <row r="21">
       <c r="A21" s="21" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B21" s="46">
         <v>2.0</v>
@@ -5327,7 +5385,7 @@
     </row>
     <row r="22">
       <c r="A22" s="21" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B22" s="46">
         <v>2.0</v>
@@ -5341,7 +5399,7 @@
     </row>
     <row r="23">
       <c r="A23" s="21" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="B23" s="46">
         <v>2.0</v>
@@ -5355,7 +5413,7 @@
     </row>
     <row r="24">
       <c r="A24" s="21" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B24" s="46">
         <v>2.0</v>
@@ -5369,7 +5427,7 @@
     </row>
     <row r="25">
       <c r="A25" s="21" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="B25" s="46">
         <v>2.0</v>
@@ -5383,7 +5441,7 @@
     </row>
     <row r="26">
       <c r="A26" s="21" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B26" s="46">
         <v>5.0</v>
@@ -5446,16 +5504,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="47" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2">
@@ -5510,18 +5568,18 @@
     </row>
     <row r="6">
       <c r="B6" s="48" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="48" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8">
@@ -5593,16 +5651,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -5638,22 +5696,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>21</v>
@@ -5665,7 +5723,7 @@
         <v>21</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>21</v>
@@ -5683,32 +5741,32 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>21</v>
@@ -5726,20 +5784,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>21</v>
@@ -5751,7 +5809,7 @@
         <v>21</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>21</v>
@@ -5769,28 +5827,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>21</v>
@@ -5814,22 +5872,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>21</v>
@@ -5841,7 +5899,7 @@
         <v>21</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>21</v>
@@ -5859,43 +5917,43 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8">
@@ -5904,41 +5962,41 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
@@ -5947,16 +6005,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="5" t="s">
@@ -5966,7 +6024,7 @@
         <v>21</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>21</v>
@@ -5975,10 +6033,10 @@
         <v>21</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N9" s="5" t="s">
         <v>21</v>
@@ -5990,16 +6048,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="5" t="s">
@@ -6009,7 +6067,7 @@
         <v>21</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>21</v>
@@ -6021,7 +6079,7 @@
         <v>21</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N10" s="5" t="s">
         <v>21</v>
@@ -6033,16 +6091,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="5" t="s">
@@ -6064,10 +6122,10 @@
         <v>21</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
@@ -6076,16 +6134,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="5" t="s">
@@ -6095,7 +6153,7 @@
         <v>21</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>21</v>
@@ -6104,7 +6162,7 @@
         <v>21</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M12" s="5" t="s">
         <v>21</v>
@@ -6119,16 +6177,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="5" t="s">
@@ -6138,7 +6196,7 @@
         <v>21</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>21</v>
@@ -6162,16 +6220,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="5" t="s">
@@ -6181,7 +6239,7 @@
         <v>21</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>21</v>
@@ -6205,16 +6263,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="5" t="s">
@@ -6224,7 +6282,7 @@
         <v>21</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>21</v>
@@ -6233,7 +6291,7 @@
         <v>21</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>21</v>
@@ -6248,16 +6306,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="5" t="s">
@@ -6267,19 +6325,19 @@
         <v>21</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N16" s="5" t="s">
         <v>21</v>
@@ -6291,16 +6349,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="5" t="s">
@@ -6310,16 +6368,16 @@
         <v>21</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>21</v>
@@ -6334,16 +6392,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="5" t="s">
@@ -6353,7 +6411,7 @@
         <v>21</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>21</v>
@@ -6362,10 +6420,10 @@
         <v>21</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N18" s="5" t="s">
         <v>21</v>
@@ -6377,16 +6435,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="14" t="s">
@@ -6396,22 +6454,22 @@
         <v>21</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J19" s="14" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M19" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N19" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
@@ -6430,16 +6488,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="5" t="s">
@@ -6449,22 +6507,22 @@
         <v>21</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21">
@@ -6473,16 +6531,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="14" t="s">
@@ -6492,7 +6550,7 @@
         <v>21</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J21" s="14" t="s">
         <v>21</v>
@@ -6501,7 +6559,7 @@
         <v>21</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M21" s="14" t="s">
         <v>21</v>
@@ -6526,16 +6584,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="14" t="s">
@@ -6545,7 +6603,7 @@
         <v>21</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J22" s="14" t="s">
         <v>21</v>
@@ -6554,7 +6612,7 @@
         <v>21</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M22" s="14" t="s">
         <v>21</v>
@@ -6579,16 +6637,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="17" t="s">
@@ -6598,7 +6656,7 @@
         <v>21</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J23" s="17" t="s">
         <v>21</v>
@@ -6610,7 +6668,7 @@
         <v>21</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N23" s="17" t="s">
         <v>21</v>
@@ -6632,16 +6690,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="5" t="s">
@@ -6651,7 +6709,7 @@
         <v>21</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>21</v>
@@ -6663,10 +6721,10 @@
         <v>21</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25">
@@ -6675,16 +6733,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="5" t="s">
@@ -6694,19 +6752,19 @@
         <v>21</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>21</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N25" s="5" t="s">
         <v>21</v>
@@ -6718,16 +6776,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="5" t="s">
@@ -6737,7 +6795,7 @@
         <v>21</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>21</v>
@@ -6746,13 +6804,13 @@
         <v>21</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
@@ -6761,23 +6819,23 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>21</v>
@@ -6786,7 +6844,7 @@
         <v>21</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>21</v>
@@ -6804,16 +6862,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="5" t="s">
@@ -6823,7 +6881,7 @@
         <v>21</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>21</v>
@@ -6832,7 +6890,7 @@
         <v>21</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M28" s="5" t="s">
         <v>21</v>
@@ -6847,32 +6905,32 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>21</v>
@@ -6890,16 +6948,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="5" t="s">
@@ -6909,13 +6967,13 @@
         <v>21</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>21</v>
@@ -6933,20 +6991,20 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>21</v>
@@ -7020,34 +7078,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2">
@@ -7056,31 +7114,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F2" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>196</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>193</v>
       </c>
       <c r="K2" s="25" t="b">
         <v>0</v>
@@ -7092,31 +7150,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G3" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="D3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="F3" s="23" t="s">
+      <c r="I3" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>199</v>
-      </c>
       <c r="J3" s="24" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K3" s="25" t="b">
         <v>0</v>
@@ -7128,31 +7186,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K4" s="25" t="b">
         <v>0</v>
@@ -7164,31 +7222,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F5" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="I5" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>199</v>
-      </c>
       <c r="J5" s="24" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K5" s="25" t="b">
         <v>0</v>
@@ -7200,31 +7258,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D6" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="H6" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>198</v>
-      </c>
       <c r="I6" s="23" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="K6" s="25" t="b">
         <v>1</v>
@@ -7236,31 +7294,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>213</v>
-      </c>
       <c r="G7" s="23" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K7" s="25" t="b">
         <v>0</v>
@@ -7272,31 +7330,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K8" s="25" t="b">
         <v>0</v>
@@ -7308,31 +7366,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F9" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>196</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>193</v>
       </c>
       <c r="K9" s="25" t="b">
         <v>0</v>
@@ -7343,22 +7401,22 @@
         <v>0</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12">
@@ -7367,7 +7425,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C12" s="27" t="b">
         <v>0</v>
@@ -7379,10 +7437,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13">
@@ -7391,7 +7449,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C13" s="27" t="b">
         <v>0</v>
@@ -7403,10 +7461,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -7466,28 +7524,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2">
@@ -7496,28 +7554,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F2" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
@@ -7526,28 +7584,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F3" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4">
@@ -7556,28 +7614,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C4" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>244</v>
-      </c>
       <c r="E4" s="33" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F4" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5">
@@ -7586,28 +7644,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>248</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>245</v>
       </c>
       <c r="F5" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6">
@@ -7616,28 +7674,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F6" s="34" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7">
@@ -7646,28 +7704,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F7" s="34" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8">
@@ -7676,28 +7734,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F8" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9">
@@ -7706,28 +7764,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F9" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I9" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10">
@@ -7736,28 +7794,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F10" s="34" t="b">
         <v>0</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -7800,10 +7858,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2">
@@ -7812,7 +7870,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3">
@@ -7821,10 +7879,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4">
@@ -7833,10 +7891,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5">
@@ -7845,10 +7903,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6">
@@ -7857,10 +7915,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7">
@@ -7869,10 +7927,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8">
@@ -7881,10 +7939,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9">
@@ -7893,10 +7951,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10">
@@ -7905,10 +7963,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11">
@@ -7917,10 +7975,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12">
@@ -7929,10 +7987,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13">
@@ -7941,10 +7999,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14">
@@ -7953,10 +8011,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15">
@@ -7965,10 +8023,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16">
@@ -7977,10 +8035,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17">
@@ -7989,10 +8047,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -8031,13 +8089,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2">
@@ -8046,13 +8104,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>195</v>
-      </c>
       <c r="D2" s="36" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3">
@@ -8061,13 +8119,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4">
@@ -8076,13 +8134,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5">
@@ -8091,13 +8149,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6">
@@ -8106,13 +8164,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8">
@@ -8120,19 +8178,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9">
@@ -8141,19 +8199,19 @@
         <v>0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10">
@@ -8162,19 +8220,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11">
@@ -8183,19 +8241,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12">
@@ -8204,19 +8262,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13">
@@ -8225,19 +8283,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14">
@@ -8246,19 +8304,19 @@
         <v>5</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15">
@@ -8267,19 +8325,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16">
@@ -8288,19 +8346,19 @@
         <v>7</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17">
@@ -8309,19 +8367,19 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19">
@@ -8423,13 +8481,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2">
@@ -8438,7 +8496,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
@@ -8449,13 +8507,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4">
@@ -8464,13 +8522,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5">
@@ -8479,13 +8537,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6">
@@ -8494,13 +8552,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7">
@@ -8509,13 +8567,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8">
@@ -8524,13 +8582,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9">
@@ -8539,13 +8597,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10">
@@ -8554,13 +8612,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11">
@@ -8569,13 +8627,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12">
@@ -8584,13 +8642,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13">
@@ -8599,13 +8657,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -8642,22 +8700,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2">
@@ -8666,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C2" s="21">
         <v>0.0</v>
@@ -8675,7 +8733,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G2" s="21"/>
     </row>
@@ -8685,7 +8743,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C3" s="21">
         <v>0.0</v>
@@ -8694,13 +8752,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4">
@@ -8709,7 +8767,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C4" s="21">
         <v>0.0</v>
@@ -8718,13 +8776,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5">
@@ -8733,7 +8791,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C5" s="21">
         <v>0.0</v>
@@ -8742,13 +8800,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6">
@@ -8757,7 +8815,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C6" s="21">
         <v>0.0</v>
@@ -8766,13 +8824,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7">
@@ -8781,7 +8839,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C7" s="21">
         <v>0.0</v>
@@ -8790,13 +8848,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8">
@@ -8805,7 +8863,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C8" s="21">
         <v>0.0</v>
@@ -8814,13 +8872,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9">
@@ -8829,7 +8887,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C9" s="21">
         <v>0.0</v>
@@ -8838,13 +8896,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10">
@@ -8853,7 +8911,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C10" s="21">
         <v>0.0</v>
@@ -8862,13 +8920,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11">
@@ -8877,7 +8935,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C11" s="21">
         <v>0.0</v>
@@ -8886,13 +8944,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12">
@@ -8901,7 +8959,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C12" s="21">
         <v>0.0</v>
@@ -8910,13 +8968,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13">
@@ -8925,7 +8983,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C13" s="21">
         <v>0.0</v>
@@ -8934,13 +8992,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -8984,25 +9042,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
@@ -9011,7 +9069,7 @@
         <v>-1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C2" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9042,13 +9100,13 @@
         <v>ITEM_NONE</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -9057,7 +9115,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="C3" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9088,13 +9146,13 @@
         <v>ITEM_POTION|ITEM_POTION_BLUE|ITEM_FOUNTAIN|ITEM_NPC_MILITO</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4">
@@ -9103,7 +9161,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C4" s="41" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9134,13 +9192,13 @@
         <v>ITEM_LAST</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Unchainers part 2
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="+OsgWlKpz3rEQBEoQqyDldkFjMoYVSJwnG0mCPZ3r+8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="RevQRioADhUqV9bUm1e5eju+pgJalEnDZytwzxc5btY="/>
     </ext>
   </extLst>
 </workbook>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="434">
   <si>
     <t>N</t>
   </si>
@@ -516,6 +516,18 @@
     <t>Makes player interact with usage data</t>
   </si>
   <si>
+    <t>UNCHAIN_TO_ITEM</t>
+  </si>
+  <si>
+    <t>UNCHAIN_TO_ITEM_DELEGATE</t>
+  </si>
+  <si>
+    <t>ItemMasterClass.UnchainToItemService</t>
+  </si>
+  <si>
+    <t>Applies an unchain event to an item such as spawn or setsprite</t>
+  </si>
+  <si>
     <t>PLAYER_REACHED_WAYPOINT</t>
   </si>
   <si>
@@ -744,19 +756,19 @@
     <t>TargetSprite</t>
   </si>
   <si>
-    <t>UNCHAIN_NONE</t>
-  </si>
-  <si>
-    <t>UNCHAIN_TYPE_NONE</t>
+    <t>TargetEvents</t>
+  </si>
+  <si>
+    <t>UNCHAIN_RED_POTION_TOOK</t>
+  </si>
+  <si>
+    <t>UNCHAIN_TYPE_DESPAWN</t>
   </si>
   <si>
     <t>SPRITE_NONE</t>
   </si>
   <si>
-    <t>UNCHAIN_RED_POTION_TOOK</t>
-  </si>
-  <si>
-    <t>UNCHAIN_TYPE_DESPAWN</t>
+    <t>UNCHAIN_FOUNTAIN_FULL</t>
   </si>
   <si>
     <t>UNCHAIN_TYPE_SET_SPRITE</t>
@@ -1936,7 +1948,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A23:B28" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A23:B27" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="15">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_TYPE_ID" id="2"/>
@@ -1946,7 +1958,7 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A30:B32" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A29:B31" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="16">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ANIMATION_ID" id="2"/>
@@ -1956,7 +1968,7 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A34:B39" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A33:B38" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="17">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_FAMILY_TYPE_ID" id="2"/>
@@ -1986,7 +1998,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N27" displayName="Table_Services" name="Table_Services" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N28" displayName="Table_Services" name="Table_Services" id="2">
   <tableColumns count="14">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SERVICE_ID" id="2"/>
@@ -2058,8 +2070,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A11:G14" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="4">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A11:H13" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="4">
+  <tableColumns count="8">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_ID" id="2"/>
     <tableColumn name="Type" id="3"/>
@@ -2067,6 +2079,7 @@
     <tableColumn name="NeededEvents" id="5"/>
     <tableColumn name="TargetItem" id="6"/>
     <tableColumn name="TargetSprite" id="7"/>
+    <tableColumn name="TargetEvents" id="8"/>
   </tableColumns>
   <tableStyleInfo name="ACTION_CONDS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -2565,7 +2578,7 @@
         <v>21</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -4193,7 +4206,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2">
@@ -4202,7 +4215,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3">
@@ -4211,7 +4224,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4">
@@ -4220,7 +4233,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5">
@@ -4229,7 +4242,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6">
@@ -4241,7 +4254,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="8">
@@ -4249,7 +4262,7 @@
         <v>0.0</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9">
@@ -4257,7 +4270,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10">
@@ -4265,7 +4278,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11">
@@ -4273,7 +4286,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12">
@@ -4281,7 +4294,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13">
@@ -4289,7 +4302,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15">
@@ -4297,7 +4310,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16">
@@ -4306,7 +4319,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17">
@@ -4315,7 +4328,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18">
@@ -4324,7 +4337,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19">
@@ -4333,7 +4346,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20">
@@ -4342,7 +4355,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21">
@@ -4351,7 +4364,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23">
@@ -4359,7 +4372,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24">
@@ -4368,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>216</v>
+        <v>392</v>
       </c>
     </row>
     <row r="25">
@@ -4377,7 +4390,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>388</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26">
@@ -4386,7 +4399,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27">
@@ -4395,93 +4408,84 @@
         <v>3</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="21">
-        <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>4</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>389</v>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>390</v>
+      <c r="A30" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="21">
-        <v>1.0</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>342</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="21">
+        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>0</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>391</v>
+      <c r="B34" s="21" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="21">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>231</v>
+        <v>1</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="21">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>392</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="21">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="21">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="21">
-        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>4</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -4523,7 +4527,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2">
@@ -4532,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
@@ -4541,7 +4545,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
@@ -4550,7 +4554,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5">
@@ -4559,7 +4563,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7">
@@ -4567,7 +4571,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8">
@@ -4783,10 +4787,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2">
@@ -4799,7 +4803,7 @@
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3">
@@ -4812,7 +4816,7 @@
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4">
@@ -4825,7 +4829,7 @@
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5">
@@ -4838,7 +4842,7 @@
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6">
@@ -5169,21 +5173,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B2" s="42">
         <v>1.0</v>
@@ -5197,7 +5201,7 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="B3" s="42">
         <v>1.0</v>
@@ -5211,7 +5215,7 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="B4" s="42">
         <v>3.0</v>
@@ -5225,7 +5229,7 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B5" s="42">
         <v>1.0</v>
@@ -5239,7 +5243,7 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B6" s="42">
         <v>3.0</v>
@@ -5253,7 +5257,7 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B7" s="42">
         <v>3.0</v>
@@ -5267,7 +5271,7 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B8" s="42">
         <v>5.0</v>
@@ -5281,7 +5285,7 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B9" s="42">
         <v>4.0</v>
@@ -5295,7 +5299,7 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B10" s="42">
         <v>4.0</v>
@@ -5309,7 +5313,7 @@
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="B11" s="42">
         <v>1.0</v>
@@ -5323,7 +5327,7 @@
     </row>
     <row r="12">
       <c r="A12" s="21" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B12" s="42">
         <v>4.0</v>
@@ -5337,7 +5341,7 @@
     </row>
     <row r="13">
       <c r="A13" s="21" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B13" s="42">
         <v>1.0</v>
@@ -5351,7 +5355,7 @@
     </row>
     <row r="14">
       <c r="A14" s="21" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B14" s="42">
         <v>2.0</v>
@@ -5365,7 +5369,7 @@
     </row>
     <row r="15">
       <c r="A15" s="21" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B15" s="42">
         <v>3.0</v>
@@ -5379,7 +5383,7 @@
     </row>
     <row r="16">
       <c r="A16" s="21" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="B16" s="42">
         <v>2.0</v>
@@ -5393,7 +5397,7 @@
     </row>
     <row r="17">
       <c r="A17" s="21" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B17" s="42">
         <v>2.0</v>
@@ -5407,7 +5411,7 @@
     </row>
     <row r="18">
       <c r="A18" s="21" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B18" s="42">
         <v>2.0</v>
@@ -5421,7 +5425,7 @@
     </row>
     <row r="19">
       <c r="A19" s="21" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="B19" s="42">
         <v>2.0</v>
@@ -5435,7 +5439,7 @@
     </row>
     <row r="20">
       <c r="A20" s="21" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B20" s="42">
         <v>3.0</v>
@@ -5449,7 +5453,7 @@
     </row>
     <row r="21">
       <c r="A21" s="21" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B21" s="42">
         <v>2.0</v>
@@ -5463,7 +5467,7 @@
     </row>
     <row r="22">
       <c r="A22" s="21" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="B22" s="42">
         <v>2.0</v>
@@ -5477,7 +5481,7 @@
     </row>
     <row r="23">
       <c r="A23" s="21" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="B23" s="42">
         <v>2.0</v>
@@ -5491,7 +5495,7 @@
     </row>
     <row r="24">
       <c r="A24" s="21" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="B24" s="42">
         <v>2.0</v>
@@ -5505,7 +5509,7 @@
     </row>
     <row r="25">
       <c r="A25" s="21" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B25" s="42">
         <v>2.0</v>
@@ -5519,7 +5523,7 @@
     </row>
     <row r="26">
       <c r="A26" s="21" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B26" s="42">
         <v>5.0</v>
@@ -5582,16 +5586,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="43" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2">
@@ -5646,18 +5650,18 @@
     </row>
     <row r="6">
       <c r="B6" s="44" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="44" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8">
@@ -5770,7 +5774,7 @@
     </row>
     <row r="2">
       <c r="A2" s="11">
-        <f t="shared" ref="A2:A27" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A28" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -6595,22 +6599,22 @@
         <v>21</v>
       </c>
       <c r="I20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="14" t="s">
+      <c r="N20" s="14" t="s">
         <v>70</v>
-      </c>
-      <c r="M20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="14" t="s">
-        <v>21</v>
       </c>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
@@ -6628,41 +6632,41 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="12" t="s">
         <v>145</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>146</v>
       </c>
       <c r="F21" s="13"/>
-      <c r="G21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="17" t="s">
+      <c r="G21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="14" t="s">
         <v>21</v>
       </c>
       <c r="I21" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="J21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M21" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="N21" s="17" t="s">
+      <c r="M21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="14" t="s">
         <v>21</v>
       </c>
       <c r="O21" s="15"/>
@@ -6681,43 +6685,53 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="5" t="s">
+      <c r="F22" s="13"/>
+      <c r="G22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="5" t="s">
+      <c r="J22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="N22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
     </row>
     <row r="23">
       <c r="A23" s="11">
@@ -6736,27 +6750,27 @@
       <c r="E23" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="N23" s="5" t="s">
         <v>21</v>
@@ -6779,24 +6793,24 @@
       <c r="E24" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="L24" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>21</v>
@@ -6824,7 +6838,7 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>21</v>
@@ -6836,10 +6850,10 @@
         <v>21</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>21</v>
@@ -6867,7 +6881,7 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>21</v>
@@ -6879,7 +6893,7 @@
         <v>21</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>21</v>
@@ -6899,31 +6913,31 @@
       <c r="B27" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>85</v>
+      <c r="C27" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="L27" s="5" t="s">
         <v>21</v>
       </c>
@@ -6931,15 +6945,58 @@
         <v>21</v>
       </c>
       <c r="N27" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="11">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="5" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A27">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A28">
       <formula1>AND(ISNUMBER(A2),(NOT(OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D")))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:N27">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:N28">
       <formula1>"W,X,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6984,31 +7041,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2">
@@ -7017,31 +7074,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G2" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>183</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="3">
@@ -7050,31 +7107,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D3" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="E3" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>184</v>
-      </c>
       <c r="I3" s="23" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
@@ -7083,31 +7140,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5">
@@ -7116,31 +7173,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F5" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="H5" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="I5" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="J5" s="24" t="s">
         <v>183</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="6">
@@ -7149,31 +7206,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7">
@@ -7182,31 +7239,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8">
@@ -7215,31 +7272,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9">
@@ -7248,31 +7305,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G9" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>183</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="11">
@@ -7280,22 +7337,25 @@
         <v>0</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>214</v>
+        <v>218</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="12">
@@ -7304,22 +7364,25 @@
         <v>0</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>217</v>
+        <v>222</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="13">
@@ -7328,51 +7391,30 @@
         <v>1</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="21">
-        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>2</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>222</v>
+        <v>226</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D12:D14">
+    <dataValidation type="list" allowBlank="1" sqref="D12:D13">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C9">
@@ -7381,10 +7423,10 @@
     <dataValidation type="list" allowBlank="1" sqref="H2:H9">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J9 E12:E14">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J9 E12:E13 H12:H13">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:G9 C12:C14 F12:G14">
+    <dataValidation type="list" allowBlank="1" sqref="D2:G9 C12:C13 F12:G13">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="I2:I9">
@@ -7430,25 +7472,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2">
@@ -7457,25 +7499,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F2" s="32" t="b">
         <v>0</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3">
@@ -7484,25 +7526,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="F3" s="32" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4">
@@ -7511,25 +7553,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="F4" s="32" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5">
@@ -7538,25 +7580,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="E5" s="31" t="s">
         <v>239</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>234</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>235</v>
       </c>
       <c r="F5" s="32" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6">
@@ -7565,25 +7607,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="F6" s="32" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7">
@@ -7592,25 +7634,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="F7" s="32" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H7" s="33" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8">
@@ -7619,25 +7661,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C8" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="D8" s="30" t="s">
-        <v>241</v>
-      </c>
       <c r="E8" s="31" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F8" s="32" t="b">
         <v>0</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9">
@@ -7646,25 +7688,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F9" s="32" t="b">
         <v>0</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10">
@@ -7673,25 +7715,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F10" s="32" t="b">
         <v>0</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -7734,10 +7776,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2">
@@ -7746,7 +7788,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3">
@@ -7755,10 +7797,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4">
@@ -7767,10 +7809,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5">
@@ -7779,10 +7821,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6">
@@ -7791,10 +7833,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7">
@@ -7803,10 +7845,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8">
@@ -7815,10 +7857,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9">
@@ -7827,10 +7869,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10">
@@ -7839,10 +7881,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11">
@@ -7851,10 +7893,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12">
@@ -7863,10 +7905,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13">
@@ -7875,10 +7917,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14">
@@ -7887,10 +7929,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15">
@@ -7899,10 +7941,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16">
@@ -7911,10 +7953,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17">
@@ -7923,10 +7965,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -7965,13 +8007,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2">
@@ -7980,13 +8022,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3">
@@ -7995,13 +8037,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4">
@@ -8010,13 +8052,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5">
@@ -8025,13 +8067,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6">
@@ -8040,13 +8082,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>288</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="8">
@@ -8054,19 +8096,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9">
@@ -8075,19 +8117,19 @@
         <v>0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10">
@@ -8096,19 +8138,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11">
@@ -8117,19 +8159,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12">
@@ -8138,19 +8180,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13">
@@ -8159,19 +8201,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>179</v>
+        <v>206</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14">
@@ -8180,19 +8222,19 @@
         <v>5</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>179</v>
+        <v>304</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15">
@@ -8201,19 +8243,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16">
@@ -8222,19 +8264,19 @@
         <v>7</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17">
@@ -8243,19 +8285,19 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19">
@@ -8314,13 +8356,13 @@
     <dataValidation type="list" allowBlank="1" sqref="F9:F17">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D9:D17">
-      <formula1>Table_Events[EVENT_ID]</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C9:C17">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D2:D6">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D9:D17">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="E9:E17">
@@ -8357,13 +8399,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2">
@@ -8372,7 +8414,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
@@ -8383,13 +8425,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4">
@@ -8398,13 +8440,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5">
@@ -8413,13 +8455,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6">
@@ -8428,13 +8470,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7">
@@ -8443,13 +8485,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8">
@@ -8458,13 +8500,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9">
@@ -8473,13 +8515,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10">
@@ -8488,13 +8530,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11">
@@ -8503,13 +8545,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12">
@@ -8518,13 +8560,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13">
@@ -8533,13 +8575,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -8576,22 +8618,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2">
@@ -8600,7 +8642,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C2" s="21">
         <v>0.0</v>
@@ -8609,7 +8651,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="G2" s="21"/>
     </row>
@@ -8619,7 +8661,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C3" s="21">
         <v>0.0</v>
@@ -8628,13 +8670,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4">
@@ -8643,7 +8685,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C4" s="21">
         <v>0.0</v>
@@ -8652,13 +8694,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5">
@@ -8667,7 +8709,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C5" s="21">
         <v>0.0</v>
@@ -8676,13 +8718,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6">
@@ -8691,7 +8733,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="C6" s="21">
         <v>0.0</v>
@@ -8700,13 +8742,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7">
@@ -8715,7 +8757,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="C7" s="21">
         <v>0.0</v>
@@ -8724,13 +8766,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8">
@@ -8739,7 +8781,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C8" s="21">
         <v>0.0</v>
@@ -8748,13 +8790,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9">
@@ -8763,7 +8805,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C9" s="21">
         <v>0.0</v>
@@ -8772,13 +8814,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10">
@@ -8787,7 +8829,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C10" s="21">
         <v>0.0</v>
@@ -8796,13 +8838,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11">
@@ -8811,7 +8853,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C11" s="21">
         <v>0.0</v>
@@ -8820,13 +8862,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12">
@@ -8835,7 +8877,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C12" s="21">
         <v>0.0</v>
@@ -8844,13 +8886,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13">
@@ -8859,7 +8901,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C13" s="21">
         <v>0.0</v>
@@ -8868,13 +8910,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -8918,25 +8960,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
@@ -8945,7 +8987,7 @@
         <v>-1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C2" s="38" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -8976,13 +9018,13 @@
         <v>ITEM_NONE</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -8991,7 +9033,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="C3" s="38" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9022,13 +9064,13 @@
         <v>ITEM_POTION|ITEM_POTION_BLUE|ITEM_FOUNTAIN|ITEM_NPC_MILITO</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4">
@@ -9037,7 +9079,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="C4" s="38" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9068,13 +9110,13 @@
         <v>ITEM_LAST</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Memento part 1
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="1rIOFNNcgLtBVNPWuph1Z1dDHHR9A1HRbdjaNIKTGHM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="9pTKa1/CSa8+HA9axHOey5TgCP61CNcau05bqhNsx28="/>
     </ext>
   </extLst>
 </workbook>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="471">
   <si>
     <t>N</t>
   </si>
@@ -411,18 +411,6 @@
     <t>Registers a player in scene</t>
   </si>
   <si>
-    <t>WP_REGISTER</t>
-  </si>
-  <si>
-    <t>WP_REGISTER_DELEGATE</t>
-  </si>
-  <si>
-    <t>LevelMasterClass.WPRegisterService</t>
-  </si>
-  <si>
-    <t>Registers a Waypoint in level</t>
-  </si>
-  <si>
     <t>DOOR_REGISTER</t>
   </si>
   <si>
@@ -459,6 +447,18 @@
     <t>Updates actual player waypoint when crossing or stopping on it</t>
   </si>
   <si>
+    <t>GET_WP_LIST</t>
+  </si>
+  <si>
+    <t>GET_WP_LIST_DELEGATE</t>
+  </si>
+  <si>
+    <t>LevelMasterClass.GetWaypointListService</t>
+  </si>
+  <si>
+    <t>Gets list of waypoints and solutions</t>
+  </si>
+  <si>
     <t>GAME_ELEMENT_HOVER</t>
   </si>
   <si>
@@ -720,6 +720,9 @@
     <t>ITEM_POTION_BLUE</t>
   </si>
   <si>
+    <t>EVENT_BLUE_POTION_TOOK</t>
+  </si>
+  <si>
     <t>COND_FOUNTAIN</t>
   </si>
   <si>
@@ -792,6 +795,12 @@
     <t>UNCHAIN_TYPE_EARN_ITEM</t>
   </si>
   <si>
+    <t>UNCHAIN_BLUE_POTION_TOOK</t>
+  </si>
+  <si>
+    <t>UNCHAIN_BLUE_POTION_TOOK_2</t>
+  </si>
+  <si>
     <t>UNCHAIN_FOUNTAIN_FULL</t>
   </si>
   <si>
@@ -1251,6 +1260,24 @@
     <t>Dicen que compilas solo con la mente</t>
   </si>
   <si>
+    <t>PHRASE_MEMENTO_POTION_1</t>
+  </si>
+  <si>
+    <t>A potion with unknown effects. What will it serve for?</t>
+  </si>
+  <si>
+    <t>Una poción con efectos desconocidos. Para qué servirá?</t>
+  </si>
+  <si>
+    <t>PHRASE_MEMENTO_POTION_2</t>
+  </si>
+  <si>
+    <t>Finally I knew it served to fill fountain</t>
+  </si>
+  <si>
+    <t>Finalmente descurí que servía para llenar la fuente</t>
+  </si>
+  <si>
     <t>ROOM_ID</t>
   </si>
   <si>
@@ -1314,6 +1341,12 @@
     <t>UNCHAIN_TYPE_EVENT</t>
   </si>
   <si>
+    <t>UNCHAIN_TYPE_NOTIF</t>
+  </si>
+  <si>
+    <t>UNCHAIN_TYPE_MEMENTO</t>
+  </si>
+  <si>
     <t>DIALOG_ANIMATION_ID</t>
   </si>
   <si>
@@ -1329,6 +1362,48 @@
     <t>EVENT_LAST</t>
   </si>
   <si>
+    <t>MEMENTO_PARENT_ID</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>MEMENTO_PARENT_NONE</t>
+  </si>
+  <si>
+    <t>MEMENTO_PARENT_RED_POTION</t>
+  </si>
+  <si>
+    <t>MEMENTO_PARENT_LAST</t>
+  </si>
+  <si>
+    <t>MEMENTO_ID</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Phrase</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>MEMENTO_NONE</t>
+  </si>
+  <si>
+    <t>MEMENTO_RED_POTION_1</t>
+  </si>
+  <si>
+    <t>MEMENTO_RED_POTION_2</t>
+  </si>
+  <si>
+    <t>MEMENTO_LAST</t>
+  </si>
+  <si>
     <t>EVENT_COMBI_ID</t>
   </si>
   <si>
@@ -1423,6 +1498,9 @@
   </si>
   <si>
     <t>Waypoint numeration in Editor</t>
+  </si>
+  <si>
+    <t>Use one raycast for all objets (Input)</t>
   </si>
   <si>
     <t>SPRITES</t>
@@ -1499,7 +1577,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1619,6 +1697,12 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1705,7 +1789,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="22">
+  <tableStyles count="24">
     <tableStyle count="4" pivot="0" name="VARMAP-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1820,6 +1904,18 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
       <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
+    <tableStyle count="4" pivot="0" name="EVENTS-style 3">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
+    <tableStyle count="4" pivot="0" name="EVENTS-style 4">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
     <tableStyle count="4" pivot="0" name="_TODO-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1923,7 +2019,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G13" displayName="Table_Phrases" name="Table_Phrases" id="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G15" displayName="Table_Phrases" name="Table_Phrases" id="10">
   <tableColumns count="7">
     <tableColumn name="N" id="1"/>
     <tableColumn name="PHRASE_ID" id="2"/>
@@ -1984,7 +2080,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A23:B29" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A23:B31" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="15">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_TYPE_ID" id="2"/>
@@ -1994,7 +2090,7 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A31:B33" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A33:B35" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="16">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ANIMATION_ID" id="2"/>
@@ -2004,7 +2100,7 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A35:B40" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A37:B42" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="17">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_FAMILY_TYPE_ID" id="2"/>
@@ -2014,7 +2110,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Events" name="Table_Events" id="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B6" displayName="Table_Events" name="Table_Events" id="18">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_ID" id="2"/>
@@ -2024,10 +2120,11 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B30" displayName="Table_EventsCombi" name="Table_EventsCombi" id="19">
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A8:C11" displayName="Table_Memento_Parent" name="Table_Memento_Parent" id="19">
+  <tableColumns count="3">
     <tableColumn name="N" id="1"/>
-    <tableColumn name="EVENT_COMBI_ID" id="2"/>
+    <tableColumn name="MEMENTO_PARENT_ID" id="2"/>
+    <tableColumn name="Sprite" id="3"/>
   </tableColumns>
   <tableStyleInfo name="EVENTS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -2056,7 +2153,31 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D26" displayName="Table_TODO" name="Table_TODO" id="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A13:F17" displayName="Table_Memento" name="Table_Memento" id="20">
+  <tableColumns count="6">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="MEMENTO_ID" id="2"/>
+    <tableColumn name="Parent" id="3"/>
+    <tableColumn name="Phrase" id="4"/>
+    <tableColumn name="Initial" id="5"/>
+    <tableColumn name="Final" id="6"/>
+  </tableColumns>
+  <tableStyleInfo name="EVENTS-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A19:B42" displayName="Table_EventsCombi" name="Table_EventsCombi" id="21">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="EVENT_COMBI_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="EVENTS-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D27" displayName="Table_TODO" name="Table_TODO" id="22">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -2067,8 +2188,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B128" displayName="Table_PickableSprites" name="Table_PickableSprites" id="21">
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B128" displayName="Table_PickableSprites" name="Table_PickableSprites" id="23">
   <tableColumns count="2">
     <tableColumn name="SPRITES" id="1"/>
     <tableColumn name="WORK" id="2"/>
@@ -2077,8 +2198,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="D1:E128" displayName="Table_PickableNames" name="Table_PickableNames" id="22">
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="D1:E128" displayName="Table_PickableNames" name="Table_PickableNames" id="24">
   <tableColumns count="2">
     <tableColumn name="NAMES" id="1"/>
     <tableColumn name="WORK" id="2"/>
@@ -2106,7 +2227,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A11:I15" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A11:I17" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="4">
   <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_ID" id="2"/>
@@ -3199,7 +3320,7 @@
         <v>21</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>21</v>
@@ -4293,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2">
@@ -4329,7 +4450,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6">
@@ -4341,7 +4462,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8">
@@ -4357,7 +4478,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10">
@@ -4373,7 +4494,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12">
@@ -4381,7 +4502,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13">
@@ -4389,7 +4510,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15">
@@ -4397,7 +4518,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16">
@@ -4415,7 +4536,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="18">
@@ -4424,7 +4545,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19">
@@ -4451,7 +4572,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23">
@@ -4459,7 +4580,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
     </row>
     <row r="24">
@@ -4468,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="25">
@@ -4477,7 +4598,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26">
@@ -4486,7 +4607,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27">
@@ -4495,7 +4616,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28">
@@ -4504,7 +4625,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29">
@@ -4513,84 +4634,102 @@
         <v>5</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>404</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="21">
+        <f>ROW()-ROW(Table_Unchain_Type[N])</f>
+        <v>6</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="21">
+        <f>ROW()-ROW(Table_Unchain_Type[N])</f>
+        <v>7</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="21">
+      <c r="B33" s="18" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="21">
         <v>0.0</v>
       </c>
-      <c r="B32" s="21" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="21">
+      <c r="B34" s="21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="21">
         <v>1.0</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="18" t="s">
+      <c r="B35" s="21" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="21">
-        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="21">
-        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>1</v>
-      </c>
       <c r="B37" s="18" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="21">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>2</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>256</v>
+        <v>0</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="21">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>266</v>
+        <v>418</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="21">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="21">
+        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="21">
+        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>4</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>249</v>
+      <c r="B42" s="18" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -4622,8 +4761,8 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="35.43"/>
     <col customWidth="1" min="3" max="3" width="43.0"/>
-    <col customWidth="1" min="4" max="4" width="15.29"/>
-    <col customWidth="1" min="6" max="6" width="18.57"/>
+    <col customWidth="1" min="4" max="4" width="36.43"/>
+    <col customWidth="1" min="5" max="6" width="10.0"/>
     <col customWidth="1" min="7" max="7" width="21.71"/>
   </cols>
   <sheetData>
@@ -4632,12 +4771,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21">
-        <f t="shared" ref="A2:A5" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A6" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -4659,7 +4798,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5">
@@ -4668,207 +4807,380 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="21">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="40">
+      <c r="B8" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="21">
+        <f>ROW()-ROW(Table_Memento_Parent[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="21">
+        <f>ROW()-ROW(Table_Memento_Parent[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="21">
+        <f>ROW()-ROW(Table_Memento_Parent[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>427</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>428</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>429</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="21">
+        <f>ROW()-ROW(Table_Memento[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="21">
+        <f>ROW()-ROW(Table_Memento[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="E15" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="21">
+        <f>ROW()-ROW(Table_Memento[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="E16" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="21">
+        <f>ROW()-ROW(Table_Memento[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>0</v>
       </c>
-      <c r="B8" s="41" t="str">
+      <c r="B20" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(FLATTEN(Table_Events[EVENT_ID],""(NOT)""&amp;Table_Events[EVENT_ID]))"),"EVENT_NONE")</f>
         <v>EVENT_NONE</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="40">
+    <row r="21">
+      <c r="A21" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>1</v>
       </c>
-      <c r="B9" s="41" t="str">
+      <c r="B21" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_RED_POTION_TOOK")</f>
         <v>EVENT_RED_POTION_TOOK</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="40">
+    <row r="22">
+      <c r="A22" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="str">
+      <c r="B22" s="43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_BLUE_POTION_TOOK")</f>
+        <v>EVENT_BLUE_POTION_TOOK</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="42">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B23" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_FOUNTAIN_FULL")</f>
         <v>EVENT_FOUNTAIN_FULL</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="40">
+    <row r="24">
+      <c r="A24" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>3</v>
-      </c>
-      <c r="B11" s="41" t="str">
+        <v>4</v>
+      </c>
+      <c r="B24" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAST")</f>
         <v>EVENT_LAST</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="40">
+    <row r="25">
+      <c r="A25" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>4</v>
-      </c>
-      <c r="B12" s="41" t="str">
+        <v>5</v>
+      </c>
+      <c r="B25" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_NONE")</f>
         <v>(NOT)EVENT_NONE</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="40">
+    <row r="26">
+      <c r="A26" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>5</v>
-      </c>
-      <c r="B13" s="41" t="str">
+        <v>6</v>
+      </c>
+      <c r="B26" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_RED_POTION_TOOK")</f>
         <v>(NOT)EVENT_RED_POTION_TOOK</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="40">
+    <row r="27">
+      <c r="A27" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>6</v>
-      </c>
-      <c r="B14" s="41" t="str">
+        <v>7</v>
+      </c>
+      <c r="B27" s="43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_BLUE_POTION_TOOK")</f>
+        <v>(NOT)EVENT_BLUE_POTION_TOOK</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="42">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>8</v>
+      </c>
+      <c r="B28" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_FOUNTAIN_FULL")</f>
         <v>(NOT)EVENT_FOUNTAIN_FULL</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="40">
+    <row r="29">
+      <c r="A29" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>7</v>
-      </c>
-      <c r="B15" s="41" t="str">
+        <v>9</v>
+      </c>
+      <c r="B29" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAST")</f>
         <v>(NOT)EVENT_LAST</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="40">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>8</v>
-      </c>
-      <c r="B16" s="41"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="40">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>9</v>
-      </c>
-      <c r="B17" s="41"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="40">
+    <row r="30">
+      <c r="A30" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>10</v>
       </c>
-      <c r="B18" s="41"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="40">
+      <c r="B30" s="43"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>11</v>
       </c>
-      <c r="B19" s="41"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="40">
+      <c r="B31" s="43"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>12</v>
       </c>
-      <c r="B20" s="41"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="40">
+      <c r="B32" s="43"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>13</v>
       </c>
-      <c r="B21" s="41"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="40">
+      <c r="B33" s="43"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>14</v>
       </c>
-      <c r="B22" s="41"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="40">
+      <c r="B34" s="43"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>15</v>
       </c>
-      <c r="B23" s="41"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="40">
+      <c r="B35" s="43"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>16</v>
       </c>
-      <c r="B24" s="41"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="40">
+      <c r="B36" s="43"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>17</v>
       </c>
-      <c r="B25" s="41"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="40">
+      <c r="B37" s="43"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>18</v>
       </c>
-      <c r="B26" s="41"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="40">
+      <c r="B38" s="43"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>19</v>
       </c>
-      <c r="B27" s="41"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="40">
+      <c r="B39" s="43"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>20</v>
       </c>
-      <c r="B28" s="41"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="40">
+      <c r="B40" s="43"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>21</v>
       </c>
-      <c r="B29" s="41"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="40">
+      <c r="B41" s="43"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="42">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>22</v>
       </c>
-      <c r="B30" s="41"/>
+      <c r="B42" s="43"/>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="C9:C11 C14:D17">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
+  <tableParts count="4">
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4892,10 +5204,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>411</v>
+        <v>436</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>412</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2">
@@ -4903,12 +5215,12 @@
         <f t="shared" ref="A2:A32" si="1">ROW()-ROW($G$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="42" t="str">
+      <c r="B2" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A2,0)</f>
         <v>ITEM_POTION</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
     </row>
     <row r="3">
@@ -4916,12 +5228,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="42" t="str">
+      <c r="B3" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A3,0)</f>
         <v>ITEM_POTION_BLUE</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4">
@@ -4929,12 +5241,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="42" t="str">
+      <c r="B4" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A4,0)</f>
         <v>ITEM_FOUNTAIN</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5">
@@ -4942,12 +5254,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="42" t="str">
+      <c r="B5" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A5,0)</f>
         <v>ITEM_NPC_MILITO</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6">
@@ -4955,297 +5267,297 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="42" t="str">
+      <c r="B6" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A6,0)</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="44"/>
     </row>
     <row r="7">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="42" t="str">
+      <c r="B7" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A7,0)</f>
         <v/>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="44"/>
     </row>
     <row r="8">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="str">
+      <c r="B8" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A8,0)</f>
         <v/>
       </c>
-      <c r="C8" s="42"/>
+      <c r="C8" s="44"/>
     </row>
     <row r="9">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="42" t="str">
+      <c r="B9" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A9,0)</f>
         <v/>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="44"/>
     </row>
     <row r="10">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="42" t="str">
+      <c r="B10" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A10,0)</f>
         <v/>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="44"/>
     </row>
     <row r="11">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="42" t="str">
+      <c r="B11" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A11,0)</f>
         <v/>
       </c>
-      <c r="C11" s="42"/>
+      <c r="C11" s="44"/>
     </row>
     <row r="12">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="42" t="str">
+      <c r="B12" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A12,0)</f>
         <v/>
       </c>
-      <c r="C12" s="42"/>
+      <c r="C12" s="44"/>
     </row>
     <row r="13">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="42" t="str">
+      <c r="B13" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A13,0)</f>
         <v/>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="44"/>
     </row>
     <row r="14">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="42" t="str">
+      <c r="B14" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A14,0)</f>
         <v/>
       </c>
-      <c r="C14" s="42"/>
+      <c r="C14" s="44"/>
     </row>
     <row r="15">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="42" t="str">
+      <c r="B15" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A15,0)</f>
         <v/>
       </c>
-      <c r="C15" s="42"/>
+      <c r="C15" s="44"/>
     </row>
     <row r="16">
       <c r="A16" s="9">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="42" t="str">
+      <c r="B16" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A16,0)</f>
         <v/>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="44"/>
     </row>
     <row r="17">
       <c r="A17" s="9">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="42" t="str">
+      <c r="B17" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A17,0)</f>
         <v/>
       </c>
-      <c r="C17" s="42"/>
+      <c r="C17" s="44"/>
     </row>
     <row r="18">
       <c r="A18" s="9">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="42" t="str">
+      <c r="B18" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A18,0)</f>
         <v/>
       </c>
-      <c r="C18" s="42"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19">
       <c r="A19" s="9">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="42" t="str">
+      <c r="B19" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A19,0)</f>
         <v/>
       </c>
-      <c r="C19" s="42"/>
+      <c r="C19" s="44"/>
     </row>
     <row r="20">
       <c r="A20" s="9">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="42" t="str">
+      <c r="B20" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A20,0)</f>
         <v/>
       </c>
-      <c r="C20" s="42"/>
+      <c r="C20" s="44"/>
     </row>
     <row r="21">
       <c r="A21" s="9">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="42" t="str">
+      <c r="B21" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A21,0)</f>
         <v/>
       </c>
-      <c r="C21" s="42"/>
+      <c r="C21" s="44"/>
     </row>
     <row r="22">
       <c r="A22" s="9">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="42" t="str">
+      <c r="B22" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A22,0)</f>
         <v/>
       </c>
-      <c r="C22" s="42"/>
+      <c r="C22" s="44"/>
     </row>
     <row r="23">
       <c r="A23" s="9">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="42" t="str">
+      <c r="B23" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A23,0)</f>
         <v/>
       </c>
-      <c r="C23" s="42"/>
+      <c r="C23" s="44"/>
     </row>
     <row r="24">
       <c r="A24" s="9">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="42" t="str">
+      <c r="B24" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A24,0)</f>
         <v/>
       </c>
-      <c r="C24" s="42"/>
+      <c r="C24" s="44"/>
     </row>
     <row r="25">
       <c r="A25" s="9">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="42" t="str">
+      <c r="B25" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A25,0)</f>
         <v/>
       </c>
-      <c r="C25" s="42"/>
+      <c r="C25" s="44"/>
     </row>
     <row r="26">
       <c r="A26" s="9">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="42" t="str">
+      <c r="B26" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A26,0)</f>
         <v/>
       </c>
-      <c r="C26" s="42"/>
+      <c r="C26" s="44"/>
     </row>
     <row r="27">
       <c r="A27" s="9">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="42" t="str">
+      <c r="B27" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A27,0)</f>
         <v/>
       </c>
-      <c r="C27" s="42"/>
+      <c r="C27" s="44"/>
     </row>
     <row r="28">
       <c r="A28" s="9">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="42" t="str">
+      <c r="B28" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A28,0)</f>
         <v/>
       </c>
-      <c r="C28" s="42"/>
+      <c r="C28" s="44"/>
     </row>
     <row r="29">
       <c r="A29" s="9">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="42" t="str">
+      <c r="B29" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A29,0)</f>
         <v/>
       </c>
-      <c r="C29" s="42"/>
+      <c r="C29" s="44"/>
     </row>
     <row r="30">
       <c r="A30" s="9">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="42" t="str">
+      <c r="B30" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A30,0)</f>
         <v/>
       </c>
-      <c r="C30" s="42"/>
+      <c r="C30" s="44"/>
     </row>
     <row r="31">
       <c r="A31" s="9">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="42" t="str">
+      <c r="B31" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A31,0)</f>
         <v/>
       </c>
-      <c r="C31" s="42"/>
+      <c r="C31" s="44"/>
     </row>
     <row r="32">
       <c r="A32" s="9">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="42" t="str">
+      <c r="B32" s="44" t="str">
         <f>OFFSET(ITEMS!$B$6,A32,0)</f>
         <v/>
       </c>
-      <c r="C32" s="42"/>
+      <c r="C32" s="44"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -5278,23 +5590,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>415</v>
+        <v>440</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>416</v>
+        <v>441</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>417</v>
+        <v>442</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="B2" s="43">
+        <v>443</v>
+      </c>
+      <c r="B2" s="45">
         <v>1.0</v>
       </c>
       <c r="C2" s="21" t="b">
@@ -5306,9 +5618,9 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>419</v>
-      </c>
-      <c r="B3" s="43">
+        <v>444</v>
+      </c>
+      <c r="B3" s="45">
         <v>1.0</v>
       </c>
       <c r="C3" s="21" t="b">
@@ -5320,23 +5632,23 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>420</v>
-      </c>
-      <c r="B4" s="43">
+        <v>445</v>
+      </c>
+      <c r="B4" s="45">
         <v>3.0</v>
       </c>
       <c r="C4" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>421</v>
-      </c>
-      <c r="B5" s="43">
+        <v>446</v>
+      </c>
+      <c r="B5" s="45">
         <v>1.0</v>
       </c>
       <c r="C5" s="21" t="b">
@@ -5348,9 +5660,9 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>422</v>
-      </c>
-      <c r="B6" s="43">
+        <v>447</v>
+      </c>
+      <c r="B6" s="45">
         <v>3.0</v>
       </c>
       <c r="C6" s="21" t="b">
@@ -5362,9 +5674,9 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>423</v>
-      </c>
-      <c r="B7" s="43">
+        <v>448</v>
+      </c>
+      <c r="B7" s="45">
         <v>3.0</v>
       </c>
       <c r="C7" s="21" t="b">
@@ -5376,9 +5688,9 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="B8" s="43">
+        <v>449</v>
+      </c>
+      <c r="B8" s="45">
         <v>5.0</v>
       </c>
       <c r="C8" s="21" t="b">
@@ -5390,9 +5702,9 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>425</v>
-      </c>
-      <c r="B9" s="43">
+        <v>450</v>
+      </c>
+      <c r="B9" s="45">
         <v>4.0</v>
       </c>
       <c r="C9" s="21" t="b">
@@ -5404,9 +5716,9 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>426</v>
-      </c>
-      <c r="B10" s="43">
+        <v>451</v>
+      </c>
+      <c r="B10" s="45">
         <v>4.0</v>
       </c>
       <c r="C10" s="21" t="b">
@@ -5418,9 +5730,9 @@
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>427</v>
-      </c>
-      <c r="B11" s="43">
+        <v>452</v>
+      </c>
+      <c r="B11" s="45">
         <v>1.0</v>
       </c>
       <c r="C11" s="21" t="b">
@@ -5432,9 +5744,9 @@
     </row>
     <row r="12">
       <c r="A12" s="21" t="s">
-        <v>428</v>
-      </c>
-      <c r="B12" s="43">
+        <v>453</v>
+      </c>
+      <c r="B12" s="45">
         <v>4.0</v>
       </c>
       <c r="C12" s="21" t="b">
@@ -5446,9 +5758,9 @@
     </row>
     <row r="13">
       <c r="A13" s="21" t="s">
-        <v>429</v>
-      </c>
-      <c r="B13" s="43">
+        <v>454</v>
+      </c>
+      <c r="B13" s="45">
         <v>1.0</v>
       </c>
       <c r="C13" s="21" t="b">
@@ -5460,9 +5772,9 @@
     </row>
     <row r="14">
       <c r="A14" s="21" t="s">
-        <v>430</v>
-      </c>
-      <c r="B14" s="43">
+        <v>455</v>
+      </c>
+      <c r="B14" s="45">
         <v>2.0</v>
       </c>
       <c r="C14" s="21" t="b">
@@ -5474,9 +5786,9 @@
     </row>
     <row r="15">
       <c r="A15" s="21" t="s">
-        <v>431</v>
-      </c>
-      <c r="B15" s="43">
+        <v>456</v>
+      </c>
+      <c r="B15" s="45">
         <v>3.0</v>
       </c>
       <c r="C15" s="21" t="b">
@@ -5488,9 +5800,9 @@
     </row>
     <row r="16">
       <c r="A16" s="21" t="s">
-        <v>432</v>
-      </c>
-      <c r="B16" s="43">
+        <v>457</v>
+      </c>
+      <c r="B16" s="45">
         <v>2.0</v>
       </c>
       <c r="C16" s="21" t="b">
@@ -5502,9 +5814,9 @@
     </row>
     <row r="17">
       <c r="A17" s="21" t="s">
-        <v>433</v>
-      </c>
-      <c r="B17" s="43">
+        <v>458</v>
+      </c>
+      <c r="B17" s="45">
         <v>2.0</v>
       </c>
       <c r="C17" s="21" t="b">
@@ -5516,9 +5828,9 @@
     </row>
     <row r="18">
       <c r="A18" s="21" t="s">
-        <v>434</v>
-      </c>
-      <c r="B18" s="43">
+        <v>459</v>
+      </c>
+      <c r="B18" s="45">
         <v>2.0</v>
       </c>
       <c r="C18" s="21" t="b">
@@ -5530,9 +5842,9 @@
     </row>
     <row r="19">
       <c r="A19" s="21" t="s">
-        <v>435</v>
-      </c>
-      <c r="B19" s="43">
+        <v>460</v>
+      </c>
+      <c r="B19" s="45">
         <v>2.0</v>
       </c>
       <c r="C19" s="21" t="b">
@@ -5544,9 +5856,9 @@
     </row>
     <row r="20">
       <c r="A20" s="21" t="s">
-        <v>436</v>
-      </c>
-      <c r="B20" s="43">
+        <v>461</v>
+      </c>
+      <c r="B20" s="45">
         <v>3.0</v>
       </c>
       <c r="C20" s="21" t="b">
@@ -5558,9 +5870,9 @@
     </row>
     <row r="21">
       <c r="A21" s="21" t="s">
-        <v>437</v>
-      </c>
-      <c r="B21" s="43">
+        <v>462</v>
+      </c>
+      <c r="B21" s="45">
         <v>2.0</v>
       </c>
       <c r="C21" s="21" t="b">
@@ -5572,9 +5884,9 @@
     </row>
     <row r="22">
       <c r="A22" s="21" t="s">
-        <v>438</v>
-      </c>
-      <c r="B22" s="43">
+        <v>463</v>
+      </c>
+      <c r="B22" s="45">
         <v>2.0</v>
       </c>
       <c r="C22" s="21" t="b">
@@ -5586,9 +5898,9 @@
     </row>
     <row r="23">
       <c r="A23" s="21" t="s">
-        <v>439</v>
-      </c>
-      <c r="B23" s="43">
+        <v>464</v>
+      </c>
+      <c r="B23" s="45">
         <v>2.0</v>
       </c>
       <c r="C23" s="21" t="b">
@@ -5600,9 +5912,9 @@
     </row>
     <row r="24">
       <c r="A24" s="21" t="s">
-        <v>440</v>
-      </c>
-      <c r="B24" s="43">
+        <v>465</v>
+      </c>
+      <c r="B24" s="45">
         <v>2.0</v>
       </c>
       <c r="C24" s="21" t="b">
@@ -5614,34 +5926,48 @@
     </row>
     <row r="25">
       <c r="A25" s="21" t="s">
-        <v>441</v>
-      </c>
-      <c r="B25" s="43">
+        <v>466</v>
+      </c>
+      <c r="B25" s="45">
         <v>2.0</v>
       </c>
       <c r="C25" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="21" t="s">
-        <v>347</v>
-      </c>
-      <c r="B26" s="43">
+        <v>467</v>
+      </c>
+      <c r="B26" s="45">
+        <v>2.0</v>
+      </c>
+      <c r="C26" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="B27" s="45">
         <v>5.0</v>
       </c>
-      <c r="C26" s="21" t="b">
+      <c r="C27" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="D26" s="21" t="b">
+      <c r="D27" s="21" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B26">
+  <conditionalFormatting sqref="B2:B27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="1"/>
@@ -5653,13 +5979,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A26">
+  <conditionalFormatting sqref="A2:A27">
     <cfRule type="expression" dxfId="5" priority="2">
       <formula>$C2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B26">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B27">
       <formula1>AND(ISNUMBER(B2),(NOT(OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -5689,110 +6015,228 @@
     <col customWidth="1" min="4" max="5" width="23.71"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="44" t="s">
-        <v>442</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>443</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>444</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="45" t="str">
+    <row r="1" ht="22.5" customHeight="1">
+      <c r="A1" s="46" t="s">
+        <v>468</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>470</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" ht="22.5" customHeight="1">
+      <c r="A2" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"SPRITE_POTION_RED")</f>
         <v>SPRITE_POTION_RED</v>
       </c>
-      <c r="B2" s="45" t="str">
+      <c r="B2" s="47" t="str">
         <f t="array" ref="B2:B10">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
         <v/>
       </c>
-      <c r="D2" s="45" t="str">
+      <c r="D2" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"NAME_ITEM_POTION")</f>
         <v>NAME_ITEM_POTION</v>
       </c>
-      <c r="E2" s="45" t="str">
+      <c r="E2" s="47" t="str">
         <f t="array" ref="E2:E10">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
         <v/>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="45" t="str">
+    <row r="3" ht="22.5" customHeight="1">
+      <c r="A3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_POTION_BLUE")</f>
         <v>SPRITE_POTION_BLUE</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="45" t="str">
+      <c r="D3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_BLUE_POTION")</f>
         <v>NAME_ITEM_BLUE_POTION</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="45" t="s">
+    <row r="4" ht="22.5" customHeight="1">
+      <c r="B4" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="45" t="s">
+    <row r="5" ht="22.5" customHeight="1">
+      <c r="B5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="45" t="s">
-        <v>259</v>
-      </c>
-      <c r="E7" s="45" t="s">
+    <row r="6" ht="22.5" customHeight="1">
+      <c r="B6" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" s="47" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" s="45" t="s">
+    <row r="7" ht="22.5" customHeight="1">
+      <c r="B7" s="47" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" ht="22.5" customHeight="1">
+      <c r="B8" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="45" t="s">
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="B9" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" s="45" t="s">
+    <row r="10" ht="22.5" customHeight="1">
+      <c r="B10" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="47" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="11" ht="22.5" customHeight="1"/>
+    <row r="12" ht="22.5" customHeight="1"/>
+    <row r="13" ht="22.5" customHeight="1"/>
+    <row r="14" ht="22.5" customHeight="1"/>
+    <row r="15" ht="22.5" customHeight="1"/>
+    <row r="16" ht="22.5" customHeight="1"/>
+    <row r="17" ht="22.5" customHeight="1"/>
+    <row r="18" ht="22.5" customHeight="1"/>
+    <row r="19" ht="22.5" customHeight="1"/>
+    <row r="20" ht="22.5" customHeight="1"/>
+    <row r="21" ht="22.5" customHeight="1"/>
+    <row r="22" ht="22.5" customHeight="1"/>
+    <row r="23" ht="22.5" customHeight="1"/>
+    <row r="24" ht="22.5" customHeight="1"/>
+    <row r="25" ht="22.5" customHeight="1"/>
+    <row r="26" ht="22.5" customHeight="1"/>
+    <row r="27" ht="22.5" customHeight="1"/>
+    <row r="28" ht="22.5" customHeight="1"/>
+    <row r="29" ht="22.5" customHeight="1"/>
+    <row r="30" ht="22.5" customHeight="1"/>
+    <row r="31" ht="22.5" customHeight="1"/>
+    <row r="32" ht="22.5" customHeight="1"/>
+    <row r="33" ht="22.5" customHeight="1"/>
+    <row r="34" ht="22.5" customHeight="1"/>
+    <row r="35" ht="22.5" customHeight="1"/>
+    <row r="36" ht="22.5" customHeight="1"/>
+    <row r="37" ht="22.5" customHeight="1"/>
+    <row r="38" ht="22.5" customHeight="1"/>
+    <row r="39" ht="22.5" customHeight="1"/>
+    <row r="40" ht="22.5" customHeight="1"/>
+    <row r="41" ht="22.5" customHeight="1"/>
+    <row r="42" ht="22.5" customHeight="1"/>
+    <row r="43" ht="22.5" customHeight="1"/>
+    <row r="44" ht="22.5" customHeight="1"/>
+    <row r="45" ht="22.5" customHeight="1"/>
+    <row r="46" ht="22.5" customHeight="1"/>
+    <row r="47" ht="22.5" customHeight="1"/>
+    <row r="48" ht="22.5" customHeight="1"/>
+    <row r="49" ht="22.5" customHeight="1"/>
+    <row r="50" ht="22.5" customHeight="1"/>
+    <row r="51" ht="22.5" customHeight="1"/>
+    <row r="52" ht="22.5" customHeight="1"/>
+    <row r="53" ht="22.5" customHeight="1"/>
+    <row r="54" ht="22.5" customHeight="1"/>
+    <row r="55" ht="22.5" customHeight="1"/>
+    <row r="56" ht="22.5" customHeight="1"/>
+    <row r="57" ht="22.5" customHeight="1"/>
+    <row r="58" ht="22.5" customHeight="1"/>
+    <row r="59" ht="22.5" customHeight="1"/>
+    <row r="60" ht="22.5" customHeight="1"/>
+    <row r="61" ht="22.5" customHeight="1"/>
+    <row r="62" ht="22.5" customHeight="1"/>
+    <row r="63" ht="22.5" customHeight="1"/>
+    <row r="64" ht="22.5" customHeight="1"/>
+    <row r="65" ht="22.5" customHeight="1"/>
+    <row r="66" ht="22.5" customHeight="1"/>
+    <row r="67" ht="22.5" customHeight="1"/>
+    <row r="68" ht="22.5" customHeight="1"/>
+    <row r="69" ht="22.5" customHeight="1"/>
+    <row r="70" ht="22.5" customHeight="1"/>
+    <row r="71" ht="22.5" customHeight="1"/>
+    <row r="72" ht="22.5" customHeight="1"/>
+    <row r="73" ht="22.5" customHeight="1"/>
+    <row r="74" ht="22.5" customHeight="1"/>
+    <row r="75" ht="22.5" customHeight="1"/>
+    <row r="76" ht="22.5" customHeight="1"/>
+    <row r="77" ht="22.5" customHeight="1"/>
+    <row r="78" ht="22.5" customHeight="1"/>
+    <row r="79" ht="22.5" customHeight="1"/>
+    <row r="80" ht="22.5" customHeight="1"/>
+    <row r="81" ht="22.5" customHeight="1"/>
+    <row r="82" ht="22.5" customHeight="1"/>
+    <row r="83" ht="22.5" customHeight="1"/>
+    <row r="84" ht="22.5" customHeight="1"/>
+    <row r="85" ht="22.5" customHeight="1"/>
+    <row r="86" ht="22.5" customHeight="1"/>
+    <row r="87" ht="22.5" customHeight="1"/>
+    <row r="88" ht="22.5" customHeight="1"/>
+    <row r="89" ht="22.5" customHeight="1"/>
+    <row r="90" ht="22.5" customHeight="1"/>
+    <row r="91" ht="22.5" customHeight="1"/>
+    <row r="92" ht="22.5" customHeight="1"/>
+    <row r="93" ht="22.5" customHeight="1"/>
+    <row r="94" ht="22.5" customHeight="1"/>
+    <row r="95" ht="22.5" customHeight="1"/>
+    <row r="96" ht="22.5" customHeight="1"/>
+    <row r="97" ht="22.5" customHeight="1"/>
+    <row r="98" ht="22.5" customHeight="1"/>
+    <row r="99" ht="22.5" customHeight="1"/>
+    <row r="100" ht="22.5" customHeight="1"/>
+    <row r="101" ht="22.5" customHeight="1"/>
+    <row r="102" ht="22.5" customHeight="1"/>
+    <row r="103" ht="22.5" customHeight="1"/>
+    <row r="104" ht="22.5" customHeight="1"/>
+    <row r="105" ht="22.5" customHeight="1"/>
+    <row r="106" ht="22.5" customHeight="1"/>
+    <row r="107" ht="22.5" customHeight="1"/>
+    <row r="108" ht="22.5" customHeight="1"/>
+    <row r="109" ht="22.5" customHeight="1"/>
+    <row r="110" ht="22.5" customHeight="1"/>
+    <row r="111" ht="22.5" customHeight="1"/>
+    <row r="112" ht="22.5" customHeight="1"/>
+    <row r="113" ht="22.5" customHeight="1"/>
+    <row r="114" ht="22.5" customHeight="1"/>
+    <row r="115" ht="22.5" customHeight="1"/>
+    <row r="116" ht="22.5" customHeight="1"/>
+    <row r="117" ht="22.5" customHeight="1"/>
+    <row r="118" ht="22.5" customHeight="1"/>
+    <row r="119" ht="22.5" customHeight="1"/>
+    <row r="120" ht="22.5" customHeight="1"/>
+    <row r="121" ht="22.5" customHeight="1"/>
+    <row r="122" ht="22.5" customHeight="1"/>
+    <row r="123" ht="22.5" customHeight="1"/>
+    <row r="124" ht="22.5" customHeight="1"/>
+    <row r="125" ht="22.5" customHeight="1"/>
+    <row r="126" ht="22.5" customHeight="1"/>
+    <row r="127" ht="22.5" customHeight="1"/>
+    <row r="128" ht="22.5" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="2">
@@ -6352,7 +6796,7 @@
         <v>21</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="N12" s="5" t="s">
         <v>21</v>
@@ -6392,10 +6836,10 @@
         <v>21</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="N13" s="5" t="s">
         <v>21</v>
@@ -7345,7 +7789,7 @@
         <v>194</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6">
@@ -7354,7 +7798,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>188</v>
@@ -7363,13 +7807,13 @@
         <v>196</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H6" s="23" t="s">
         <v>193</v>
@@ -7378,7 +7822,7 @@
         <v>194</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7">
@@ -7387,7 +7831,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>188</v>
@@ -7399,13 +7843,13 @@
         <v>206</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I7" s="23" t="s">
         <v>194</v>
@@ -7420,7 +7864,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>188</v>
@@ -7432,13 +7876,13 @@
         <v>190</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>201</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>194</v>
@@ -7453,7 +7897,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>188</v>
@@ -7485,28 +7929,28 @@
         <v>0</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>179</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12">
@@ -7515,10 +7959,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>188</v>
@@ -7527,10 +7971,10 @@
         <v>198</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>189</v>
@@ -7545,10 +7989,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>198</v>
@@ -7557,10 +8001,10 @@
         <v>198</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>196</v>
@@ -7575,22 +8019,22 @@
         <v>2</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>188</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="H14" s="28" t="s">
         <v>189</v>
@@ -7605,33 +8049,93 @@
         <v>3</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="I15" s="27" t="s">
         <v>188</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="21">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>4</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="21">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>5</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D12:D15">
+    <dataValidation type="list" allowBlank="1" sqref="D12:D17">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C9">
@@ -7640,10 +8144,10 @@
     <dataValidation type="list" allowBlank="1" sqref="H2:H9">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J9 E12:E15 I12:I15">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J9 E12:E17 I12:I17">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:G9 C12:C15 F12:H15">
+    <dataValidation type="list" allowBlank="1" sqref="D2:G9 C12:C17 F12:H17">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="I2:I9">
@@ -7689,28 +8193,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
@@ -7722,22 +8226,22 @@
         <v>190</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G2" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>187</v>
@@ -7749,25 +8253,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G3" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I3" s="34" t="s">
         <v>187</v>
@@ -7779,25 +8283,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C4" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="D4" s="31" t="s">
-        <v>249</v>
-      </c>
       <c r="E4" s="32" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G4" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I4" s="34" t="s">
         <v>187</v>
@@ -7809,25 +8313,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>250</v>
-      </c>
       <c r="F5" s="30" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G5" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I5" s="34" t="s">
         <v>187</v>
@@ -7839,28 +8343,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G6" s="33" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7">
@@ -7872,22 +8376,22 @@
         <v>206</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="G7" s="33" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="I7" s="34" t="s">
         <v>204</v>
@@ -7899,28 +8403,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="G8" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9">
@@ -7929,28 +8433,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G9" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I9" s="34" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10">
@@ -7959,25 +8463,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G10" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I10" s="34" t="s">
         <v>187</v>
@@ -8023,10 +8527,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2">
@@ -8035,7 +8539,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
@@ -8044,10 +8548,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4">
@@ -8056,10 +8560,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5">
@@ -8068,10 +8572,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6">
@@ -8080,10 +8584,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7">
@@ -8092,10 +8596,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8">
@@ -8104,10 +8608,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9">
@@ -8116,10 +8620,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10">
@@ -8128,10 +8632,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11">
@@ -8140,10 +8644,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12">
@@ -8152,10 +8656,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13">
@@ -8164,10 +8668,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14">
@@ -8176,10 +8680,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15">
@@ -8188,10 +8692,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16">
@@ -8200,10 +8704,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17">
@@ -8212,10 +8716,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -8254,13 +8758,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2">
@@ -8275,7 +8779,7 @@
         <v>190</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3">
@@ -8290,7 +8794,7 @@
         <v>190</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4">
@@ -8299,13 +8803,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>190</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5">
@@ -8314,13 +8818,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>190</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6">
@@ -8329,13 +8833,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>190</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8">
@@ -8343,19 +8847,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>179</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9">
@@ -8364,7 +8868,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>188</v>
@@ -8385,7 +8889,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>188</v>
@@ -8406,7 +8910,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>188</v>
@@ -8418,7 +8922,7 @@
         <v>193</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12">
@@ -8427,7 +8931,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>188</v>
@@ -8439,7 +8943,7 @@
         <v>193</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13">
@@ -8448,10 +8952,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>188</v>
@@ -8460,7 +8964,7 @@
         <v>193</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14">
@@ -8469,10 +8973,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>188</v>
@@ -8481,7 +8985,7 @@
         <v>193</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15">
@@ -8490,7 +8994,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>188</v>
@@ -8502,7 +9006,7 @@
         <v>193</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16">
@@ -8511,7 +9015,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>188</v>
@@ -8523,7 +9027,7 @@
         <v>193</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17">
@@ -8532,7 +9036,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>188</v>
@@ -8646,13 +9150,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2">
@@ -8661,7 +9165,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
@@ -8672,13 +9176,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4">
@@ -8687,13 +9191,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5">
@@ -8702,13 +9206,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6">
@@ -8717,13 +9221,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7">
@@ -8732,13 +9236,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8">
@@ -8747,13 +9251,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9">
@@ -8762,13 +9266,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10">
@@ -8777,13 +9281,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11">
@@ -8792,13 +9296,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12">
@@ -8807,13 +9311,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13">
@@ -8822,13 +9326,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -8865,22 +9369,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2">
@@ -8898,7 +9402,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="G2" s="21"/>
     </row>
@@ -8908,7 +9412,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C3" s="21">
         <v>0.0</v>
@@ -8917,13 +9421,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4">
@@ -8932,7 +9436,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C4" s="21">
         <v>0.0</v>
@@ -8941,13 +9445,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5">
@@ -8956,7 +9460,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C5" s="21">
         <v>0.0</v>
@@ -8965,13 +9469,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6">
@@ -8980,7 +9484,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C6" s="21">
         <v>0.0</v>
@@ -8989,13 +9493,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7">
@@ -9004,7 +9508,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C7" s="21">
         <v>0.0</v>
@@ -9013,13 +9517,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8">
@@ -9028,7 +9532,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C8" s="21">
         <v>0.0</v>
@@ -9037,13 +9541,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9">
@@ -9052,7 +9556,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C9" s="21">
         <v>0.0</v>
@@ -9061,13 +9565,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10">
@@ -9076,7 +9580,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C10" s="21">
         <v>0.0</v>
@@ -9085,13 +9589,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11">
@@ -9109,13 +9613,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12">
@@ -9124,7 +9628,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C12" s="21">
         <v>0.0</v>
@@ -9133,13 +9637,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13">
@@ -9148,7 +9652,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C13" s="21">
         <v>0.0</v>
@@ -9157,18 +9661,66 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>383</v>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="21">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>12</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>387</v>
+      </c>
+      <c r="C14" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="D14" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="21">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>390</v>
+      </c>
+      <c r="C15" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="D15" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E13">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E15">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -9207,25 +9759,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
@@ -9234,7 +9786,7 @@
         <v>-1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="C2" s="39" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9265,13 +9817,13 @@
         <v>ITEM_NONE</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G2" s="34" t="s">
         <v>190</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -9280,7 +9832,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="C3" s="39" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9311,13 +9863,13 @@
         <v>ITEM_POTION|ITEM_POTION_BLUE|ITEM_FOUNTAIN|ITEM_NPC_MILITO</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4">
@@ -9326,7 +9878,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C4" s="39" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -9357,13 +9909,13 @@
         <v>ITEM_LAST</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Memento Part 6 -Double click trigger
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -1494,7 +1494,7 @@
     <t>Memento2</t>
   </si>
   <si>
-    <t>TriggeredEvents</t>
+    <t>TriggeredEvent</t>
   </si>
   <si>
     <t>MEMENTO_COMBI_NONE</t>
@@ -2295,7 +2295,7 @@
     <tableColumn name="MEMENTO_COMBI_ID" id="2"/>
     <tableColumn name="Memento1" id="3"/>
     <tableColumn name="Memento2" id="4"/>
-    <tableColumn name="TriggeredEvents" id="5"/>
+    <tableColumn name="TriggeredEvent" id="5"/>
   </tableColumns>
   <tableStyleInfo name="EVENTS-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -5601,10 +5601,7 @@
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E26:E27">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C11:D14 C17:D23 C26:D27">
+    <dataValidation type="list" allowBlank="1" sqref="C11:D14 C17:D23 C26:E27">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Boost in Room loading -Pending GameEventManager to manage only items or to do everything at the beginning -Bug of name not loaded of MEMENTO_CHASE. Only happened once
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="1hvTGMjp64ENmBfCwPA3bZaIlReLpNavBHh+62leDQk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="+cumPAp/7fk/zp3OQ2CmVaZozmRfAsI72TWrj48Ox0Y="/>
     </ext>
   </extLst>
 </workbook>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="552">
   <si>
     <t>N</t>
   </si>
@@ -813,6 +813,42 @@
     <t>COND_ROOM1_NOT_CROSS_DOOR, COND_ROOM1_NOT_CROSS_MAIN_DOOR</t>
   </si>
   <si>
+    <t>ITEM_DOOR_UNCONDITIONAL</t>
+  </si>
+  <si>
+    <t>ITEM_ROOM1_SPOON</t>
+  </si>
+  <si>
+    <t>NAME_SPOON</t>
+  </si>
+  <si>
+    <t>ITEM_FAMILY_TYPE_OBJECT</t>
+  </si>
+  <si>
+    <t>SPRITE_ROOM1_SPOON</t>
+  </si>
+  <si>
+    <t>SPRITE_PICKABLE_SPOON</t>
+  </si>
+  <si>
+    <t>ITEM_ROOM1_DRAWER</t>
+  </si>
+  <si>
+    <t>NAME_DRAWER</t>
+  </si>
+  <si>
+    <t>SPRITE_ROOM1_DRAWER</t>
+  </si>
+  <si>
+    <t>ITEM_ROOM1_WINDOW</t>
+  </si>
+  <si>
+    <t>NAME_WINDOW</t>
+  </si>
+  <si>
+    <t>SPRITE_ROOM1_WINDOW_CLOSED</t>
+  </si>
+  <si>
     <t>ITEM_LAST</t>
   </si>
   <si>
@@ -984,7 +1020,7 @@
     <t>UNCHAIN_ROOM1_NEED_FLEE</t>
   </si>
   <si>
-    <t>EVENT_ROOM1_AWARE_CHASE_1, EVENT_ROOM1_AWARE_CHASE_2</t>
+    <t>EVENT_ROOM1_AWARE_CHASE_1, EVENT_ROOM1_AWARE_CHASE_2, EVENT_ROOM1_OBSERVE_VICTIM</t>
   </si>
   <si>
     <t>UNCHAIN_ROOM1_MEMENTO_CHASE_1</t>
@@ -1083,6 +1119,36 @@
     <t>SPRITE_ATLAS_UI_0[SPRITE_CURSOR_DOOR]</t>
   </si>
   <si>
+    <t>BACKGROUND_ROOM1_KITCHEN</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_ROOM1_2[BACKGROUND_ROOM1_KITCHEN]</t>
+  </si>
+  <si>
+    <t>SPRITE_ROOM1_KITCHEN_BASIN</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_ROOM1_2[SPRITE_ROOM1_KITCHEN_BASIN]</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_ROOM1_2[SPRITE_ROOM1_SPOON]</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_ROOM1_2[SPRITE_ROOM1_DRAWER]</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_ROOM1_2[SPRITE_ROOM1_WINDOW_CLOSED]</t>
+  </si>
+  <si>
+    <t>SPRITE_ROOM1_JAM</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_ROOM1_2[SPRITE_ROOM1_JAM]</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_PICKABLES_0[SPRITE_PICKABLE_SPOON]</t>
+  </si>
+  <si>
     <t>DIALOG_ID</t>
   </si>
   <si>
@@ -1215,6 +1281,24 @@
     <t>Cruzar puerta</t>
   </si>
   <si>
+    <t>Spoon</t>
+  </si>
+  <si>
+    <t>Cuchara</t>
+  </si>
+  <si>
+    <t>Drawer</t>
+  </si>
+  <si>
+    <t>Cajonera</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>Ventana</t>
+  </si>
+  <si>
     <t>Last</t>
   </si>
   <si>
@@ -1449,6 +1533,15 @@
     <t>ITEM_VICTIM, ITEM_WITNESS1, ITEM_WITNESS2, ITEM_WITNESS3, ITEM_ROOM1_DOOR_KITCHEN, ITEM_ROOM1_DOOR_MAIN</t>
   </si>
   <si>
+    <t>ROOM1_KITCHEN</t>
+  </si>
+  <si>
+    <t>BACKGROUND_ROOM1_KITCHEN, SPRITE_ROOM1_JAM, SPRITE_ROOM1_KITCHEN_BASIN</t>
+  </si>
+  <si>
+    <t>ITEM_ROOM1_SPOON, ITEM_ROOM1_DRAWER, ITEM_ROOM1_WINDOW, ITEM_DOOR_UNCONDITIONAL</t>
+  </si>
+  <si>
     <t>ROOM_LAST</t>
   </si>
   <si>
@@ -1513,9 +1606,6 @@
   </si>
   <si>
     <t>ITEM_FAMILY_TYPE_ID</t>
-  </si>
-  <si>
-    <t>ITEM_FAMILY_TYPE_OBJECT</t>
   </si>
   <si>
     <t>EVENT_ID</t>
@@ -2226,7 +2316,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H4" displayName="Table_Rooms" name="Table_Rooms" id="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H5" displayName="Table_Rooms" name="Table_Rooms" id="11">
   <tableColumns count="8">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
@@ -2414,7 +2504,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I12" displayName="Table_Items" name="Table_Items" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I16" displayName="Table_Items" name="Table_Items" id="3">
   <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_ID" id="2"/>
@@ -2467,7 +2557,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C19" displayName="Table_sprites" name="Table_sprites" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C26" displayName="Table_sprites" name="Table_sprites" id="6">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SPRITE_ID" id="2"/>
@@ -2504,7 +2594,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D14" displayName="Table_Name" name="Table_Name" id="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D17" displayName="Table_Name" name="Table_Name" id="9">
   <tableColumns count="4">
     <tableColumn name="N" id="1"/>
     <tableColumn name="NAME_ID" id="2"/>
@@ -3114,7 +3204,7 @@
       </c>
       <c r="E8" s="7">
         <f>COUNTIF(Table_Items[PICKABLE],"=TRUE")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>38</v>
@@ -4721,7 +4811,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>445</v>
+        <v>476</v>
       </c>
     </row>
     <row r="2">
@@ -4730,7 +4820,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3">
@@ -4739,7 +4829,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4">
@@ -4748,7 +4838,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>446</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5">
@@ -4757,7 +4847,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>447</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6">
@@ -4769,7 +4859,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8">
@@ -4777,7 +4867,7 @@
         <v>0.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9">
@@ -4785,7 +4875,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>449</v>
+        <v>480</v>
       </c>
     </row>
     <row r="10">
@@ -4793,7 +4883,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11">
@@ -4801,7 +4891,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12">
@@ -4809,7 +4899,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13">
@@ -4817,7 +4907,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
     </row>
     <row r="15">
@@ -4825,7 +4915,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>453</v>
+        <v>484</v>
       </c>
     </row>
     <row r="16">
@@ -4834,7 +4924,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17">
@@ -4843,7 +4933,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
     </row>
     <row r="18">
@@ -4852,7 +4942,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>455</v>
+        <v>486</v>
       </c>
     </row>
     <row r="19">
@@ -4861,7 +4951,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
     </row>
     <row r="20">
@@ -4870,7 +4960,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21">
@@ -4879,7 +4969,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22">
@@ -4888,7 +4978,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24">
@@ -4896,7 +4986,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>457</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25">
@@ -4905,7 +4995,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26">
@@ -4914,7 +5004,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
     </row>
     <row r="27">
@@ -4923,7 +5013,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
     </row>
     <row r="28">
@@ -4932,7 +5022,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>461</v>
+        <v>492</v>
       </c>
     </row>
     <row r="29">
@@ -4941,7 +5031,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
     </row>
     <row r="30">
@@ -4950,7 +5040,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31">
@@ -4959,7 +5049,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>463</v>
+        <v>494</v>
       </c>
     </row>
     <row r="32">
@@ -4968,7 +5058,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34">
@@ -4976,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
     </row>
     <row r="35">
@@ -4984,7 +5074,7 @@
         <v>0.0</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>374</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36">
@@ -4992,7 +5082,7 @@
         <v>1.0</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38">
@@ -5000,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>465</v>
+        <v>496</v>
       </c>
     </row>
     <row r="39">
@@ -5027,7 +5117,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>466</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42">
@@ -5088,7 +5178,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>467</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2">
@@ -5097,7 +5187,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
@@ -5106,7 +5196,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4">
@@ -5115,7 +5205,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5">
@@ -5124,7 +5214,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6">
@@ -5133,7 +5223,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7">
@@ -5142,7 +5232,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8">
@@ -5151,7 +5241,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>468</v>
+        <v>498</v>
       </c>
     </row>
     <row r="10">
@@ -5159,16 +5249,16 @@
         <v>0</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="C10" s="41" t="s">
         <v>193</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>470</v>
+        <v>500</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
     </row>
     <row r="11">
@@ -5177,7 +5267,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>472</v>
+        <v>502</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>201</v>
@@ -5196,10 +5286,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>473</v>
+        <v>503</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>215</v>
@@ -5215,13 +5305,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>474</v>
+        <v>504</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>361</v>
+        <v>383</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="E13" s="42" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B13,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_CHASE_0|MEMENTO_CHASE_1")</f>
@@ -5234,10 +5324,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>475</v>
+        <v>505</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>203</v>
@@ -5252,19 +5342,19 @@
         <v>0</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>476</v>
+        <v>506</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>477</v>
+        <v>507</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>478</v>
+        <v>508</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>479</v>
+        <v>509</v>
       </c>
       <c r="F16" s="43" t="s">
-        <v>480</v>
+        <v>510</v>
       </c>
     </row>
     <row r="17">
@@ -5273,16 +5363,16 @@
         <v>0</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>472</v>
+        <v>502</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="F17" s="45" t="b">
         <v>0</v>
@@ -5294,16 +5384,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>473</v>
+        <v>503</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="F18" s="45" t="b">
         <v>0</v>
@@ -5315,16 +5405,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>473</v>
+        <v>503</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>400</v>
+        <v>428</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="F19" s="45" t="b">
         <v>0</v>
@@ -5336,16 +5426,16 @@
         <v>3</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>474</v>
+        <v>504</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>423</v>
+        <v>451</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="F20" s="45" t="b">
         <v>0</v>
@@ -5357,16 +5447,16 @@
         <v>4</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>474</v>
+        <v>504</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>426</v>
+        <v>454</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="F21" s="45" t="b">
         <v>0</v>
@@ -5378,16 +5468,16 @@
         <v>5</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>482</v>
+        <v>512</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>475</v>
+        <v>505</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="F22" s="45" t="b">
         <v>0</v>
@@ -5398,10 +5488,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>483</v>
+        <v>513</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>484</v>
+        <v>514</v>
       </c>
     </row>
     <row r="25">
@@ -5410,10 +5500,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27">
@@ -5421,7 +5511,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>485</v>
+        <v>515</v>
       </c>
     </row>
     <row r="28">
@@ -5666,10 +5756,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>486</v>
+        <v>516</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>487</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2">
@@ -5682,7 +5772,7 @@
         <v>#REF!</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>488</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3">
@@ -5695,7 +5785,7 @@
         <v>#REF!</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>488</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4">
@@ -5708,7 +5798,7 @@
         <v>#REF!</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>488</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5">
@@ -5721,7 +5811,7 @@
         <v>#REF!</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>488</v>
+        <v>518</v>
       </c>
     </row>
     <row r="6">
@@ -6052,21 +6142,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>489</v>
+        <v>519</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>490</v>
+        <v>520</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>491</v>
+        <v>521</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>492</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>493</v>
+        <v>523</v>
       </c>
       <c r="B2" s="50">
         <v>1.0</v>
@@ -6080,7 +6170,7 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>494</v>
+        <v>524</v>
       </c>
       <c r="B3" s="50">
         <v>1.0</v>
@@ -6094,7 +6184,7 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>495</v>
+        <v>525</v>
       </c>
       <c r="B4" s="50">
         <v>3.0</v>
@@ -6108,7 +6198,7 @@
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>496</v>
+        <v>526</v>
       </c>
       <c r="B5" s="50">
         <v>1.0</v>
@@ -6122,7 +6212,7 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>497</v>
+        <v>527</v>
       </c>
       <c r="B6" s="50">
         <v>3.0</v>
@@ -6136,7 +6226,7 @@
     </row>
     <row r="7">
       <c r="A7" s="28" t="s">
-        <v>498</v>
+        <v>528</v>
       </c>
       <c r="B7" s="50">
         <v>3.0</v>
@@ -6150,7 +6240,7 @@
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>499</v>
+        <v>529</v>
       </c>
       <c r="B8" s="50">
         <v>5.0</v>
@@ -6164,7 +6254,7 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>500</v>
+        <v>530</v>
       </c>
       <c r="B9" s="50">
         <v>4.0</v>
@@ -6178,7 +6268,7 @@
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>501</v>
+        <v>531</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="28" t="b">
@@ -6190,7 +6280,7 @@
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>502</v>
+        <v>532</v>
       </c>
       <c r="B11" s="50">
         <v>4.0</v>
@@ -6204,7 +6294,7 @@
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
-        <v>503</v>
+        <v>533</v>
       </c>
       <c r="B12" s="50">
         <v>1.0</v>
@@ -6218,7 +6308,7 @@
     </row>
     <row r="13">
       <c r="A13" s="28" t="s">
-        <v>504</v>
+        <v>534</v>
       </c>
       <c r="B13" s="50">
         <v>4.0</v>
@@ -6232,7 +6322,7 @@
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
-        <v>505</v>
+        <v>535</v>
       </c>
       <c r="B14" s="50">
         <v>1.0</v>
@@ -6246,7 +6336,7 @@
     </row>
     <row r="15">
       <c r="A15" s="28" t="s">
-        <v>506</v>
+        <v>536</v>
       </c>
       <c r="B15" s="50">
         <v>2.0</v>
@@ -6260,7 +6350,7 @@
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
-        <v>507</v>
+        <v>537</v>
       </c>
       <c r="B16" s="50">
         <v>3.0</v>
@@ -6274,7 +6364,7 @@
     </row>
     <row r="17">
       <c r="A17" s="28" t="s">
-        <v>508</v>
+        <v>538</v>
       </c>
       <c r="B17" s="50">
         <v>2.0</v>
@@ -6288,7 +6378,7 @@
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
-        <v>509</v>
+        <v>539</v>
       </c>
       <c r="B18" s="50">
         <v>2.0</v>
@@ -6302,7 +6392,7 @@
     </row>
     <row r="19">
       <c r="A19" s="28" t="s">
-        <v>510</v>
+        <v>540</v>
       </c>
       <c r="B19" s="50">
         <v>2.0</v>
@@ -6316,7 +6406,7 @@
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
-        <v>511</v>
+        <v>541</v>
       </c>
       <c r="B20" s="50">
         <v>2.0</v>
@@ -6330,7 +6420,7 @@
     </row>
     <row r="21">
       <c r="A21" s="28" t="s">
-        <v>512</v>
+        <v>542</v>
       </c>
       <c r="B21" s="50">
         <v>3.0</v>
@@ -6344,7 +6434,7 @@
     </row>
     <row r="22">
       <c r="A22" s="28" t="s">
-        <v>513</v>
+        <v>543</v>
       </c>
       <c r="B22" s="50">
         <v>2.0</v>
@@ -6358,7 +6448,7 @@
     </row>
     <row r="23">
       <c r="A23" s="28" t="s">
-        <v>514</v>
+        <v>544</v>
       </c>
       <c r="B23" s="50">
         <v>2.0</v>
@@ -6372,7 +6462,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>515</v>
+        <v>545</v>
       </c>
       <c r="B24" s="50">
         <v>2.0</v>
@@ -6386,7 +6476,7 @@
     </row>
     <row r="25">
       <c r="A25" s="28" t="s">
-        <v>516</v>
+        <v>546</v>
       </c>
       <c r="B25" s="50">
         <v>2.0</v>
@@ -6400,7 +6490,7 @@
     </row>
     <row r="26">
       <c r="A26" s="28" t="s">
-        <v>517</v>
+        <v>547</v>
       </c>
       <c r="B26" s="50">
         <v>2.0</v>
@@ -6414,7 +6504,7 @@
     </row>
     <row r="27">
       <c r="A27" s="28" t="s">
-        <v>518</v>
+        <v>548</v>
       </c>
       <c r="B27" s="50">
         <v>2.0</v>
@@ -6428,7 +6518,7 @@
     </row>
     <row r="28">
       <c r="A28" s="28" t="s">
-        <v>366</v>
+        <v>394</v>
       </c>
       <c r="B28" s="50">
         <v>5.0</v>
@@ -6491,33 +6581,33 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="51" t="s">
-        <v>519</v>
+        <v>549</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>520</v>
+        <v>550</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>521</v>
+        <v>551</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>520</v>
+        <v>550</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
       <c r="A2" s="52" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"#N/A")</f>
-        <v>#N/A</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"SPRITE_PICKABLE_SPOON")</f>
+        <v>SPRITE_PICKABLE_SPOON</v>
       </c>
       <c r="B2" s="52" t="str">
-        <f t="array" ref="B2:B12">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
+        <f t="array" ref="B2:B16">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
         <v/>
       </c>
       <c r="D2" s="52" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"#N/A")</f>
-        <v>#N/A</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"NAME_SPOON")</f>
+        <v>NAME_SPOON</v>
       </c>
       <c r="E2" s="52" t="str">
-        <f t="array" ref="E2:E12">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
+        <f t="array" ref="E2:E16">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
         <v/>
       </c>
     </row>
@@ -6601,10 +6691,38 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" ht="22.5" customHeight="1"/>
-    <row r="14" ht="22.5" customHeight="1"/>
-    <row r="15" ht="22.5" customHeight="1"/>
-    <row r="16" ht="22.5" customHeight="1"/>
+    <row r="13" ht="22.5" customHeight="1">
+      <c r="B13" s="52" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" ht="22.5" customHeight="1">
+      <c r="B14" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" ht="22.5" customHeight="1">
+      <c r="B15" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" ht="22.5" customHeight="1">
+      <c r="B16" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="17" ht="22.5" customHeight="1"/>
     <row r="18" ht="22.5" customHeight="1"/>
     <row r="19" ht="22.5" customHeight="1"/>
@@ -8295,7 +8413,7 @@
     </row>
     <row r="2">
       <c r="A2" s="22">
-        <f t="shared" ref="A2:A12" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A16" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -8602,16 +8720,16 @@
         <v>232</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="G12" s="26" t="b">
         <v>0</v>
@@ -8623,12 +8741,132 @@
         <v>204</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="22">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="G13" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="22">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="G14" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="22">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="22">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="G16" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E12 I2:I12">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E16 I2:I16">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:D12 F2:F12 H2:H12">
+    <dataValidation type="list" allowBlank="1" sqref="C2:D16 F2:F16 H2:H16">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -8673,31 +8911,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2">
@@ -8709,28 +8947,28 @@
         <v>204</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>200</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
@@ -8742,28 +8980,28 @@
         <v>216</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>200</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
@@ -8775,28 +9013,28 @@
         <v>220</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>200</v>
       </c>
       <c r="F4" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="J4" s="33" t="s">
         <v>256</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="5">
@@ -8808,28 +9046,28 @@
         <v>223</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>200</v>
       </c>
       <c r="F5" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="J5" s="33" t="s">
         <v>256</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="6">
@@ -8841,28 +9079,28 @@
         <v>229</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>200</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7">
@@ -8871,31 +9109,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>262</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>250</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>200</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="J7" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8">
@@ -8904,31 +9142,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>200</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10">
@@ -8936,31 +9174,31 @@
         <v>0</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11">
@@ -8969,16 +9207,16 @@
         <v>0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="F11" s="34" t="s">
         <v>200</v>
@@ -8987,13 +9225,13 @@
         <v>203</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="J11" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12">
@@ -9002,16 +9240,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>200</v>
@@ -9020,13 +9258,13 @@
         <v>203</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="J12" s="33" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13">
@@ -9035,16 +9273,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="F13" s="34" t="s">
         <v>200</v>
@@ -9053,13 +9291,13 @@
         <v>203</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14">
@@ -9068,16 +9306,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>200</v>
@@ -9086,13 +9324,13 @@
         <v>203</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15">
@@ -9101,16 +9339,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>200</v>
@@ -9119,13 +9357,13 @@
         <v>203</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16">
@@ -9134,16 +9372,16 @@
         <v>5</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="F16" s="34" t="s">
         <v>200</v>
@@ -9152,13 +9390,13 @@
         <v>203</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17">
@@ -9167,16 +9405,16 @@
         <v>6</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="C17" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="D17" s="34" t="s">
-        <v>263</v>
-      </c>
       <c r="E17" s="33" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>200</v>
@@ -9185,13 +9423,13 @@
         <v>203</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -9237,7 +9475,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="28.29"/>
+    <col customWidth="1" min="2" max="2" width="34.29"/>
     <col customWidth="1" min="3" max="3" width="73.0"/>
     <col customWidth="1" min="4" max="4" width="26.0"/>
   </cols>
@@ -9247,10 +9485,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2">
@@ -9268,10 +9506,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4">
@@ -9280,10 +9518,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5">
@@ -9292,10 +9530,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6">
@@ -9304,10 +9542,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7">
@@ -9316,10 +9554,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8">
@@ -9328,10 +9566,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9">
@@ -9340,10 +9578,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10">
@@ -9352,10 +9590,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11">
@@ -9364,10 +9602,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12">
@@ -9379,7 +9617,7 @@
         <v>215</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13">
@@ -9391,7 +9629,7 @@
         <v>219</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14">
@@ -9403,7 +9641,7 @@
         <v>222</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15">
@@ -9415,7 +9653,7 @@
         <v>225</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16">
@@ -9424,10 +9662,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17">
@@ -9436,10 +9674,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18">
@@ -9448,10 +9686,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19">
@@ -9460,10 +9698,94 @@
         <v>17</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>234</v>
+        <v>334</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>234</v>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>18</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>19</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>20</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>21</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>22</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>23</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>24</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -9502,13 +9824,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>322</v>
+        <v>344</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>323</v>
+        <v>345</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>324</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2">
@@ -9517,13 +9839,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>200</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3">
@@ -9532,13 +9854,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>200</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4">
@@ -9547,13 +9869,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>200</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5">
@@ -9562,13 +9884,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>200</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>328</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6">
@@ -9577,13 +9899,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>329</v>
+        <v>351</v>
       </c>
       <c r="C6" s="33" t="s">
         <v>200</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8">
@@ -9591,19 +9913,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>330</v>
+        <v>352</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>331</v>
+        <v>353</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>332</v>
+        <v>354</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>333</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9">
@@ -9612,19 +9934,19 @@
         <v>0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10">
@@ -9633,19 +9955,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11">
@@ -9654,19 +9976,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12">
@@ -9675,19 +9997,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>328</v>
+        <v>350</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>335</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13">
@@ -9696,19 +10018,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>336</v>
+        <v>358</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15">
@@ -9810,13 +10132,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>337</v>
+        <v>359</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>338</v>
+        <v>360</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2">
@@ -9839,10 +10161,10 @@
         <v>206</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4">
@@ -9854,10 +10176,10 @@
         <v>209</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>341</v>
+        <v>363</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>342</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5">
@@ -9869,10 +10191,10 @@
         <v>211</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6">
@@ -9881,13 +10203,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7">
@@ -9896,13 +10218,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>348</v>
+        <v>370</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>350</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8">
@@ -9911,13 +10233,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>352</v>
+        <v>374</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9">
@@ -9926,13 +10248,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>355</v>
+        <v>377</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>356</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10">
@@ -9944,10 +10266,10 @@
         <v>213</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>358</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11">
@@ -9959,10 +10281,10 @@
         <v>218</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>359</v>
+        <v>381</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>360</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12">
@@ -9971,13 +10293,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>361</v>
+        <v>383</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>362</v>
+        <v>384</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>363</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13">
@@ -9989,10 +10311,10 @@
         <v>227</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>364</v>
+        <v>386</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>365</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14">
@@ -10001,13 +10323,58 @@
         <v>12</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>367</v>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="22">
+        <f>ROW()-ROW(Table_Name[NAME_ID])</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>390</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="22">
+        <f>ROW()-ROW(Table_Name[NAME_ID])</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="22">
+        <f>ROW()-ROW(Table_Name[NAME_ID])</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -10044,22 +10411,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>368</v>
+        <v>396</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>369</v>
+        <v>397</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>370</v>
+        <v>398</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>371</v>
+        <v>399</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>372</v>
+        <v>400</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>373</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2">
@@ -10068,7 +10435,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="C2" s="28">
         <v>0.0</v>
@@ -10077,7 +10444,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>374</v>
+        <v>402</v>
       </c>
       <c r="G2" s="28"/>
     </row>
@@ -10087,7 +10454,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>375</v>
+        <v>403</v>
       </c>
       <c r="C3" s="28">
         <v>0.0</v>
@@ -10096,13 +10463,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>377</v>
+        <v>405</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>378</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4">
@@ -10111,7 +10478,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>379</v>
+        <v>407</v>
       </c>
       <c r="C4" s="28">
         <v>0.0</v>
@@ -10120,13 +10487,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>380</v>
+        <v>408</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>381</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5">
@@ -10135,7 +10502,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>382</v>
+        <v>410</v>
       </c>
       <c r="C5" s="28">
         <v>0.0</v>
@@ -10144,13 +10511,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>383</v>
+        <v>411</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>384</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6">
@@ -10159,7 +10526,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>385</v>
+        <v>413</v>
       </c>
       <c r="C6" s="28">
         <v>0.0</v>
@@ -10168,13 +10535,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>386</v>
+        <v>414</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>387</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7">
@@ -10183,7 +10550,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>388</v>
+        <v>416</v>
       </c>
       <c r="C7" s="28">
         <v>0.0</v>
@@ -10192,13 +10559,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>389</v>
+        <v>417</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>390</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8">
@@ -10207,7 +10574,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>391</v>
+        <v>419</v>
       </c>
       <c r="C8" s="28">
         <v>0.0</v>
@@ -10216,13 +10583,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>392</v>
+        <v>420</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>393</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9">
@@ -10231,7 +10598,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>394</v>
+        <v>422</v>
       </c>
       <c r="C9" s="28">
         <v>0.0</v>
@@ -10240,13 +10607,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>395</v>
+        <v>423</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>396</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10">
@@ -10255,7 +10622,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
       <c r="C10" s="28">
         <v>0.0</v>
@@ -10264,13 +10631,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>374</v>
+        <v>402</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>398</v>
+        <v>426</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>399</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11">
@@ -10279,7 +10646,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>400</v>
+        <v>428</v>
       </c>
       <c r="C11" s="28">
         <v>0.0</v>
@@ -10288,13 +10655,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>374</v>
+        <v>402</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>401</v>
+        <v>429</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>402</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12">
@@ -10303,7 +10670,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="C12" s="28">
         <v>0.0</v>
@@ -10312,13 +10679,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>403</v>
+        <v>431</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>404</v>
+        <v>432</v>
       </c>
     </row>
     <row r="13">
@@ -10327,7 +10694,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>405</v>
+        <v>433</v>
       </c>
       <c r="C13" s="28">
         <v>0.0</v>
@@ -10336,13 +10703,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>406</v>
+        <v>434</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>407</v>
+        <v>435</v>
       </c>
     </row>
     <row r="14">
@@ -10351,7 +10718,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>408</v>
+        <v>436</v>
       </c>
       <c r="C14" s="28">
         <v>1.0</v>
@@ -10360,13 +10727,13 @@
         <v>0.0</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>409</v>
+        <v>437</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>410</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15">
@@ -10375,7 +10742,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>411</v>
+        <v>439</v>
       </c>
       <c r="C15" s="28">
         <v>0.0</v>
@@ -10384,13 +10751,13 @@
         <v>0.0</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>412</v>
+        <v>440</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>413</v>
+        <v>441</v>
       </c>
     </row>
     <row r="16">
@@ -10399,7 +10766,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>414</v>
+        <v>442</v>
       </c>
       <c r="C16" s="28">
         <v>1.0</v>
@@ -10408,13 +10775,13 @@
         <v>0.0</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>415</v>
+        <v>443</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>416</v>
+        <v>444</v>
       </c>
     </row>
     <row r="17">
@@ -10423,7 +10790,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>417</v>
+        <v>445</v>
       </c>
       <c r="C17" s="28">
         <v>1.0</v>
@@ -10432,13 +10799,13 @@
         <v>0.0</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>418</v>
+        <v>446</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>419</v>
+        <v>447</v>
       </c>
     </row>
     <row r="18">
@@ -10447,7 +10814,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>420</v>
+        <v>448</v>
       </c>
       <c r="C18" s="28">
         <v>0.0</v>
@@ -10456,13 +10823,13 @@
         <v>0.0</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>421</v>
+        <v>449</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>422</v>
+        <v>450</v>
       </c>
     </row>
     <row r="19">
@@ -10471,7 +10838,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>423</v>
+        <v>451</v>
       </c>
       <c r="C19" s="28">
         <v>0.0</v>
@@ -10480,13 +10847,13 @@
         <v>0.0</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>424</v>
+        <v>452</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>425</v>
+        <v>453</v>
       </c>
     </row>
     <row r="20">
@@ -10495,7 +10862,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>426</v>
+        <v>454</v>
       </c>
       <c r="C20" s="28">
         <v>0.0</v>
@@ -10504,13 +10871,13 @@
         <v>0.0</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>427</v>
+        <v>455</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>428</v>
+        <v>456</v>
       </c>
     </row>
     <row r="21">
@@ -10519,7 +10886,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="C21" s="28">
         <v>0.0</v>
@@ -10528,13 +10895,13 @@
         <v>0.0</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>429</v>
+        <v>457</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>430</v>
+        <v>458</v>
       </c>
     </row>
     <row r="22">
@@ -10543,7 +10910,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="C22" s="28">
         <v>0.0</v>
@@ -10552,13 +10919,13 @@
         <v>0.0</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>431</v>
+        <v>459</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>432</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -10588,10 +10955,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="15.14"/>
+    <col customWidth="1" min="2" max="2" width="17.86"/>
     <col customWidth="1" min="3" max="3" width="25.57"/>
     <col customWidth="1" min="4" max="5" width="29.86"/>
-    <col customWidth="1" min="6" max="6" width="34.57"/>
+    <col customWidth="1" min="6" max="6" width="48.29"/>
     <col customWidth="1" min="7" max="7" width="41.14"/>
     <col customWidth="1" min="8" max="8" width="42.86"/>
     <col customWidth="1" min="9" max="9" width="31.71"/>
@@ -10602,34 +10969,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>433</v>
+        <v>461</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>434</v>
+        <v>462</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>435</v>
+        <v>463</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>436</v>
+        <v>464</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>437</v>
+        <v>465</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>438</v>
+        <v>466</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>439</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
       <c r="A2" s="22">
-        <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)-1</f>
+        <f t="shared" ref="A2:A5" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>440</v>
+        <v>468</v>
       </c>
       <c r="C2" s="40" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -10644,7 +11011,7 @@
         <v>SPRITE_NONE</v>
       </c>
       <c r="D2" s="40" t="str">
-        <f t="shared" ref="D2:D4" si="2">SUBSTITUTE(H2,", ","|")</f>
+        <f t="shared" ref="D2:D5" si="2">SUBSTITUTE(H2,", ","|")</f>
         <v>PHRASE_NONSENSE</v>
       </c>
       <c r="E2" s="40" t="str">
@@ -10666,7 +11033,7 @@
         <v>200</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>375</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -10675,7 +11042,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>441</v>
+        <v>469</v>
       </c>
       <c r="C3" s="40" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -10706,13 +11073,13 @@
         <v>ITEM_VICTIM|ITEM_WITNESS1|ITEM_WITNESS2|ITEM_WITNESS3|ITEM_ROOM1_DOOR_KITCHEN|ITEM_ROOM1_DOOR_MAIN</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>442</v>
+        <v>470</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>443</v>
+        <v>471</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>375</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4">
@@ -10721,7 +11088,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>444</v>
+        <v>472</v>
       </c>
       <c r="C4" s="40" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -10732,8 +11099,8 @@
 ),"", "")
 ))
 )
-)"),"SPRITE_LAST")</f>
-        <v>SPRITE_LAST</v>
+)"),"BACKGROUND_ROOM1_KITCHEN|SPRITE_ROOM1_JAM|SPRITE_ROOM1_KITCHEN_BASIN")</f>
+        <v>BACKGROUND_ROOM1_KITCHEN|SPRITE_ROOM1_JAM|SPRITE_ROOM1_KITCHEN_BASIN</v>
       </c>
       <c r="D4" s="40" t="str">
         <f t="shared" si="2"/>
@@ -10748,22 +11115,68 @@
 ),"", "")
 ))
 )
+)"),"ITEM_ROOM1_SPOON|ITEM_ROOM1_DRAWER|ITEM_ROOM1_WINDOW|ITEM_DOOR_UNCONDITIONAL")</f>
+        <v>ITEM_ROOM1_SPOON|ITEM_ROOM1_DRAWER|ITEM_ROOM1_WINDOW|ITEM_DOOR_UNCONDITIONAL</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>474</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>475</v>
+      </c>
+      <c r="C5" s="40" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+F5
+),"", "")
+))
+)
+)"),"SPRITE_LAST")</f>
+        <v>SPRITE_LAST</v>
+      </c>
+      <c r="D5" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="E5" s="40" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G5
+),"", "")
+))
+)
 )"),"ITEM_LAST")</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>375</v>
+      <c r="F5" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="F2:H4">
+    <dataValidation type="list" allowBlank="1" sqref="F2:H5">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
-Also Item related unchainers can be ignored -Pending more robust change of room camera disposition -Unselect player when changing room
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="553">
   <si>
     <t>N</t>
   </si>
@@ -1501,6 +1501,9 @@
   </si>
   <si>
     <t>ROOM_ID</t>
+  </si>
+  <si>
+    <t>BackgroundSprite</t>
   </si>
   <si>
     <t>CompoundSpritesText</t>
@@ -2316,16 +2319,17 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H5" displayName="Table_Rooms" name="Table_Rooms" id="11">
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I5" displayName="Table_Rooms" name="Table_Rooms" id="11">
+  <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
-    <tableColumn name="CompoundSpritesText" id="3"/>
-    <tableColumn name="CompoundPhrasesText" id="4"/>
-    <tableColumn name="CompoundItemsText" id="5"/>
-    <tableColumn name="NeededBackgrounds_Sprites" id="6"/>
-    <tableColumn name="NeededItems" id="7"/>
-    <tableColumn name="NeededPhrases" id="8"/>
+    <tableColumn name="BackgroundSprite" id="3"/>
+    <tableColumn name="CompoundSpritesText" id="4"/>
+    <tableColumn name="CompoundPhrasesText" id="5"/>
+    <tableColumn name="CompoundItemsText" id="6"/>
+    <tableColumn name="NeededBackgrounds_Sprites" id="7"/>
+    <tableColumn name="NeededItems" id="8"/>
+    <tableColumn name="NeededPhrases" id="9"/>
   </tableColumns>
   <tableStyleInfo name="ROOMS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -3367,7 +3371,7 @@
         <v>23</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>30</v>
@@ -3385,7 +3389,7 @@
         <v>30</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
@@ -4811,7 +4815,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2">
@@ -4838,7 +4842,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5">
@@ -4847,7 +4851,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6">
@@ -4859,7 +4863,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8">
@@ -4875,7 +4879,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10">
@@ -4891,7 +4895,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12">
@@ -4899,7 +4903,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13">
@@ -4907,7 +4911,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15">
@@ -4915,7 +4919,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16">
@@ -4933,7 +4937,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="18">
@@ -4942,7 +4946,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="19">
@@ -4951,7 +4955,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="20">
@@ -4986,7 +4990,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="25">
@@ -4995,7 +4999,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="26">
@@ -5004,7 +5008,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="27">
@@ -5013,7 +5017,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="28">
@@ -5022,7 +5026,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="29">
@@ -5031,7 +5035,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="30">
@@ -5049,7 +5053,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="32">
@@ -5066,7 +5070,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="35">
@@ -5090,7 +5094,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="39">
@@ -5178,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2">
@@ -5241,7 +5245,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="10">
@@ -5249,16 +5253,16 @@
         <v>0</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C10" s="41" t="s">
         <v>193</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11">
@@ -5267,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>201</v>
@@ -5286,7 +5290,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>376</v>
@@ -5305,7 +5309,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>383</v>
@@ -5324,7 +5328,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>245</v>
@@ -5342,19 +5346,19 @@
         <v>0</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F16" s="43" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="17">
@@ -5366,13 +5370,13 @@
         <v>292</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>261</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F17" s="45" t="b">
         <v>0</v>
@@ -5387,13 +5391,13 @@
         <v>289</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>425</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F18" s="45" t="b">
         <v>0</v>
@@ -5408,13 +5412,13 @@
         <v>294</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>428</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F19" s="45" t="b">
         <v>0</v>
@@ -5429,13 +5433,13 @@
         <v>297</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>451</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F20" s="45" t="b">
         <v>0</v>
@@ -5450,13 +5454,13 @@
         <v>303</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>454</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F21" s="45" t="b">
         <v>0</v>
@@ -5468,16 +5472,16 @@
         <v>5</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>261</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F22" s="45" t="b">
         <v>0</v>
@@ -5488,10 +5492,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="25">
@@ -5500,7 +5504,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C25" s="46" t="s">
         <v>256</v>
@@ -5511,7 +5515,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="28">
@@ -5756,10 +5760,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="2">
@@ -5772,7 +5776,7 @@
         <v>#REF!</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3">
@@ -5785,7 +5789,7 @@
         <v>#REF!</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="4">
@@ -5798,7 +5802,7 @@
         <v>#REF!</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="5">
@@ -5811,7 +5815,7 @@
         <v>#REF!</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="6">
@@ -6142,21 +6146,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B2" s="50">
         <v>1.0</v>
@@ -6170,7 +6174,7 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B3" s="50">
         <v>1.0</v>
@@ -6184,7 +6188,7 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B4" s="50">
         <v>3.0</v>
@@ -6198,7 +6202,7 @@
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B5" s="50">
         <v>1.0</v>
@@ -6212,7 +6216,7 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B6" s="50">
         <v>3.0</v>
@@ -6226,7 +6230,7 @@
     </row>
     <row r="7">
       <c r="A7" s="28" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B7" s="50">
         <v>3.0</v>
@@ -6240,7 +6244,7 @@
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B8" s="50">
         <v>5.0</v>
@@ -6254,7 +6258,7 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B9" s="50">
         <v>4.0</v>
@@ -6268,7 +6272,7 @@
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="28" t="b">
@@ -6280,7 +6284,7 @@
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B11" s="50">
         <v>4.0</v>
@@ -6294,7 +6298,7 @@
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B12" s="50">
         <v>1.0</v>
@@ -6308,7 +6312,7 @@
     </row>
     <row r="13">
       <c r="A13" s="28" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B13" s="50">
         <v>4.0</v>
@@ -6322,7 +6326,7 @@
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B14" s="50">
         <v>1.0</v>
@@ -6336,7 +6340,7 @@
     </row>
     <row r="15">
       <c r="A15" s="28" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B15" s="50">
         <v>2.0</v>
@@ -6350,7 +6354,7 @@
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B16" s="50">
         <v>3.0</v>
@@ -6364,7 +6368,7 @@
     </row>
     <row r="17">
       <c r="A17" s="28" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B17" s="50">
         <v>2.0</v>
@@ -6378,7 +6382,7 @@
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B18" s="50">
         <v>2.0</v>
@@ -6392,7 +6396,7 @@
     </row>
     <row r="19">
       <c r="A19" s="28" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B19" s="50">
         <v>2.0</v>
@@ -6406,7 +6410,7 @@
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B20" s="50">
         <v>2.0</v>
@@ -6420,7 +6424,7 @@
     </row>
     <row r="21">
       <c r="A21" s="28" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B21" s="50">
         <v>3.0</v>
@@ -6434,7 +6438,7 @@
     </row>
     <row r="22">
       <c r="A22" s="28" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B22" s="50">
         <v>2.0</v>
@@ -6448,7 +6452,7 @@
     </row>
     <row r="23">
       <c r="A23" s="28" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B23" s="50">
         <v>2.0</v>
@@ -6462,7 +6466,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B24" s="50">
         <v>2.0</v>
@@ -6476,7 +6480,7 @@
     </row>
     <row r="25">
       <c r="A25" s="28" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B25" s="50">
         <v>2.0</v>
@@ -6490,7 +6494,7 @@
     </row>
     <row r="26">
       <c r="A26" s="28" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B26" s="50">
         <v>2.0</v>
@@ -6504,7 +6508,7 @@
     </row>
     <row r="27">
       <c r="A27" s="28" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B27" s="50">
         <v>2.0</v>
@@ -6581,16 +6585,16 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="51" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D1" s="51" t="s">
+        <v>552</v>
+      </c>
+      <c r="E1" s="51" t="s">
         <v>551</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
@@ -10956,7 +10960,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="17.86"/>
-    <col customWidth="1" min="3" max="3" width="25.57"/>
+    <col customWidth="1" min="3" max="3" width="38.29"/>
     <col customWidth="1" min="4" max="5" width="29.86"/>
     <col customWidth="1" min="6" max="6" width="48.29"/>
     <col customWidth="1" min="7" max="7" width="41.14"/>
@@ -10989,6 +10993,9 @@
       <c r="H1" s="21" t="s">
         <v>467</v>
       </c>
+      <c r="I1" s="21" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
       <c r="A2" s="22">
@@ -10996,25 +11003,12 @@
         <v>-1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>468</v>
-      </c>
-      <c r="C2" s="40" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-F2
-),"", "")
-))
-)
-)"),"SPRITE_NONE")</f>
-        <v>SPRITE_NONE</v>
+        <v>469</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="D2" s="40" t="str">
-        <f t="shared" ref="D2:D5" si="2">SUBSTITUTE(H2,", ","|")</f>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="E2" s="40" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -11023,16 +11017,32 @@
 ),"", "")
 ))
 )
+)"),"SPRITE_NONE")</f>
+        <v>SPRITE_NONE</v>
+      </c>
+      <c r="E2" s="40" t="str">
+        <f t="shared" ref="E2:E5" si="2">SUBSTITUTE(I2,", ","|")</f>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F2" s="40" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H2
+),"", "")
+))
+)
 )"),"ITEM_NONE")</f>
         <v>ITEM_NONE</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="H2" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="I2" s="27" t="s">
         <v>403</v>
       </c>
     </row>
@@ -11042,25 +11052,12 @@
         <v>0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>469</v>
-      </c>
-      <c r="C3" s="40" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-F3
-),"", "")
-))
-)
-)"),"BACKGROUND_ROOM1|SPRITE_ROOM1_DECO_TABLE")</f>
-        <v>BACKGROUND_ROOM1|SPRITE_ROOM1_DECO_TABLE</v>
+        <v>470</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>322</v>
       </c>
       <c r="D3" s="40" t="str">
-        <f t="shared" si="2"/>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="E3" s="40" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -11069,16 +11066,32 @@
 ),"", "")
 ))
 )
+)"),"BACKGROUND_ROOM1|SPRITE_ROOM1_DECO_TABLE")</f>
+        <v>BACKGROUND_ROOM1|SPRITE_ROOM1_DECO_TABLE</v>
+      </c>
+      <c r="E3" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F3" s="40" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H3
+),"", "")
+))
+)
 )"),"ITEM_VICTIM|ITEM_WITNESS1|ITEM_WITNESS2|ITEM_WITNESS3|ITEM_ROOM1_DOOR_KITCHEN|ITEM_ROOM1_DOOR_MAIN")</f>
         <v>ITEM_VICTIM|ITEM_WITNESS1|ITEM_WITNESS2|ITEM_WITNESS3|ITEM_ROOM1_DOOR_KITCHEN|ITEM_ROOM1_DOOR_MAIN</v>
       </c>
-      <c r="F3" s="27" t="s">
-        <v>470</v>
-      </c>
       <c r="G3" s="27" t="s">
         <v>471</v>
       </c>
       <c r="H3" s="27" t="s">
+        <v>472</v>
+      </c>
+      <c r="I3" s="27" t="s">
         <v>403</v>
       </c>
     </row>
@@ -11088,25 +11101,12 @@
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>472</v>
-      </c>
-      <c r="C4" s="40" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-F4
-),"", "")
-))
-)
-)"),"BACKGROUND_ROOM1_KITCHEN|SPRITE_ROOM1_JAM|SPRITE_ROOM1_KITCHEN_BASIN")</f>
-        <v>BACKGROUND_ROOM1_KITCHEN|SPRITE_ROOM1_JAM|SPRITE_ROOM1_KITCHEN_BASIN</v>
+        <v>473</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>334</v>
       </c>
       <c r="D4" s="40" t="str">
-        <f t="shared" si="2"/>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="E4" s="40" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -11115,16 +11115,32 @@
 ),"", "")
 ))
 )
+)"),"BACKGROUND_ROOM1_KITCHEN|SPRITE_ROOM1_JAM|SPRITE_ROOM1_KITCHEN_BASIN")</f>
+        <v>BACKGROUND_ROOM1_KITCHEN|SPRITE_ROOM1_JAM|SPRITE_ROOM1_KITCHEN_BASIN</v>
+      </c>
+      <c r="E4" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F4" s="40" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H4
+),"", "")
+))
+)
 )"),"ITEM_ROOM1_SPOON|ITEM_ROOM1_DRAWER|ITEM_ROOM1_WINDOW|ITEM_DOOR_UNCONDITIONAL")</f>
         <v>ITEM_ROOM1_SPOON|ITEM_ROOM1_DRAWER|ITEM_ROOM1_WINDOW|ITEM_DOOR_UNCONDITIONAL</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>473</v>
-      </c>
       <c r="G4" s="27" t="s">
         <v>474</v>
       </c>
       <c r="H4" s="27" t="s">
+        <v>475</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>403</v>
       </c>
     </row>
@@ -11134,25 +11150,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>475</v>
-      </c>
-      <c r="C5" s="40" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-F5
-),"", "")
-))
-)
-)"),"SPRITE_LAST")</f>
-        <v>SPRITE_LAST</v>
+        <v>476</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="D5" s="40" t="str">
-        <f t="shared" si="2"/>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="E5" s="40" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -11161,22 +11164,41 @@
 ),"", "")
 ))
 )
+)"),"SPRITE_LAST")</f>
+        <v>SPRITE_LAST</v>
+      </c>
+      <c r="E5" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F5" s="40" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H5
+),"", "")
+))
+)
 )"),"ITEM_LAST")</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="G5" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="H5" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="I5" s="27" t="s">
         <v>403</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="F2:H5">
+    <dataValidation type="list" allowBlank="1" sqref="G2:I5">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C5">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[Partial] Hive 1 Corridor done
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="Nd8JqOZIvfX3CGrPaUjEddhy1HuKpPIxJqVNv0wMJG4="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="JajZFS4bxvZPfcm3DhUxFUNZ+8T58xWWr6wrNuCHdkE="/>
     </ext>
   </extLst>
 </workbook>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="485">
   <si>
     <t>N</t>
   </si>
@@ -753,18 +753,69 @@
     <t>ITEM_FAMILY_TYPE_PLAYER</t>
   </si>
   <si>
+    <t>ITEM_HIVE1_CHEST</t>
+  </si>
+  <si>
+    <t>NAME_ITEM_SECR_DESK</t>
+  </si>
+  <si>
+    <t>ITEM_FAMILY_TYPE_OBJECT</t>
+  </si>
+  <si>
+    <t>SPRITE_ITEM_CHEST_OPENED, SPRITE_ITEM_CHEST_CLOSED</t>
+  </si>
+  <si>
+    <t>SPRITE_ITEM_CHEST_CLOSED</t>
+  </si>
+  <si>
+    <t>COND_OPEN_CHEST, COND_CLOSE_CHEST</t>
+  </si>
+  <si>
     <t>ITEM_CARDS_PICKABLE</t>
   </si>
   <si>
     <t>NAME_ITEM_CARDS</t>
   </si>
   <si>
-    <t>ITEM_FAMILY_TYPE_OBJECT</t>
+    <t>SPRITE_ITEM_CARDS</t>
   </si>
   <si>
     <t>SPRITE_ITEM_CARDS_PICKABLE</t>
   </si>
   <si>
+    <t>COND_TAKE_CARDS</t>
+  </si>
+  <si>
+    <t>ITEM_HIVE1_WARDROBE</t>
+  </si>
+  <si>
+    <t>NAME_ITEM_WARDROBE</t>
+  </si>
+  <si>
+    <t>SPRITE_BLANK</t>
+  </si>
+  <si>
+    <t>COND_OPEN_HIVE1_WARDROBE</t>
+  </si>
+  <si>
+    <t>ITEM_HIVE1_WARDROBE_OPENED</t>
+  </si>
+  <si>
+    <t>SPRITE_ITEM_WARDROBE_OPENED</t>
+  </si>
+  <si>
+    <t>COND_CLOSE_HIVE1_WARDROBE</t>
+  </si>
+  <si>
+    <t>ITEM_GENERIC_DOOR1</t>
+  </si>
+  <si>
+    <t>NAME_ITEM_CROSS</t>
+  </si>
+  <si>
+    <t>ITEM_FAMILY_TYPE_DOOR</t>
+  </si>
+  <si>
     <t>ITEM_LAST</t>
   </si>
   <si>
@@ -819,15 +870,48 @@
     <t>PHRASE_NONE</t>
   </si>
   <si>
+    <t>COND_OPEN_CHEST</t>
+  </si>
+  <si>
+    <t>(NOT)EVENT_HIVE1_CHEST_OPENED</t>
+  </si>
+  <si>
+    <t>CHARACTER_MAIN</t>
+  </si>
+  <si>
+    <t>INTERACTION_TAKE</t>
+  </si>
+  <si>
+    <t>ITEM_USE_ANIMATION_TAKE</t>
+  </si>
+  <si>
+    <t>EVENT_HIVE1_CHEST_OPENED</t>
+  </si>
+  <si>
+    <t>COND_CLOSE_CHEST</t>
+  </si>
+  <si>
+    <t>(NOT)EVENT_CARDS_PICKABLE_TAKEN</t>
+  </si>
+  <si>
+    <t>EVENT_CARDS_PICKABLE_TAKEN</t>
+  </si>
+  <si>
+    <t>(NOT)EVENT_HIVE1_WARDROBE_OPENED</t>
+  </si>
+  <si>
+    <t>EVENT_HIVE1_WARDROBE_OPENED</t>
+  </si>
+  <si>
     <t>COND_LAST</t>
   </si>
   <si>
-    <t>ITEM_USE_ANIMATION_TAKE</t>
-  </si>
-  <si>
     <t>UNCHAIN_ID</t>
   </si>
   <si>
+    <t>Repeat</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -861,12 +945,63 @@
     <t>MEMENTO_NONE</t>
   </si>
   <si>
+    <t>UNCHAIN_HIVE1_OPEN_CHEST_1</t>
+  </si>
+  <si>
+    <t>UNCHAIN_TYPE_SET_SPRITE</t>
+  </si>
+  <si>
+    <t>SPRITE_ITEM_CHEST_OPENED</t>
+  </si>
+  <si>
+    <t>UNCHAIN_HIVE1_OPEN_CHEST_2</t>
+  </si>
+  <si>
+    <t>UNCHAIN_TYPE_SPAWN</t>
+  </si>
+  <si>
+    <t>UNCHAIN_HIVE1_CLOSE_CHEST_1</t>
+  </si>
+  <si>
+    <t>UNCHAIN_HIVE1_CLOSE_CHEST_2</t>
+  </si>
+  <si>
+    <t>UNCHAIN_TYPE_DESPAWN</t>
+  </si>
+  <si>
+    <t>UNCHAIN_CARDS_PICKABLE_TAKE_1</t>
+  </si>
+  <si>
+    <t>UNCHAIN_TYPE_DESTROY</t>
+  </si>
+  <si>
+    <t>UNCHAIN_CARDS_PICKABLE_TAKE_2</t>
+  </si>
+  <si>
+    <t>UNCHAIN_TYPE_EARN_ITEM</t>
+  </si>
+  <si>
+    <t>UNCHAIN_HIVE1_OPEN_WARDROBE_1</t>
+  </si>
+  <si>
+    <t>UNCHAIN_HIVE1_OPEN_WARDROBE_2</t>
+  </si>
+  <si>
+    <t>UNCHAIN_HIVE1_CLOSE_WARDROBE_1</t>
+  </si>
+  <si>
+    <t>UNCHAIN_HIVE1_CLOSE_WARDROBE_2</t>
+  </si>
+  <si>
     <t>SPRITE_ID</t>
   </si>
   <si>
     <t>PATH</t>
   </si>
   <si>
+    <t>SPRITE_ATLAS_UI_0[SPRITE_BLANK]</t>
+  </si>
+  <si>
     <t>SPRITE_CURSOR_NORMAL</t>
   </si>
   <si>
@@ -927,9 +1062,27 @@
     <t>SPRITE_ATLAS_HIVE1_0[BACKGROUND_HIVE1_ROOM1]</t>
   </si>
   <si>
+    <t>SPRITE_ATLAS_HIVE1_0[SPRITE_HIVE1_CHEST_CLOSED]</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_0[SPRITE_HIVE1_CHEST_OPENED]</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_0[SPRITE_HIVE1_CHEST_CARDS]</t>
+  </si>
+  <si>
     <t>SPRITE_ATLAS_PICKABLE_0[SPRITE_PICKABLE_CARDS]</t>
   </si>
   <si>
+    <t>SPRITE_ITEM_DECO_BED_LAYER</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_0[SPRITE_HIVE1_BED_LAYER]</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_0[SPRITE_HIVE1_WARDROBE_OPENED]</t>
+  </si>
+  <si>
     <t>DIALOG_ID</t>
   </si>
   <si>
@@ -1005,9 +1158,6 @@
     <t>Tomar</t>
   </si>
   <si>
-    <t>NAME_ITEM_SECR_DESK</t>
-  </si>
-  <si>
     <t>Secretary desk</t>
   </si>
   <si>
@@ -1053,6 +1203,18 @@
     <t>Bolsa de aseo</t>
   </si>
   <si>
+    <t>Wardrobe</t>
+  </si>
+  <si>
+    <t>Armario</t>
+  </si>
+  <si>
+    <t>Cross</t>
+  </si>
+  <si>
+    <t>Cruzar</t>
+  </si>
+  <si>
     <t>Last</t>
   </si>
   <si>
@@ -1176,15 +1338,18 @@
     <t>ROOM_1</t>
   </si>
   <si>
+    <t>BACKGROUND_HIVE1_ROOM1, SPRITE_ITEM_DECO_BED_LAYER</t>
+  </si>
+  <si>
+    <t>ITEM_CARDS_PICKABLE, ITEM_HIVE1_CHEST, ITEM_HIVE1_WARDROBE, ITEM_HIVE1_WARDROBE_OPENED, ITEM_GENERIC_DOOR1</t>
+  </si>
+  <si>
     <t>ROOM_LAST</t>
   </si>
   <si>
     <t>CHARACTER_TYPE_ID</t>
   </si>
   <si>
-    <t>CHARACTER_MAIN</t>
-  </si>
-  <si>
     <t>CHARACTER_PARROT</t>
   </si>
   <si>
@@ -1215,9 +1380,6 @@
     <t>INTERACTION_USE</t>
   </si>
   <si>
-    <t>INTERACTION_TAKE</t>
-  </si>
-  <si>
     <t>INTERACTION_OBSERVE</t>
   </si>
   <si>
@@ -1230,16 +1392,7 @@
     <t>UNCHAIN_TYPE_ID</t>
   </si>
   <si>
-    <t>UNCHAIN_TYPE_SPAWN</t>
-  </si>
-  <si>
-    <t>UNCHAIN_TYPE_DESPAWN</t>
-  </si>
-  <si>
-    <t>UNCHAIN_TYPE_SET_SPRITE</t>
-  </si>
-  <si>
-    <t>UNCHAIN_TYPE_EARN_ITEM</t>
+    <t>UNCHAIN_TYPE_UNCLICKABLE</t>
   </si>
   <si>
     <t>UNCHAIN_TYPE_LOSE_ITEM</t>
@@ -1255,9 +1408,6 @@
   </si>
   <si>
     <t>ITEM_FAMILY_TYPE_ID</t>
-  </si>
-  <si>
-    <t>ITEM_FAMILY_TYPE_DOOR</t>
   </si>
   <si>
     <t>ITEM_FAMILY_TYPE_NPC</t>
@@ -1487,7 +1637,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1585,10 +1735,16 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -2015,7 +2171,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A24:B32" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A24:B34" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="15">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_TYPE_ID" id="2"/>
@@ -2025,7 +2181,7 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A34:B36" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A36:B38" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="16">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ANIMATION_ID" id="2"/>
@@ -2035,7 +2191,7 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A38:B43" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A40:B45" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="17">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_FAMILY_TYPE_ID" id="2"/>
@@ -2045,7 +2201,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B4" displayName="Table_Events" name="Table_Events" id="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B7" displayName="Table_Events" name="Table_Events" id="18">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_ID" id="2"/>
@@ -2055,7 +2211,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A6:E8" displayName="Table_Memento_Parent" name="Table_Memento_Parent" id="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A9:E11" displayName="Table_Memento_Parent" name="Table_Memento_Parent" id="19">
   <tableColumns count="5">
     <tableColumn name="N" id="1"/>
     <tableColumn name="MEMENTO_PARENT_ID" id="2"/>
@@ -2090,7 +2246,7 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A10:F12" displayName="Table_Memento" name="Table_Memento" id="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A13:F15" displayName="Table_Memento" name="Table_Memento" id="20">
   <tableColumns count="6">
     <tableColumn name="N" id="1"/>
     <tableColumn name="MEMENTO_ID" id="2"/>
@@ -2104,7 +2260,7 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A14:C15" displayName="Table_Memento_Combi" name="Table_Memento_Combi" id="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A17:C18" displayName="Table_Memento_Combi" name="Table_Memento_Combi" id="21">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="MEMENTO_COMBI_ID" id="2"/>
@@ -2115,7 +2271,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A17:B59" displayName="Table_EventsCombi" name="Table_EventsCombi" id="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A20:B62" displayName="Table_EventsCombi" name="Table_EventsCombi" id="22">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_COMBI_ID" id="2"/>
@@ -2157,7 +2313,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I5" displayName="Table_Items" name="Table_Items" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I9" displayName="Table_Items" name="Table_Items" id="3">
   <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_ID" id="2"/>
@@ -2174,7 +2330,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J3" displayName="Table_Action_Conditions" name="Table_Action_Conditions" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J8" displayName="Table_Action_Conditions" name="Table_Action_Conditions" id="4">
   <tableColumns count="10">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ACTION_COND_ID" id="2"/>
@@ -2192,25 +2348,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A5:J6" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="5">
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A10:K21" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="5">
+  <tableColumns count="11">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_ID" id="2"/>
-    <tableColumn name="Type" id="3"/>
-    <tableColumn name="IgnoreIfEvent" id="4"/>
-    <tableColumn name="NeededEvents" id="5"/>
-    <tableColumn name="TargetItem" id="6"/>
-    <tableColumn name="TargetSprite" id="7"/>
-    <tableColumn name="TargetCharacter" id="8"/>
-    <tableColumn name="TargetMemento" id="9"/>
-    <tableColumn name="TargetEvents" id="10"/>
+    <tableColumn name="Repeat" id="3"/>
+    <tableColumn name="Type" id="4"/>
+    <tableColumn name="IgnoreIfEvent" id="5"/>
+    <tableColumn name="NeededEvents" id="6"/>
+    <tableColumn name="TargetItem" id="7"/>
+    <tableColumn name="TargetSprite" id="8"/>
+    <tableColumn name="TargetCharacter" id="9"/>
+    <tableColumn name="TargetMemento" id="10"/>
+    <tableColumn name="TargetEvents" id="11"/>
   </tableColumns>
   <tableStyleInfo name="ACTION_CONDS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C14" displayName="Table_sprites" name="Table_sprites" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C20" displayName="Table_sprites" name="Table_sprites" id="6">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SPRITE_ID" id="2"/>
@@ -2247,7 +2404,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D13" displayName="Table_Name" name="Table_Name" id="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D15" displayName="Table_Name" name="Table_Name" id="9">
   <tableColumns count="4">
     <tableColumn name="N" id="1"/>
     <tableColumn name="NAME_ID" id="2"/>
@@ -4464,7 +4621,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>354</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2">
@@ -4473,7 +4630,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3">
@@ -4482,7 +4639,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>355</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
@@ -4491,7 +4648,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>356</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5">
@@ -4500,7 +4657,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>357</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6">
@@ -4512,7 +4669,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>358</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8">
@@ -4520,7 +4677,7 @@
         <v>0.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9">
@@ -4528,7 +4685,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>359</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10">
@@ -4536,7 +4693,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11">
@@ -4544,7 +4701,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>360</v>
+        <v>415</v>
       </c>
     </row>
     <row r="12">
@@ -4552,7 +4709,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>361</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13">
@@ -4560,7 +4717,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>362</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15">
@@ -4568,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>363</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16">
@@ -4577,7 +4734,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17">
@@ -4586,7 +4743,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>364</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18">
@@ -4595,7 +4752,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>365</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19">
@@ -4604,7 +4761,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>366</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20">
@@ -4613,7 +4770,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>367</v>
+        <v>421</v>
       </c>
     </row>
     <row r="21">
@@ -4622,7 +4779,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>368</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22">
@@ -4631,7 +4788,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>369</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24">
@@ -4639,7 +4796,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>370</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25">
@@ -4648,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>371</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26">
@@ -4657,7 +4814,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>372</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27">
@@ -4666,7 +4823,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>373</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28">
@@ -4675,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>374</v>
+        <v>425</v>
       </c>
     </row>
     <row r="29">
@@ -4684,7 +4841,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>375</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30">
@@ -4693,7 +4850,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>376</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31">
@@ -4702,7 +4859,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>245</v>
+        <v>426</v>
       </c>
     </row>
     <row r="32">
@@ -4711,83 +4868,101 @@
         <v>7</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>377</v>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="28">
+        <f>ROW()-ROW(Table_Unchain_Type[N])</f>
+        <v>8</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="28">
+        <f>ROW()-ROW(Table_Unchain_Type[N])</f>
+        <v>9</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="28">
+      <c r="B36" s="19" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="28">
         <v>0.0</v>
       </c>
-      <c r="B35" s="28" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="28">
+      <c r="B37" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="28">
         <v>1.0</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="19" t="s">
+      <c r="B38" s="28" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="28">
-        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="28">
-        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>1</v>
-      </c>
       <c r="B40" s="19" t="s">
-        <v>380</v>
+        <v>430</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="28">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>2</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>214</v>
+        <v>0</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="28">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>381</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="28">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="28">
+        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="28">
+        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>4</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B45" s="19" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4831,16 +5006,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>382</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28">
-        <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A7" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
@@ -4849,7 +5024,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4">
@@ -4858,147 +5033,151 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>383</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="28">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>384</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>385</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>386</v>
+      <c r="A6" s="28">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="28">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>434</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>435</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="28">
         <f>ROW()-ROW(Table_Memento_Parent[N])</f>
         <v>0</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>387</v>
-      </c>
-      <c r="C7" s="30" t="s">
+      <c r="B10" s="28" t="s">
+        <v>437</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D10" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="E7" s="43" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B7,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_NONE")</f>
+      <c r="E10" s="45" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B10,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_NONE")</f>
         <v>MEMENTO_NONE</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="28">
+    <row r="11">
+      <c r="A11" s="28">
         <f>ROW()-ROW(Table_Memento_Parent[N])</f>
         <v>1</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>388</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="D8" s="30" t="s">
+      <c r="B11" s="28" t="s">
+        <v>438</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="E8" s="43" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B8,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_LAST")</f>
+      <c r="E11" s="45" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B11,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_LAST")</f>
         <v>MEMENTO_LAST</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="19" t="s">
+    <row r="13">
+      <c r="A13" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>389</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>390</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>391</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>392</v>
-      </c>
-      <c r="F10" s="44" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="28">
+      <c r="B13" s="19" t="s">
+        <v>439</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>440</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>441</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>442</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="28">
         <f>ROW()-ROW(Table_Memento[N])</f>
         <v>0</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>387</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="E11" s="45" t="s">
-        <v>394</v>
-      </c>
-      <c r="F11" s="46" t="b">
+      <c r="B14" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>437</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="F14" s="48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="28">
+    <row r="15">
+      <c r="A15" s="28">
         <f>ROW()-ROW(Table_Memento[N])</f>
         <v>1</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>395</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>388</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="E12" s="45" t="s">
-        <v>394</v>
-      </c>
-      <c r="F12" s="46" t="b">
+      <c r="B15" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>438</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="F15" s="48" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>396</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="28">
-        <f>ROW()-ROW(Table_Memento_Combi[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>394</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="17">
@@ -5006,327 +5185,368 @@
         <v>0</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>398</v>
+        <v>446</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="48">
+      <c r="A18" s="28">
+        <f>ROW()-ROW(Table_Memento_Combi[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>444</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>0</v>
       </c>
-      <c r="B18" s="49" t="str">
+      <c r="B21" s="51" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(FLATTEN(Table_Events[EVENT_ID],""(NOT)""&amp;Table_Events[EVENT_ID]))"),"EVENT_NONE")</f>
         <v>EVENT_NONE</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="48">
+    <row r="22">
+      <c r="A22" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>1</v>
       </c>
-      <c r="B19" s="49" t="str">
+      <c r="B22" s="51" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_FIRST")</f>
         <v>EVENT_FIRST</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="48">
+    <row r="23">
+      <c r="A23" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>2</v>
       </c>
-      <c r="B20" s="49" t="str">
+      <c r="B23" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_CHEST_OPENED")</f>
+        <v>EVENT_HIVE1_CHEST_OPENED</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="50">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B24" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_CARDS_PICKABLE_TAKEN")</f>
+        <v>EVENT_CARDS_PICKABLE_TAKEN</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="50">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>4</v>
+      </c>
+      <c r="B25" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_WARDROBE_OPENED")</f>
+        <v>EVENT_HIVE1_WARDROBE_OPENED</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="50">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>5</v>
+      </c>
+      <c r="B26" s="51" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAST")</f>
         <v>EVENT_LAST</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="48">
+    <row r="27">
+      <c r="A27" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>3</v>
-      </c>
-      <c r="B21" s="49" t="str">
+        <v>6</v>
+      </c>
+      <c r="B27" s="51" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_NONE")</f>
         <v>(NOT)EVENT_NONE</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="48">
+    <row r="28">
+      <c r="A28" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>4</v>
-      </c>
-      <c r="B22" s="49" t="str">
+        <v>7</v>
+      </c>
+      <c r="B28" s="51" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_FIRST")</f>
         <v>(NOT)EVENT_FIRST</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="48">
+    <row r="29">
+      <c r="A29" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>5</v>
-      </c>
-      <c r="B23" s="49" t="str">
+        <v>8</v>
+      </c>
+      <c r="B29" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_CHEST_OPENED")</f>
+        <v>(NOT)EVENT_HIVE1_CHEST_OPENED</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="50">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>9</v>
+      </c>
+      <c r="B30" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_CARDS_PICKABLE_TAKEN")</f>
+        <v>(NOT)EVENT_CARDS_PICKABLE_TAKEN</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="50">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>10</v>
+      </c>
+      <c r="B31" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_WARDROBE_OPENED")</f>
+        <v>(NOT)EVENT_HIVE1_WARDROBE_OPENED</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="50">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>11</v>
+      </c>
+      <c r="B32" s="51" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAST")</f>
         <v>(NOT)EVENT_LAST</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="48">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>6</v>
-      </c>
-      <c r="B24" s="49"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="48">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>7</v>
-      </c>
-      <c r="B25" s="49"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="48">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>8</v>
-      </c>
-      <c r="B26" s="49"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="48">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>9</v>
-      </c>
-      <c r="B27" s="49"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="48">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>10</v>
-      </c>
-      <c r="B28" s="49"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="48">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>11</v>
-      </c>
-      <c r="B29" s="49"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="48">
+    <row r="33">
+      <c r="A33" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>12</v>
       </c>
-      <c r="B30" s="49"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="48">
+      <c r="B33" s="51"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>13</v>
       </c>
-      <c r="B31" s="49"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="48">
+      <c r="B34" s="51"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>14</v>
       </c>
-      <c r="B32" s="49"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="48">
+      <c r="B35" s="51"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>15</v>
       </c>
-      <c r="B33" s="49"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="48">
+      <c r="B36" s="51"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>16</v>
       </c>
-      <c r="B34" s="49"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="48">
+      <c r="B37" s="51"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>17</v>
       </c>
-      <c r="B35" s="49"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="48">
+      <c r="B38" s="51"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>18</v>
       </c>
-      <c r="B36" s="49"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="48">
+      <c r="B39" s="51"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>19</v>
       </c>
-      <c r="B37" s="49"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="48">
+      <c r="B40" s="51"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>20</v>
       </c>
-      <c r="B38" s="49"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="48">
+      <c r="B41" s="51"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>21</v>
       </c>
-      <c r="B39" s="49"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="48">
+      <c r="B42" s="51"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>22</v>
       </c>
-      <c r="B40" s="49"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="48">
+      <c r="B43" s="51"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>23</v>
       </c>
-      <c r="B41" s="49"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="48">
+      <c r="B44" s="51"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>24</v>
       </c>
-      <c r="B42" s="49"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="48">
+      <c r="B45" s="51"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>25</v>
       </c>
-      <c r="B43" s="49"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="48">
+      <c r="B46" s="51"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>26</v>
       </c>
-      <c r="B44" s="49"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="48">
+      <c r="B47" s="51"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>27</v>
       </c>
-      <c r="B45" s="49"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="48">
+      <c r="B48" s="51"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>28</v>
       </c>
-      <c r="B46" s="49"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="48">
+      <c r="B49" s="51"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>29</v>
       </c>
-      <c r="B47" s="49"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="48">
+      <c r="B50" s="51"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>30</v>
       </c>
-      <c r="B48" s="49"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="48">
+      <c r="B51" s="51"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>31</v>
       </c>
-      <c r="B49" s="49"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="48">
+      <c r="B52" s="51"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>32</v>
       </c>
-      <c r="B50" s="49"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="48">
+      <c r="B53" s="51"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>33</v>
       </c>
-      <c r="B51" s="49"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="48">
+      <c r="B54" s="51"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>34</v>
       </c>
-      <c r="B52" s="49"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="48">
+      <c r="B55" s="51"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>35</v>
       </c>
-      <c r="B53" s="49"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="48">
+      <c r="B56" s="51"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>36</v>
       </c>
-      <c r="B54" s="49"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="48">
+      <c r="B57" s="51"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>37</v>
       </c>
-      <c r="B55" s="49"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="48">
+      <c r="B58" s="51"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>38</v>
       </c>
-      <c r="B56" s="49"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="48">
+      <c r="B59" s="51"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>39</v>
       </c>
-      <c r="B57" s="49"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="48">
+      <c r="B60" s="51"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>40</v>
       </c>
-      <c r="B58" s="49"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="48">
+      <c r="B61" s="51"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="50">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>41</v>
       </c>
-      <c r="B59" s="49"/>
+      <c r="B62" s="51"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E11:E12">
+    <dataValidation type="list" allowBlank="1" sqref="E14:E15">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C7:D8 C11:D12 C15">
+    <dataValidation type="list" allowBlank="1" sqref="C10:D11 C14:D15 C18">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -5360,10 +5580,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>399</v>
+        <v>449</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>400</v>
+        <v>450</v>
       </c>
     </row>
     <row r="2">
@@ -5371,12 +5591,12 @@
         <f t="shared" ref="A2:A32" si="1">ROW()-ROW($G$2)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="50" t="str">
+      <c r="B2" s="52" t="str">
         <f t="shared" ref="B2:B32" si="2">OFFSET(#REF!,A2,0)</f>
         <v>#REF!</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>401</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3">
@@ -5384,12 +5604,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B3" s="50" t="str">
+      <c r="B3" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>401</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4">
@@ -5397,12 +5617,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B4" s="50" t="str">
+      <c r="B4" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>401</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5">
@@ -5410,12 +5630,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="50" t="str">
+      <c r="B5" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>401</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6">
@@ -5423,297 +5643,297 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" s="50" t="str">
+      <c r="B6" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C6" s="50"/>
+      <c r="C6" s="52"/>
     </row>
     <row r="7">
       <c r="A7" s="10">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="50" t="str">
+      <c r="B7" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="50"/>
+      <c r="C7" s="52"/>
     </row>
     <row r="8">
       <c r="A8" s="10">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="50" t="str">
+      <c r="B8" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C8" s="50"/>
+      <c r="C8" s="52"/>
     </row>
     <row r="9">
       <c r="A9" s="10">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="50" t="str">
+      <c r="B9" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C9" s="50"/>
+      <c r="C9" s="52"/>
     </row>
     <row r="10">
       <c r="A10" s="10">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="50" t="str">
+      <c r="B10" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C10" s="50"/>
+      <c r="C10" s="52"/>
     </row>
     <row r="11">
       <c r="A11" s="10">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="50" t="str">
+      <c r="B11" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C11" s="50"/>
+      <c r="C11" s="52"/>
     </row>
     <row r="12">
       <c r="A12" s="10">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="50" t="str">
+      <c r="B12" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C12" s="50"/>
+      <c r="C12" s="52"/>
     </row>
     <row r="13">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="50" t="str">
+      <c r="B13" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C13" s="50"/>
+      <c r="C13" s="52"/>
     </row>
     <row r="14">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="50" t="str">
+      <c r="B14" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C14" s="50"/>
+      <c r="C14" s="52"/>
     </row>
     <row r="15">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="50" t="str">
+      <c r="B15" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C15" s="50"/>
+      <c r="C15" s="52"/>
     </row>
     <row r="16">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="50" t="str">
+      <c r="B16" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C16" s="50"/>
+      <c r="C16" s="52"/>
     </row>
     <row r="17">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="50" t="str">
+      <c r="B17" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="52"/>
     </row>
     <row r="18">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="50" t="str">
+      <c r="B18" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C18" s="50"/>
+      <c r="C18" s="52"/>
     </row>
     <row r="19">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="50" t="str">
+      <c r="B19" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C19" s="50"/>
+      <c r="C19" s="52"/>
     </row>
     <row r="20">
       <c r="A20" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="50" t="str">
+      <c r="B20" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C20" s="50"/>
+      <c r="C20" s="52"/>
     </row>
     <row r="21">
       <c r="A21" s="10">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="50" t="str">
+      <c r="B21" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C21" s="50"/>
+      <c r="C21" s="52"/>
     </row>
     <row r="22">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="50" t="str">
+      <c r="B22" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C22" s="50"/>
+      <c r="C22" s="52"/>
     </row>
     <row r="23">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="50" t="str">
+      <c r="B23" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C23" s="50"/>
+      <c r="C23" s="52"/>
     </row>
     <row r="24">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="50" t="str">
+      <c r="B24" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C24" s="50"/>
+      <c r="C24" s="52"/>
     </row>
     <row r="25">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="50" t="str">
+      <c r="B25" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C25" s="50"/>
+      <c r="C25" s="52"/>
     </row>
     <row r="26">
       <c r="A26" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="50" t="str">
+      <c r="B26" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C26" s="50"/>
+      <c r="C26" s="52"/>
     </row>
     <row r="27">
       <c r="A27" s="10">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="50" t="str">
+      <c r="B27" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C27" s="50"/>
+      <c r="C27" s="52"/>
     </row>
     <row r="28">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="50" t="str">
+      <c r="B28" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C28" s="50"/>
+      <c r="C28" s="52"/>
     </row>
     <row r="29">
       <c r="A29" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="50" t="str">
+      <c r="B29" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C29" s="50"/>
+      <c r="C29" s="52"/>
     </row>
     <row r="30">
       <c r="A30" s="10">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="50" t="str">
+      <c r="B30" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C30" s="50"/>
+      <c r="C30" s="52"/>
     </row>
     <row r="31">
       <c r="A31" s="10">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="50" t="str">
+      <c r="B31" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C31" s="50"/>
+      <c r="C31" s="52"/>
     </row>
     <row r="32">
       <c r="A32" s="10">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="50" t="str">
+      <c r="B32" s="52" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="C32" s="50"/>
+      <c r="C32" s="52"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -5746,23 +5966,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>402</v>
+        <v>452</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>403</v>
+        <v>453</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>404</v>
+        <v>454</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>405</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>406</v>
-      </c>
-      <c r="B2" s="51">
+        <v>456</v>
+      </c>
+      <c r="B2" s="53">
         <v>1.0</v>
       </c>
       <c r="C2" s="28" t="b">
@@ -5774,9 +5994,9 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>407</v>
-      </c>
-      <c r="B3" s="51">
+        <v>457</v>
+      </c>
+      <c r="B3" s="53">
         <v>1.0</v>
       </c>
       <c r="C3" s="28" t="b">
@@ -5788,9 +6008,9 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>408</v>
-      </c>
-      <c r="B4" s="51">
+        <v>458</v>
+      </c>
+      <c r="B4" s="53">
         <v>3.0</v>
       </c>
       <c r="C4" s="28" t="b">
@@ -5802,9 +6022,9 @@
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>409</v>
-      </c>
-      <c r="B5" s="51">
+        <v>459</v>
+      </c>
+      <c r="B5" s="53">
         <v>1.0</v>
       </c>
       <c r="C5" s="28" t="b">
@@ -5816,9 +6036,9 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>410</v>
-      </c>
-      <c r="B6" s="51">
+        <v>460</v>
+      </c>
+      <c r="B6" s="53">
         <v>3.0</v>
       </c>
       <c r="C6" s="28" t="b">
@@ -5830,9 +6050,9 @@
     </row>
     <row r="7">
       <c r="A7" s="28" t="s">
-        <v>411</v>
-      </c>
-      <c r="B7" s="51">
+        <v>461</v>
+      </c>
+      <c r="B7" s="53">
         <v>3.0</v>
       </c>
       <c r="C7" s="28" t="b">
@@ -5844,9 +6064,9 @@
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>412</v>
-      </c>
-      <c r="B8" s="51">
+        <v>462</v>
+      </c>
+      <c r="B8" s="53">
         <v>5.0</v>
       </c>
       <c r="C8" s="28" t="b">
@@ -5858,9 +6078,9 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>413</v>
-      </c>
-      <c r="B9" s="51">
+        <v>463</v>
+      </c>
+      <c r="B9" s="53">
         <v>4.0</v>
       </c>
       <c r="C9" s="28" t="b">
@@ -5872,9 +6092,9 @@
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>414</v>
-      </c>
-      <c r="B10" s="51"/>
+        <v>464</v>
+      </c>
+      <c r="B10" s="53"/>
       <c r="C10" s="28" t="b">
         <v>0</v>
       </c>
@@ -5884,9 +6104,9 @@
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>415</v>
-      </c>
-      <c r="B11" s="51">
+        <v>465</v>
+      </c>
+      <c r="B11" s="53">
         <v>4.0</v>
       </c>
       <c r="C11" s="28" t="b">
@@ -5898,9 +6118,9 @@
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
-        <v>416</v>
-      </c>
-      <c r="B12" s="51">
+        <v>466</v>
+      </c>
+      <c r="B12" s="53">
         <v>1.0</v>
       </c>
       <c r="C12" s="28" t="b">
@@ -5912,9 +6132,9 @@
     </row>
     <row r="13">
       <c r="A13" s="28" t="s">
-        <v>417</v>
-      </c>
-      <c r="B13" s="51">
+        <v>467</v>
+      </c>
+      <c r="B13" s="53">
         <v>4.0</v>
       </c>
       <c r="C13" s="28" t="b">
@@ -5926,9 +6146,9 @@
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
-        <v>418</v>
-      </c>
-      <c r="B14" s="51">
+        <v>468</v>
+      </c>
+      <c r="B14" s="53">
         <v>1.0</v>
       </c>
       <c r="C14" s="28" t="b">
@@ -5940,9 +6160,9 @@
     </row>
     <row r="15">
       <c r="A15" s="28" t="s">
-        <v>419</v>
-      </c>
-      <c r="B15" s="51">
+        <v>469</v>
+      </c>
+      <c r="B15" s="53">
         <v>2.0</v>
       </c>
       <c r="C15" s="28" t="b">
@@ -5954,9 +6174,9 @@
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
-        <v>420</v>
-      </c>
-      <c r="B16" s="51">
+        <v>470</v>
+      </c>
+      <c r="B16" s="53">
         <v>3.0</v>
       </c>
       <c r="C16" s="28" t="b">
@@ -5968,9 +6188,9 @@
     </row>
     <row r="17">
       <c r="A17" s="28" t="s">
-        <v>421</v>
-      </c>
-      <c r="B17" s="51">
+        <v>471</v>
+      </c>
+      <c r="B17" s="53">
         <v>2.0</v>
       </c>
       <c r="C17" s="28" t="b">
@@ -5982,9 +6202,9 @@
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
-        <v>422</v>
-      </c>
-      <c r="B18" s="51">
+        <v>472</v>
+      </c>
+      <c r="B18" s="53">
         <v>2.0</v>
       </c>
       <c r="C18" s="28" t="b">
@@ -5996,9 +6216,9 @@
     </row>
     <row r="19">
       <c r="A19" s="28" t="s">
-        <v>423</v>
-      </c>
-      <c r="B19" s="51">
+        <v>473</v>
+      </c>
+      <c r="B19" s="53">
         <v>2.0</v>
       </c>
       <c r="C19" s="28" t="b">
@@ -6010,9 +6230,9 @@
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
-        <v>424</v>
-      </c>
-      <c r="B20" s="51">
+        <v>474</v>
+      </c>
+      <c r="B20" s="53">
         <v>2.0</v>
       </c>
       <c r="C20" s="28" t="b">
@@ -6024,9 +6244,9 @@
     </row>
     <row r="21">
       <c r="A21" s="28" t="s">
-        <v>425</v>
-      </c>
-      <c r="B21" s="51">
+        <v>475</v>
+      </c>
+      <c r="B21" s="53">
         <v>3.0</v>
       </c>
       <c r="C21" s="28" t="b">
@@ -6038,9 +6258,9 @@
     </row>
     <row r="22">
       <c r="A22" s="28" t="s">
-        <v>426</v>
-      </c>
-      <c r="B22" s="51">
+        <v>476</v>
+      </c>
+      <c r="B22" s="53">
         <v>2.0</v>
       </c>
       <c r="C22" s="28" t="b">
@@ -6052,9 +6272,9 @@
     </row>
     <row r="23">
       <c r="A23" s="28" t="s">
-        <v>427</v>
-      </c>
-      <c r="B23" s="51">
+        <v>477</v>
+      </c>
+      <c r="B23" s="53">
         <v>2.0</v>
       </c>
       <c r="C23" s="28" t="b">
@@ -6066,9 +6286,9 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>428</v>
-      </c>
-      <c r="B24" s="51">
+        <v>478</v>
+      </c>
+      <c r="B24" s="53">
         <v>2.0</v>
       </c>
       <c r="C24" s="28" t="b">
@@ -6080,9 +6300,9 @@
     </row>
     <row r="25">
       <c r="A25" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="B25" s="51">
+        <v>479</v>
+      </c>
+      <c r="B25" s="53">
         <v>2.0</v>
       </c>
       <c r="C25" s="28" t="b">
@@ -6094,9 +6314,9 @@
     </row>
     <row r="26">
       <c r="A26" s="28" t="s">
-        <v>430</v>
-      </c>
-      <c r="B26" s="51">
+        <v>480</v>
+      </c>
+      <c r="B26" s="53">
         <v>2.0</v>
       </c>
       <c r="C26" s="28" t="b">
@@ -6108,9 +6328,9 @@
     </row>
     <row r="27">
       <c r="A27" s="28" t="s">
-        <v>431</v>
-      </c>
-      <c r="B27" s="51">
+        <v>481</v>
+      </c>
+      <c r="B27" s="53">
         <v>2.0</v>
       </c>
       <c r="C27" s="28" t="b">
@@ -6122,9 +6342,9 @@
     </row>
     <row r="28">
       <c r="A28" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="B28" s="51">
+        <v>366</v>
+      </c>
+      <c r="B28" s="53">
         <v>5.0</v>
       </c>
       <c r="C28" s="28" t="b">
@@ -6184,65 +6404,93 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="52" t="s">
-        <v>432</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>433</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>434</v>
-      </c>
-      <c r="E1" s="52" t="s">
-        <v>433</v>
+      <c r="A1" s="54" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>484</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="53" t="str">
+      <c r="A2" s="55" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"SPRITE_ITEM_CARDS_PICKABLE")</f>
         <v>SPRITE_ITEM_CARDS_PICKABLE</v>
       </c>
-      <c r="B2" s="53" t="str">
-        <f t="array" ref="B2:B5">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
+      <c r="B2" s="55" t="str">
+        <f t="array" ref="B2:B9">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
         <v/>
       </c>
-      <c r="D2" s="53" t="str">
+      <c r="D2" s="55" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"NAME_ITEM_CARDS")</f>
         <v>NAME_ITEM_CARDS</v>
       </c>
-      <c r="E2" s="53" t="str">
-        <f t="array" ref="E2:E5">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
+      <c r="E2" s="55" t="str">
+        <f t="array" ref="E2:E9">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
         <v/>
       </c>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" ht="22.5" customHeight="1">
-      <c r="B4" s="53" t="s">
-        <v>215</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>213</v>
+      <c r="B4" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" ht="22.5" customHeight="1">
+      <c r="B6" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E6" s="55" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" ht="22.5" customHeight="1"/>
-    <row r="7" ht="22.5" customHeight="1"/>
-    <row r="8" ht="22.5" customHeight="1"/>
-    <row r="9" ht="22.5" customHeight="1"/>
+    <row r="7" ht="22.5" customHeight="1">
+      <c r="B7" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" ht="22.5" customHeight="1">
+      <c r="B8" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="B9" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="10" ht="22.5" customHeight="1"/>
     <row r="11" ht="22.5" customHeight="1"/>
     <row r="12" ht="22.5" customHeight="1"/>
@@ -7983,7 +8231,7 @@
     </row>
     <row r="2">
       <c r="A2" s="22">
-        <f t="shared" ref="A2:A5" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A9" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -8059,16 +8307,16 @@
         <v>215</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G4" s="26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5">
@@ -8077,36 +8325,156 @@
         <v>3</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D5" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="G5" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="22">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="G6" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="22">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="22">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="G8" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="22">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="E5" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="G5" s="26" t="b">
+      <c r="E9" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="G9" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I9" s="27" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E5 I2:I5">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E9 I2:I9">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:D5 F2:F5 H2:H5">
+    <dataValidation type="list" allowBlank="1" sqref="C2:D9 F2:F9 H2:H9">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -8151,31 +8519,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2">
@@ -8187,28 +8555,28 @@
         <v>208</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
@@ -8217,122 +8585,653 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>228</v>
+        <v>251</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>252</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>233</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>228</v>
+        <v>250</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="28">
+        <f>ROW()-ROW(Table_Action_Conditions[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>243</v>
+      <c r="A5" s="28">
+        <f>ROW()-ROW(Table_Action_Conditions[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="28">
+        <f>ROW()-ROW(Table_Action_Conditions[N])</f>
+        <v>4</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="28">
+        <f>ROW()-ROW(Table_Action_Conditions[N])</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="28">
+        <f>ROW()-ROW(Table_Action_Conditions[N])</f>
+        <v>6</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
         <v>0</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="B11" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="F11" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="G11" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="I11" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="J11" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K11" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="I12" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="J13" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="C14" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>4</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="C15" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="I15" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K15" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>5</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C16" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="I16" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="J16" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>6</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="I17" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J17" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>7</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="C18" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H18" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>207</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="J6" s="33" t="s">
+      <c r="I18" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J18" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K18" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>8</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="C19" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>228</v>
+      </c>
+      <c r="I19" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K19" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>9</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="C20" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K20" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>10</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="I21" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J21" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K21" s="33" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J3">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J8">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H2:H3">
+    <dataValidation type="list" allowBlank="1" sqref="H2:H8">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C3">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C8">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J6">
+    <dataValidation type="list" allowBlank="1" sqref="K11:K21">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D6">
+    <dataValidation type="list" allowBlank="1" sqref="E11:E21">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E6">
+    <dataValidation type="list" allowBlank="1" sqref="F11:F21">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:G3 C6 F6:I6">
+    <dataValidation type="list" allowBlank="1" sqref="D2:G8 D11:D21 G11:J21">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I3">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I8">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -8368,10 +9267,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>248</v>
+        <v>292</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>249</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2">
@@ -8389,10 +9288,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>251</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4">
@@ -8401,10 +9300,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>252</v>
+        <v>295</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>253</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5">
@@ -8413,10 +9312,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>255</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6">
@@ -8425,10 +9324,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>256</v>
+        <v>299</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>257</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7">
@@ -8437,10 +9336,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>258</v>
+        <v>301</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>259</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8">
@@ -8449,10 +9348,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>260</v>
+        <v>303</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>261</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9">
@@ -8461,10 +9360,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>262</v>
+        <v>305</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>263</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10">
@@ -8473,10 +9372,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>264</v>
+        <v>307</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>265</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11">
@@ -8485,10 +9384,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>266</v>
+        <v>309</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>267</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12">
@@ -8497,10 +9396,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>268</v>
+        <v>311</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>269</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13">
@@ -8509,10 +9408,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>215</v>
+        <v>313</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>270</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14">
@@ -8521,10 +9420,82 @@
         <v>12</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>218</v>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>16</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>17</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>18</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -8563,13 +9534,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>271</v>
+        <v>322</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>272</v>
+        <v>323</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2">
@@ -8578,13 +9549,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>204</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3">
@@ -8593,13 +9564,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>204</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>276</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4">
@@ -8608,13 +9579,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>277</v>
+        <v>328</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>204</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6">
@@ -8622,19 +9593,19 @@
         <v>0</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>278</v>
+        <v>329</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>279</v>
+        <v>330</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>280</v>
+        <v>331</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>281</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7">
@@ -8643,19 +9614,19 @@
         <v>0</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8">
@@ -8664,19 +9635,19 @@
         <v>1</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>276</v>
+        <v>327</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9">
@@ -8685,68 +9656,68 @@
         <v>2</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>282</v>
+        <v>333</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -8795,17 +9766,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>283</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>284</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>285</v>
+      <c r="B1" s="39" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="2">
@@ -8816,8 +9787,8 @@
       <c r="B2" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3">
       <c r="A3" s="22">
@@ -8828,10 +9799,10 @@
         <v>210</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>286</v>
+        <v>337</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>286</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4">
@@ -8840,13 +9811,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>289</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5">
@@ -8855,13 +9826,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>292</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6">
@@ -8870,13 +9841,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>293</v>
+        <v>344</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>294</v>
+        <v>345</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>295</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7">
@@ -8885,13 +9856,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>296</v>
+        <v>213</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>297</v>
+        <v>347</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8">
@@ -8900,13 +9871,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>299</v>
+        <v>349</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>300</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9">
@@ -8915,13 +9886,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>303</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10">
@@ -8930,13 +9901,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>304</v>
+        <v>354</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>305</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11">
@@ -8945,13 +9916,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>306</v>
+        <v>356</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>307</v>
+        <v>357</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>308</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12">
@@ -8960,13 +9931,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>309</v>
+        <v>359</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>310</v>
+        <v>360</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>311</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13">
@@ -8975,13 +9946,43 @@
         <v>11</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>312</v>
+        <v>362</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>313</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="22">
+        <f>ROW()-ROW(Table_Name[NAME_ID])</f>
+        <v>12</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="22">
+        <f>ROW()-ROW(Table_Name[NAME_ID])</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -9018,22 +10019,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>315</v>
+        <v>369</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>316</v>
+        <v>370</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>319</v>
+        <v>372</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="2">
@@ -9042,7 +10043,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="C2" s="28">
         <v>0.0</v>
@@ -9050,10 +10051,10 @@
       <c r="D2" s="28">
         <v>0.0</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="F2" s="40"/>
+      <c r="E2" s="35" t="s">
+        <v>374</v>
+      </c>
+      <c r="F2" s="42"/>
       <c r="G2" s="29"/>
     </row>
     <row r="3">
@@ -9062,7 +10063,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>321</v>
+        <v>375</v>
       </c>
       <c r="C3" s="28">
         <v>0.0</v>
@@ -9070,14 +10071,14 @@
       <c r="D3" s="28">
         <v>0.0</v>
       </c>
-      <c r="E3" s="32" t="s">
-        <v>322</v>
+      <c r="E3" s="35" t="s">
+        <v>376</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>323</v>
+        <v>377</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>324</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4">
@@ -9086,7 +10087,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>325</v>
+        <v>379</v>
       </c>
       <c r="C4" s="28">
         <v>0.0</v>
@@ -9094,14 +10095,14 @@
       <c r="D4" s="28">
         <v>0.0</v>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>322</v>
+      <c r="E4" s="35" t="s">
+        <v>376</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>326</v>
+        <v>380</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>327</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5">
@@ -9110,7 +10111,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>328</v>
+        <v>382</v>
       </c>
       <c r="C5" s="28">
         <v>0.0</v>
@@ -9118,14 +10119,14 @@
       <c r="D5" s="28">
         <v>0.0</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>322</v>
+      <c r="E5" s="35" t="s">
+        <v>376</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>330</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6">
@@ -9134,7 +10135,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>331</v>
+        <v>385</v>
       </c>
       <c r="C6" s="28">
         <v>0.0</v>
@@ -9142,14 +10143,14 @@
       <c r="D6" s="28">
         <v>0.0</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>322</v>
+      <c r="E6" s="35" t="s">
+        <v>376</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>332</v>
+        <v>386</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>333</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7">
@@ -9158,7 +10159,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>334</v>
+        <v>388</v>
       </c>
       <c r="C7" s="28">
         <v>0.0</v>
@@ -9166,14 +10167,14 @@
       <c r="D7" s="28">
         <v>0.0</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>322</v>
+      <c r="E7" s="35" t="s">
+        <v>376</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>335</v>
+        <v>389</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>336</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8">
@@ -9182,7 +10183,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>337</v>
+        <v>391</v>
       </c>
       <c r="C8" s="28">
         <v>0.0</v>
@@ -9190,14 +10191,14 @@
       <c r="D8" s="28">
         <v>0.0</v>
       </c>
-      <c r="E8" s="32" t="s">
-        <v>322</v>
+      <c r="E8" s="35" t="s">
+        <v>376</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>338</v>
+        <v>392</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>339</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9">
@@ -9206,7 +10207,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>340</v>
+        <v>394</v>
       </c>
       <c r="C9" s="28">
         <v>0.0</v>
@@ -9214,14 +10215,14 @@
       <c r="D9" s="28">
         <v>0.0</v>
       </c>
-      <c r="E9" s="32" t="s">
-        <v>322</v>
+      <c r="E9" s="35" t="s">
+        <v>376</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>341</v>
+        <v>395</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>342</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -9265,28 +10266,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>343</v>
+        <v>397</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>344</v>
+        <v>398</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>345</v>
+        <v>399</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>346</v>
+        <v>400</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>347</v>
+        <v>401</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>348</v>
+        <v>402</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>349</v>
+        <v>403</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>350</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
@@ -9295,12 +10296,12 @@
         <v>-1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>351</v>
+        <v>405</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="41" t="str">
+      <c r="D2" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -9312,11 +10313,11 @@
 )"),"SPRITE_NONE")</f>
         <v>SPRITE_NONE</v>
       </c>
-      <c r="E2" s="41" t="str">
+      <c r="E2" s="43" t="str">
         <f t="shared" ref="E2:E4" si="2">SUBSTITUTE(I2,", ","|")</f>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="F2" s="41" t="str">
+      <c r="F2" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -9335,7 +10336,7 @@
         <v>204</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>321</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -9344,12 +10345,12 @@
         <v>0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>352</v>
+        <v>406</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>268</v>
-      </c>
-      <c r="D3" s="41" t="str">
+        <v>313</v>
+      </c>
+      <c r="D3" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -9358,14 +10359,14 @@
 ),"", "")
 ))
 )
-)"),"BACKGROUND_HIVE1_ROOM1")</f>
-        <v>BACKGROUND_HIVE1_ROOM1</v>
-      </c>
-      <c r="E3" s="41" t="str">
+)"),"BACKGROUND_HIVE1_ROOM1|SPRITE_ITEM_DECO_BED_LAYER")</f>
+        <v>BACKGROUND_HIVE1_ROOM1|SPRITE_ITEM_DECO_BED_LAYER</v>
+      </c>
+      <c r="E3" s="43" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="F3" s="41" t="str">
+      <c r="F3" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -9374,17 +10375,17 @@
 ),"", "")
 ))
 )
-)"),"ITEM_CARDS_PICKABLE")</f>
-        <v>ITEM_CARDS_PICKABLE</v>
+)"),"ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1")</f>
+        <v>ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>268</v>
+        <v>407</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>212</v>
+        <v>408</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>321</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4">
@@ -9393,12 +10394,12 @@
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>353</v>
+        <v>409</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="D4" s="41" t="str">
+      <c r="D4" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -9410,11 +10411,11 @@
 )"),"SPRITE_LAST")</f>
         <v>SPRITE_LAST</v>
       </c>
-      <c r="E4" s="41" t="str">
+      <c r="E4" s="43" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="F4" s="41" t="str">
+      <c r="F4" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -9427,13 +10428,13 @@
         <v>ITEM_LAST</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>321</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Partial] Hive 1 Hall
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="JajZFS4bxvZPfcm3DhUxFUNZ+8T58xWWr6wrNuCHdkE="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="iUZbEbSsLXPBycyS5vEpc4QSLEm/7Zie+YCTBzHQemw="/>
     </ext>
   </extLst>
 </workbook>
@@ -74,13 +74,13 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="D6">
+    <comment authorId="0" ref="D8">
       <text>
         <t xml:space="preserve">Event triggered after all phrases
 ======</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E6">
+    <comment authorId="0" ref="E8">
       <text>
         <t xml:space="preserve">New dialog shown after all phrases have been said
 ======</t>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="528">
   <si>
     <t>N</t>
   </si>
@@ -816,6 +816,27 @@
     <t>ITEM_FAMILY_TYPE_DOOR</t>
   </si>
   <si>
+    <t>ITEM_HIVE1_NPC_REME</t>
+  </si>
+  <si>
+    <t>NAME_NPC_REME</t>
+  </si>
+  <si>
+    <t>ITEM_FAMILY_TYPE_NPC</t>
+  </si>
+  <si>
+    <t>SPRITE_NPC_REME_IDLE</t>
+  </si>
+  <si>
+    <t>COND_TALK_REME_1</t>
+  </si>
+  <si>
+    <t>ITEM_GENERIC_DOOR2</t>
+  </si>
+  <si>
+    <t>ITEM_GENERIC_DOOR3</t>
+  </si>
+  <si>
     <t>ITEM_LAST</t>
   </si>
   <si>
@@ -903,6 +924,12 @@
     <t>EVENT_HIVE1_WARDROBE_OPENED</t>
   </si>
   <si>
+    <t>INTERACTION_TALK</t>
+  </si>
+  <si>
+    <t>DIALOG_REME_INTRO</t>
+  </si>
+  <si>
     <t>COND_LAST</t>
   </si>
   <si>
@@ -1083,6 +1110,21 @@
     <t>SPRITE_ATLAS_HIVE1_0[SPRITE_HIVE1_WARDROBE_OPENED]</t>
   </si>
   <si>
+    <t>BACKGROUND_HIVE1_CORRIDOR1</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_1[BACKGROUND_HIVE1_CORRIDOR1]</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_1[SPRITE_HIVE1_REME_IDLE]</t>
+  </si>
+  <si>
+    <t>BACKGROUND_HIVE1_HALL1</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_2[BACKGROUND_HIVE1_HALL1]</t>
+  </si>
+  <si>
     <t>DIALOG_ID</t>
   </si>
   <si>
@@ -1101,6 +1143,15 @@
     <t>DIALOG_OPTION_SIMPLE</t>
   </si>
   <si>
+    <t>DIALOG_OPTION_REME_INTRO</t>
+  </si>
+  <si>
+    <t>DIALOG_REME</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_REME_1, DIALOG_OPTION_REME_2</t>
+  </si>
+  <si>
     <t>DIALOG_LAST</t>
   </si>
   <si>
@@ -1116,6 +1167,21 @@
     <t>Phrases</t>
   </si>
   <si>
+    <t>PHRASE_DIALOG_REME_INTRO_1, PHRASE_DIALOG_REME_INTRO_2, PHRASE_DIALOG_REME_INTRO_3</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_REME_1</t>
+  </si>
+  <si>
+    <t>PHRASE_DIALOG_REME_1_1, PHRASE_DIALOG_REME_1_2, PHRASE_DIALOG_REME_1_3</t>
+  </si>
+  <si>
+    <t>DIALOG_OPTION_REME_2</t>
+  </si>
+  <si>
+    <t>PHRASE_DIALOG_REME_2_1</t>
+  </si>
+  <si>
     <t>DIALOG_OPTION_LAST</t>
   </si>
   <si>
@@ -1164,9 +1230,6 @@
     <t>Cajonera</t>
   </si>
   <si>
-    <t>NAME_NPC_REME</t>
-  </si>
-  <si>
     <t>Remedios</t>
   </si>
   <si>
@@ -1308,6 +1371,66 @@
     <t>Es una genial idea!</t>
   </si>
   <si>
+    <t>PHRASE_DIALOG_REME_INTRO_1</t>
+  </si>
+  <si>
+    <t>Good morning Reme</t>
+  </si>
+  <si>
+    <t>Buenos días Reme</t>
+  </si>
+  <si>
+    <t>PHRASE_DIALOG_REME_INTRO_2</t>
+  </si>
+  <si>
+    <t>Be careful! It's just cleaned</t>
+  </si>
+  <si>
+    <t>Me vas a pisar lo fregado!</t>
+  </si>
+  <si>
+    <t>PHRASE_DIALOG_REME_INTRO_3</t>
+  </si>
+  <si>
+    <t>(Oh... pretty clean)</t>
+  </si>
+  <si>
+    <t>(Limpísimo está)</t>
+  </si>
+  <si>
+    <t>PHRASE_DIALOG_REME_1_1</t>
+  </si>
+  <si>
+    <t>Do you know if WC is usable today?</t>
+  </si>
+  <si>
+    <t>Sabes si el aseo está usable hoy?</t>
+  </si>
+  <si>
+    <t>PHRASE_DIALOG_REME_1_2</t>
+  </si>
+  <si>
+    <t>It always works. It's you and all the scum living here who think you are highborn</t>
+  </si>
+  <si>
+    <t>Claro que funciona. Tú y toda la morralla que vivís aquí os pensáis que sois marqueses</t>
+  </si>
+  <si>
+    <t>PHRASE_DIALOG_REME_1_3</t>
+  </si>
+  <si>
+    <t>It's downstairs as always! Be fast. Now there is nobody using it</t>
+  </si>
+  <si>
+    <t>Está en el piso de abajo como siempre! Sé rápido. Ahora mismo no hay nadie usándolo</t>
+  </si>
+  <si>
+    <t>Well! Have a nice day Reme!</t>
+  </si>
+  <si>
+    <t>Bueno! Que tengas un florido día Reme!</t>
+  </si>
+  <si>
     <t>ROOM_ID</t>
   </si>
   <si>
@@ -1335,7 +1458,7 @@
     <t>ROOM_NONE</t>
   </si>
   <si>
-    <t>ROOM_1</t>
+    <t>HIVE1_ROOM_1</t>
   </si>
   <si>
     <t>BACKGROUND_HIVE1_ROOM1, SPRITE_ITEM_DECO_BED_LAYER</t>
@@ -1344,6 +1467,18 @@
     <t>ITEM_CARDS_PICKABLE, ITEM_HIVE1_CHEST, ITEM_HIVE1_WARDROBE, ITEM_HIVE1_WARDROBE_OPENED, ITEM_GENERIC_DOOR1</t>
   </si>
   <si>
+    <t>HIVE1_CORRIDOR_1</t>
+  </si>
+  <si>
+    <t>ITEM_GENERIC_DOOR1, ITEM_HIVE1_NPC_REME</t>
+  </si>
+  <si>
+    <t>HIVE1_HALL_1</t>
+  </si>
+  <si>
+    <t>ITEM_GENERIC_DOOR1, ITEM_GENERIC_DOOR2, ITEM_GENERIC_DOOR3</t>
+  </si>
+  <si>
     <t>ROOM_LAST</t>
   </si>
   <si>
@@ -1383,9 +1518,6 @@
     <t>INTERACTION_OBSERVE</t>
   </si>
   <si>
-    <t>INTERACTION_TALK</t>
-  </si>
-  <si>
     <t>INTERACTION_CROSS_DOOR</t>
   </si>
   <si>
@@ -1408,9 +1540,6 @@
   </si>
   <si>
     <t>ITEM_FAMILY_TYPE_ID</t>
-  </si>
-  <si>
-    <t>ITEM_FAMILY_TYPE_NPC</t>
   </si>
   <si>
     <t>EVENT_ID</t>
@@ -2109,7 +2238,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G9" displayName="Table_Phrases" name="Table_Phrases" id="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G16" displayName="Table_Phrases" name="Table_Phrases" id="10">
   <tableColumns count="7">
     <tableColumn name="N" id="1"/>
     <tableColumn name="PHRASE_ID" id="2"/>
@@ -2124,7 +2253,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I4" displayName="Table_Rooms" name="Table_Rooms" id="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I6" displayName="Table_Rooms" name="Table_Rooms" id="11">
   <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
@@ -2313,7 +2442,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I9" displayName="Table_Items" name="Table_Items" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I12" displayName="Table_Items" name="Table_Items" id="3">
   <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_ID" id="2"/>
@@ -2330,7 +2459,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J8" displayName="Table_Action_Conditions" name="Table_Action_Conditions" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J9" displayName="Table_Action_Conditions" name="Table_Action_Conditions" id="4">
   <tableColumns count="10">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ACTION_COND_ID" id="2"/>
@@ -2348,7 +2477,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A10:K21" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A11:K22" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="5">
   <tableColumns count="11">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_ID" id="2"/>
@@ -2367,7 +2496,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C20" displayName="Table_sprites" name="Table_sprites" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C23" displayName="Table_sprites" name="Table_sprites" id="6">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SPRITE_ID" id="2"/>
@@ -2378,7 +2507,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D4" displayName="Table_Dialogs" name="Table_Dialogs" id="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D6" displayName="Table_Dialogs" name="Table_Dialogs" id="7">
   <tableColumns count="4">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ID" id="2"/>
@@ -2390,7 +2519,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A6:F9" displayName="Table_Dialog_Options" name="Table_Dialog_Options" id="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A8:F14" displayName="Table_Dialog_Options" name="Table_Dialog_Options" id="8">
   <tableColumns count="6">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_OPTION_ID" id="2"/>
@@ -4621,7 +4750,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>410</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2">
@@ -4630,7 +4759,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3">
@@ -4639,7 +4768,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4">
@@ -4648,7 +4777,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>411</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5">
@@ -4657,7 +4786,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>412</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6">
@@ -4669,7 +4798,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>413</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8">
@@ -4677,7 +4806,7 @@
         <v>0.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9">
@@ -4685,7 +4814,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>414</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10">
@@ -4693,7 +4822,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11">
@@ -4701,7 +4830,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>415</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12">
@@ -4709,7 +4838,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>416</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13">
@@ -4717,7 +4846,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>417</v>
+        <v>462</v>
       </c>
     </row>
     <row r="15">
@@ -4725,7 +4854,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>418</v>
+        <v>463</v>
       </c>
     </row>
     <row r="16">
@@ -4734,7 +4863,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17">
@@ -4743,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>419</v>
+        <v>464</v>
       </c>
     </row>
     <row r="18">
@@ -4752,7 +4881,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>420</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19">
@@ -4761,7 +4890,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20">
@@ -4770,7 +4899,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>421</v>
+        <v>466</v>
       </c>
     </row>
     <row r="21">
@@ -4779,7 +4908,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>422</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22">
@@ -4788,7 +4917,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>423</v>
+        <v>467</v>
       </c>
     </row>
     <row r="24">
@@ -4796,7 +4925,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>424</v>
+        <v>468</v>
       </c>
     </row>
     <row r="25">
@@ -4805,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26">
@@ -4814,7 +4943,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
     </row>
     <row r="27">
@@ -4823,7 +4952,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28">
@@ -4832,7 +4961,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>425</v>
+        <v>469</v>
       </c>
     </row>
     <row r="29">
@@ -4841,7 +4970,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30">
@@ -4850,7 +4979,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31">
@@ -4859,7 +4988,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>426</v>
+        <v>470</v>
       </c>
     </row>
     <row r="32">
@@ -4868,7 +4997,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>427</v>
+        <v>471</v>
       </c>
     </row>
     <row r="33">
@@ -4877,7 +5006,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34">
@@ -4886,7 +5015,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>428</v>
+        <v>472</v>
       </c>
     </row>
     <row r="36">
@@ -4894,7 +5023,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>429</v>
+        <v>473</v>
       </c>
     </row>
     <row r="37">
@@ -4902,7 +5031,7 @@
         <v>0.0</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>374</v>
+        <v>395</v>
       </c>
     </row>
     <row r="38">
@@ -4910,7 +5039,7 @@
         <v>1.0</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40">
@@ -4918,7 +5047,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>430</v>
+        <v>474</v>
       </c>
     </row>
     <row r="41">
@@ -4954,7 +5083,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>431</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45">
@@ -5006,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>432</v>
+        <v>475</v>
       </c>
     </row>
     <row r="2">
@@ -5015,7 +5144,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3">
@@ -5024,7 +5153,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4">
@@ -5033,7 +5162,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5">
@@ -5042,7 +5171,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6">
@@ -5051,7 +5180,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7">
@@ -5060,7 +5189,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>433</v>
+        <v>476</v>
       </c>
     </row>
     <row r="9">
@@ -5068,16 +5197,16 @@
         <v>0</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="C9" s="44" t="s">
         <v>197</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>435</v>
+        <v>478</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>436</v>
+        <v>479</v>
       </c>
     </row>
     <row r="10">
@@ -5086,7 +5215,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>205</v>
@@ -5105,10 +5234,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>438</v>
+        <v>481</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>207</v>
@@ -5123,19 +5252,19 @@
         <v>0</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>439</v>
+        <v>482</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>440</v>
+        <v>483</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>441</v>
+        <v>484</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>442</v>
+        <v>485</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>443</v>
+        <v>486</v>
       </c>
     </row>
     <row r="14">
@@ -5144,16 +5273,16 @@
         <v>0</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E14" s="47" t="s">
-        <v>444</v>
+        <v>487</v>
       </c>
       <c r="F14" s="48" t="b">
         <v>0</v>
@@ -5165,16 +5294,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>445</v>
+        <v>488</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>438</v>
+        <v>481</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E15" s="47" t="s">
-        <v>444</v>
+        <v>487</v>
       </c>
       <c r="F15" s="48" t="b">
         <v>0</v>
@@ -5185,10 +5314,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>446</v>
+        <v>489</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>447</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18">
@@ -5197,10 +5326,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>444</v>
+        <v>487</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20">
@@ -5208,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>448</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21">
@@ -5580,10 +5709,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>450</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2">
@@ -5596,7 +5725,7 @@
         <v>#REF!</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>451</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3">
@@ -5609,7 +5738,7 @@
         <v>#REF!</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>451</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4">
@@ -5622,7 +5751,7 @@
         <v>#REF!</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>451</v>
+        <v>494</v>
       </c>
     </row>
     <row r="5">
@@ -5635,7 +5764,7 @@
         <v>#REF!</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>451</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6">
@@ -5966,21 +6095,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>452</v>
+        <v>495</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>453</v>
+        <v>496</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>454</v>
+        <v>497</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>455</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>456</v>
+        <v>499</v>
       </c>
       <c r="B2" s="53">
         <v>1.0</v>
@@ -5994,7 +6123,7 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>457</v>
+        <v>500</v>
       </c>
       <c r="B3" s="53">
         <v>1.0</v>
@@ -6008,7 +6137,7 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>458</v>
+        <v>501</v>
       </c>
       <c r="B4" s="53">
         <v>3.0</v>
@@ -6022,7 +6151,7 @@
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>459</v>
+        <v>502</v>
       </c>
       <c r="B5" s="53">
         <v>1.0</v>
@@ -6036,7 +6165,7 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>460</v>
+        <v>503</v>
       </c>
       <c r="B6" s="53">
         <v>3.0</v>
@@ -6050,7 +6179,7 @@
     </row>
     <row r="7">
       <c r="A7" s="28" t="s">
-        <v>461</v>
+        <v>504</v>
       </c>
       <c r="B7" s="53">
         <v>3.0</v>
@@ -6064,7 +6193,7 @@
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>462</v>
+        <v>505</v>
       </c>
       <c r="B8" s="53">
         <v>5.0</v>
@@ -6078,7 +6207,7 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>463</v>
+        <v>506</v>
       </c>
       <c r="B9" s="53">
         <v>4.0</v>
@@ -6092,7 +6221,7 @@
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>464</v>
+        <v>507</v>
       </c>
       <c r="B10" s="53"/>
       <c r="C10" s="28" t="b">
@@ -6104,7 +6233,7 @@
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>465</v>
+        <v>508</v>
       </c>
       <c r="B11" s="53">
         <v>4.0</v>
@@ -6118,7 +6247,7 @@
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
-        <v>466</v>
+        <v>509</v>
       </c>
       <c r="B12" s="53">
         <v>1.0</v>
@@ -6132,7 +6261,7 @@
     </row>
     <row r="13">
       <c r="A13" s="28" t="s">
-        <v>467</v>
+        <v>510</v>
       </c>
       <c r="B13" s="53">
         <v>4.0</v>
@@ -6146,7 +6275,7 @@
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
-        <v>468</v>
+        <v>511</v>
       </c>
       <c r="B14" s="53">
         <v>1.0</v>
@@ -6160,7 +6289,7 @@
     </row>
     <row r="15">
       <c r="A15" s="28" t="s">
-        <v>469</v>
+        <v>512</v>
       </c>
       <c r="B15" s="53">
         <v>2.0</v>
@@ -6174,7 +6303,7 @@
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
-        <v>470</v>
+        <v>513</v>
       </c>
       <c r="B16" s="53">
         <v>3.0</v>
@@ -6188,7 +6317,7 @@
     </row>
     <row r="17">
       <c r="A17" s="28" t="s">
-        <v>471</v>
+        <v>514</v>
       </c>
       <c r="B17" s="53">
         <v>2.0</v>
@@ -6202,7 +6331,7 @@
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
-        <v>472</v>
+        <v>515</v>
       </c>
       <c r="B18" s="53">
         <v>2.0</v>
@@ -6216,7 +6345,7 @@
     </row>
     <row r="19">
       <c r="A19" s="28" t="s">
-        <v>473</v>
+        <v>516</v>
       </c>
       <c r="B19" s="53">
         <v>2.0</v>
@@ -6230,7 +6359,7 @@
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
-        <v>474</v>
+        <v>517</v>
       </c>
       <c r="B20" s="53">
         <v>2.0</v>
@@ -6244,7 +6373,7 @@
     </row>
     <row r="21">
       <c r="A21" s="28" t="s">
-        <v>475</v>
+        <v>518</v>
       </c>
       <c r="B21" s="53">
         <v>3.0</v>
@@ -6258,7 +6387,7 @@
     </row>
     <row r="22">
       <c r="A22" s="28" t="s">
-        <v>476</v>
+        <v>519</v>
       </c>
       <c r="B22" s="53">
         <v>2.0</v>
@@ -6272,7 +6401,7 @@
     </row>
     <row r="23">
       <c r="A23" s="28" t="s">
-        <v>477</v>
+        <v>520</v>
       </c>
       <c r="B23" s="53">
         <v>2.0</v>
@@ -6286,7 +6415,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>478</v>
+        <v>521</v>
       </c>
       <c r="B24" s="53">
         <v>2.0</v>
@@ -6300,7 +6429,7 @@
     </row>
     <row r="25">
       <c r="A25" s="28" t="s">
-        <v>479</v>
+        <v>522</v>
       </c>
       <c r="B25" s="53">
         <v>2.0</v>
@@ -6314,7 +6443,7 @@
     </row>
     <row r="26">
       <c r="A26" s="28" t="s">
-        <v>480</v>
+        <v>523</v>
       </c>
       <c r="B26" s="53">
         <v>2.0</v>
@@ -6328,7 +6457,7 @@
     </row>
     <row r="27">
       <c r="A27" s="28" t="s">
-        <v>481</v>
+        <v>524</v>
       </c>
       <c r="B27" s="53">
         <v>2.0</v>
@@ -6342,7 +6471,7 @@
     </row>
     <row r="28">
       <c r="A28" s="28" t="s">
-        <v>366</v>
+        <v>387</v>
       </c>
       <c r="B28" s="53">
         <v>5.0</v>
@@ -6405,16 +6534,16 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="54" t="s">
-        <v>482</v>
+        <v>525</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>483</v>
+        <v>526</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>484</v>
+        <v>527</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>483</v>
+        <v>526</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
@@ -6423,7 +6552,7 @@
         <v>SPRITE_ITEM_CARDS_PICKABLE</v>
       </c>
       <c r="B2" s="55" t="str">
-        <f t="array" ref="B2:B9">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
+        <f t="array" ref="B2:B12">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
         <v/>
       </c>
       <c r="D2" s="55" t="str">
@@ -6431,7 +6560,7 @@
         <v>NAME_ITEM_CARDS</v>
       </c>
       <c r="E2" s="55" t="str">
-        <f t="array" ref="E2:E9">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
+        <f t="array" ref="E2:E12">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
         <v/>
       </c>
     </row>
@@ -6491,9 +6620,30 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" ht="22.5" customHeight="1"/>
-    <row r="11" ht="22.5" customHeight="1"/>
-    <row r="12" ht="22.5" customHeight="1"/>
+    <row r="10" ht="22.5" customHeight="1">
+      <c r="B10" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" ht="22.5" customHeight="1">
+      <c r="B11" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" ht="22.5" customHeight="1">
+      <c r="B12" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="13" ht="22.5" customHeight="1"/>
     <row r="14" ht="22.5" customHeight="1"/>
     <row r="15" ht="22.5" customHeight="1"/>
@@ -8231,7 +8381,7 @@
     </row>
     <row r="2">
       <c r="A2" s="22">
-        <f t="shared" ref="A2:A9" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A12" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -8451,13 +8601,13 @@
         <v>234</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>206</v>
+        <v>235</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G9" s="26" t="b">
         <v>0</v>
@@ -8466,15 +8616,105 @@
         <v>207</v>
       </c>
       <c r="I9" s="27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="22">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="G11" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="22">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="G12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I12" s="27" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E9 I2:I9">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E12 I2:I12">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:D9 F2:F9 H2:H9">
+    <dataValidation type="list" allowBlank="1" sqref="C2:D12 F2:F12 H2:H12">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -8519,31 +8759,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
@@ -8555,28 +8795,28 @@
         <v>208</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3">
@@ -8585,31 +8825,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4">
@@ -8618,31 +8858,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5">
@@ -8654,28 +8894,28 @@
         <v>222</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6">
@@ -8687,28 +8927,28 @@
         <v>226</v>
       </c>
       <c r="C6" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>260</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>253</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7">
@@ -8720,28 +8960,28 @@
         <v>229</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="J7" s="33" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8">
@@ -8750,264 +8990,261 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>262</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>245</v>
+        <v>237</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>252</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>204</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="G8" s="30" t="s">
         <v>255</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>249</v>
+        <v>270</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>250</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="28">
+        <f>ROW()-ROW(Table_Action_Conditions[N])</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>263</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>270</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="28">
-        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="C11" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="30" t="s">
+      <c r="C11" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="D11" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="F11" s="33" t="s">
-        <v>245</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>207</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="J11" s="35" t="s">
+      <c r="E11" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="K11" s="33" t="s">
-        <v>245</v>
+      <c r="F11" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C12" s="34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>245</v>
+        <v>283</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>278</v>
+        <v>207</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K12" s="33" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C13" s="34" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>207</v>
+        <v>287</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="C14" s="34" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="F14" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="K14" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="I14" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="J14" s="35" t="s">
-        <v>275</v>
-      </c>
-      <c r="K14" s="33" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="C15" s="34" t="b">
         <v>1</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E15" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="F15" s="33" t="s">
         <v>259</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="G15" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="I15" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="K15" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>207</v>
-      </c>
-      <c r="I15" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="J15" s="35" t="s">
-        <v>275</v>
-      </c>
-      <c r="K15" s="33" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="C16" s="34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="F16" s="33" t="s">
         <v>259</v>
@@ -9019,34 +9256,34 @@
         <v>207</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="J16" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K16" s="33" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C17" s="34" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="G17" s="35" t="s">
         <v>218</v>
@@ -9058,180 +9295,216 @@
         <v>253</v>
       </c>
       <c r="J17" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K17" s="33" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="C18" s="34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="G18" s="35" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H18" s="35" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="J18" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="C19" s="34" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="G19" s="35" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="H19" s="35" t="s">
         <v>228</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="J19" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C20" s="34" t="b">
         <v>1</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="G20" s="35" t="s">
         <v>223</v>
       </c>
       <c r="H20" s="35" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="I20" s="36" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="J20" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="28">
         <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="C21" s="34" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H21" s="35" t="s">
         <v>225</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="J21" s="35" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>245</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>10</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="C22" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="I22" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="J22" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="K22" s="33" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J8">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J9">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H2:H8">
+    <dataValidation type="list" allowBlank="1" sqref="H2:H9">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C8">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C9">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K11:K21">
+    <dataValidation type="list" allowBlank="1" sqref="K12:K22">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E11:E21">
+    <dataValidation type="list" allowBlank="1" sqref="E12:E22">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F11:F21">
+    <dataValidation type="list" allowBlank="1" sqref="F12:F22">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:G8 D11:D21 G11:J21">
+    <dataValidation type="list" allowBlank="1" sqref="D2:G9 D12:D22 G12:J22">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I8">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I9">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -9267,10 +9540,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2">
@@ -9291,7 +9564,7 @@
         <v>225</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4">
@@ -9300,10 +9573,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5">
@@ -9312,10 +9585,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6">
@@ -9324,10 +9597,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7">
@@ -9336,10 +9609,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8">
@@ -9348,10 +9621,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9">
@@ -9360,10 +9633,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10">
@@ -9372,10 +9645,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11">
@@ -9384,10 +9657,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12">
@@ -9396,10 +9669,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13">
@@ -9408,10 +9681,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14">
@@ -9423,7 +9696,7 @@
         <v>216</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15">
@@ -9432,10 +9705,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16">
@@ -9447,7 +9720,7 @@
         <v>220</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17">
@@ -9459,7 +9732,7 @@
         <v>221</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18">
@@ -9468,10 +9741,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19">
@@ -9483,7 +9756,7 @@
         <v>228</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20">
@@ -9492,10 +9765,46 @@
         <v>18</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>235</v>
+        <v>331</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>235</v>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>19</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>20</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>21</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -9534,13 +9843,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2">
@@ -9549,13 +9858,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>204</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3">
@@ -9564,13 +9873,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>204</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4">
@@ -9579,137 +9888,190 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>328</v>
+        <v>270</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="D4" s="31" t="s">
-        <v>325</v>
+      <c r="D4" s="33" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="28">
+        <f>ROW()-ROW(Table_Dialogs[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="28">
+        <f>ROW()-ROW(Table_Dialogs[N])</f>
+        <v>4</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>345</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>330</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="28">
-        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>325</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="28">
-        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
-        <v>1</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>327</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>250</v>
+      <c r="B8" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>347</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>348</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="28">
         <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="28">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="28">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
         <v>2</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>333</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="B11" s="28" t="s">
+        <v>342</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>343</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
+      <c r="A12" s="28">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>343</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
+      <c r="A13" s="28">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>4</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
+      <c r="A14" s="28">
+        <f>ROW()-ROW(Table_Dialog_Options[N])</f>
+        <v>5</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="37"/>
@@ -9719,25 +10081,65 @@
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
     </row>
+    <row r="17">
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E7:E9">
-      <formula1>Table_Dialogs[DIALOG_ID]</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C4">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C6">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F7:F9">
+    <dataValidation type="list" allowBlank="1" sqref="F9:F14">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C7:C9">
+    <dataValidation type="list" allowBlank="1" sqref="C9:C14">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D4">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D6">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D7:D9">
+    <dataValidation type="list" allowBlank="1" sqref="D9:D14">
       <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="E9:E14">
+      <formula1>Table_Dialogs[DIALOG_ID]</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId2"/>
@@ -9770,13 +10172,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>335</v>
+        <v>357</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>336</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
@@ -9799,10 +10201,10 @@
         <v>210</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>337</v>
+        <v>359</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>337</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4">
@@ -9811,13 +10213,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>338</v>
+        <v>360</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
@@ -9826,13 +10228,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>341</v>
+        <v>363</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>342</v>
+        <v>364</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6">
@@ -9841,13 +10243,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7">
@@ -9859,10 +10261,10 @@
         <v>213</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>348</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8">
@@ -9871,13 +10273,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>349</v>
+        <v>234</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>350</v>
+        <v>371</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>350</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9">
@@ -9886,13 +10288,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>351</v>
+        <v>372</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>352</v>
+        <v>373</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10">
@@ -9904,10 +10306,10 @@
         <v>219</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>354</v>
+        <v>375</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>355</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11">
@@ -9916,13 +10318,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>356</v>
+        <v>377</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>357</v>
+        <v>378</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>358</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12">
@@ -9931,13 +10333,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>359</v>
+        <v>380</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>361</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13">
@@ -9949,10 +10351,10 @@
         <v>224</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>362</v>
+        <v>383</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>363</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14">
@@ -9964,10 +10366,10 @@
         <v>231</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>364</v>
+        <v>385</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>365</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15">
@@ -9976,13 +10378,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>366</v>
+        <v>387</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>367</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -10019,22 +10421,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>368</v>
+        <v>389</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>369</v>
+        <v>390</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>370</v>
+        <v>391</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>371</v>
+        <v>392</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>372</v>
+        <v>393</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>373</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2">
@@ -10043,7 +10445,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="C2" s="28">
         <v>0.0</v>
@@ -10052,7 +10454,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>374</v>
+        <v>395</v>
       </c>
       <c r="F2" s="42"/>
       <c r="G2" s="29"/>
@@ -10063,7 +10465,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
       <c r="C3" s="28">
         <v>0.0</v>
@@ -10072,13 +10474,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>377</v>
+        <v>398</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>378</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4">
@@ -10087,7 +10489,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>379</v>
+        <v>400</v>
       </c>
       <c r="C4" s="28">
         <v>0.0</v>
@@ -10096,13 +10498,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>380</v>
+        <v>401</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5">
@@ -10111,7 +10513,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>382</v>
+        <v>403</v>
       </c>
       <c r="C5" s="28">
         <v>0.0</v>
@@ -10120,13 +10522,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>383</v>
+        <v>404</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>384</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6">
@@ -10135,7 +10537,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>385</v>
+        <v>406</v>
       </c>
       <c r="C6" s="28">
         <v>0.0</v>
@@ -10144,13 +10546,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>386</v>
+        <v>407</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>387</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7">
@@ -10159,7 +10561,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>388</v>
+        <v>409</v>
       </c>
       <c r="C7" s="28">
         <v>0.0</v>
@@ -10168,13 +10570,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>389</v>
+        <v>410</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>390</v>
+        <v>411</v>
       </c>
     </row>
     <row r="8">
@@ -10183,7 +10585,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>391</v>
+        <v>412</v>
       </c>
       <c r="C8" s="28">
         <v>0.0</v>
@@ -10192,13 +10594,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>392</v>
+        <v>413</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>393</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9">
@@ -10207,7 +10609,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>394</v>
+        <v>415</v>
       </c>
       <c r="C9" s="28">
         <v>0.0</v>
@@ -10216,18 +10618,186 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>395</v>
+        <v>416</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>396</v>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>418</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="D10" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>419</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>421</v>
+      </c>
+      <c r="C11" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>422</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>10</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>424</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>11</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>427</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>12</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>430</v>
+      </c>
+      <c r="C14" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="D14" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="C15" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="C16" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>437</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E9">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E16">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -10252,7 +10822,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="17.86"/>
+    <col customWidth="1" min="2" max="2" width="20.0"/>
     <col customWidth="1" min="3" max="3" width="38.29"/>
     <col customWidth="1" min="4" max="5" width="29.86"/>
     <col customWidth="1" min="6" max="6" width="48.29"/>
@@ -10266,37 +10836,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>397</v>
+        <v>438</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>398</v>
+        <v>439</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>399</v>
+        <v>440</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>400</v>
+        <v>441</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>401</v>
+        <v>442</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>402</v>
+        <v>443</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>403</v>
+        <v>444</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>404</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
       <c r="A2" s="22">
-        <f t="shared" ref="A2:A4" si="1">ROW()-ROW($A$2)-1</f>
+        <f t="shared" ref="A2:A6" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>405</v>
+        <v>446</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>207</v>
@@ -10314,7 +10884,7 @@
         <v>SPRITE_NONE</v>
       </c>
       <c r="E2" s="43" t="str">
-        <f t="shared" ref="E2:E4" si="2">SUBSTITUTE(I2,", ","|")</f>
+        <f t="shared" ref="E2:E6" si="2">SUBSTITUTE(I2,", ","|")</f>
         <v>PHRASE_NONSENSE</v>
       </c>
       <c r="F2" s="43" t="str">
@@ -10336,7 +10906,7 @@
         <v>204</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -10345,10 +10915,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>406</v>
+        <v>447</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="D3" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -10379,13 +10949,13 @@
         <v>ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>407</v>
+        <v>448</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>408</v>
+        <v>449</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4">
@@ -10394,10 +10964,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>409</v>
+        <v>450</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>207</v>
+        <v>331</v>
       </c>
       <c r="D4" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -10408,8 +10978,8 @@
 ),"", "")
 ))
 )
-)"),"SPRITE_LAST")</f>
-        <v>SPRITE_LAST</v>
+)"),"BACKGROUND_HIVE1_CORRIDOR1")</f>
+        <v>BACKGROUND_HIVE1_CORRIDOR1</v>
       </c>
       <c r="E4" s="43" t="str">
         <f t="shared" si="2"/>
@@ -10424,25 +10994,123 @@
 ),"", "")
 ))
 )
+)"),"ITEM_GENERIC_DOOR1|ITEM_HIVE1_NPC_REME")</f>
+        <v>ITEM_GENERIC_DOOR1|ITEM_HIVE1_NPC_REME</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>451</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="D5" s="43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G5
+),"", "")
+))
+)
+)"),"BACKGROUND_HIVE1_HALL1")</f>
+        <v>BACKGROUND_HIVE1_HALL1</v>
+      </c>
+      <c r="E5" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F5" s="43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H5
+),"", "")
+))
+)
+)"),"ITEM_GENERIC_DOOR1|ITEM_GENERIC_DOOR2|ITEM_GENERIC_DOOR3")</f>
+        <v>ITEM_GENERIC_DOOR1|ITEM_GENERIC_DOOR2|ITEM_GENERIC_DOOR3</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>453</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="22">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G6
+),"", "")
+))
+)
+)"),"SPRITE_LAST")</f>
+        <v>SPRITE_LAST</v>
+      </c>
+      <c r="E6" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F6" s="43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H6
+),"", "")
+))
+)
 )"),"ITEM_LAST")</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="G4" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>375</v>
+      <c r="G6" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="G2:I4">
+    <dataValidation type="list" allowBlank="1" sqref="G2:I6">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C4">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C6">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[Partial] Hive 1 WC
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="iUZbEbSsLXPBycyS5vEpc4QSLEm/7Zie+YCTBzHQemw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="WmR+e/A3djqB8MlQCkyxoD++reBna5ZzGwsXFxshat0="/>
     </ext>
   </extLst>
 </workbook>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="531">
   <si>
     <t>N</t>
   </si>
@@ -1125,6 +1125,12 @@
     <t>SPRITE_ATLAS_HIVE1_2[BACKGROUND_HIVE1_HALL1]</t>
   </si>
   <si>
+    <t>BACKGROUND_HIVE1_WC</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_3[BACKGROUND_HIVE1_WC]</t>
+  </si>
+  <si>
     <t>DIALOG_ID</t>
   </si>
   <si>
@@ -1477,6 +1483,9 @@
   </si>
   <si>
     <t>ITEM_GENERIC_DOOR1, ITEM_GENERIC_DOOR2, ITEM_GENERIC_DOOR3</t>
+  </si>
+  <si>
+    <t>HIVE1_WC_1</t>
   </si>
   <si>
     <t>ROOM_LAST</t>
@@ -2253,7 +2262,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I6" displayName="Table_Rooms" name="Table_Rooms" id="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I7" displayName="Table_Rooms" name="Table_Rooms" id="11">
   <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
@@ -2496,7 +2505,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C23" displayName="Table_sprites" name="Table_sprites" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C24" displayName="Table_sprites" name="Table_sprites" id="6">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SPRITE_ID" id="2"/>
@@ -4750,7 +4759,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2">
@@ -4777,7 +4786,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5">
@@ -4786,7 +4795,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6">
@@ -4798,7 +4807,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8">
@@ -4814,7 +4823,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10">
@@ -4830,7 +4839,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12">
@@ -4838,7 +4847,7 @@
         <v>4.0</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13">
@@ -4846,7 +4855,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15">
@@ -4854,7 +4863,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="16">
@@ -4872,7 +4881,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18">
@@ -4881,7 +4890,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="19">
@@ -4899,7 +4908,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="21">
@@ -4917,7 +4926,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="24">
@@ -4925,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="25">
@@ -4961,7 +4970,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="29">
@@ -4988,7 +4997,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="32">
@@ -4997,7 +5006,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="33">
@@ -5015,7 +5024,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="36">
@@ -5023,7 +5032,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="37">
@@ -5031,7 +5040,7 @@
         <v>0.0</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="38">
@@ -5039,7 +5048,7 @@
         <v>1.0</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="40">
@@ -5047,7 +5056,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="41">
@@ -5135,7 +5144,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
@@ -5189,7 +5198,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9">
@@ -5197,16 +5206,16 @@
         <v>0</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C9" s="44" t="s">
         <v>197</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10">
@@ -5215,7 +5224,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>205</v>
@@ -5234,7 +5243,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>241</v>
@@ -5252,19 +5261,19 @@
         <v>0</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="14">
@@ -5276,13 +5285,13 @@
         <v>284</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="D14" s="35" t="s">
         <v>257</v>
       </c>
       <c r="E14" s="47" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F14" s="48" t="b">
         <v>0</v>
@@ -5294,16 +5303,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>257</v>
       </c>
       <c r="E15" s="47" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F15" s="48" t="b">
         <v>0</v>
@@ -5314,10 +5323,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="18">
@@ -5326,7 +5335,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="C18" s="49" t="s">
         <v>252</v>
@@ -5337,7 +5346,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="21">
@@ -5709,10 +5718,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2">
@@ -5725,7 +5734,7 @@
         <v>#REF!</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3">
@@ -5738,7 +5747,7 @@
         <v>#REF!</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4">
@@ -5751,7 +5760,7 @@
         <v>#REF!</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="5">
@@ -5764,7 +5773,7 @@
         <v>#REF!</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6">
@@ -6095,21 +6104,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="B2" s="53">
         <v>1.0</v>
@@ -6123,7 +6132,7 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="B3" s="53">
         <v>1.0</v>
@@ -6137,7 +6146,7 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="B4" s="53">
         <v>3.0</v>
@@ -6151,7 +6160,7 @@
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="B5" s="53">
         <v>1.0</v>
@@ -6165,7 +6174,7 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B6" s="53">
         <v>3.0</v>
@@ -6179,7 +6188,7 @@
     </row>
     <row r="7">
       <c r="A7" s="28" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="B7" s="53">
         <v>3.0</v>
@@ -6193,7 +6202,7 @@
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B8" s="53">
         <v>5.0</v>
@@ -6207,7 +6216,7 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B9" s="53">
         <v>4.0</v>
@@ -6221,7 +6230,7 @@
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="B10" s="53"/>
       <c r="C10" s="28" t="b">
@@ -6233,7 +6242,7 @@
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="B11" s="53">
         <v>4.0</v>
@@ -6247,7 +6256,7 @@
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="B12" s="53">
         <v>1.0</v>
@@ -6261,7 +6270,7 @@
     </row>
     <row r="13">
       <c r="A13" s="28" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="B13" s="53">
         <v>4.0</v>
@@ -6275,7 +6284,7 @@
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="B14" s="53">
         <v>1.0</v>
@@ -6289,7 +6298,7 @@
     </row>
     <row r="15">
       <c r="A15" s="28" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B15" s="53">
         <v>2.0</v>
@@ -6303,7 +6312,7 @@
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="B16" s="53">
         <v>3.0</v>
@@ -6317,7 +6326,7 @@
     </row>
     <row r="17">
       <c r="A17" s="28" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B17" s="53">
         <v>2.0</v>
@@ -6331,7 +6340,7 @@
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="B18" s="53">
         <v>2.0</v>
@@ -6345,7 +6354,7 @@
     </row>
     <row r="19">
       <c r="A19" s="28" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B19" s="53">
         <v>2.0</v>
@@ -6359,7 +6368,7 @@
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B20" s="53">
         <v>2.0</v>
@@ -6373,7 +6382,7 @@
     </row>
     <row r="21">
       <c r="A21" s="28" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B21" s="53">
         <v>3.0</v>
@@ -6387,7 +6396,7 @@
     </row>
     <row r="22">
       <c r="A22" s="28" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="B22" s="53">
         <v>2.0</v>
@@ -6401,7 +6410,7 @@
     </row>
     <row r="23">
       <c r="A23" s="28" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B23" s="53">
         <v>2.0</v>
@@ -6415,7 +6424,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="B24" s="53">
         <v>2.0</v>
@@ -6429,7 +6438,7 @@
     </row>
     <row r="25">
       <c r="A25" s="28" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B25" s="53">
         <v>2.0</v>
@@ -6443,7 +6452,7 @@
     </row>
     <row r="26">
       <c r="A26" s="28" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="B26" s="53">
         <v>2.0</v>
@@ -6457,7 +6466,7 @@
     </row>
     <row r="27">
       <c r="A27" s="28" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="B27" s="53">
         <v>2.0</v>
@@ -6471,7 +6480,7 @@
     </row>
     <row r="28">
       <c r="A28" s="28" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B28" s="53">
         <v>5.0</v>
@@ -6534,16 +6543,16 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="54" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
@@ -9801,9 +9810,21 @@
         <v>21</v>
       </c>
       <c r="B23" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>22</v>
+      </c>
+      <c r="B24" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C24" s="28" t="s">
         <v>242</v>
       </c>
     </row>
@@ -9843,13 +9864,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2">
@@ -9864,7 +9885,7 @@
         <v>204</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3">
@@ -9873,13 +9894,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>204</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4">
@@ -9894,7 +9915,7 @@
         <v>204</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5">
@@ -9903,13 +9924,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>204</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6">
@@ -9918,13 +9939,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C6" s="33" t="s">
         <v>204</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8">
@@ -9932,19 +9953,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>244</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9">
@@ -9953,7 +9974,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>252</v>
@@ -9974,7 +9995,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>252</v>
@@ -9995,7 +10016,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>252</v>
@@ -10004,10 +10025,10 @@
         <v>252</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12">
@@ -10016,7 +10037,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>252</v>
@@ -10025,10 +10046,10 @@
         <v>252</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13">
@@ -10037,7 +10058,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>252</v>
@@ -10049,7 +10070,7 @@
         <v>256</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14">
@@ -10058,7 +10079,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C14" s="29" t="s">
         <v>252</v>
@@ -10172,13 +10193,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2">
@@ -10201,10 +10222,10 @@
         <v>210</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4">
@@ -10213,13 +10234,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5">
@@ -10228,13 +10249,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6">
@@ -10243,13 +10264,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7">
@@ -10261,10 +10282,10 @@
         <v>213</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8">
@@ -10276,10 +10297,10 @@
         <v>234</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9">
@@ -10288,13 +10309,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10">
@@ -10306,10 +10327,10 @@
         <v>219</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11">
@@ -10318,13 +10339,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12">
@@ -10333,13 +10354,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13">
@@ -10351,10 +10372,10 @@
         <v>224</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14">
@@ -10366,10 +10387,10 @@
         <v>231</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15">
@@ -10381,10 +10402,10 @@
         <v>241</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -10421,22 +10442,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2">
@@ -10454,7 +10475,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F2" s="42"/>
       <c r="G2" s="29"/>
@@ -10465,7 +10486,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C3" s="28">
         <v>0.0</v>
@@ -10474,13 +10495,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4">
@@ -10489,7 +10510,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C4" s="28">
         <v>0.0</v>
@@ -10498,13 +10519,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5">
@@ -10513,7 +10534,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C5" s="28">
         <v>0.0</v>
@@ -10522,13 +10543,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6">
@@ -10537,7 +10558,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C6" s="28">
         <v>0.0</v>
@@ -10546,13 +10567,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="7">
@@ -10561,7 +10582,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C7" s="28">
         <v>0.0</v>
@@ -10570,13 +10591,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8">
@@ -10585,7 +10606,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C8" s="28">
         <v>0.0</v>
@@ -10594,13 +10615,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9">
@@ -10609,7 +10630,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C9" s="28">
         <v>0.0</v>
@@ -10618,13 +10639,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="10">
@@ -10633,7 +10654,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C10" s="28">
         <v>0.0</v>
@@ -10642,13 +10663,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11">
@@ -10657,7 +10678,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C11" s="28">
         <v>1.0</v>
@@ -10666,13 +10687,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12">
@@ -10681,7 +10702,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C12" s="28">
         <v>0.0</v>
@@ -10690,13 +10711,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13">
@@ -10705,7 +10726,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C13" s="28">
         <v>0.0</v>
@@ -10714,13 +10735,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="14">
@@ -10729,7 +10750,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C14" s="28">
         <v>1.0</v>
@@ -10738,13 +10759,13 @@
         <v>0.0</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="15">
@@ -10753,7 +10774,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C15" s="28">
         <v>1.0</v>
@@ -10762,13 +10783,13 @@
         <v>0.0</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16">
@@ -10777,7 +10798,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C16" s="28">
         <v>1.0</v>
@@ -10786,13 +10807,13 @@
         <v>0.0</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -10836,37 +10857,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
       <c r="A2" s="22">
-        <f t="shared" ref="A2:A6" si="1">ROW()-ROW($A$2)-1</f>
+        <f t="shared" ref="A2:A7" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>207</v>
@@ -10884,7 +10905,7 @@
         <v>SPRITE_NONE</v>
       </c>
       <c r="E2" s="43" t="str">
-        <f t="shared" ref="E2:E6" si="2">SUBSTITUTE(I2,", ","|")</f>
+        <f t="shared" ref="E2:E7" si="2">SUBSTITUTE(I2,", ","|")</f>
         <v>PHRASE_NONSENSE</v>
       </c>
       <c r="F2" s="43" t="str">
@@ -10906,7 +10927,7 @@
         <v>204</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" ht="98.25" customHeight="1">
@@ -10915,7 +10936,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>322</v>
@@ -10949,13 +10970,13 @@
         <v>ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4">
@@ -10964,7 +10985,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>331</v>
@@ -11001,10 +11022,10 @@
         <v>331</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5">
@@ -11013,7 +11034,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>334</v>
@@ -11050,10 +11071,10 @@
         <v>334</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6">
@@ -11062,10 +11083,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>207</v>
+        <v>336</v>
       </c>
       <c r="D6" s="43" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
@@ -11076,8 +11097,8 @@
 ),"", "")
 ))
 )
-)"),"SPRITE_LAST")</f>
-        <v>SPRITE_LAST</v>
+)"),"BACKGROUND_HIVE1_WC")</f>
+        <v>BACKGROUND_HIVE1_WC</v>
       </c>
       <c r="E6" s="43" t="str">
         <f t="shared" si="2"/>
@@ -11092,25 +11113,74 @@
 ),"", "")
 ))
 )
+)"),"ITEM_GENERIC_DOOR1")</f>
+        <v>ITEM_GENERIC_DOOR1</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="22">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>457</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G7
+),"", "")
+))
+)
+)"),"SPRITE_LAST")</f>
+        <v>SPRITE_LAST</v>
+      </c>
+      <c r="E7" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F7" s="43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H7
+),"", "")
+))
+)
 )"),"ITEM_LAST")</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G7" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H7" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="I6" s="27" t="s">
-        <v>396</v>
+      <c r="I7" s="27" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="G2:I6">
+    <dataValidation type="list" allowBlank="1" sqref="G2:I7">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C6">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C7">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[Partial] Building Decisions as game element and state
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -9,19 +9,20 @@
     <sheet state="visible" name="ACTION_CONDS" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="SPRITES" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="DIALOGS" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="NAMES" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="PHRASES" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="ROOMS" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="TYPES" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="EVENTS" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="_TODO" sheetId="12" r:id="rId15"/>
-    <sheet state="visible" name="_CONSTANTS" sheetId="13" r:id="rId16"/>
+    <sheet state="visible" name="DECISIONS" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="NAMES" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="PHRASES" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="ROOMS" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="TYPES" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="EVENTS" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="_TODO" sheetId="13" r:id="rId16"/>
+    <sheet state="visible" name="_CONSTANTS" sheetId="14" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId17" roundtripDataChecksum="DrZSqdpBkeOmoIRhVt8H7jF34Bb/sHMtS7KC4nWjq2A="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="5tFQ7vvm8ABagsRZL0pF7aJginsEKagokaVFLScxL48="/>
     </ext>
   </extLst>
 </workbook>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="655">
   <si>
     <t>N</t>
   </si>
@@ -1409,6 +1410,54 @@
     <t>DIALOG_OPTION_LAST</t>
   </si>
   <si>
+    <t>DECISION_ID</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>DECISION_SLEEP_1</t>
+  </si>
+  <si>
+    <t>DECISION_OPTION_NOT_SLEEP, DECISION_OPTION_SLEEP_NAP, DECISION_OPTION_SLEEP_LONG</t>
+  </si>
+  <si>
+    <t>DECISION_ID_LAST</t>
+  </si>
+  <si>
+    <t>DECISION_OPTION_LAST</t>
+  </si>
+  <si>
+    <t>DECISION_OPTION_ID</t>
+  </si>
+  <si>
+    <t>Phrase</t>
+  </si>
+  <si>
+    <t>DECISION_OPTION_NOT_SLEEP</t>
+  </si>
+  <si>
+    <t>PHRASE_DECISION_NOT_SLEEP</t>
+  </si>
+  <si>
+    <t>DECISION_OPTION_SLEEP_NAP</t>
+  </si>
+  <si>
+    <t>PHRASE_DECISION_SLEEP_NAP</t>
+  </si>
+  <si>
+    <t>EVENT_PENDING_SLEEP_NAP</t>
+  </si>
+  <si>
+    <t>DECISION_OPTION_SLEEP_LONG</t>
+  </si>
+  <si>
+    <t>PHRASE_DECISION_SLEEP_LONG</t>
+  </si>
+  <si>
+    <t>EVENT_PENDING_SLEEP_LONG</t>
+  </si>
+  <si>
     <t>NAME_ID</t>
   </si>
   <si>
@@ -1751,6 +1800,24 @@
     <t>QUIEN se ha creido que soy? Los juegos de naipes son el mismísimo demonio</t>
   </si>
   <si>
+    <t>Don't sleep</t>
+  </si>
+  <si>
+    <t>No dormir</t>
+  </si>
+  <si>
+    <t>Sleep for a while</t>
+  </si>
+  <si>
+    <t>Echarse un rato</t>
+  </si>
+  <si>
+    <t>Sleep until next day</t>
+  </si>
+  <si>
+    <t>Dormir hasta el día siguiente</t>
+  </si>
+  <si>
     <t>ROOM_ID</t>
   </si>
   <si>
@@ -1884,9 +1951,6 @@
   </si>
   <si>
     <t>Parent</t>
-  </si>
-  <si>
-    <t>Phrase</t>
   </si>
   <si>
     <t>Combinations</t>
@@ -2083,7 +2147,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2202,6 +2266,18 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -2318,7 +2394,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="26">
+  <tableStyles count="28">
     <tableStyle count="4" pivot="0" name="VARMAP-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -2362,6 +2438,18 @@
       <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
     <tableStyle count="4" pivot="0" name="DIALOGS-style 2">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
+    <tableStyle count="4" pivot="0" name="DECISIONS-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
+    <tableStyle count="4" pivot="0" name="DECISIONS-style 2">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -2499,6 +2587,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
@@ -2556,7 +2648,31 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G27" displayName="Table_Phrases" name="Table_Phrases" id="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A5:D9" displayName="Table_Decision_Options" name="Table_Decision_Options" id="10">
+  <tableColumns count="4">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="DECISION_OPTION_ID" id="2"/>
+    <tableColumn name="Phrase" id="3"/>
+    <tableColumn name="EventTriggered" id="4"/>
+  </tableColumns>
+  <tableStyleInfo name="DECISIONS-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D19" displayName="Table_Name" name="Table_Name" id="11">
+  <tableColumns count="4">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="NAME_ID" id="2"/>
+    <tableColumn name="Name_English" id="3"/>
+    <tableColumn name="Name_Spanish" id="4"/>
+  </tableColumns>
+  <tableStyleInfo name="NAMES-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G30" displayName="Table_Phrases" name="Table_Phrases" id="12">
   <tableColumns count="7">
     <tableColumn name="N" id="1"/>
     <tableColumn name="PHRASE_ID" id="2"/>
@@ -2570,8 +2686,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I7" displayName="Table_Rooms" name="Table_Rooms" id="11">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I7" displayName="Table_Rooms" name="Table_Rooms" id="13">
   <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
@@ -2587,8 +2703,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="12">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B5" displayName="Table_Characters" name="Table_Characters" id="14">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="CHARACTER_TYPE_ID" id="2"/>
@@ -2597,8 +2713,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="13">
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:B13" displayName="Table_ItemUse_Animation" name="Table_ItemUse_Animation" id="15">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ANIMATION_ID" id="2"/>
@@ -2607,8 +2723,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B22" displayName="Table_Interaction" name="Table_Interaction" id="14">
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B22" displayName="Table_Interaction" name="Table_Interaction" id="16">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="INTERACTION_ID" id="2"/>
@@ -2617,8 +2733,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A24:B34" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="15">
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A24:B34" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="17">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_TYPE_ID" id="2"/>
@@ -2627,8 +2743,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A36:B38" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="16">
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A36:B38" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="18">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ANIMATION_ID" id="2"/>
@@ -2637,33 +2753,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A40:B45" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="17">
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A40:B45" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="19">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_FAMILY_TYPE_ID" id="2"/>
   </tableColumns>
   <tableStyleInfo name="TYPES-style 6" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A47:B50" displayName="Table_Moment_Day" name="Table_Moment_Day" id="18">
-  <tableColumns count="2">
-    <tableColumn name="N" id="1"/>
-    <tableColumn name="MOMENT_TYPE_ID" id="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TYPES-style 7" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B11" displayName="Table_Events" name="Table_Events" id="19">
-  <tableColumns count="2">
-    <tableColumn name="N" id="1"/>
-    <tableColumn name="EVENT_ID" id="2"/>
-  </tableColumns>
-  <tableStyleInfo name="EVENTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -2690,7 +2786,27 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A13:E16" displayName="Table_Memento_Parent" name="Table_Memento_Parent" id="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A47:B50" displayName="Table_Moment_Day" name="Table_Moment_Day" id="20">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="MOMENT_TYPE_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TYPES-style 7" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B13" displayName="Table_Events" name="Table_Events" id="21">
+  <tableColumns count="2">
+    <tableColumn name="N" id="1"/>
+    <tableColumn name="EVENT_ID" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="EVENTS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:E18" displayName="Table_Memento_Parent" name="Table_Memento_Parent" id="22">
   <tableColumns count="5">
     <tableColumn name="N" id="1"/>
     <tableColumn name="MEMENTO_PARENT_ID" id="2"/>
@@ -2702,8 +2818,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A18:F22" displayName="Table_Memento" name="Table_Memento" id="21">
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A20:F24" displayName="Table_Memento" name="Table_Memento" id="23">
   <tableColumns count="6">
     <tableColumn name="N" id="1"/>
     <tableColumn name="MEMENTO_ID" id="2"/>
@@ -2716,8 +2832,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A24:C25" displayName="Table_Memento_Combi" name="Table_Memento_Combi" id="22">
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A26:C27" displayName="Table_Memento_Combi" name="Table_Memento_Combi" id="24">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="MEMENTO_COMBI_ID" id="2"/>
@@ -2727,8 +2843,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A27:B69" displayName="Table_EventsCombi" name="Table_EventsCombi" id="23">
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A29:B71" displayName="Table_EventsCombi" name="Table_EventsCombi" id="25">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="EVENT_COMBI_ID" id="2"/>
@@ -2737,8 +2853,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D31" displayName="Table_TODO" name="Table_TODO" id="24">
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D31" displayName="Table_TODO" name="Table_TODO" id="26">
   <tableColumns count="4">
     <tableColumn name="TASK" id="1"/>
     <tableColumn name="PRIO" id="2"/>
@@ -2749,8 +2865,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B128" displayName="Table_PickableSprites" name="Table_PickableSprites" id="25">
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B128" displayName="Table_PickableSprites" name="Table_PickableSprites" id="27">
   <tableColumns count="2">
     <tableColumn name="SPRITES" id="1"/>
     <tableColumn name="WORK" id="2"/>
@@ -2759,8 +2875,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="D1:E128" displayName="Table_PickableNames" name="Table_PickableNames" id="26">
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="D1:E128" displayName="Table_PickableNames" name="Table_PickableNames" id="28">
   <tableColumns count="2">
     <tableColumn name="NAMES" id="1"/>
     <tableColumn name="WORK" id="2"/>
@@ -2862,14 +2978,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D19" displayName="Table_Name" name="Table_Name" id="9">
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C3" displayName="Table_Decisions" name="Table_Decisions" id="9">
+  <tableColumns count="3">
     <tableColumn name="N" id="1"/>
-    <tableColumn name="NAME_ID" id="2"/>
-    <tableColumn name="Name_English" id="3"/>
-    <tableColumn name="Name_Spanish" id="4"/>
+    <tableColumn name="DECISION_ID" id="2"/>
+    <tableColumn name="OPTIONS" id="3"/>
   </tableColumns>
-  <tableStyleInfo name="NAMES-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="DECISIONS-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -5106,6 +5221,365 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="20.0"/>
+    <col customWidth="1" min="3" max="3" width="38.29"/>
+    <col customWidth="1" min="4" max="5" width="29.86"/>
+    <col customWidth="1" min="6" max="6" width="48.29"/>
+    <col customWidth="1" min="7" max="7" width="41.14"/>
+    <col customWidth="1" min="8" max="8" width="42.86"/>
+    <col customWidth="1" min="9" max="9" width="31.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>568</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>569</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>571</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>572</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>573</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="2" ht="186.0" customHeight="1">
+      <c r="A2" s="22">
+        <f t="shared" ref="A2:A7" si="1">ROW()-ROW($A$2)-1</f>
+        <v>-1</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G2
+),"", "")
+))
+)
+)"),"SPRITE_NONE")</f>
+        <v>SPRITE_NONE</v>
+      </c>
+      <c r="E2" s="49" t="str">
+        <f t="shared" ref="E2:E7" si="2">SUBSTITUTE(I2,", ","|")</f>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F2" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H2
+),"", "")
+))
+)
+)"),"ITEM_NONE")</f>
+        <v>ITEM_NONE</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" ht="98.25" customHeight="1">
+      <c r="A3" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>391</v>
+      </c>
+      <c r="D3" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G3
+),"", "")
+))
+)
+)"),"BACKGROUND_HIVE1_ROOM1|SPRITE_ITEM_DECO_BED_LAYER")</f>
+        <v>BACKGROUND_HIVE1_ROOM1|SPRITE_ITEM_DECO_BED_LAYER</v>
+      </c>
+      <c r="E3" s="49" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F3" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H3
+),"", "")
+))
+)
+)"),"ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1|ITEM_HIVE1_PERFUME|ITEM_SOAP_PICKABLE")</f>
+        <v>ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1|ITEM_HIVE1_PERFUME|ITEM_SOAP_PICKABLE</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>578</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>400</v>
+      </c>
+      <c r="D4" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G4
+),"", "")
+))
+)
+)"),"BACKGROUND_HIVE1_CORRIDOR1")</f>
+        <v>BACKGROUND_HIVE1_CORRIDOR1</v>
+      </c>
+      <c r="E4" s="49" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F4" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H4
+),"", "")
+))
+)
+)"),"ITEM_GENERIC_DOOR1|ITEM_HIVE1_NPC_REME")</f>
+        <v>ITEM_GENERIC_DOOR1|ITEM_HIVE1_NPC_REME</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>580</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="D5" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G5
+),"", "")
+))
+)
+)"),"BACKGROUND_HIVE1_HALL1")</f>
+        <v>BACKGROUND_HIVE1_HALL1</v>
+      </c>
+      <c r="E5" s="49" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F5" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H5
+),"", "")
+))
+)
+)"),"ITEM_GENERIC_DOOR1|ITEM_GENERIC_DOOR2|ITEM_HIVE1_AD_BOARD|ITEM_HIVE1_EXIT_DOOR")</f>
+        <v>ITEM_GENERIC_DOOR1|ITEM_GENERIC_DOOR2|ITEM_HIVE1_AD_BOARD|ITEM_HIVE1_EXIT_DOOR</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>403</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>582</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="22">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>583</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G6
+),"", "")
+))
+)
+)"),"BACKGROUND_HIVE1_WC")</f>
+        <v>BACKGROUND_HIVE1_WC</v>
+      </c>
+      <c r="E6" s="49" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F6" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H6
+),"", "")
+))
+)
+)"),"ITEM_GENERIC_DOOR1|ITEM_HIVE1_BASIN")</f>
+        <v>ITEM_GENERIC_DOOR1|ITEM_HIVE1_BASIN</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>405</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>584</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="22">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>585</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G7
+),"", "")
+))
+)
+)"),"SPRITE_LAST")</f>
+        <v>SPRITE_LAST</v>
+      </c>
+      <c r="E7" s="49" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F7" s="49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H7
+),"", "")
+))
+)
+)"),"ITEM_LAST")</f>
+        <v>ITEM_LAST</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>495</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C7 G2:I7">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <tabColor rgb="FF990000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5128,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>564</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2">
@@ -5155,7 +5629,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>565</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5">
@@ -5164,7 +5638,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>566</v>
+        <v>588</v>
       </c>
     </row>
     <row r="6">
@@ -5176,7 +5650,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>567</v>
+        <v>589</v>
       </c>
     </row>
     <row r="8">
@@ -5224,7 +5698,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
     </row>
     <row r="15">
@@ -5232,7 +5706,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>569</v>
+        <v>591</v>
       </c>
     </row>
     <row r="16">
@@ -5250,7 +5724,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>570</v>
+        <v>592</v>
       </c>
     </row>
     <row r="18">
@@ -5303,7 +5777,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>571</v>
+        <v>593</v>
       </c>
     </row>
     <row r="25">
@@ -5339,7 +5813,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>572</v>
+        <v>594</v>
       </c>
     </row>
     <row r="29">
@@ -5366,7 +5840,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>573</v>
+        <v>595</v>
       </c>
     </row>
     <row r="32">
@@ -5384,7 +5858,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>574</v>
+        <v>596</v>
       </c>
     </row>
     <row r="34">
@@ -5401,7 +5875,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>575</v>
+        <v>597</v>
       </c>
     </row>
     <row r="37">
@@ -5409,7 +5883,7 @@
         <v>0.0</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>478</v>
+        <v>494</v>
       </c>
     </row>
     <row r="38">
@@ -5417,7 +5891,7 @@
         <v>1.0</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
     </row>
     <row r="40">
@@ -5425,7 +5899,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>576</v>
+        <v>598</v>
       </c>
     </row>
     <row r="41">
@@ -5478,7 +5952,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>577</v>
+        <v>599</v>
       </c>
     </row>
     <row r="48">
@@ -5487,7 +5961,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>578</v>
+        <v>600</v>
       </c>
     </row>
     <row r="49">
@@ -5496,7 +5970,7 @@
         <v>1</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>579</v>
+        <v>601</v>
       </c>
     </row>
     <row r="50">
@@ -5522,7 +5996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF00FF00"/>
@@ -5549,12 +6023,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>580</v>
+        <v>602</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28">
-        <f t="shared" ref="A2:A11" si="1">ROW()-ROW($A$2)</f>
+        <f t="shared" ref="A2:A13" si="1">ROW()-ROW($A$2)</f>
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
@@ -5639,161 +6113,137 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>581</v>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="28">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="28">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>582</v>
-      </c>
-      <c r="C13" s="46" t="s">
+      <c r="B15" s="19" t="s">
+        <v>604</v>
+      </c>
+      <c r="C15" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="46" t="s">
-        <v>583</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="28">
-        <f>ROW()-ROW(Table_Memento_Parent[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>585</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E14" s="47" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B14,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_NONE")</f>
-        <v>MEMENTO_NONE</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="28">
-        <f>ROW()-ROW(Table_Memento_Parent[N])</f>
-        <v>1</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>586</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>461</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>407</v>
-      </c>
-      <c r="E15" s="47" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B15,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_JOB_FIND_1_1|MEMENTO_JOB_FIND_1_2")</f>
-        <v>MEMENTO_JOB_FIND_1_1|MEMENTO_JOB_FIND_1_2</v>
+      <c r="D15" s="50" t="s">
+        <v>605</v>
+      </c>
+      <c r="E15" s="50" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="28">
         <f>ROW()-ROW(Table_Memento_Parent[N])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>587</v>
+        <v>607</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>259</v>
+        <v>208</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="E16" s="47" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B16,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_LAST")</f>
+      <c r="E16" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B16,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_NONE")</f>
+        <v>MEMENTO_NONE</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="28">
+        <f>ROW()-ROW(Table_Memento_Parent[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>608</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="E17" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B17,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_JOB_FIND_1_1|MEMENTO_JOB_FIND_1_2")</f>
+        <v>MEMENTO_JOB_FIND_1_1|MEMENTO_JOB_FIND_1_2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="28">
+        <f>ROW()-ROW(Table_Memento_Parent[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E18" s="51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B18,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_LAST")</f>
         <v>MEMENTO_LAST</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="19" t="s">
+    <row r="20">
+      <c r="A20" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>588</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>589</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>590</v>
-      </c>
-      <c r="E18" s="46" t="s">
-        <v>591</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="28">
-        <f>ROW()-ROW(Table_Memento[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>342</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>585</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>275</v>
-      </c>
-      <c r="E19" s="49" t="s">
-        <v>593</v>
-      </c>
-      <c r="F19" s="38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="28">
-        <f>ROW()-ROW(Table_Memento[N])</f>
-        <v>1</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>345</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>586</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>520</v>
-      </c>
-      <c r="E20" s="49" t="s">
-        <v>593</v>
-      </c>
-      <c r="F20" s="38" t="b">
-        <v>0</v>
+      <c r="B20" s="19" t="s">
+        <v>610</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>611</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>438</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>612</v>
+      </c>
+      <c r="F20" s="52" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="28">
         <f>ROW()-ROW(Table_Memento[N])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>586</v>
+        <v>607</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="E21" s="49" t="s">
-        <v>593</v>
+        <v>275</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>614</v>
       </c>
       <c r="F21" s="38" t="b">
         <v>0</v>
@@ -5802,415 +6252,469 @@
     <row r="22">
       <c r="A22" s="28">
         <f>ROW()-ROW(Table_Memento[N])</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>594</v>
+        <v>345</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>587</v>
+        <v>608</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>275</v>
-      </c>
-      <c r="E22" s="49" t="s">
-        <v>593</v>
+        <v>536</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>614</v>
       </c>
       <c r="F22" s="38" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="28">
+        <f>ROW()-ROW(Table_Memento[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>608</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>614</v>
+      </c>
+      <c r="F23" s="38" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="24">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="28">
+        <f>ROW()-ROW(Table_Memento[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>615</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>609</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="E24" s="53" t="s">
+        <v>614</v>
+      </c>
+      <c r="F24" s="38" t="b">
         <v>0</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>595</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="28">
+    </row>
+    <row r="26">
+      <c r="A26" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>616</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="28">
         <f>ROW()-ROW(Table_Memento_Combi[N])</f>
         <v>0</v>
       </c>
-      <c r="B25" s="28" t="s">
-        <v>593</v>
-      </c>
-      <c r="C25" s="50" t="s">
+      <c r="B27" s="28" t="s">
+        <v>614</v>
+      </c>
+      <c r="C27" s="54" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="19" t="s">
+    <row r="29">
+      <c r="A29" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="37">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B28" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(FLATTEN(Table_Events[EVENT_ID],""(NOT)""&amp;Table_Events[EVENT_ID]))"),"EVENT_NONE")</f>
-        <v>EVENT_NONE</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="37">
-        <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>1</v>
-      </c>
-      <c r="B29" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_FIRST")</f>
-        <v>EVENT_FIRST</v>
+      <c r="B29" s="19" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>2</v>
-      </c>
-      <c r="B30" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_CHEST_OPENED")</f>
-        <v>EVENT_HIVE1_CHEST_OPENED</v>
+        <v>0</v>
+      </c>
+      <c r="B30" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(FLATTEN(Table_Events[EVENT_ID],""(NOT)""&amp;Table_Events[EVENT_ID]))"),"EVENT_NONE")</f>
+        <v>EVENT_NONE</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>3</v>
-      </c>
-      <c r="B31" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_CARDS_PICKABLE_TAKEN")</f>
-        <v>EVENT_CARDS_PICKABLE_TAKEN</v>
+        <v>1</v>
+      </c>
+      <c r="B31" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_FIRST")</f>
+        <v>EVENT_FIRST</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>4</v>
-      </c>
-      <c r="B32" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_WARDROBE_OPENED")</f>
-        <v>EVENT_HIVE1_WARDROBE_OPENED</v>
+        <v>2</v>
+      </c>
+      <c r="B32" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_CHEST_OPENED")</f>
+        <v>EVENT_HIVE1_CHEST_OPENED</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>5</v>
-      </c>
-      <c r="B33" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_AD_BOARD_OBSERVED_1")</f>
-        <v>EVENT_HIVE1_AD_BOARD_OBSERVED_1</v>
+        <v>3</v>
+      </c>
+      <c r="B33" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_CARDS_PICKABLE_TAKEN")</f>
+        <v>EVENT_CARDS_PICKABLE_TAKEN</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>6</v>
-      </c>
-      <c r="B34" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_USED_PERFUME")</f>
-        <v>EVENT_HIVE1_USED_PERFUME</v>
+        <v>4</v>
+      </c>
+      <c r="B34" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_WARDROBE_OPENED")</f>
+        <v>EVENT_HIVE1_WARDROBE_OPENED</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>7</v>
-      </c>
-      <c r="B35" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_USED_BASIN")</f>
-        <v>EVENT_HIVE1_USED_BASIN</v>
+        <v>5</v>
+      </c>
+      <c r="B35" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_AD_BOARD_OBSERVED_1")</f>
+        <v>EVENT_HIVE1_AD_BOARD_OBSERVED_1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>8</v>
-      </c>
-      <c r="B36" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_SOAP_PICKABLE_TAKEN")</f>
-        <v>EVENT_SOAP_PICKABLE_TAKEN</v>
+        <v>6</v>
+      </c>
+      <c r="B36" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_USED_PERFUME")</f>
+        <v>EVENT_HIVE1_USED_PERFUME</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>9</v>
-      </c>
-      <c r="B37" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAST")</f>
-        <v>EVENT_LAST</v>
+        <v>7</v>
+      </c>
+      <c r="B37" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_USED_BASIN")</f>
+        <v>EVENT_HIVE1_USED_BASIN</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>10</v>
-      </c>
-      <c r="B38" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_NONE")</f>
-        <v>(NOT)EVENT_NONE</v>
+        <v>8</v>
+      </c>
+      <c r="B38" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_SOAP_PICKABLE_TAKEN")</f>
+        <v>EVENT_SOAP_PICKABLE_TAKEN</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>11</v>
-      </c>
-      <c r="B39" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_FIRST")</f>
-        <v>(NOT)EVENT_FIRST</v>
+        <v>9</v>
+      </c>
+      <c r="B39" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_PENDING_SLEEP_NAP")</f>
+        <v>EVENT_PENDING_SLEEP_NAP</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>12</v>
-      </c>
-      <c r="B40" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_CHEST_OPENED")</f>
-        <v>(NOT)EVENT_HIVE1_CHEST_OPENED</v>
+        <v>10</v>
+      </c>
+      <c r="B40" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_PENDING_SLEEP_LONG")</f>
+        <v>EVENT_PENDING_SLEEP_LONG</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>13</v>
-      </c>
-      <c r="B41" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_CARDS_PICKABLE_TAKEN")</f>
-        <v>(NOT)EVENT_CARDS_PICKABLE_TAKEN</v>
+        <v>11</v>
+      </c>
+      <c r="B41" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAST")</f>
+        <v>EVENT_LAST</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>14</v>
-      </c>
-      <c r="B42" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_WARDROBE_OPENED")</f>
-        <v>(NOT)EVENT_HIVE1_WARDROBE_OPENED</v>
+        <v>12</v>
+      </c>
+      <c r="B42" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_NONE")</f>
+        <v>(NOT)EVENT_NONE</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>15</v>
-      </c>
-      <c r="B43" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_AD_BOARD_OBSERVED_1")</f>
-        <v>(NOT)EVENT_HIVE1_AD_BOARD_OBSERVED_1</v>
+        <v>13</v>
+      </c>
+      <c r="B43" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_FIRST")</f>
+        <v>(NOT)EVENT_FIRST</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>16</v>
-      </c>
-      <c r="B44" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_USED_PERFUME")</f>
-        <v>(NOT)EVENT_HIVE1_USED_PERFUME</v>
+        <v>14</v>
+      </c>
+      <c r="B44" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_CHEST_OPENED")</f>
+        <v>(NOT)EVENT_HIVE1_CHEST_OPENED</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>17</v>
-      </c>
-      <c r="B45" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_USED_BASIN")</f>
-        <v>(NOT)EVENT_HIVE1_USED_BASIN</v>
+        <v>15</v>
+      </c>
+      <c r="B45" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_CARDS_PICKABLE_TAKEN")</f>
+        <v>(NOT)EVENT_CARDS_PICKABLE_TAKEN</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>18</v>
-      </c>
-      <c r="B46" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_SOAP_PICKABLE_TAKEN")</f>
-        <v>(NOT)EVENT_SOAP_PICKABLE_TAKEN</v>
+        <v>16</v>
+      </c>
+      <c r="B46" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_WARDROBE_OPENED")</f>
+        <v>(NOT)EVENT_HIVE1_WARDROBE_OPENED</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>19</v>
-      </c>
-      <c r="B47" s="51" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAST")</f>
-        <v>(NOT)EVENT_LAST</v>
+        <v>17</v>
+      </c>
+      <c r="B47" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_AD_BOARD_OBSERVED_1")</f>
+        <v>(NOT)EVENT_HIVE1_AD_BOARD_OBSERVED_1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>20</v>
-      </c>
-      <c r="B48" s="51"/>
+        <v>18</v>
+      </c>
+      <c r="B48" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_USED_PERFUME")</f>
+        <v>(NOT)EVENT_HIVE1_USED_PERFUME</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>21</v>
-      </c>
-      <c r="B49" s="51"/>
+        <v>19</v>
+      </c>
+      <c r="B49" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_USED_BASIN")</f>
+        <v>(NOT)EVENT_HIVE1_USED_BASIN</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>22</v>
-      </c>
-      <c r="B50" s="51"/>
+        <v>20</v>
+      </c>
+      <c r="B50" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_SOAP_PICKABLE_TAKEN")</f>
+        <v>(NOT)EVENT_SOAP_PICKABLE_TAKEN</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>23</v>
-      </c>
-      <c r="B51" s="51"/>
+        <v>21</v>
+      </c>
+      <c r="B51" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_PENDING_SLEEP_NAP")</f>
+        <v>(NOT)EVENT_PENDING_SLEEP_NAP</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>24</v>
-      </c>
-      <c r="B52" s="51"/>
+        <v>22</v>
+      </c>
+      <c r="B52" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_PENDING_SLEEP_LONG")</f>
+        <v>(NOT)EVENT_PENDING_SLEEP_LONG</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>25</v>
-      </c>
-      <c r="B53" s="51"/>
+        <v>23</v>
+      </c>
+      <c r="B53" s="55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAST")</f>
+        <v>(NOT)EVENT_LAST</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>26</v>
-      </c>
-      <c r="B54" s="51"/>
+        <v>24</v>
+      </c>
+      <c r="B54" s="55"/>
     </row>
     <row r="55">
       <c r="A55" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>27</v>
-      </c>
-      <c r="B55" s="51"/>
+        <v>25</v>
+      </c>
+      <c r="B55" s="55"/>
     </row>
     <row r="56">
       <c r="A56" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>28</v>
-      </c>
-      <c r="B56" s="51"/>
+        <v>26</v>
+      </c>
+      <c r="B56" s="55"/>
     </row>
     <row r="57">
       <c r="A57" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>29</v>
-      </c>
-      <c r="B57" s="51"/>
+        <v>27</v>
+      </c>
+      <c r="B57" s="55"/>
     </row>
     <row r="58">
       <c r="A58" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>30</v>
-      </c>
-      <c r="B58" s="51"/>
+        <v>28</v>
+      </c>
+      <c r="B58" s="55"/>
     </row>
     <row r="59">
       <c r="A59" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>31</v>
-      </c>
-      <c r="B59" s="51"/>
+        <v>29</v>
+      </c>
+      <c r="B59" s="55"/>
     </row>
     <row r="60">
       <c r="A60" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>32</v>
-      </c>
-      <c r="B60" s="51"/>
+        <v>30</v>
+      </c>
+      <c r="B60" s="55"/>
     </row>
     <row r="61">
       <c r="A61" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>33</v>
-      </c>
-      <c r="B61" s="51"/>
+        <v>31</v>
+      </c>
+      <c r="B61" s="55"/>
     </row>
     <row r="62">
       <c r="A62" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>34</v>
-      </c>
-      <c r="B62" s="51"/>
+        <v>32</v>
+      </c>
+      <c r="B62" s="55"/>
     </row>
     <row r="63">
       <c r="A63" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>35</v>
-      </c>
-      <c r="B63" s="51"/>
+        <v>33</v>
+      </c>
+      <c r="B63" s="55"/>
     </row>
     <row r="64">
       <c r="A64" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>36</v>
-      </c>
-      <c r="B64" s="51"/>
+        <v>34</v>
+      </c>
+      <c r="B64" s="55"/>
     </row>
     <row r="65">
       <c r="A65" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>37</v>
-      </c>
-      <c r="B65" s="51"/>
+        <v>35</v>
+      </c>
+      <c r="B65" s="55"/>
     </row>
     <row r="66">
       <c r="A66" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>38</v>
-      </c>
-      <c r="B66" s="51"/>
+        <v>36</v>
+      </c>
+      <c r="B66" s="55"/>
     </row>
     <row r="67">
       <c r="A67" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>39</v>
-      </c>
-      <c r="B67" s="51"/>
+        <v>37</v>
+      </c>
+      <c r="B67" s="55"/>
     </row>
     <row r="68">
       <c r="A68" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
-        <v>40</v>
-      </c>
-      <c r="B68" s="51"/>
+        <v>38</v>
+      </c>
+      <c r="B68" s="55"/>
     </row>
     <row r="69">
       <c r="A69" s="37">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>39</v>
+      </c>
+      <c r="B69" s="55"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="37">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
+        <v>40</v>
+      </c>
+      <c r="B70" s="55"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="37">
+        <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>41</v>
       </c>
-      <c r="B69" s="51"/>
+      <c r="B71" s="55"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E19:E22">
+    <dataValidation type="list" allowBlank="1" sqref="E21:E24">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C14:D16 C19:D22 C25">
+    <dataValidation type="list" allowBlank="1" sqref="C16:D18 C21:D24 C27">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -6225,7 +6729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6246,23 +6750,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>598</v>
+        <v>619</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>599</v>
+        <v>620</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>600</v>
+        <v>621</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>601</v>
+        <v>622</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>602</v>
-      </c>
-      <c r="B2" s="52">
+        <v>623</v>
+      </c>
+      <c r="B2" s="56">
         <v>1.0</v>
       </c>
       <c r="C2" s="28" t="b">
@@ -6274,9 +6778,9 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>603</v>
-      </c>
-      <c r="B3" s="52">
+        <v>624</v>
+      </c>
+      <c r="B3" s="56">
         <v>1.0</v>
       </c>
       <c r="C3" s="28" t="b">
@@ -6288,9 +6792,9 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>604</v>
-      </c>
-      <c r="B4" s="52">
+        <v>625</v>
+      </c>
+      <c r="B4" s="56">
         <v>3.0</v>
       </c>
       <c r="C4" s="28" t="b">
@@ -6302,9 +6806,9 @@
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>605</v>
-      </c>
-      <c r="B5" s="52">
+        <v>626</v>
+      </c>
+      <c r="B5" s="56">
         <v>1.0</v>
       </c>
       <c r="C5" s="28" t="b">
@@ -6316,9 +6820,9 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>606</v>
-      </c>
-      <c r="B6" s="52">
+        <v>627</v>
+      </c>
+      <c r="B6" s="56">
         <v>3.0</v>
       </c>
       <c r="C6" s="28" t="b">
@@ -6330,9 +6834,9 @@
     </row>
     <row r="7">
       <c r="A7" s="28" t="s">
-        <v>607</v>
-      </c>
-      <c r="B7" s="52">
+        <v>628</v>
+      </c>
+      <c r="B7" s="56">
         <v>3.0</v>
       </c>
       <c r="C7" s="28" t="b">
@@ -6344,9 +6848,9 @@
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>608</v>
-      </c>
-      <c r="B8" s="52">
+        <v>629</v>
+      </c>
+      <c r="B8" s="56">
         <v>5.0</v>
       </c>
       <c r="C8" s="28" t="b">
@@ -6358,9 +6862,9 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>609</v>
-      </c>
-      <c r="B9" s="52">
+        <v>630</v>
+      </c>
+      <c r="B9" s="56">
         <v>4.0</v>
       </c>
       <c r="C9" s="28" t="b">
@@ -6372,9 +6876,9 @@
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>610</v>
-      </c>
-      <c r="B10" s="52">
+        <v>631</v>
+      </c>
+      <c r="B10" s="56">
         <v>5.0</v>
       </c>
       <c r="C10" s="28" t="b">
@@ -6386,9 +6890,9 @@
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>611</v>
-      </c>
-      <c r="B11" s="52">
+        <v>632</v>
+      </c>
+      <c r="B11" s="56">
         <v>4.0</v>
       </c>
       <c r="C11" s="28" t="b">
@@ -6400,9 +6904,9 @@
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
-        <v>612</v>
-      </c>
-      <c r="B12" s="52">
+        <v>633</v>
+      </c>
+      <c r="B12" s="56">
         <v>1.0</v>
       </c>
       <c r="C12" s="28" t="b">
@@ -6414,9 +6918,9 @@
     </row>
     <row r="13">
       <c r="A13" s="28" t="s">
-        <v>613</v>
-      </c>
-      <c r="B13" s="52">
+        <v>634</v>
+      </c>
+      <c r="B13" s="56">
         <v>4.0</v>
       </c>
       <c r="C13" s="28" t="b">
@@ -6428,9 +6932,9 @@
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
-        <v>614</v>
-      </c>
-      <c r="B14" s="52">
+        <v>635</v>
+      </c>
+      <c r="B14" s="56">
         <v>1.0</v>
       </c>
       <c r="C14" s="28" t="b">
@@ -6442,9 +6946,9 @@
     </row>
     <row r="15">
       <c r="A15" s="28" t="s">
-        <v>615</v>
-      </c>
-      <c r="B15" s="52">
+        <v>636</v>
+      </c>
+      <c r="B15" s="56">
         <v>2.0</v>
       </c>
       <c r="C15" s="28" t="b">
@@ -6456,9 +6960,9 @@
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
-        <v>616</v>
-      </c>
-      <c r="B16" s="52">
+        <v>637</v>
+      </c>
+      <c r="B16" s="56">
         <v>3.0</v>
       </c>
       <c r="C16" s="28" t="b">
@@ -6470,9 +6974,9 @@
     </row>
     <row r="17">
       <c r="A17" s="28" t="s">
-        <v>617</v>
-      </c>
-      <c r="B17" s="52">
+        <v>638</v>
+      </c>
+      <c r="B17" s="56">
         <v>2.0</v>
       </c>
       <c r="C17" s="28" t="b">
@@ -6484,9 +6988,9 @@
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
-        <v>618</v>
-      </c>
-      <c r="B18" s="52">
+        <v>639</v>
+      </c>
+      <c r="B18" s="56">
         <v>2.0</v>
       </c>
       <c r="C18" s="28" t="b">
@@ -6498,9 +7002,9 @@
     </row>
     <row r="19">
       <c r="A19" s="28" t="s">
-        <v>619</v>
-      </c>
-      <c r="B19" s="52">
+        <v>640</v>
+      </c>
+      <c r="B19" s="56">
         <v>2.0</v>
       </c>
       <c r="C19" s="28" t="b">
@@ -6512,9 +7016,9 @@
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
-        <v>620</v>
-      </c>
-      <c r="B20" s="52">
+        <v>641</v>
+      </c>
+      <c r="B20" s="56">
         <v>2.0</v>
       </c>
       <c r="C20" s="28" t="b">
@@ -6526,9 +7030,9 @@
     </row>
     <row r="21">
       <c r="A21" s="28" t="s">
-        <v>621</v>
-      </c>
-      <c r="B21" s="52">
+        <v>642</v>
+      </c>
+      <c r="B21" s="56">
         <v>3.0</v>
       </c>
       <c r="C21" s="28" t="b">
@@ -6540,9 +7044,9 @@
     </row>
     <row r="22">
       <c r="A22" s="28" t="s">
-        <v>622</v>
-      </c>
-      <c r="B22" s="52">
+        <v>643</v>
+      </c>
+      <c r="B22" s="56">
         <v>2.0</v>
       </c>
       <c r="C22" s="28" t="b">
@@ -6554,9 +7058,9 @@
     </row>
     <row r="23">
       <c r="A23" s="28" t="s">
-        <v>623</v>
-      </c>
-      <c r="B23" s="52">
+        <v>644</v>
+      </c>
+      <c r="B23" s="56">
         <v>2.0</v>
       </c>
       <c r="C23" s="28" t="b">
@@ -6568,9 +7072,9 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>624</v>
-      </c>
-      <c r="B24" s="52">
+        <v>645</v>
+      </c>
+      <c r="B24" s="56">
         <v>2.0</v>
       </c>
       <c r="C24" s="28" t="b">
@@ -6582,9 +7086,9 @@
     </row>
     <row r="25">
       <c r="A25" s="28" t="s">
-        <v>625</v>
-      </c>
-      <c r="B25" s="52">
+        <v>646</v>
+      </c>
+      <c r="B25" s="56">
         <v>2.0</v>
       </c>
       <c r="C25" s="28" t="b">
@@ -6596,9 +7100,9 @@
     </row>
     <row r="26">
       <c r="A26" s="28" t="s">
-        <v>626</v>
-      </c>
-      <c r="B26" s="52">
+        <v>647</v>
+      </c>
+      <c r="B26" s="56">
         <v>2.0</v>
       </c>
       <c r="C26" s="28" t="b">
@@ -6610,9 +7114,9 @@
     </row>
     <row r="27">
       <c r="A27" s="28" t="s">
-        <v>627</v>
-      </c>
-      <c r="B27" s="52">
+        <v>648</v>
+      </c>
+      <c r="B27" s="56">
         <v>2.0</v>
       </c>
       <c r="C27" s="28" t="b">
@@ -6624,9 +7128,9 @@
     </row>
     <row r="28">
       <c r="A28" s="28" t="s">
-        <v>628</v>
-      </c>
-      <c r="B28" s="52">
+        <v>649</v>
+      </c>
+      <c r="B28" s="56">
         <v>2.0</v>
       </c>
       <c r="C28" s="28" t="b">
@@ -6638,9 +7142,9 @@
     </row>
     <row r="29">
       <c r="A29" s="28" t="s">
-        <v>629</v>
-      </c>
-      <c r="B29" s="52">
+        <v>650</v>
+      </c>
+      <c r="B29" s="56">
         <v>4.0</v>
       </c>
       <c r="C29" s="28" t="b">
@@ -6652,9 +7156,9 @@
     </row>
     <row r="30">
       <c r="A30" s="28" t="s">
-        <v>630</v>
-      </c>
-      <c r="B30" s="52">
+        <v>651</v>
+      </c>
+      <c r="B30" s="56">
         <v>2.0</v>
       </c>
       <c r="C30" s="28" t="b">
@@ -6666,9 +7170,9 @@
     </row>
     <row r="31">
       <c r="A31" s="28" t="s">
-        <v>470</v>
-      </c>
-      <c r="B31" s="52">
+        <v>486</v>
+      </c>
+      <c r="B31" s="56">
         <v>5.0</v>
       </c>
       <c r="C31" s="28" t="b">
@@ -6709,7 +7213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FFB45F06"/>
@@ -6728,186 +7232,186 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="53" t="s">
-        <v>631</v>
-      </c>
-      <c r="B1" s="53" t="s">
-        <v>632</v>
-      </c>
-      <c r="D1" s="53" t="s">
-        <v>633</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>632</v>
+      <c r="A1" s="57" t="s">
+        <v>652</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>653</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>654</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="54" t="str">
+      <c r="A2" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"SPRITE_ITEM_CARDS_PICKABLE")</f>
         <v>SPRITE_ITEM_CARDS_PICKABLE</v>
       </c>
-      <c r="B2" s="54" t="str">
+      <c r="B2" s="58" t="str">
         <f t="array" ref="B2:B17">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
         <v/>
       </c>
-      <c r="D2" s="54" t="str">
+      <c r="D2" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"NAME_ITEM_CARDS")</f>
         <v>NAME_ITEM_CARDS</v>
       </c>
-      <c r="E2" s="54" t="str">
+      <c r="E2" s="58" t="str">
         <f t="array" ref="E2:E17">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
         <v/>
       </c>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="54" t="str">
+      <c r="A3" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_BLANK")</f>
         <v>SPRITE_BLANK</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="54" t="str">
+      <c r="D3" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_AD_BOARD")</f>
         <v>NAME_ITEM_AD_BOARD</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" ht="22.5" customHeight="1">
-      <c r="A4" s="54" t="str">
+      <c r="A4" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_BLANK")</f>
         <v>SPRITE_BLANK</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="54" t="str">
+      <c r="D4" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_CROSS")</f>
         <v>NAME_ITEM_CROSS</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
-      <c r="A5" s="54" t="str">
+      <c r="A5" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_BLANK")</f>
         <v>SPRITE_BLANK</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="54" t="str">
+      <c r="D5" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_BASIN")</f>
         <v>NAME_ITEM_BASIN</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="58" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
-      <c r="A6" s="54" t="str">
+      <c r="A6" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_PICKABLE_SOAP")</f>
         <v>SPRITE_PICKABLE_SOAP</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="54" t="str">
+      <c r="D6" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_SOAP")</f>
         <v>NAME_ITEM_SOAP</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" ht="22.5" customHeight="1">
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" ht="22.5" customHeight="1">
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="22.5" customHeight="1">
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" ht="22.5" customHeight="1">
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="54" t="s">
+      <c r="E12" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="58" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="58" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="15" ht="22.5" customHeight="1">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="16" ht="22.5" customHeight="1">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="58" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="17" ht="22.5" customHeight="1">
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="54" t="s">
+      <c r="E17" s="58" t="s">
         <v>20</v>
       </c>
     </row>
@@ -11382,6 +11886,151 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="33.43"/>
+    <col customWidth="1" min="3" max="3" width="45.43"/>
+    <col customWidth="1" min="4" max="4" width="37.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="28">
+        <f>ROW()-ROW(Table_Decisions[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="28">
+        <f>ROW()-ROW(Table_Decisions[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>437</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>438</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="42">
+        <f>ROW()-ROW(Table_Decision_Options[N])</f>
+        <v>0</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="42">
+        <f>ROW()-ROW(Table_Decision_Options[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>441</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="42">
+        <f>ROW()-ROW(Table_Decision_Options[N])</f>
+        <v>2</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>444</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>445</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="42">
+        <f>ROW()-ROW(Table_Decision_Options[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C3 D6:D9">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C6:C9">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <tabColor rgb="FF20124D"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -11396,17 +12045,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>431</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>432</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>433</v>
+      <c r="B1" s="45" t="s">
+        <v>447</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="2">
@@ -11417,8 +12066,8 @@
       <c r="B2" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3">
       <c r="A3" s="22">
@@ -11429,10 +12078,10 @@
         <v>213</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>434</v>
+        <v>450</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>434</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4">
@@ -11441,13 +12090,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>435</v>
+        <v>451</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>437</v>
+        <v>453</v>
       </c>
     </row>
     <row r="5">
@@ -11456,13 +12105,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>438</v>
+        <v>454</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>440</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6">
@@ -11471,13 +12120,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>441</v>
+        <v>457</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>442</v>
+        <v>458</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>443</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7">
@@ -11489,10 +12138,10 @@
         <v>216</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>444</v>
+        <v>460</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>445</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8">
@@ -11504,10 +12153,10 @@
         <v>237</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>446</v>
+        <v>462</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>446</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9">
@@ -11519,10 +12168,10 @@
         <v>244</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>447</v>
+        <v>463</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>448</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10">
@@ -11534,10 +12183,10 @@
         <v>222</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>449</v>
+        <v>465</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>450</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11">
@@ -11546,13 +12195,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>451</v>
+        <v>467</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>453</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12">
@@ -11561,13 +12210,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>454</v>
+        <v>470</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>455</v>
+        <v>471</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>456</v>
+        <v>472</v>
       </c>
     </row>
     <row r="13">
@@ -11579,10 +12228,10 @@
         <v>227</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>457</v>
+        <v>473</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14">
@@ -11594,10 +12243,10 @@
         <v>234</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>460</v>
+        <v>476</v>
       </c>
     </row>
     <row r="15">
@@ -11606,13 +12255,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>461</v>
+        <v>477</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>462</v>
+        <v>478</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>463</v>
+        <v>479</v>
       </c>
     </row>
     <row r="16">
@@ -11624,10 +12273,10 @@
         <v>247</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>464</v>
+        <v>480</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>465</v>
+        <v>481</v>
       </c>
     </row>
     <row r="17">
@@ -11639,10 +12288,10 @@
         <v>252</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>466</v>
+        <v>482</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>467</v>
+        <v>483</v>
       </c>
     </row>
     <row r="18">
@@ -11654,10 +12303,10 @@
         <v>255</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>468</v>
+        <v>484</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>469</v>
+        <v>485</v>
       </c>
     </row>
     <row r="19">
@@ -11669,10 +12318,10 @@
         <v>259</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>470</v>
+        <v>486</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>471</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -11683,7 +12332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF674EA7"/>
@@ -11709,22 +12358,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>472</v>
+        <v>488</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>473</v>
+        <v>489</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>474</v>
+        <v>490</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>475</v>
+        <v>491</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>476</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>477</v>
+        <v>492</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="2">
@@ -11742,9 +12391,9 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>478</v>
-      </c>
-      <c r="F2" s="44"/>
+        <v>494</v>
+      </c>
+      <c r="F2" s="48"/>
       <c r="G2" s="29"/>
     </row>
     <row r="3">
@@ -11753,7 +12402,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>479</v>
+        <v>495</v>
       </c>
       <c r="C3" s="28">
         <v>0.0</v>
@@ -11762,13 +12411,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>481</v>
+        <v>497</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>482</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4">
@@ -11777,7 +12426,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>483</v>
+        <v>499</v>
       </c>
       <c r="C4" s="28">
         <v>0.0</v>
@@ -11786,13 +12435,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>484</v>
+        <v>500</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>485</v>
+        <v>501</v>
       </c>
     </row>
     <row r="5">
@@ -11801,7 +12450,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>486</v>
+        <v>502</v>
       </c>
       <c r="C5" s="28">
         <v>0.0</v>
@@ -11810,13 +12459,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>487</v>
+        <v>503</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>488</v>
+        <v>504</v>
       </c>
     </row>
     <row r="6">
@@ -11825,7 +12474,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>489</v>
+        <v>505</v>
       </c>
       <c r="C6" s="28">
         <v>0.0</v>
@@ -11834,13 +12483,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>490</v>
+        <v>506</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>491</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7">
@@ -11849,7 +12498,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>492</v>
+        <v>508</v>
       </c>
       <c r="C7" s="28">
         <v>0.0</v>
@@ -11858,13 +12507,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>493</v>
+        <v>509</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>494</v>
+        <v>510</v>
       </c>
     </row>
     <row r="8">
@@ -11882,13 +12531,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>495</v>
+        <v>511</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>496</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9">
@@ -11897,7 +12546,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>497</v>
+        <v>513</v>
       </c>
       <c r="C9" s="28">
         <v>0.0</v>
@@ -11906,13 +12555,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>498</v>
+        <v>514</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>499</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10">
@@ -11921,7 +12570,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>500</v>
+        <v>516</v>
       </c>
       <c r="C10" s="28">
         <v>0.0</v>
@@ -11930,13 +12579,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>501</v>
+        <v>517</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>502</v>
+        <v>518</v>
       </c>
     </row>
     <row r="11">
@@ -11945,7 +12594,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="C11" s="28">
         <v>1.0</v>
@@ -11954,13 +12603,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>504</v>
+        <v>520</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>505</v>
+        <v>521</v>
       </c>
     </row>
     <row r="12">
@@ -11969,7 +12618,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>506</v>
+        <v>522</v>
       </c>
       <c r="C12" s="28">
         <v>0.0</v>
@@ -11978,13 +12627,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>507</v>
+        <v>523</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>508</v>
+        <v>524</v>
       </c>
     </row>
     <row r="13">
@@ -11993,7 +12642,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>509</v>
+        <v>525</v>
       </c>
       <c r="C13" s="28">
         <v>0.0</v>
@@ -12002,13 +12651,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>510</v>
+        <v>526</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>511</v>
+        <v>527</v>
       </c>
     </row>
     <row r="14">
@@ -12017,7 +12666,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="C14" s="28">
         <v>1.0</v>
@@ -12026,13 +12675,13 @@
         <v>0.0</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>513</v>
+        <v>529</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>514</v>
+        <v>530</v>
       </c>
     </row>
     <row r="15">
@@ -12041,7 +12690,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>515</v>
+        <v>531</v>
       </c>
       <c r="C15" s="28">
         <v>1.0</v>
@@ -12050,13 +12699,13 @@
         <v>0.0</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>517</v>
+        <v>533</v>
       </c>
     </row>
     <row r="16">
@@ -12074,13 +12723,13 @@
         <v>0.0</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>518</v>
+        <v>534</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>519</v>
+        <v>535</v>
       </c>
     </row>
     <row r="17">
@@ -12089,7 +12738,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
       <c r="C17" s="28">
         <v>0.0</v>
@@ -12098,13 +12747,13 @@
         <v>0.0</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>522</v>
+        <v>538</v>
       </c>
     </row>
     <row r="18">
@@ -12122,13 +12771,13 @@
         <v>0.0</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>523</v>
+        <v>539</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>524</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19">
@@ -12146,13 +12795,13 @@
         <v>0.0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>525</v>
+        <v>541</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>526</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20">
@@ -12170,13 +12819,13 @@
         <v>0.0</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>527</v>
+        <v>543</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>528</v>
+        <v>544</v>
       </c>
     </row>
     <row r="21">
@@ -12194,13 +12843,13 @@
         <v>0.0</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>529</v>
+        <v>545</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>530</v>
+        <v>546</v>
       </c>
     </row>
     <row r="22">
@@ -12218,13 +12867,13 @@
         <v>0.0</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>531</v>
+        <v>547</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>532</v>
+        <v>548</v>
       </c>
     </row>
     <row r="23">
@@ -12242,13 +12891,13 @@
         <v>0.0</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>533</v>
+        <v>549</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>534</v>
+        <v>550</v>
       </c>
     </row>
     <row r="24">
@@ -12266,13 +12915,13 @@
         <v>0.0</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>535</v>
+        <v>551</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>536</v>
+        <v>552</v>
       </c>
     </row>
     <row r="25">
@@ -12290,13 +12939,13 @@
         <v>0.0</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>537</v>
+        <v>553</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>538</v>
+        <v>554</v>
       </c>
     </row>
     <row r="26">
@@ -12305,7 +12954,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>539</v>
+        <v>555</v>
       </c>
       <c r="C26" s="28">
         <v>0.0</v>
@@ -12314,13 +12963,13 @@
         <v>0.0</v>
       </c>
       <c r="E26" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>540</v>
+        <v>556</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>541</v>
+        <v>557</v>
       </c>
     </row>
     <row r="27">
@@ -12329,7 +12978,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>542</v>
+        <v>558</v>
       </c>
       <c r="C27" s="28">
         <v>1.0</v>
@@ -12338,377 +12987,90 @@
         <v>0.0</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>543</v>
+        <v>559</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>544</v>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>26</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="C28" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="D28" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>496</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>561</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>27</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>442</v>
+      </c>
+      <c r="C29" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="D29" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>496</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>563</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="28">
+        <f>ROW()-ROW(Table_Phrases[N])</f>
+        <v>28</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="C30" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="D30" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>496</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>565</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>566</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E27">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="20.0"/>
-    <col customWidth="1" min="3" max="3" width="38.29"/>
-    <col customWidth="1" min="4" max="5" width="29.86"/>
-    <col customWidth="1" min="6" max="6" width="48.29"/>
-    <col customWidth="1" min="7" max="7" width="41.14"/>
-    <col customWidth="1" min="8" max="8" width="42.86"/>
-    <col customWidth="1" min="9" max="9" width="31.71"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>545</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>546</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>547</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>548</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>549</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>550</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>551</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="2" ht="186.0" customHeight="1">
-      <c r="A2" s="22">
-        <f t="shared" ref="A2:A7" si="1">ROW()-ROW($A$2)-1</f>
-        <v>-1</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="D2" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-G2
-),"", "")
-))
-)
-)"),"SPRITE_NONE")</f>
-        <v>SPRITE_NONE</v>
-      </c>
-      <c r="E2" s="45" t="str">
-        <f t="shared" ref="E2:E7" si="2">SUBSTITUTE(I2,", ","|")</f>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="F2" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-H2
-),"", "")
-))
-)
-)"),"ITEM_NONE")</f>
-        <v>ITEM_NONE</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="3" ht="98.25" customHeight="1">
-      <c r="A3" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>554</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>391</v>
-      </c>
-      <c r="D3" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-G3
-),"", "")
-))
-)
-)"),"BACKGROUND_HIVE1_ROOM1|SPRITE_ITEM_DECO_BED_LAYER")</f>
-        <v>BACKGROUND_HIVE1_ROOM1|SPRITE_ITEM_DECO_BED_LAYER</v>
-      </c>
-      <c r="E3" s="45" t="str">
-        <f t="shared" si="2"/>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="F3" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-H3
-),"", "")
-))
-)
-)"),"ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1|ITEM_HIVE1_PERFUME|ITEM_SOAP_PICKABLE")</f>
-        <v>ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1|ITEM_HIVE1_PERFUME|ITEM_SOAP_PICKABLE</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>555</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>556</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="22">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>400</v>
-      </c>
-      <c r="D4" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-G4
-),"", "")
-))
-)
-)"),"BACKGROUND_HIVE1_CORRIDOR1")</f>
-        <v>BACKGROUND_HIVE1_CORRIDOR1</v>
-      </c>
-      <c r="E4" s="45" t="str">
-        <f t="shared" si="2"/>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="F4" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-H4
-),"", "")
-))
-)
-)"),"ITEM_GENERIC_DOOR1|ITEM_HIVE1_NPC_REME")</f>
-        <v>ITEM_GENERIC_DOOR1|ITEM_HIVE1_NPC_REME</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>400</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>558</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="22">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>559</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>403</v>
-      </c>
-      <c r="D5" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-G5
-),"", "")
-))
-)
-)"),"BACKGROUND_HIVE1_HALL1")</f>
-        <v>BACKGROUND_HIVE1_HALL1</v>
-      </c>
-      <c r="E5" s="45" t="str">
-        <f t="shared" si="2"/>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="F5" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-H5
-),"", "")
-))
-)
-)"),"ITEM_GENERIC_DOOR1|ITEM_GENERIC_DOOR2|ITEM_HIVE1_AD_BOARD|ITEM_HIVE1_EXIT_DOOR")</f>
-        <v>ITEM_GENERIC_DOOR1|ITEM_GENERIC_DOOR2|ITEM_HIVE1_AD_BOARD|ITEM_HIVE1_EXIT_DOOR</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>403</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>560</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="22">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>405</v>
-      </c>
-      <c r="D6" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-G6
-),"", "")
-))
-)
-)"),"BACKGROUND_HIVE1_WC")</f>
-        <v>BACKGROUND_HIVE1_WC</v>
-      </c>
-      <c r="E6" s="45" t="str">
-        <f t="shared" si="2"/>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="F6" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-H6
-),"", "")
-))
-)
-)"),"ITEM_GENERIC_DOOR1|ITEM_HIVE1_BASIN")</f>
-        <v>ITEM_GENERIC_DOOR1|ITEM_HIVE1_BASIN</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>562</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="22">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="D7" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-G7
-),"", "")
-))
-)
-)"),"SPRITE_LAST")</f>
-        <v>SPRITE_LAST</v>
-      </c>
-      <c r="E7" s="45" t="str">
-        <f t="shared" si="2"/>
-        <v>PHRASE_NONSENSE</v>
-      </c>
-      <c r="F7" s="45" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
-TEXTJOIN(""|"",TRUE,
-UNIQUE(TRANSPOSE(
-SPLIT(TEXTJOIN("", "",TRUE,
-H7
-),"", "")
-))
-)
-)"),"ITEM_LAST")</f>
-        <v>ITEM_LAST</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>479</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C7 G2:I7">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E30">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Need to advance plot before game design
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -22,7 +22,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="YFJKiRHnbLaReT0fElVWCmQaqsqOboXpCeFk/pjr01I="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataChecksum="Ase+1se9b+EjWhlP2XrZzGEgrT2jRKe9xel5CRKylSM="/>
     </ext>
   </extLst>
 </workbook>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="697">
   <si>
     <t>N</t>
   </si>
@@ -1287,6 +1287,12 @@
     <t>(NOT)EVENT_LAUNCH_SLEEP_DECISION</t>
   </si>
   <si>
+    <t>UNCHAIN_REME_DAY</t>
+  </si>
+  <si>
+    <t>MOMENT_MORNING</t>
+  </si>
+  <si>
     <t>SPRITE_ID</t>
   </si>
   <si>
@@ -1407,6 +1413,36 @@
     <t>SPRITE_ATLAS_PICKABLE_0[SPRITE_PICKABLE_SOAP]</t>
   </si>
   <si>
+    <t>BACKGROUND_HIVE1_CORRIDOR1_N</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_4[BACKGROUND_HIVE1_CORRIDOR1_NIGHT]</t>
+  </si>
+  <si>
+    <t>BACKGROUND_HIVE1_HALL1_N</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_5[BACKGROUND_HIVE1_HALL1_NIGHT]</t>
+  </si>
+  <si>
+    <t>BACKGROUND_HIVE1_WC_N</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_HIVE1_6[BACKGROUND_HIVE1_WC_NIGHT]</t>
+  </si>
+  <si>
+    <t>BACKGROUND_CITY1_STREET1</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_CITY1_1[BACKGROUND_CITY1_STREET1]</t>
+  </si>
+  <si>
+    <t>BACKGROUND_CITY1_STREET1_N</t>
+  </si>
+  <si>
+    <t>SPRITE_ATLAS_CITY1_2[BACKGROUND_CITY1_STREET1_NIGHT]</t>
+  </si>
+  <si>
     <t>DIALOG_ID</t>
   </si>
   <si>
@@ -1506,7 +1542,7 @@
     <t>PHRASE_DECISION_SLEEP_NAP</t>
   </si>
   <si>
-    <t>EVENT_PENDING_SLEEP_NAP</t>
+    <t>EVENT_MASTER_PENDING_SLEEP_NAP</t>
   </si>
   <si>
     <t>DECISION_OPTION_SLEEP_LONG</t>
@@ -1515,7 +1551,7 @@
     <t>PHRASE_DECISION_SLEEP_LONG</t>
   </si>
   <si>
-    <t>EVENT_PENDING_SLEEP_LONG</t>
+    <t>EVENT_MASTER_PENDING_SLEEP_LONG</t>
   </si>
   <si>
     <t>NAME_ID</t>
@@ -1926,21 +1962,36 @@
     <t>HIVE1_CORRIDOR_1</t>
   </si>
   <si>
+    <t>BACKGROUND_HIVE1_CORRIDOR1, BACKGROUND_HIVE1_CORRIDOR1_N</t>
+  </si>
+  <si>
     <t>ITEM_GENERIC_DOOR1, ITEM_HIVE1_NPC_REME</t>
   </si>
   <si>
     <t>HIVE1_HALL_1</t>
   </si>
   <si>
+    <t>BACKGROUND_HIVE1_HALL1, BACKGROUND_HIVE1_HALL1_N</t>
+  </si>
+  <si>
     <t>ITEM_GENERIC_DOOR1, ITEM_GENERIC_DOOR2, ITEM_HIVE1_AD_BOARD, ITEM_HIVE1_EXIT_DOOR</t>
   </si>
   <si>
     <t>HIVE1_WC_1</t>
   </si>
   <si>
+    <t>BACKGROUND_HIVE1_WC, BACKGROUND_HIVE1_WC_N</t>
+  </si>
+  <si>
     <t>ITEM_GENERIC_DOOR1, ITEM_HIVE1_BASIN</t>
   </si>
   <si>
+    <t>CITY1_STREET_1</t>
+  </si>
+  <si>
+    <t>BACKGROUND_CITY1_STREET1, BACKGROUND_CITY1_STREET1_N</t>
+  </si>
+  <si>
     <t>ROOM_LAST</t>
   </si>
   <si>
@@ -1987,9 +2038,6 @@
   </si>
   <si>
     <t>MOMENT_TYPE_ID</t>
-  </si>
-  <si>
-    <t>MOMENT_MORNING</t>
   </si>
   <si>
     <t>MOMENT_NIGHT</t>
@@ -2225,7 +2273,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2346,6 +2394,18 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -2370,6 +2430,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -2765,7 +2828,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I7" displayName="Table_Rooms" name="Table_Rooms" id="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I8" displayName="Table_Rooms" name="Table_Rooms" id="13">
   <tableColumns count="9">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ROOM_ID" id="2"/>
@@ -2999,7 +3062,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A24:N45" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A24:N46" displayName="Table_Unchain_Conditions" name="Table_Unchain_Conditions" id="5">
   <tableColumns count="14">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_ID" id="2"/>
@@ -3021,7 +3084,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C26" displayName="Table_sprites" name="Table_sprites" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C31" displayName="Table_sprites" name="Table_sprites" id="6">
   <tableColumns count="3">
     <tableColumn name="N" id="1"/>
     <tableColumn name="SPRITE_ID" id="2"/>
@@ -5313,7 +5376,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="20.0"/>
-    <col customWidth="1" min="3" max="3" width="38.29"/>
+    <col customWidth="1" min="3" max="3" width="45.71"/>
     <col customWidth="1" min="4" max="5" width="29.86"/>
     <col customWidth="1" min="6" max="6" width="48.29"/>
     <col customWidth="1" min="7" max="7" width="41.14"/>
@@ -5326,42 +5389,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>589</v>
+        <v>601</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>591</v>
+        <v>603</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>592</v>
+        <v>604</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>593</v>
+        <v>605</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>594</v>
+        <v>606</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>595</v>
+        <v>607</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>596</v>
+        <v>608</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
       <c r="A2" s="22">
-        <f t="shared" ref="A2:A7" si="1">ROW()-ROW($A$2)-1</f>
+        <f t="shared" ref="A2:A8" si="1">ROW()-ROW($A$2)-1</f>
         <v>-1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="C2" s="22" t="s">
+        <v>609</v>
+      </c>
+      <c r="C2" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="D2" s="49" t="str">
+      <c r="D2" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5373,11 +5436,11 @@
 )"),"SPRITE_NONE")</f>
         <v>SPRITE_NONE</v>
       </c>
-      <c r="E2" s="49" t="str">
-        <f t="shared" ref="E2:E7" si="2">SUBSTITUTE(I2,", ","|")</f>
+      <c r="E2" s="54" t="str">
+        <f t="shared" ref="E2:E8" si="2">SUBSTITUTE(I2,", ","|")</f>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="F2" s="49" t="str">
+      <c r="F2" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5396,7 +5459,7 @@
         <v>215</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3">
@@ -5405,12 +5468,12 @@
         <v>0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>598</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>411</v>
-      </c>
-      <c r="D3" s="49" t="str">
+        <v>610</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5422,11 +5485,11 @@
 )"),"BACKGROUND_HIVE1_ROOM1|SPRITE_ITEM_DECO_BED_LAYER")</f>
         <v>BACKGROUND_HIVE1_ROOM1|SPRITE_ITEM_DECO_BED_LAYER</v>
       </c>
-      <c r="E3" s="49" t="str">
+      <c r="E3" s="54" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE|PHRASE_DECISION_NOT_SLEEP|PHRASE_DECISION_SLEEP_NAP|PHRASE_DECISION_SLEEP_LONG</v>
       </c>
-      <c r="F3" s="49" t="str">
+      <c r="F3" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5439,13 +5502,13 @@
         <v>ITEM_CARDS_PICKABLE|ITEM_HIVE1_CHEST|ITEM_HIVE1_WARDROBE|ITEM_HIVE1_WARDROBE_OPENED|ITEM_GENERIC_DOOR1|ITEM_HIVE1_PERFUME|ITEM_SOAP_PICKABLE|ITEM_HIVE1_BED</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>599</v>
+        <v>611</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>600</v>
+        <v>612</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>601</v>
+        <v>613</v>
       </c>
     </row>
     <row r="4">
@@ -5454,12 +5517,12 @@
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="D4" s="49" t="str">
+        <v>614</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>615</v>
+      </c>
+      <c r="D4" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5468,14 +5531,14 @@
 ),"", "")
 ))
 )
-)"),"BACKGROUND_HIVE1_CORRIDOR1")</f>
-        <v>BACKGROUND_HIVE1_CORRIDOR1</v>
-      </c>
-      <c r="E4" s="49" t="str">
+)"),"BACKGROUND_HIVE1_CORRIDOR1|BACKGROUND_HIVE1_CORRIDOR1_N")</f>
+        <v>BACKGROUND_HIVE1_CORRIDOR1|BACKGROUND_HIVE1_CORRIDOR1_N</v>
+      </c>
+      <c r="E4" s="54" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="F4" s="49" t="str">
+      <c r="F4" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5488,13 +5551,13 @@
         <v>ITEM_GENERIC_DOOR1|ITEM_HIVE1_NPC_REME</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>420</v>
+        <v>615</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>603</v>
+        <v>616</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
     </row>
     <row r="5">
@@ -5503,12 +5566,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>604</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="D5" s="49" t="str">
+        <v>617</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>618</v>
+      </c>
+      <c r="D5" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5517,14 +5580,14 @@
 ),"", "")
 ))
 )
-)"),"BACKGROUND_HIVE1_HALL1")</f>
-        <v>BACKGROUND_HIVE1_HALL1</v>
-      </c>
-      <c r="E5" s="49" t="str">
+)"),"BACKGROUND_HIVE1_HALL1|BACKGROUND_HIVE1_HALL1_N")</f>
+        <v>BACKGROUND_HIVE1_HALL1|BACKGROUND_HIVE1_HALL1_N</v>
+      </c>
+      <c r="E5" s="54" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="F5" s="49" t="str">
+      <c r="F5" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5537,13 +5600,13 @@
         <v>ITEM_GENERIC_DOOR1|ITEM_GENERIC_DOOR2|ITEM_HIVE1_AD_BOARD|ITEM_HIVE1_EXIT_DOOR</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>423</v>
+        <v>618</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>605</v>
+        <v>619</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
     </row>
     <row r="6">
@@ -5552,12 +5615,12 @@
         <v>3</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>606</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>425</v>
-      </c>
-      <c r="D6" s="49" t="str">
+        <v>620</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>621</v>
+      </c>
+      <c r="D6" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5566,14 +5629,14 @@
 ),"", "")
 ))
 )
-)"),"BACKGROUND_HIVE1_WC")</f>
-        <v>BACKGROUND_HIVE1_WC</v>
-      </c>
-      <c r="E6" s="49" t="str">
+)"),"BACKGROUND_HIVE1_WC|BACKGROUND_HIVE1_WC_N")</f>
+        <v>BACKGROUND_HIVE1_WC|BACKGROUND_HIVE1_WC_N</v>
+      </c>
+      <c r="E6" s="54" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="F6" s="49" t="str">
+      <c r="F6" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5586,13 +5649,13 @@
         <v>ITEM_GENERIC_DOOR1|ITEM_HIVE1_BASIN</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>425</v>
+        <v>621</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>607</v>
+        <v>622</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7">
@@ -5601,12 +5664,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>608</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="D7" s="49" t="str">
+        <v>623</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>624</v>
+      </c>
+      <c r="D7" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5615,14 +5678,14 @@
 ),"", "")
 ))
 )
-)"),"SPRITE_LAST")</f>
-        <v>SPRITE_LAST</v>
-      </c>
-      <c r="E7" s="49" t="str">
+)"),"BACKGROUND_CITY1_STREET1|BACKGROUND_CITY1_STREET1_N")</f>
+        <v>BACKGROUND_CITY1_STREET1|BACKGROUND_CITY1_STREET1_N</v>
+      </c>
+      <c r="E7" s="54" t="str">
         <f t="shared" si="2"/>
         <v>PHRASE_NONSENSE</v>
       </c>
-      <c r="F7" s="49" t="str">
+      <c r="F7" s="54" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
 TEXTJOIN(""|"",TRUE,
 UNIQUE(TRANSPOSE(
@@ -5631,22 +5694,71 @@
 ),"", "")
 ))
 )
+)"),"ITEM_GENERIC_DOOR1")</f>
+        <v>ITEM_GENERIC_DOOR1</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>624</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="22">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>625</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="D8" s="54" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+G8
+),"", "")
+))
+)
+)"),"SPRITE_LAST")</f>
+        <v>SPRITE_LAST</v>
+      </c>
+      <c r="E8" s="54" t="str">
+        <f t="shared" si="2"/>
+        <v>PHRASE_NONSENSE</v>
+      </c>
+      <c r="F8" s="54" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(
+TEXTJOIN(""|"",TRUE,
+UNIQUE(TRANSPOSE(
+SPLIT(TEXTJOIN("", "",TRUE,
+H8
+),"", "")
+))
+)
 )"),"ITEM_LAST")</f>
         <v>ITEM_LAST</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G8" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H8" s="27" t="s">
         <v>269</v>
       </c>
-      <c r="I7" s="27" t="s">
-        <v>517</v>
+      <c r="I8" s="27" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C7 G2:I7">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C8 G2:I8">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -5683,7 +5795,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>609</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2">
@@ -5710,7 +5822,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>610</v>
+        <v>627</v>
       </c>
     </row>
     <row r="5">
@@ -5719,7 +5831,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>611</v>
+        <v>628</v>
       </c>
     </row>
     <row r="6">
@@ -5731,7 +5843,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>612</v>
+        <v>629</v>
       </c>
     </row>
     <row r="8">
@@ -5779,7 +5891,7 @@
         <v>5.0</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
     </row>
     <row r="15">
@@ -5787,7 +5899,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>614</v>
+        <v>631</v>
       </c>
     </row>
     <row r="16">
@@ -5805,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>615</v>
+        <v>632</v>
       </c>
     </row>
     <row r="18">
@@ -5858,7 +5970,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>616</v>
+        <v>633</v>
       </c>
     </row>
     <row r="25">
@@ -5894,7 +6006,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>617</v>
+        <v>634</v>
       </c>
     </row>
     <row r="29">
@@ -5921,7 +6033,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>618</v>
+        <v>635</v>
       </c>
     </row>
     <row r="32">
@@ -5939,7 +6051,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>619</v>
+        <v>636</v>
       </c>
     </row>
     <row r="34">
@@ -5966,7 +6078,7 @@
         <v>11</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>620</v>
+        <v>637</v>
       </c>
     </row>
     <row r="38">
@@ -5974,7 +6086,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>621</v>
+        <v>638</v>
       </c>
     </row>
     <row r="39">
@@ -5982,7 +6094,7 @@
         <v>0.0</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
     </row>
     <row r="40">
@@ -5990,7 +6102,7 @@
         <v>1.0</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
     <row r="42">
@@ -5998,7 +6110,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>622</v>
+        <v>639</v>
       </c>
     </row>
     <row r="43">
@@ -6051,7 +6163,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>623</v>
+        <v>640</v>
       </c>
     </row>
     <row r="50">
@@ -6060,7 +6172,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>624</v>
+        <v>391</v>
       </c>
     </row>
     <row r="51">
@@ -6069,7 +6181,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>625</v>
+        <v>641</v>
       </c>
     </row>
     <row r="52">
@@ -6122,7 +6234,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>626</v>
+        <v>642</v>
       </c>
     </row>
     <row r="2">
@@ -6140,7 +6252,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>627</v>
+        <v>643</v>
       </c>
     </row>
     <row r="4">
@@ -6149,7 +6261,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>628</v>
+        <v>644</v>
       </c>
     </row>
     <row r="5">
@@ -6158,7 +6270,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>354</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6">
@@ -6167,7 +6279,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>292</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7">
@@ -6176,7 +6288,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>295</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8">
@@ -6185,7 +6297,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9">
@@ -6194,7 +6306,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10">
@@ -6203,7 +6315,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>330</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11">
@@ -6212,7 +6324,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12">
@@ -6221,7 +6333,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13">
@@ -6230,7 +6342,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14">
@@ -6239,7 +6351,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>463</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15">
@@ -6248,7 +6360,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>466</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16">
@@ -6257,7 +6369,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>629</v>
+        <v>645</v>
       </c>
     </row>
     <row r="18">
@@ -6265,16 +6377,16 @@
         <v>0</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>630</v>
-      </c>
-      <c r="C18" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="C18" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="D18" s="50" t="s">
-        <v>631</v>
-      </c>
-      <c r="E18" s="50" t="s">
-        <v>632</v>
+      <c r="D18" s="55" t="s">
+        <v>647</v>
+      </c>
+      <c r="E18" s="55" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="19">
@@ -6283,7 +6395,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>633</v>
+        <v>649</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>216</v>
@@ -6291,7 +6403,7 @@
       <c r="D19" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="E19" s="51" t="str">
+      <c r="E19" s="56" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B19,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_NONE")</f>
         <v>MEMENTO_NONE</v>
       </c>
@@ -6302,15 +6414,15 @@
         <v>1</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>634</v>
+        <v>650</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>497</v>
+        <v>509</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>427</v>
-      </c>
-      <c r="E20" s="51" t="str">
+        <v>429</v>
+      </c>
+      <c r="E20" s="56" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B20,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_JOB_FIND_1_1|MEMENTO_JOB_FIND_1_2")</f>
         <v>MEMENTO_JOB_FIND_1_1|MEMENTO_JOB_FIND_1_2</v>
       </c>
@@ -6321,7 +6433,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>635</v>
+        <v>651</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>270</v>
@@ -6329,7 +6441,7 @@
       <c r="D21" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="E21" s="51" t="str">
+      <c r="E21" s="56" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(SUBSTITUTE(SUBSTITUTE(JOIN(""|"",UNIQUE(IF(Table_Memento[Parent]=B21,Table_Memento[MEMENTO_ID],""Ñ""))),""Ñ|"",""""),""|Ñ"",""""))"),"MEMENTO_LAST")</f>
         <v>MEMENTO_LAST</v>
       </c>
@@ -6339,19 +6451,19 @@
         <v>0</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>636</v>
-      </c>
-      <c r="C23" s="52" t="s">
-        <v>637</v>
-      </c>
-      <c r="D23" s="52" t="s">
-        <v>458</v>
-      </c>
-      <c r="E23" s="50" t="s">
-        <v>638</v>
-      </c>
-      <c r="F23" s="52" t="s">
-        <v>639</v>
+        <v>652</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>653</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>470</v>
+      </c>
+      <c r="E23" s="55" t="s">
+        <v>654</v>
+      </c>
+      <c r="F23" s="57" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="24">
@@ -6363,13 +6475,13 @@
         <v>356</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>633</v>
+        <v>649</v>
       </c>
       <c r="D24" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="E24" s="53" t="s">
-        <v>640</v>
+      <c r="E24" s="58" t="s">
+        <v>656</v>
       </c>
       <c r="F24" s="39" t="b">
         <v>0</v>
@@ -6384,13 +6496,13 @@
         <v>360</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>634</v>
+        <v>650</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>558</v>
-      </c>
-      <c r="E25" s="53" t="s">
-        <v>640</v>
+        <v>570</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>656</v>
       </c>
       <c r="F25" s="39" t="b">
         <v>0</v>
@@ -6405,13 +6517,13 @@
         <v>382</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>634</v>
+        <v>650</v>
       </c>
       <c r="D26" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="E26" s="53" t="s">
-        <v>640</v>
+      <c r="E26" s="58" t="s">
+        <v>656</v>
       </c>
       <c r="F26" s="39" t="b">
         <v>0</v>
@@ -6423,16 +6535,16 @@
         <v>3</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>641</v>
+        <v>657</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>635</v>
+        <v>651</v>
       </c>
       <c r="D27" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="E27" s="53" t="s">
-        <v>640</v>
+      <c r="E27" s="58" t="s">
+        <v>656</v>
       </c>
       <c r="F27" s="39" t="b">
         <v>0</v>
@@ -6443,10 +6555,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>642</v>
+        <v>658</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>643</v>
+        <v>659</v>
       </c>
     </row>
     <row r="30">
@@ -6455,9 +6567,9 @@
         <v>0</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>640</v>
-      </c>
-      <c r="C30" s="54" t="s">
+        <v>656</v>
+      </c>
+      <c r="C30" s="59" t="s">
         <v>281</v>
       </c>
     </row>
@@ -6466,7 +6578,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>644</v>
+        <v>660</v>
       </c>
     </row>
     <row r="33">
@@ -6474,7 +6586,7 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>0</v>
       </c>
-      <c r="B33" s="55" t="str">
+      <c r="B33" s="60" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(FLATTEN(Table_Events[EVENT_ID],""(NOT)""&amp;Table_Events[EVENT_ID]))"),"EVENT_NONE")</f>
         <v>EVENT_NONE</v>
       </c>
@@ -6484,7 +6596,7 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>1</v>
       </c>
-      <c r="B34" s="55" t="str">
+      <c r="B34" s="60" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_MASTER_CHANGE_ROOM")</f>
         <v>EVENT_MASTER_CHANGE_ROOM</v>
       </c>
@@ -6494,7 +6606,7 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>2</v>
       </c>
-      <c r="B35" s="55" t="str">
+      <c r="B35" s="60" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_MASTER_CHANGE_MOMENT_DAY")</f>
         <v>EVENT_MASTER_CHANGE_MOMENT_DAY</v>
       </c>
@@ -6504,9 +6616,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>3</v>
       </c>
-      <c r="B36" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_FIRST")</f>
-        <v>EVENT_FIRST</v>
+      <c r="B36" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_MASTER_PENDING_SLEEP_NAP")</f>
+        <v>EVENT_MASTER_PENDING_SLEEP_NAP</v>
       </c>
     </row>
     <row r="37">
@@ -6514,9 +6626,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>4</v>
       </c>
-      <c r="B37" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_CHEST_OPENED")</f>
-        <v>EVENT_HIVE1_CHEST_OPENED</v>
+      <c r="B37" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_MASTER_PENDING_SLEEP_LONG")</f>
+        <v>EVENT_MASTER_PENDING_SLEEP_LONG</v>
       </c>
     </row>
     <row r="38">
@@ -6524,9 +6636,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>5</v>
       </c>
-      <c r="B38" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_CARDS_PICKABLE_TAKEN")</f>
-        <v>EVENT_CARDS_PICKABLE_TAKEN</v>
+      <c r="B38" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_FIRST")</f>
+        <v>EVENT_FIRST</v>
       </c>
     </row>
     <row r="39">
@@ -6534,9 +6646,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>6</v>
       </c>
-      <c r="B39" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_WARDROBE_OPENED")</f>
-        <v>EVENT_HIVE1_WARDROBE_OPENED</v>
+      <c r="B39" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_CHEST_OPENED")</f>
+        <v>EVENT_HIVE1_CHEST_OPENED</v>
       </c>
     </row>
     <row r="40">
@@ -6544,9 +6656,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>7</v>
       </c>
-      <c r="B40" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_AD_BOARD_OBSERVED_1")</f>
-        <v>EVENT_HIVE1_AD_BOARD_OBSERVED_1</v>
+      <c r="B40" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_CARDS_PICKABLE_TAKEN")</f>
+        <v>EVENT_CARDS_PICKABLE_TAKEN</v>
       </c>
     </row>
     <row r="41">
@@ -6554,9 +6666,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>8</v>
       </c>
-      <c r="B41" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_USED_PERFUME")</f>
-        <v>EVENT_HIVE1_USED_PERFUME</v>
+      <c r="B41" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_WARDROBE_OPENED")</f>
+        <v>EVENT_HIVE1_WARDROBE_OPENED</v>
       </c>
     </row>
     <row r="42">
@@ -6564,9 +6676,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>9</v>
       </c>
-      <c r="B42" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_USED_BASIN")</f>
-        <v>EVENT_HIVE1_USED_BASIN</v>
+      <c r="B42" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_AD_BOARD_OBSERVED_1")</f>
+        <v>EVENT_HIVE1_AD_BOARD_OBSERVED_1</v>
       </c>
     </row>
     <row r="43">
@@ -6574,9 +6686,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>10</v>
       </c>
-      <c r="B43" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_SOAP_PICKABLE_TAKEN")</f>
-        <v>EVENT_SOAP_PICKABLE_TAKEN</v>
+      <c r="B43" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_USED_PERFUME")</f>
+        <v>EVENT_HIVE1_USED_PERFUME</v>
       </c>
     </row>
     <row r="44">
@@ -6584,9 +6696,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>11</v>
       </c>
-      <c r="B44" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAUNCH_SLEEP_DECISION")</f>
-        <v>EVENT_LAUNCH_SLEEP_DECISION</v>
+      <c r="B44" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_HIVE1_USED_BASIN")</f>
+        <v>EVENT_HIVE1_USED_BASIN</v>
       </c>
     </row>
     <row r="45">
@@ -6594,9 +6706,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>12</v>
       </c>
-      <c r="B45" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_PENDING_SLEEP_NAP")</f>
-        <v>EVENT_PENDING_SLEEP_NAP</v>
+      <c r="B45" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_SOAP_PICKABLE_TAKEN")</f>
+        <v>EVENT_SOAP_PICKABLE_TAKEN</v>
       </c>
     </row>
     <row r="46">
@@ -6604,9 +6716,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>13</v>
       </c>
-      <c r="B46" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_PENDING_SLEEP_LONG")</f>
-        <v>EVENT_PENDING_SLEEP_LONG</v>
+      <c r="B46" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAUNCH_SLEEP_DECISION")</f>
+        <v>EVENT_LAUNCH_SLEEP_DECISION</v>
       </c>
     </row>
     <row r="47">
@@ -6614,7 +6726,7 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>14</v>
       </c>
-      <c r="B47" s="55" t="str">
+      <c r="B47" s="60" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EVENT_LAST")</f>
         <v>EVENT_LAST</v>
       </c>
@@ -6624,7 +6736,7 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>15</v>
       </c>
-      <c r="B48" s="55" t="str">
+      <c r="B48" s="60" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_NONE")</f>
         <v>(NOT)EVENT_NONE</v>
       </c>
@@ -6634,7 +6746,7 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>16</v>
       </c>
-      <c r="B49" s="55" t="str">
+      <c r="B49" s="60" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_MASTER_CHANGE_ROOM")</f>
         <v>(NOT)EVENT_MASTER_CHANGE_ROOM</v>
       </c>
@@ -6644,7 +6756,7 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>17</v>
       </c>
-      <c r="B50" s="55" t="str">
+      <c r="B50" s="60" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_MASTER_CHANGE_MOMENT_DAY")</f>
         <v>(NOT)EVENT_MASTER_CHANGE_MOMENT_DAY</v>
       </c>
@@ -6654,9 +6766,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>18</v>
       </c>
-      <c r="B51" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_FIRST")</f>
-        <v>(NOT)EVENT_FIRST</v>
+      <c r="B51" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_MASTER_PENDING_SLEEP_NAP")</f>
+        <v>(NOT)EVENT_MASTER_PENDING_SLEEP_NAP</v>
       </c>
     </row>
     <row r="52">
@@ -6664,9 +6776,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>19</v>
       </c>
-      <c r="B52" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_CHEST_OPENED")</f>
-        <v>(NOT)EVENT_HIVE1_CHEST_OPENED</v>
+      <c r="B52" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_MASTER_PENDING_SLEEP_LONG")</f>
+        <v>(NOT)EVENT_MASTER_PENDING_SLEEP_LONG</v>
       </c>
     </row>
     <row r="53">
@@ -6674,9 +6786,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>20</v>
       </c>
-      <c r="B53" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_CARDS_PICKABLE_TAKEN")</f>
-        <v>(NOT)EVENT_CARDS_PICKABLE_TAKEN</v>
+      <c r="B53" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_FIRST")</f>
+        <v>(NOT)EVENT_FIRST</v>
       </c>
     </row>
     <row r="54">
@@ -6684,9 +6796,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>21</v>
       </c>
-      <c r="B54" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_WARDROBE_OPENED")</f>
-        <v>(NOT)EVENT_HIVE1_WARDROBE_OPENED</v>
+      <c r="B54" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_CHEST_OPENED")</f>
+        <v>(NOT)EVENT_HIVE1_CHEST_OPENED</v>
       </c>
     </row>
     <row r="55">
@@ -6694,9 +6806,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>22</v>
       </c>
-      <c r="B55" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_AD_BOARD_OBSERVED_1")</f>
-        <v>(NOT)EVENT_HIVE1_AD_BOARD_OBSERVED_1</v>
+      <c r="B55" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_CARDS_PICKABLE_TAKEN")</f>
+        <v>(NOT)EVENT_CARDS_PICKABLE_TAKEN</v>
       </c>
     </row>
     <row r="56">
@@ -6704,9 +6816,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>23</v>
       </c>
-      <c r="B56" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_USED_PERFUME")</f>
-        <v>(NOT)EVENT_HIVE1_USED_PERFUME</v>
+      <c r="B56" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_WARDROBE_OPENED")</f>
+        <v>(NOT)EVENT_HIVE1_WARDROBE_OPENED</v>
       </c>
     </row>
     <row r="57">
@@ -6714,9 +6826,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>24</v>
       </c>
-      <c r="B57" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_USED_BASIN")</f>
-        <v>(NOT)EVENT_HIVE1_USED_BASIN</v>
+      <c r="B57" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_AD_BOARD_OBSERVED_1")</f>
+        <v>(NOT)EVENT_HIVE1_AD_BOARD_OBSERVED_1</v>
       </c>
     </row>
     <row r="58">
@@ -6724,9 +6836,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>25</v>
       </c>
-      <c r="B58" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_SOAP_PICKABLE_TAKEN")</f>
-        <v>(NOT)EVENT_SOAP_PICKABLE_TAKEN</v>
+      <c r="B58" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_USED_PERFUME")</f>
+        <v>(NOT)EVENT_HIVE1_USED_PERFUME</v>
       </c>
     </row>
     <row r="59">
@@ -6734,9 +6846,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>26</v>
       </c>
-      <c r="B59" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAUNCH_SLEEP_DECISION")</f>
-        <v>(NOT)EVENT_LAUNCH_SLEEP_DECISION</v>
+      <c r="B59" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_HIVE1_USED_BASIN")</f>
+        <v>(NOT)EVENT_HIVE1_USED_BASIN</v>
       </c>
     </row>
     <row r="60">
@@ -6744,9 +6856,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>27</v>
       </c>
-      <c r="B60" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_PENDING_SLEEP_NAP")</f>
-        <v>(NOT)EVENT_PENDING_SLEEP_NAP</v>
+      <c r="B60" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_SOAP_PICKABLE_TAKEN")</f>
+        <v>(NOT)EVENT_SOAP_PICKABLE_TAKEN</v>
       </c>
     </row>
     <row r="61">
@@ -6754,9 +6866,9 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>28</v>
       </c>
-      <c r="B61" s="55" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_PENDING_SLEEP_LONG")</f>
-        <v>(NOT)EVENT_PENDING_SLEEP_LONG</v>
+      <c r="B61" s="60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAUNCH_SLEEP_DECISION")</f>
+        <v>(NOT)EVENT_LAUNCH_SLEEP_DECISION</v>
       </c>
     </row>
     <row r="62">
@@ -6764,7 +6876,7 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>29</v>
       </c>
-      <c r="B62" s="55" t="str">
+      <c r="B62" s="60" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"(NOT)EVENT_LAST")</f>
         <v>(NOT)EVENT_LAST</v>
       </c>
@@ -6774,84 +6886,84 @@
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>30</v>
       </c>
-      <c r="B63" s="55"/>
+      <c r="B63" s="60"/>
     </row>
     <row r="64">
       <c r="A64" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>31</v>
       </c>
-      <c r="B64" s="55"/>
+      <c r="B64" s="60"/>
     </row>
     <row r="65">
       <c r="A65" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>32</v>
       </c>
-      <c r="B65" s="55"/>
+      <c r="B65" s="60"/>
     </row>
     <row r="66">
       <c r="A66" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>33</v>
       </c>
-      <c r="B66" s="55"/>
+      <c r="B66" s="60"/>
     </row>
     <row r="67">
       <c r="A67" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>34</v>
       </c>
-      <c r="B67" s="55"/>
+      <c r="B67" s="60"/>
     </row>
     <row r="68">
       <c r="A68" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>35</v>
       </c>
-      <c r="B68" s="55"/>
+      <c r="B68" s="60"/>
     </row>
     <row r="69">
       <c r="A69" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>36</v>
       </c>
-      <c r="B69" s="55"/>
+      <c r="B69" s="60"/>
     </row>
     <row r="70">
       <c r="A70" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>37</v>
       </c>
-      <c r="B70" s="55"/>
+      <c r="B70" s="60"/>
     </row>
     <row r="71">
       <c r="A71" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>38</v>
       </c>
-      <c r="B71" s="55"/>
+      <c r="B71" s="60"/>
     </row>
     <row r="72">
       <c r="A72" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>39</v>
       </c>
-      <c r="B72" s="55"/>
+      <c r="B72" s="60"/>
     </row>
     <row r="73">
       <c r="A73" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>40</v>
       </c>
-      <c r="B73" s="55"/>
+      <c r="B73" s="60"/>
     </row>
     <row r="74">
       <c r="A74" s="38">
         <f>ROW()-ROW(Table_EventsCombi[N])</f>
         <v>41</v>
       </c>
-      <c r="B74" s="55"/>
+      <c r="B74" s="60"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -6894,23 +7006,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>645</v>
+        <v>661</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>646</v>
+        <v>662</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>647</v>
+        <v>663</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>648</v>
+        <v>664</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>649</v>
-      </c>
-      <c r="B2" s="56">
+        <v>665</v>
+      </c>
+      <c r="B2" s="61">
         <v>1.0</v>
       </c>
       <c r="C2" s="28" t="b">
@@ -6922,9 +7034,9 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>650</v>
-      </c>
-      <c r="B3" s="56">
+        <v>666</v>
+      </c>
+      <c r="B3" s="61">
         <v>1.0</v>
       </c>
       <c r="C3" s="28" t="b">
@@ -6936,9 +7048,9 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>651</v>
-      </c>
-      <c r="B4" s="56">
+        <v>667</v>
+      </c>
+      <c r="B4" s="61">
         <v>3.0</v>
       </c>
       <c r="C4" s="28" t="b">
@@ -6950,9 +7062,9 @@
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>652</v>
-      </c>
-      <c r="B5" s="56">
+        <v>668</v>
+      </c>
+      <c r="B5" s="61">
         <v>1.0</v>
       </c>
       <c r="C5" s="28" t="b">
@@ -6964,9 +7076,9 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>653</v>
-      </c>
-      <c r="B6" s="56">
+        <v>669</v>
+      </c>
+      <c r="B6" s="61">
         <v>3.0</v>
       </c>
       <c r="C6" s="28" t="b">
@@ -6978,9 +7090,9 @@
     </row>
     <row r="7">
       <c r="A7" s="28" t="s">
-        <v>654</v>
-      </c>
-      <c r="B7" s="56">
+        <v>670</v>
+      </c>
+      <c r="B7" s="61">
         <v>3.0</v>
       </c>
       <c r="C7" s="28" t="b">
@@ -6992,9 +7104,9 @@
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>655</v>
-      </c>
-      <c r="B8" s="56">
+        <v>671</v>
+      </c>
+      <c r="B8" s="61">
         <v>5.0</v>
       </c>
       <c r="C8" s="28" t="b">
@@ -7006,9 +7118,9 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>656</v>
-      </c>
-      <c r="B9" s="56">
+        <v>672</v>
+      </c>
+      <c r="B9" s="61">
         <v>4.0</v>
       </c>
       <c r="C9" s="28" t="b">
@@ -7020,9 +7132,9 @@
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>657</v>
-      </c>
-      <c r="B10" s="56">
+        <v>673</v>
+      </c>
+      <c r="B10" s="61">
         <v>5.0</v>
       </c>
       <c r="C10" s="28" t="b">
@@ -7034,9 +7146,9 @@
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>658</v>
-      </c>
-      <c r="B11" s="56">
+        <v>674</v>
+      </c>
+      <c r="B11" s="61">
         <v>4.0</v>
       </c>
       <c r="C11" s="28" t="b">
@@ -7048,9 +7160,9 @@
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
-        <v>659</v>
-      </c>
-      <c r="B12" s="56">
+        <v>675</v>
+      </c>
+      <c r="B12" s="61">
         <v>1.0</v>
       </c>
       <c r="C12" s="28" t="b">
@@ -7062,9 +7174,9 @@
     </row>
     <row r="13">
       <c r="A13" s="28" t="s">
-        <v>660</v>
-      </c>
-      <c r="B13" s="56">
+        <v>676</v>
+      </c>
+      <c r="B13" s="61">
         <v>4.0</v>
       </c>
       <c r="C13" s="28" t="b">
@@ -7076,9 +7188,9 @@
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
-        <v>661</v>
-      </c>
-      <c r="B14" s="56">
+        <v>677</v>
+      </c>
+      <c r="B14" s="61">
         <v>1.0</v>
       </c>
       <c r="C14" s="28" t="b">
@@ -7090,9 +7202,9 @@
     </row>
     <row r="15">
       <c r="A15" s="28" t="s">
-        <v>662</v>
-      </c>
-      <c r="B15" s="56">
+        <v>678</v>
+      </c>
+      <c r="B15" s="61">
         <v>2.0</v>
       </c>
       <c r="C15" s="28" t="b">
@@ -7104,9 +7216,9 @@
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
-        <v>663</v>
-      </c>
-      <c r="B16" s="56">
+        <v>679</v>
+      </c>
+      <c r="B16" s="61">
         <v>3.0</v>
       </c>
       <c r="C16" s="28" t="b">
@@ -7118,9 +7230,9 @@
     </row>
     <row r="17">
       <c r="A17" s="28" t="s">
-        <v>664</v>
-      </c>
-      <c r="B17" s="56">
+        <v>680</v>
+      </c>
+      <c r="B17" s="61">
         <v>2.0</v>
       </c>
       <c r="C17" s="28" t="b">
@@ -7132,9 +7244,9 @@
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
-        <v>665</v>
-      </c>
-      <c r="B18" s="56">
+        <v>681</v>
+      </c>
+      <c r="B18" s="61">
         <v>2.0</v>
       </c>
       <c r="C18" s="28" t="b">
@@ -7146,9 +7258,9 @@
     </row>
     <row r="19">
       <c r="A19" s="28" t="s">
-        <v>666</v>
-      </c>
-      <c r="B19" s="56">
+        <v>682</v>
+      </c>
+      <c r="B19" s="61">
         <v>2.0</v>
       </c>
       <c r="C19" s="28" t="b">
@@ -7160,9 +7272,9 @@
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
-        <v>667</v>
-      </c>
-      <c r="B20" s="56">
+        <v>683</v>
+      </c>
+      <c r="B20" s="61">
         <v>2.0</v>
       </c>
       <c r="C20" s="28" t="b">
@@ -7174,9 +7286,9 @@
     </row>
     <row r="21">
       <c r="A21" s="28" t="s">
-        <v>668</v>
-      </c>
-      <c r="B21" s="56">
+        <v>684</v>
+      </c>
+      <c r="B21" s="61">
         <v>3.0</v>
       </c>
       <c r="C21" s="28" t="b">
@@ -7188,9 +7300,9 @@
     </row>
     <row r="22">
       <c r="A22" s="28" t="s">
-        <v>669</v>
-      </c>
-      <c r="B22" s="56">
+        <v>685</v>
+      </c>
+      <c r="B22" s="61">
         <v>2.0</v>
       </c>
       <c r="C22" s="28" t="b">
@@ -7202,9 +7314,9 @@
     </row>
     <row r="23">
       <c r="A23" s="28" t="s">
-        <v>670</v>
-      </c>
-      <c r="B23" s="56">
+        <v>686</v>
+      </c>
+      <c r="B23" s="61">
         <v>2.0</v>
       </c>
       <c r="C23" s="28" t="b">
@@ -7216,9 +7328,9 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>671</v>
-      </c>
-      <c r="B24" s="56">
+        <v>687</v>
+      </c>
+      <c r="B24" s="61">
         <v>2.0</v>
       </c>
       <c r="C24" s="28" t="b">
@@ -7230,9 +7342,9 @@
     </row>
     <row r="25">
       <c r="A25" s="28" t="s">
-        <v>672</v>
-      </c>
-      <c r="B25" s="56">
+        <v>688</v>
+      </c>
+      <c r="B25" s="61">
         <v>2.0</v>
       </c>
       <c r="C25" s="28" t="b">
@@ -7244,9 +7356,9 @@
     </row>
     <row r="26">
       <c r="A26" s="28" t="s">
-        <v>673</v>
-      </c>
-      <c r="B26" s="56">
+        <v>689</v>
+      </c>
+      <c r="B26" s="61">
         <v>2.0</v>
       </c>
       <c r="C26" s="28" t="b">
@@ -7258,9 +7370,9 @@
     </row>
     <row r="27">
       <c r="A27" s="28" t="s">
-        <v>674</v>
-      </c>
-      <c r="B27" s="56">
+        <v>690</v>
+      </c>
+      <c r="B27" s="61">
         <v>2.0</v>
       </c>
       <c r="C27" s="28" t="b">
@@ -7272,9 +7384,9 @@
     </row>
     <row r="28">
       <c r="A28" s="28" t="s">
-        <v>675</v>
-      </c>
-      <c r="B28" s="56">
+        <v>691</v>
+      </c>
+      <c r="B28" s="61">
         <v>2.0</v>
       </c>
       <c r="C28" s="28" t="b">
@@ -7286,9 +7398,9 @@
     </row>
     <row r="29">
       <c r="A29" s="28" t="s">
-        <v>676</v>
-      </c>
-      <c r="B29" s="56">
+        <v>692</v>
+      </c>
+      <c r="B29" s="61">
         <v>4.0</v>
       </c>
       <c r="C29" s="28" t="b">
@@ -7300,9 +7412,9 @@
     </row>
     <row r="30">
       <c r="A30" s="28" t="s">
-        <v>677</v>
-      </c>
-      <c r="B30" s="56">
+        <v>693</v>
+      </c>
+      <c r="B30" s="61">
         <v>2.0</v>
       </c>
       <c r="C30" s="28" t="b">
@@ -7314,9 +7426,9 @@
     </row>
     <row r="31">
       <c r="A31" s="28" t="s">
-        <v>508</v>
-      </c>
-      <c r="B31" s="56">
+        <v>520</v>
+      </c>
+      <c r="B31" s="61">
         <v>5.0</v>
       </c>
       <c r="C31" s="28" t="b">
@@ -7376,170 +7488,170 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="57" t="s">
-        <v>678</v>
-      </c>
-      <c r="B1" s="57" t="s">
-        <v>679</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>680</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>679</v>
+      <c r="A1" s="62" t="s">
+        <v>694</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1" s="62" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="58" t="str">
+      <c r="A2" s="63" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableSprites[WORK],Table_PickableSprites[WORK]&lt;&gt;"""")"),"SPRITE_ITEM_CARDS_PICKABLE")</f>
         <v>SPRITE_ITEM_CARDS_PICKABLE</v>
       </c>
-      <c r="B2" s="58" t="str">
+      <c r="B2" s="63" t="str">
         <f t="array" ref="B2:B18">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[SpritePickable],"")</f>
         <v/>
       </c>
-      <c r="D2" s="58" t="str">
+      <c r="D2" s="63" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(Table_PickableNames[WORK],Table_PickableNames[WORK]&lt;&gt;"""")"),"NAME_ITEM_CARDS")</f>
         <v>NAME_ITEM_CARDS</v>
       </c>
-      <c r="E2" s="58" t="str">
+      <c r="E2" s="63" t="str">
         <f t="array" ref="E2:E18">IF(Table_Items[SpritePickable]&lt;&gt;"SPRITE_NONE",Table_Items[Name],"")</f>
         <v/>
       </c>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="58" t="str">
+      <c r="A3" s="63" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SPRITE_PICKABLE_SOAP")</f>
         <v>SPRITE_PICKABLE_SOAP</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="58" t="str">
+      <c r="D3" s="63" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"NAME_ITEM_SOAP")</f>
         <v>NAME_ITEM_SOAP</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" ht="22.5" customHeight="1">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="63" t="s">
         <v>232</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="63" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" ht="22.5" customHeight="1">
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" ht="22.5" customHeight="1">
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="22.5" customHeight="1">
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" ht="22.5" customHeight="1">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" ht="22.5" customHeight="1">
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" ht="22.5" customHeight="1">
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="63" t="s">
         <v>264</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="63" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="17" ht="22.5" customHeight="1">
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="63" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" ht="22.5" customHeight="1">
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="58" t="s">
+      <c r="E18" s="63" t="s">
         <v>20</v>
       </c>
     </row>
@@ -9909,7 +10021,7 @@
     <col customWidth="1" min="9" max="9" width="48.29"/>
     <col customWidth="1" min="10" max="10" width="41.0"/>
     <col customWidth="1" min="11" max="11" width="31.71"/>
-    <col customWidth="1" min="12" max="12" width="22.57"/>
+    <col customWidth="1" min="12" max="12" width="47.14"/>
     <col customWidth="1" min="13" max="13" width="25.29"/>
     <col customWidth="1" min="14" max="14" width="24.29"/>
   </cols>
@@ -11625,6 +11737,51 @@
         <v>357</v>
       </c>
       <c r="N45" s="30" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="28">
+        <f>ROW()-ROW(Table_Unchain_Conditions[N])</f>
+        <v>21</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="C46" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" s="41" t="s">
+        <v>365</v>
+      </c>
+      <c r="E46" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="F46" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="G46" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="I46" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="J46" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="K46" s="41" t="s">
+        <v>356</v>
+      </c>
+      <c r="L46" s="43" t="s">
+        <v>281</v>
+      </c>
+      <c r="M46" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="N46" s="41" t="s">
         <v>355</v>
       </c>
     </row>
@@ -11639,16 +11796,16 @@
     <dataValidation type="list" allowBlank="1" sqref="C2:C22">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="L25:L45">
+    <dataValidation type="list" allowBlank="1" sqref="L25:L46">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E25:E45">
+    <dataValidation type="list" allowBlank="1" sqref="E25:E46">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F25:F45">
+    <dataValidation type="list" allowBlank="1" sqref="F25:F46">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:G22 D25:D45 G25:K45 M25:N45">
+    <dataValidation type="list" allowBlank="1" sqref="D2:G22 D25:D46 G25:K46 M25:N46">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="I2:I22">
@@ -11687,10 +11844,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2">
@@ -11711,7 +11868,7 @@
         <v>236</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4">
@@ -11720,10 +11877,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5">
@@ -11732,10 +11889,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6">
@@ -11744,10 +11901,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7">
@@ -11756,10 +11913,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8">
@@ -11768,10 +11925,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9">
@@ -11780,10 +11937,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="10">
@@ -11792,10 +11949,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="11">
@@ -11804,10 +11961,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12">
@@ -11816,10 +11973,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13">
@@ -11828,10 +11985,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14">
@@ -11843,7 +12000,7 @@
         <v>227</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15">
@@ -11855,7 +12012,7 @@
         <v>363</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16">
@@ -11867,7 +12024,7 @@
         <v>231</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17">
@@ -11879,7 +12036,7 @@
         <v>232</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18">
@@ -11888,10 +12045,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19">
@@ -11903,7 +12060,7 @@
         <v>239</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20">
@@ -11912,10 +12069,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21">
@@ -11927,7 +12084,7 @@
         <v>247</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22">
@@ -11936,10 +12093,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="23">
@@ -11948,10 +12105,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24">
@@ -11960,10 +12117,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25">
@@ -11975,7 +12132,7 @@
         <v>264</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26">
@@ -11984,9 +12141,69 @@
         <v>24</v>
       </c>
       <c r="B26" s="28" t="s">
+        <v>432</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>25</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>434</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>26</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>27</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>438</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>28</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="28">
+        <f>ROW()-ROW(Table_sprites[N])</f>
+        <v>29</v>
+      </c>
+      <c r="B31" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C31" s="28" t="s">
         <v>271</v>
       </c>
     </row>
@@ -12026,13 +12243,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2">
@@ -12047,7 +12264,7 @@
         <v>215</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3">
@@ -12062,7 +12279,7 @@
         <v>215</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4">
@@ -12077,7 +12294,7 @@
         <v>215</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5">
@@ -12086,13 +12303,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>215</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="6">
@@ -12107,7 +12324,7 @@
         <v>215</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7">
@@ -12116,13 +12333,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>215</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9">
@@ -12130,19 +12347,19 @@
         <v>0</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>273</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10">
@@ -12151,7 +12368,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>281</v>
@@ -12172,7 +12389,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>281</v>
@@ -12193,7 +12410,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>281</v>
@@ -12202,10 +12419,10 @@
         <v>281</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13">
@@ -12214,7 +12431,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>281</v>
@@ -12223,10 +12440,10 @@
         <v>281</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
     </row>
     <row r="14">
@@ -12235,7 +12452,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>281</v>
@@ -12247,7 +12464,7 @@
         <v>285</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
     </row>
     <row r="15">
@@ -12256,7 +12473,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>281</v>
@@ -12268,7 +12485,7 @@
         <v>285</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
     </row>
     <row r="16">
@@ -12277,7 +12494,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C16" s="29" t="s">
         <v>281</v>
@@ -12293,52 +12510,52 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
     </row>
     <row r="19">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="20">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
     </row>
     <row r="21">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
     </row>
     <row r="22">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -12386,7 +12603,7 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="33.43"/>
     <col customWidth="1" min="3" max="3" width="45.43"/>
-    <col customWidth="1" min="4" max="4" width="37.0"/>
+    <col customWidth="1" min="4" max="4" width="48.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -12394,10 +12611,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>452</v>
+        <v>463</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="2">
@@ -12409,7 +12626,7 @@
         <v>357</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3">
@@ -12421,7 +12638,7 @@
         <v>387</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4">
@@ -12430,10 +12647,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6">
@@ -12441,87 +12658,87 @@
         <v>0</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="42">
+      <c r="A7" s="46">
         <f>ROW()-ROW(Table_Decision_Options[N])</f>
         <v>0</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>286</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="47" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="42">
+      <c r="A8" s="46">
         <f>ROW()-ROW(Table_Decision_Options[N])</f>
         <v>1</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>460</v>
-      </c>
-      <c r="D8" s="43" t="s">
+        <v>472</v>
+      </c>
+      <c r="D8" s="47" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="42">
+      <c r="A9" s="46">
         <f>ROW()-ROW(Table_Decision_Options[N])</f>
         <v>2</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>462</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>463</v>
+        <v>474</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="42">
+      <c r="A10" s="46">
         <f>ROW()-ROW(Table_Decision_Options[N])</f>
         <v>3</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>465</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>466</v>
+        <v>477</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="42">
+      <c r="A11" s="46">
         <f>ROW()-ROW(Table_Decision_Options[N])</f>
         <v>4</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>286</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="47" t="s">
         <v>281</v>
       </c>
     </row>
@@ -12559,17 +12776,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>467</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>468</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>469</v>
+      <c r="B1" s="49" t="s">
+        <v>479</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="2">
@@ -12580,8 +12797,8 @@
       <c r="B2" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
     </row>
     <row r="3">
       <c r="A3" s="22">
@@ -12592,10 +12809,10 @@
         <v>221</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4">
@@ -12604,13 +12821,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5">
@@ -12619,13 +12836,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>476</v>
+        <v>488</v>
       </c>
     </row>
     <row r="6">
@@ -12634,13 +12851,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7">
@@ -12652,10 +12869,10 @@
         <v>224</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
     </row>
     <row r="8">
@@ -12667,10 +12884,10 @@
         <v>245</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9">
@@ -12682,10 +12899,10 @@
         <v>252</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>483</v>
+        <v>495</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
     </row>
     <row r="10">
@@ -12697,10 +12914,10 @@
         <v>230</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>486</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11">
@@ -12709,13 +12926,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>487</v>
+        <v>499</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>488</v>
+        <v>500</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
     </row>
     <row r="12">
@@ -12724,13 +12941,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>490</v>
+        <v>502</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
     </row>
     <row r="13">
@@ -12742,10 +12959,10 @@
         <v>235</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>493</v>
+        <v>505</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14">
@@ -12757,10 +12974,10 @@
         <v>242</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
     </row>
     <row r="15">
@@ -12769,13 +12986,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>497</v>
+        <v>509</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>499</v>
+        <v>511</v>
       </c>
     </row>
     <row r="16">
@@ -12787,10 +13004,10 @@
         <v>255</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>501</v>
+        <v>513</v>
       </c>
     </row>
     <row r="17">
@@ -12802,10 +13019,10 @@
         <v>260</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>502</v>
+        <v>514</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>503</v>
+        <v>515</v>
       </c>
     </row>
     <row r="18">
@@ -12817,10 +13034,10 @@
         <v>263</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
     </row>
     <row r="19">
@@ -12832,10 +13049,10 @@
         <v>267</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
     </row>
     <row r="20">
@@ -12847,10 +13064,10 @@
         <v>270</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -12887,22 +13104,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>510</v>
+        <v>522</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>515</v>
+        <v>526</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="2">
@@ -12920,9 +13137,9 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>516</v>
-      </c>
-      <c r="F2" s="48"/>
+        <v>528</v>
+      </c>
+      <c r="F2" s="52"/>
       <c r="G2" s="29"/>
     </row>
     <row r="3">
@@ -12931,7 +13148,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="C3" s="28">
         <v>0.0</v>
@@ -12940,13 +13157,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>520</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4">
@@ -12955,7 +13172,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C4" s="28">
         <v>0.0</v>
@@ -12964,13 +13181,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>523</v>
+        <v>535</v>
       </c>
     </row>
     <row r="5">
@@ -12979,7 +13196,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>524</v>
+        <v>536</v>
       </c>
       <c r="C5" s="28">
         <v>0.0</v>
@@ -12988,13 +13205,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>525</v>
+        <v>537</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6">
@@ -13003,7 +13220,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="C6" s="28">
         <v>0.0</v>
@@ -13012,13 +13229,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>528</v>
+        <v>540</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7">
@@ -13027,7 +13244,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>530</v>
+        <v>542</v>
       </c>
       <c r="C7" s="28">
         <v>0.0</v>
@@ -13036,13 +13253,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>531</v>
+        <v>543</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>532</v>
+        <v>544</v>
       </c>
     </row>
     <row r="8">
@@ -13060,13 +13277,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>533</v>
+        <v>545</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>534</v>
+        <v>546</v>
       </c>
     </row>
     <row r="9">
@@ -13075,7 +13292,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>535</v>
+        <v>547</v>
       </c>
       <c r="C9" s="28">
         <v>0.0</v>
@@ -13084,13 +13301,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>536</v>
+        <v>548</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>537</v>
+        <v>549</v>
       </c>
     </row>
     <row r="10">
@@ -13099,7 +13316,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>538</v>
+        <v>550</v>
       </c>
       <c r="C10" s="28">
         <v>0.0</v>
@@ -13108,13 +13325,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>539</v>
+        <v>551</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>540</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11">
@@ -13123,7 +13340,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>541</v>
+        <v>553</v>
       </c>
       <c r="C11" s="28">
         <v>1.0</v>
@@ -13132,13 +13349,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>542</v>
+        <v>554</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>543</v>
+        <v>555</v>
       </c>
     </row>
     <row r="12">
@@ -13147,7 +13364,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>544</v>
+        <v>556</v>
       </c>
       <c r="C12" s="28">
         <v>0.0</v>
@@ -13156,13 +13373,13 @@
         <v>0.0</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>546</v>
+        <v>558</v>
       </c>
     </row>
     <row r="13">
@@ -13171,7 +13388,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>547</v>
+        <v>559</v>
       </c>
       <c r="C13" s="28">
         <v>0.0</v>
@@ -13180,13 +13397,13 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>548</v>
+        <v>560</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>549</v>
+        <v>561</v>
       </c>
     </row>
     <row r="14">
@@ -13195,7 +13412,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
       <c r="C14" s="28">
         <v>1.0</v>
@@ -13204,13 +13421,13 @@
         <v>0.0</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>552</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15">
@@ -13219,7 +13436,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>553</v>
+        <v>565</v>
       </c>
       <c r="C15" s="28">
         <v>1.0</v>
@@ -13228,13 +13445,13 @@
         <v>0.0</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>554</v>
+        <v>566</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>555</v>
+        <v>567</v>
       </c>
     </row>
     <row r="16">
@@ -13243,7 +13460,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="C16" s="28">
         <v>1.0</v>
@@ -13252,13 +13469,13 @@
         <v>0.0</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>556</v>
+        <v>568</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>557</v>
+        <v>569</v>
       </c>
     </row>
     <row r="17">
@@ -13267,7 +13484,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>558</v>
+        <v>570</v>
       </c>
       <c r="C17" s="28">
         <v>0.0</v>
@@ -13276,13 +13493,13 @@
         <v>0.0</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>559</v>
+        <v>571</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>560</v>
+        <v>572</v>
       </c>
     </row>
     <row r="18">
@@ -13300,13 +13517,13 @@
         <v>0.0</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>561</v>
+        <v>573</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>562</v>
+        <v>574</v>
       </c>
     </row>
     <row r="19">
@@ -13324,13 +13541,13 @@
         <v>0.0</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>564</v>
+        <v>576</v>
       </c>
     </row>
     <row r="20">
@@ -13348,13 +13565,13 @@
         <v>0.0</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>565</v>
+        <v>577</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>566</v>
+        <v>578</v>
       </c>
     </row>
     <row r="21">
@@ -13372,13 +13589,13 @@
         <v>0.0</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>567</v>
+        <v>579</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>568</v>
+        <v>580</v>
       </c>
     </row>
     <row r="22">
@@ -13396,13 +13613,13 @@
         <v>0.0</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>569</v>
+        <v>581</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
     </row>
     <row r="23">
@@ -13420,13 +13637,13 @@
         <v>0.0</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>572</v>
+        <v>584</v>
       </c>
     </row>
     <row r="24">
@@ -13444,13 +13661,13 @@
         <v>0.0</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>573</v>
+        <v>585</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
     </row>
     <row r="25">
@@ -13468,13 +13685,13 @@
         <v>0.0</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>575</v>
+        <v>587</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>576</v>
+        <v>588</v>
       </c>
     </row>
     <row r="26">
@@ -13483,7 +13700,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>577</v>
+        <v>589</v>
       </c>
       <c r="C26" s="28">
         <v>0.0</v>
@@ -13492,13 +13709,13 @@
         <v>0.0</v>
       </c>
       <c r="E26" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>578</v>
+        <v>590</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>579</v>
+        <v>591</v>
       </c>
     </row>
     <row r="27">
@@ -13507,7 +13724,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="C27" s="28">
         <v>1.0</v>
@@ -13516,13 +13733,13 @@
         <v>0.0</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>581</v>
+        <v>593</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>582</v>
+        <v>594</v>
       </c>
     </row>
     <row r="28">
@@ -13531,7 +13748,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="C28" s="28">
         <v>0.0</v>
@@ -13540,13 +13757,13 @@
         <v>0.0</v>
       </c>
       <c r="E28" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>583</v>
+        <v>595</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>584</v>
+        <v>596</v>
       </c>
     </row>
     <row r="29">
@@ -13555,7 +13772,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="C29" s="28">
         <v>0.0</v>
@@ -13564,13 +13781,13 @@
         <v>0.0</v>
       </c>
       <c r="E29" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>585</v>
+        <v>597</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>586</v>
+        <v>598</v>
       </c>
     </row>
     <row r="30">
@@ -13579,7 +13796,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="C30" s="28">
         <v>0.0</v>
@@ -13588,13 +13805,13 @@
         <v>0.0</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="F30" s="29" t="s">
-        <v>587</v>
+        <v>599</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>588</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug of Triggered Dialog not showing recently Triggered event-dependant dialog
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -8232,7 +8232,7 @@
         <v>1086</v>
       </c>
       <c r="C103" s="34">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D103" s="34">
         <v>0.0</v>
@@ -8280,7 +8280,7 @@
         <v>1090</v>
       </c>
       <c r="C105" s="34">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D105" s="34">
         <v>0.0</v>
@@ -8328,7 +8328,7 @@
         <v>1094</v>
       </c>
       <c r="C107" s="34">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D107" s="34">
         <v>0.0</v>
@@ -8376,7 +8376,7 @@
         <v>1098</v>
       </c>
       <c r="C109" s="34">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D109" s="34">
         <v>0.0</v>
@@ -8424,7 +8424,7 @@
         <v>1102</v>
       </c>
       <c r="C111" s="34">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D111" s="34">
         <v>0.0</v>
@@ -8520,7 +8520,7 @@
         <v>1108</v>
       </c>
       <c r="C115" s="34">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D115" s="34">
         <v>0.0</v>
@@ -12451,7 +12451,7 @@
         <v>68</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Making possible Observe inventory items
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3233" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3234" uniqueCount="1261">
   <si>
     <t>NewItem</t>
   </si>
@@ -3185,105 +3185,159 @@
     <t>Is this going to end somewhen?</t>
   </si>
   <si>
+    <t>Esto va a acabar algún día?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_BCKG_POOR_MAN_WC_OPTION_2_0</t>
   </si>
   <si>
     <t>This is torture</t>
   </si>
   <si>
+    <t>Esto es una tortura</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_BCKG_POOR_MAN_WC_OPTION_3_0</t>
   </si>
   <si>
     <t>I should have never eat that dinner</t>
   </si>
   <si>
+    <t>Nunca debí cenar allí</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_0_0</t>
   </si>
   <si>
     <t>Terrible night. Ah?</t>
   </si>
   <si>
+    <t>Terrible noche. No?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_0_1</t>
   </si>
   <si>
     <t>It was that Maño restaurant. Boar was terrible</t>
   </si>
   <si>
+    <t>Era el restaurante del Maño. El jabalí estaba horrible</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_0_2</t>
   </si>
   <si>
     <t>I saw it full of people. Don't think it was in bad state</t>
   </si>
   <si>
+    <t>Lo vi a reventar de gente. No creo que estuviera precisamente malo</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_0_3</t>
   </si>
   <si>
     <t>Well. Maybe my stomach is not in mood!</t>
   </si>
   <si>
+    <t>Bueno. Mi estómago no está por la labor</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_1_0</t>
   </si>
   <si>
     <t>Are you going to end today?</t>
   </si>
   <si>
+    <t>Piensas terminar algún día?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_1_1</t>
   </si>
   <si>
     <t>Haha. Very funny. If I could. I would be out there. Night is young</t>
   </si>
   <si>
+    <t>Jaja. Muy gracioso. Si pudiera. Estaría por allí. La noche es joven</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_2_0</t>
   </si>
   <si>
     <t>How can I help you?</t>
   </si>
   <si>
+    <t>Como podría ayudarte?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_2_1</t>
   </si>
   <si>
     <t>This nasty Inn is cutting water at night. I cannot let this in this state</t>
   </si>
   <si>
+    <t>Esta asquerosa pocilga está cortando el agua por las noches. No puedo dejar esto así</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_2_2</t>
   </si>
   <si>
     <t>Ahh. I see...</t>
   </si>
   <si>
+    <t>Ahh. Ya veo..</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_2_3</t>
   </si>
   <si>
     <t>Could you please talk to someone to bring water again?</t>
   </si>
   <si>
+    <t>Podrías por favor hablar con alguien para que vuelva el agua?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_OPTION_2_4</t>
   </si>
   <si>
     <t>I will see what can I do. But personnel is absent during day. Even worse at night</t>
   </si>
   <si>
+    <t>Veré lo que puedo hacer. Pero si ya el personal está ausente durante el día. Imagina por la noche</t>
+  </si>
+  <si>
     <t>I need to go. Sorry for your situation!</t>
   </si>
   <si>
+    <t>Necesito irme. Lamento la situación!</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_INTRO_0</t>
   </si>
   <si>
     <t>Did you come to laugh at my disgrace?</t>
   </si>
   <si>
+    <t>Viniste a reirte de mi desgracia?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_INTRO_1</t>
   </si>
   <si>
     <t>Did I wake you up?</t>
   </si>
   <si>
+    <t>Te desperté?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_HIVE1_POOR_MAN_WC_INTRO_2</t>
   </si>
   <si>
     <t>Are you from health department?</t>
   </si>
   <si>
+    <t>Eres del ministerio de sanidad?</t>
+  </si>
+  <si>
     <t>PHRASE_MEMENTO_POOR_MAN_WC_1</t>
   </si>
   <si>
@@ -3365,6 +3419,9 @@
     <t>It's a shoelace lost from some guest</t>
   </si>
   <si>
+    <t>Es el cordón de bota de algún huesped</t>
+  </si>
+  <si>
     <t>I don't have a reason to take it</t>
   </si>
   <si>
@@ -3413,30 +3470,45 @@
     <t>So. Isn't it the end of the night for you?</t>
   </si>
   <si>
+    <t>Entonces. La noche no acaba aquí?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_0_1</t>
   </si>
   <si>
     <t>Nope. As I told you night is so young</t>
   </si>
   <si>
+    <t>No. Como te dije la noche es joven</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_0_2</t>
   </si>
   <si>
     <t>Where are you facing to?</t>
   </si>
   <si>
+    <t>A dónde irás ahora?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_0_3</t>
   </si>
   <si>
     <t xml:space="preserve">There is a club in the south neighborhood </t>
   </si>
   <si>
+    <t>Hay un club en el barrio sur</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_1_0</t>
   </si>
   <si>
     <t>This pub you mentioned...</t>
   </si>
   <si>
+    <t>Este club que comentas...</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_1_1</t>
   </si>
   <si>
@@ -3449,42 +3521,66 @@
     <t>You think I could meet people there or ask for job?</t>
   </si>
   <si>
+    <t>Crees que puedo conocer a gente allí o encontrar trabajo?</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_1_3</t>
   </si>
   <si>
     <t>For sure gentleman. Even if it's in south neighborhood. Some business are running well there. You should go some day</t>
   </si>
   <si>
+    <t>Por supuesto caballero. Incluso siendo el barrio sur. Algunos negocios están yendo bien. Deberías pasarte un día</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_1_4</t>
   </si>
   <si>
     <t>I would be pleased</t>
   </si>
   <si>
+    <t>Me encantaría</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_1_5</t>
   </si>
   <si>
     <t>For sure. Take this invitation. It's kind of private and they won't let strangers go inside</t>
   </si>
   <si>
+    <t>Por supuesto. Toma esta invitación. Es un poco privado y no dejan entrar a desconocidos</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_OPTION_1_6</t>
   </si>
   <si>
     <t>Thank you!</t>
   </si>
   <si>
+    <t>Gracias!</t>
+  </si>
+  <si>
+    <t>Bueno. Nos vemos pronto!</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_INTRO_0</t>
   </si>
   <si>
     <t>I'm happy to see you in a better state!</t>
   </si>
   <si>
+    <t>Me alegro de verte en mejor estado</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_ARTURO_HALL_INN_INTRO_1</t>
   </si>
   <si>
     <t>I really appreciate your help this night</t>
   </si>
   <si>
+    <t>Agradezco en verdad tu ayuda esta noche</t>
+  </si>
+  <si>
     <t>PHRASE_DIALOG_LAST</t>
   </si>
   <si>
@@ -3609,6 +3705,9 @@
   </si>
   <si>
     <t>INTERACTION_MOVE</t>
+  </si>
+  <si>
+    <t>INTERACTION_COMBINE</t>
   </si>
   <si>
     <t>UNCHAIN_TYPE_ID</t>
@@ -5136,7 +5235,7 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B23" displayName="Table_Interaction" name="Table_Interaction" id="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A15:B24" displayName="Table_Interaction" name="Table_Interaction" id="20">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="INTERACTION_ID" id="2"/>
@@ -5146,7 +5245,7 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A25:B37" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A26:B38" displayName="Table_Unchain_Type" name="Table_Unchain_Type" id="21">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="UNCHAIN_TYPE_ID" id="2"/>
@@ -5156,7 +5255,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A39:B41" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A40:B42" displayName="Table_Dialog_Animation" name="Table_Dialog_Animation" id="22">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="DIALOG_ANIMATION_ID" id="2"/>
@@ -5166,7 +5265,7 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A43:B48" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A44:B49" displayName="Table_Item_Family_Type" name="Table_Item_Family_Type" id="23">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="ITEM_FAMILY_TYPE_ID" id="2"/>
@@ -5176,7 +5275,7 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A50:B53" displayName="Table_Moment_Day" name="Table_Moment_Day" id="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A51:B54" displayName="Table_Moment_Day" name="Table_Moment_Day" id="24">
   <tableColumns count="2">
     <tableColumn name="N" id="1"/>
     <tableColumn name="MOMENT_TYPE_ID" id="2"/>
@@ -7346,7 +7445,7 @@
         <v>1020</v>
       </c>
       <c r="G64" s="36" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="65">
@@ -7355,7 +7454,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="35" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C65" s="35">
         <v>0.0</v>
@@ -7367,10 +7466,10 @@
         <v>857</v>
       </c>
       <c r="F65" s="36" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="G65" s="36" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="66">
@@ -7379,7 +7478,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="35" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="C66" s="35">
         <v>0.0</v>
@@ -7391,10 +7490,10 @@
         <v>857</v>
       </c>
       <c r="F66" s="36" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="G66" s="36" t="s">
-        <v>1024</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="67">
@@ -7403,7 +7502,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="35" t="s">
-        <v>1025</v>
+        <v>1028</v>
       </c>
       <c r="C67" s="35">
         <v>0.0</v>
@@ -7415,10 +7514,10 @@
         <v>857</v>
       </c>
       <c r="F67" s="36" t="s">
-        <v>1026</v>
+        <v>1029</v>
       </c>
       <c r="G67" s="36" t="s">
-        <v>1026</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="68">
@@ -7427,7 +7526,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="35" t="s">
-        <v>1027</v>
+        <v>1031</v>
       </c>
       <c r="C68" s="35">
         <v>1.0</v>
@@ -7439,10 +7538,10 @@
         <v>857</v>
       </c>
       <c r="F68" s="36" t="s">
-        <v>1028</v>
+        <v>1032</v>
       </c>
       <c r="G68" s="36" t="s">
-        <v>1028</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="69">
@@ -7451,7 +7550,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="35" t="s">
-        <v>1029</v>
+        <v>1034</v>
       </c>
       <c r="C69" s="35">
         <v>0.0</v>
@@ -7463,10 +7562,10 @@
         <v>857</v>
       </c>
       <c r="F69" s="36" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="G69" s="36" t="s">
-        <v>1030</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="70">
@@ -7475,7 +7574,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="35" t="s">
-        <v>1031</v>
+        <v>1037</v>
       </c>
       <c r="C70" s="35">
         <v>1.0</v>
@@ -7487,10 +7586,10 @@
         <v>857</v>
       </c>
       <c r="F70" s="36" t="s">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="G70" s="36" t="s">
-        <v>1032</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="71">
@@ -7499,7 +7598,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="35" t="s">
-        <v>1033</v>
+        <v>1040</v>
       </c>
       <c r="C71" s="35">
         <v>0.0</v>
@@ -7511,10 +7610,10 @@
         <v>857</v>
       </c>
       <c r="F71" s="36" t="s">
-        <v>1034</v>
+        <v>1041</v>
       </c>
       <c r="G71" s="36" t="s">
-        <v>1034</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="72">
@@ -7523,7 +7622,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="35" t="s">
-        <v>1035</v>
+        <v>1043</v>
       </c>
       <c r="C72" s="35">
         <v>1.0</v>
@@ -7535,10 +7634,10 @@
         <v>857</v>
       </c>
       <c r="F72" s="36" t="s">
-        <v>1036</v>
+        <v>1044</v>
       </c>
       <c r="G72" s="36" t="s">
-        <v>1036</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="73">
@@ -7547,7 +7646,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="35" t="s">
-        <v>1037</v>
+        <v>1046</v>
       </c>
       <c r="C73" s="35">
         <v>0.0</v>
@@ -7559,10 +7658,10 @@
         <v>857</v>
       </c>
       <c r="F73" s="36" t="s">
-        <v>1038</v>
+        <v>1047</v>
       </c>
       <c r="G73" s="36" t="s">
-        <v>1038</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="74">
@@ -7571,7 +7670,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="35" t="s">
-        <v>1039</v>
+        <v>1049</v>
       </c>
       <c r="C74" s="35">
         <v>1.0</v>
@@ -7583,10 +7682,10 @@
         <v>857</v>
       </c>
       <c r="F74" s="36" t="s">
-        <v>1040</v>
+        <v>1050</v>
       </c>
       <c r="G74" s="36" t="s">
-        <v>1040</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="75">
@@ -7595,7 +7694,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="35" t="s">
-        <v>1041</v>
+        <v>1052</v>
       </c>
       <c r="C75" s="35">
         <v>0.0</v>
@@ -7607,10 +7706,10 @@
         <v>857</v>
       </c>
       <c r="F75" s="36" t="s">
-        <v>1042</v>
+        <v>1053</v>
       </c>
       <c r="G75" s="36" t="s">
-        <v>1042</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="76">
@@ -7619,7 +7718,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="35" t="s">
-        <v>1043</v>
+        <v>1055</v>
       </c>
       <c r="C76" s="35">
         <v>1.0</v>
@@ -7631,10 +7730,10 @@
         <v>857</v>
       </c>
       <c r="F76" s="36" t="s">
-        <v>1044</v>
+        <v>1056</v>
       </c>
       <c r="G76" s="36" t="s">
-        <v>1044</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="77">
@@ -7643,7 +7742,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="35" t="s">
-        <v>1045</v>
+        <v>1058</v>
       </c>
       <c r="C77" s="35">
         <v>0.0</v>
@@ -7655,10 +7754,10 @@
         <v>857</v>
       </c>
       <c r="F77" s="36" t="s">
-        <v>1046</v>
+        <v>1059</v>
       </c>
       <c r="G77" s="36" t="s">
-        <v>1046</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="78">
@@ -7679,10 +7778,10 @@
         <v>857</v>
       </c>
       <c r="F78" s="36" t="s">
-        <v>1047</v>
+        <v>1061</v>
       </c>
       <c r="G78" s="36" t="s">
-        <v>1047</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="79">
@@ -7691,7 +7790,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="35" t="s">
-        <v>1048</v>
+        <v>1063</v>
       </c>
       <c r="C79" s="35">
         <v>1.0</v>
@@ -7703,10 +7802,10 @@
         <v>857</v>
       </c>
       <c r="F79" s="36" t="s">
-        <v>1049</v>
+        <v>1064</v>
       </c>
       <c r="G79" s="36" t="s">
-        <v>1049</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="80">
@@ -7715,7 +7814,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="35" t="s">
-        <v>1050</v>
+        <v>1066</v>
       </c>
       <c r="C80" s="35">
         <v>1.0</v>
@@ -7727,10 +7826,10 @@
         <v>857</v>
       </c>
       <c r="F80" s="36" t="s">
-        <v>1051</v>
+        <v>1067</v>
       </c>
       <c r="G80" s="36" t="s">
-        <v>1051</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="81">
@@ -7739,7 +7838,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="35" t="s">
-        <v>1052</v>
+        <v>1069</v>
       </c>
       <c r="C81" s="35">
         <v>1.0</v>
@@ -7751,10 +7850,10 @@
         <v>857</v>
       </c>
       <c r="F81" s="36" t="s">
-        <v>1053</v>
+        <v>1070</v>
       </c>
       <c r="G81" s="36" t="s">
-        <v>1053</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="82">
@@ -7763,7 +7862,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="35" t="s">
-        <v>1054</v>
+        <v>1072</v>
       </c>
       <c r="C82" s="35">
         <v>0.0</v>
@@ -7775,10 +7874,10 @@
         <v>857</v>
       </c>
       <c r="F82" s="36" t="s">
-        <v>1055</v>
+        <v>1073</v>
       </c>
       <c r="G82" s="36" t="s">
-        <v>1056</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="83">
@@ -7787,7 +7886,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="35" t="s">
-        <v>1057</v>
+        <v>1075</v>
       </c>
       <c r="C83" s="35">
         <v>0.0</v>
@@ -7799,10 +7898,10 @@
         <v>857</v>
       </c>
       <c r="F83" s="36" t="s">
-        <v>1058</v>
+        <v>1076</v>
       </c>
       <c r="G83" s="36" t="s">
-        <v>1059</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="84">
@@ -7811,7 +7910,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="35" t="s">
-        <v>1060</v>
+        <v>1078</v>
       </c>
       <c r="C84" s="35">
         <v>0.0</v>
@@ -7823,10 +7922,10 @@
         <v>857</v>
       </c>
       <c r="F84" s="36" t="s">
-        <v>1061</v>
+        <v>1079</v>
       </c>
       <c r="G84" s="36" t="s">
-        <v>1062</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="85">
@@ -7847,10 +7946,10 @@
         <v>857</v>
       </c>
       <c r="F85" s="36" t="s">
-        <v>1063</v>
+        <v>1081</v>
       </c>
       <c r="G85" s="36" t="s">
-        <v>1064</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="86">
@@ -7871,10 +7970,10 @@
         <v>857</v>
       </c>
       <c r="F86" s="36" t="s">
-        <v>1065</v>
+        <v>1083</v>
       </c>
       <c r="G86" s="36" t="s">
-        <v>1065</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="87">
@@ -7895,10 +7994,10 @@
         <v>857</v>
       </c>
       <c r="F87" s="36" t="s">
-        <v>1066</v>
+        <v>1084</v>
       </c>
       <c r="G87" s="36" t="s">
-        <v>1067</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="88">
@@ -7919,10 +8018,10 @@
         <v>857</v>
       </c>
       <c r="F88" s="36" t="s">
-        <v>1068</v>
+        <v>1086</v>
       </c>
       <c r="G88" s="36" t="s">
-        <v>1069</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="89">
@@ -7943,10 +8042,10 @@
         <v>857</v>
       </c>
       <c r="F89" s="36" t="s">
-        <v>1070</v>
+        <v>1088</v>
       </c>
       <c r="G89" s="36" t="s">
-        <v>1071</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="90">
@@ -7967,10 +8066,10 @@
         <v>857</v>
       </c>
       <c r="F90" s="36" t="s">
-        <v>1072</v>
+        <v>1090</v>
       </c>
       <c r="G90" s="36" t="s">
-        <v>1073</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="91">
@@ -7991,10 +8090,10 @@
         <v>857</v>
       </c>
       <c r="F91" s="36" t="s">
-        <v>1074</v>
+        <v>1092</v>
       </c>
       <c r="G91" s="36" t="s">
-        <v>1075</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="92">
@@ -8015,10 +8114,10 @@
         <v>857</v>
       </c>
       <c r="F92" s="36" t="s">
-        <v>1076</v>
+        <v>1094</v>
       </c>
       <c r="G92" s="36" t="s">
-        <v>1077</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="93">
@@ -8039,10 +8138,10 @@
         <v>857</v>
       </c>
       <c r="F93" s="36" t="s">
-        <v>1078</v>
+        <v>1096</v>
       </c>
       <c r="G93" s="36" t="s">
-        <v>1079</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="94">
@@ -8063,10 +8162,10 @@
         <v>857</v>
       </c>
       <c r="F94" s="36" t="s">
-        <v>1080</v>
+        <v>1098</v>
       </c>
       <c r="G94" s="36" t="s">
-        <v>1080</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="95">
@@ -8087,10 +8186,10 @@
         <v>857</v>
       </c>
       <c r="F95" s="36" t="s">
-        <v>1081</v>
+        <v>1100</v>
       </c>
       <c r="G95" s="36" t="s">
-        <v>1082</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="96">
@@ -8111,10 +8210,10 @@
         <v>857</v>
       </c>
       <c r="F96" s="36" t="s">
-        <v>1083</v>
+        <v>1102</v>
       </c>
       <c r="G96" s="36" t="s">
-        <v>1084</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="97">
@@ -8135,10 +8234,10 @@
         <v>857</v>
       </c>
       <c r="F97" s="36" t="s">
-        <v>1085</v>
+        <v>1104</v>
       </c>
       <c r="G97" s="36" t="s">
-        <v>1086</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="98">
@@ -8159,10 +8258,10 @@
         <v>855</v>
       </c>
       <c r="F98" s="36" t="s">
-        <v>1087</v>
+        <v>1106</v>
       </c>
       <c r="G98" s="36" t="s">
-        <v>1088</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="99">
@@ -8183,10 +8282,10 @@
         <v>857</v>
       </c>
       <c r="F99" s="36" t="s">
-        <v>1089</v>
+        <v>1108</v>
       </c>
       <c r="G99" s="36" t="s">
-        <v>1090</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="100">
@@ -8207,10 +8306,10 @@
         <v>857</v>
       </c>
       <c r="F100" s="36" t="s">
-        <v>1091</v>
+        <v>1110</v>
       </c>
       <c r="G100" s="36" t="s">
-        <v>1092</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="101">
@@ -8231,10 +8330,10 @@
         <v>857</v>
       </c>
       <c r="F101" s="36" t="s">
-        <v>1093</v>
+        <v>1112</v>
       </c>
       <c r="G101" s="36" t="s">
-        <v>1094</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="102">
@@ -8243,7 +8342,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="35" t="s">
-        <v>1095</v>
+        <v>1114</v>
       </c>
       <c r="C102" s="35">
         <v>0.0</v>
@@ -8255,10 +8354,10 @@
         <v>857</v>
       </c>
       <c r="F102" s="36" t="s">
-        <v>1096</v>
+        <v>1115</v>
       </c>
       <c r="G102" s="36" t="s">
-        <v>1096</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="103">
@@ -8267,7 +8366,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="35" t="s">
-        <v>1097</v>
+        <v>1117</v>
       </c>
       <c r="C103" s="35">
         <v>1.0</v>
@@ -8279,10 +8378,10 @@
         <v>857</v>
       </c>
       <c r="F103" s="36" t="s">
-        <v>1098</v>
+        <v>1118</v>
       </c>
       <c r="G103" s="36" t="s">
-        <v>1098</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="104">
@@ -8291,7 +8390,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="35" t="s">
-        <v>1099</v>
+        <v>1120</v>
       </c>
       <c r="C104" s="35">
         <v>0.0</v>
@@ -8303,10 +8402,10 @@
         <v>857</v>
       </c>
       <c r="F104" s="36" t="s">
-        <v>1100</v>
+        <v>1121</v>
       </c>
       <c r="G104" s="36" t="s">
-        <v>1100</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="105">
@@ -8315,7 +8414,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="35" t="s">
-        <v>1101</v>
+        <v>1123</v>
       </c>
       <c r="C105" s="35">
         <v>1.0</v>
@@ -8327,10 +8426,10 @@
         <v>857</v>
       </c>
       <c r="F105" s="36" t="s">
-        <v>1102</v>
+        <v>1124</v>
       </c>
       <c r="G105" s="36" t="s">
-        <v>1102</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="106">
@@ -8339,7 +8438,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="35" t="s">
-        <v>1103</v>
+        <v>1126</v>
       </c>
       <c r="C106" s="35">
         <v>0.0</v>
@@ -8351,10 +8450,10 @@
         <v>857</v>
       </c>
       <c r="F106" s="36" t="s">
-        <v>1104</v>
+        <v>1127</v>
       </c>
       <c r="G106" s="36" t="s">
-        <v>1104</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="107">
@@ -8363,7 +8462,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="35" t="s">
-        <v>1105</v>
+        <v>1129</v>
       </c>
       <c r="C107" s="35">
         <v>1.0</v>
@@ -8375,10 +8474,10 @@
         <v>857</v>
       </c>
       <c r="F107" s="36" t="s">
-        <v>1106</v>
+        <v>1130</v>
       </c>
       <c r="G107" s="36" t="s">
-        <v>1106</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="108">
@@ -8387,7 +8486,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="35" t="s">
-        <v>1107</v>
+        <v>1131</v>
       </c>
       <c r="C108" s="35">
         <v>0.0</v>
@@ -8399,10 +8498,10 @@
         <v>857</v>
       </c>
       <c r="F108" s="36" t="s">
-        <v>1108</v>
+        <v>1132</v>
       </c>
       <c r="G108" s="36" t="s">
-        <v>1108</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="109">
@@ -8411,7 +8510,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="35" t="s">
-        <v>1109</v>
+        <v>1134</v>
       </c>
       <c r="C109" s="35">
         <v>1.0</v>
@@ -8423,10 +8522,10 @@
         <v>857</v>
       </c>
       <c r="F109" s="36" t="s">
-        <v>1110</v>
+        <v>1135</v>
       </c>
       <c r="G109" s="36" t="s">
-        <v>1110</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="110">
@@ -8435,7 +8534,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="35" t="s">
-        <v>1111</v>
+        <v>1137</v>
       </c>
       <c r="C110" s="35">
         <v>0.0</v>
@@ -8447,10 +8546,10 @@
         <v>857</v>
       </c>
       <c r="F110" s="36" t="s">
-        <v>1112</v>
+        <v>1138</v>
       </c>
       <c r="G110" s="36" t="s">
-        <v>1112</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="111">
@@ -8459,7 +8558,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="35" t="s">
-        <v>1113</v>
+        <v>1140</v>
       </c>
       <c r="C111" s="35">
         <v>1.0</v>
@@ -8471,10 +8570,10 @@
         <v>857</v>
       </c>
       <c r="F111" s="36" t="s">
-        <v>1114</v>
+        <v>1141</v>
       </c>
       <c r="G111" s="36" t="s">
-        <v>1114</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="112">
@@ -8483,7 +8582,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="35" t="s">
-        <v>1115</v>
+        <v>1143</v>
       </c>
       <c r="C112" s="35">
         <v>0.0</v>
@@ -8495,10 +8594,10 @@
         <v>857</v>
       </c>
       <c r="F112" s="36" t="s">
-        <v>1116</v>
+        <v>1144</v>
       </c>
       <c r="G112" s="36" t="s">
-        <v>1116</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="113">
@@ -8522,7 +8621,7 @@
         <v>35</v>
       </c>
       <c r="G113" s="36" t="s">
-        <v>35</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="114">
@@ -8531,7 +8630,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="35" t="s">
-        <v>1117</v>
+        <v>1147</v>
       </c>
       <c r="C114" s="35">
         <v>0.0</v>
@@ -8543,10 +8642,10 @@
         <v>857</v>
       </c>
       <c r="F114" s="36" t="s">
-        <v>1118</v>
+        <v>1148</v>
       </c>
       <c r="G114" s="36" t="s">
-        <v>1118</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="115">
@@ -8555,7 +8654,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="35" t="s">
-        <v>1119</v>
+        <v>1150</v>
       </c>
       <c r="C115" s="35">
         <v>1.0</v>
@@ -8567,10 +8666,10 @@
         <v>857</v>
       </c>
       <c r="F115" s="36" t="s">
-        <v>1120</v>
+        <v>1151</v>
       </c>
       <c r="G115" s="36" t="s">
-        <v>1120</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="116">
@@ -8579,7 +8678,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="35" t="s">
-        <v>1121</v>
+        <v>1153</v>
       </c>
       <c r="C116" s="35">
         <v>0.0</v>
@@ -8591,10 +8690,10 @@
         <v>857</v>
       </c>
       <c r="F116" s="36" t="s">
-        <v>1122</v>
+        <v>1154</v>
       </c>
       <c r="G116" s="36" t="s">
-        <v>1122</v>
+        <v>1154</v>
       </c>
     </row>
   </sheetData>
@@ -8638,25 +8737,25 @@
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1123</v>
+        <v>1155</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>1124</v>
+        <v>1156</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>1125</v>
+        <v>1157</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>1126</v>
+        <v>1158</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>1127</v>
+        <v>1159</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>1128</v>
+        <v>1160</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>1129</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="2" ht="186.0" customHeight="1">
@@ -8692,16 +8791,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>1130</v>
+        <v>1162</v>
       </c>
       <c r="C3" s="62" t="s">
         <v>620</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>1131</v>
+        <v>1163</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>1132</v>
+        <v>1164</v>
       </c>
       <c r="F3" s="33" t="s">
         <v>258</v>
@@ -8710,7 +8809,7 @@
         <v>261</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>1133</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="4">
@@ -8719,16 +8818,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>1134</v>
+        <v>1166</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>1135</v>
+        <v>1167</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>1135</v>
+        <v>1167</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>1136</v>
+        <v>1168</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>258</v>
@@ -8746,16 +8845,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>1137</v>
+        <v>1169</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>1138</v>
+        <v>1170</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>1138</v>
+        <v>1170</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>1139</v>
+        <v>1171</v>
       </c>
       <c r="F5" s="33" t="s">
         <v>258</v>
@@ -8773,16 +8872,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>1140</v>
+        <v>1172</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>1141</v>
+        <v>1173</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>1141</v>
+        <v>1173</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>1142</v>
+        <v>1174</v>
       </c>
       <c r="F6" s="33" t="s">
         <v>258</v>
@@ -8800,16 +8899,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>1143</v>
+        <v>1175</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>1144</v>
+        <v>1176</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>1144</v>
+        <v>1176</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>1145</v>
+        <v>1177</v>
       </c>
       <c r="F7" s="33" t="s">
         <v>258</v>
@@ -8827,16 +8926,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>1146</v>
+        <v>1178</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>1147</v>
+        <v>1179</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>1147</v>
+        <v>1179</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>1148</v>
+        <v>1180</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>258</v>
@@ -8854,7 +8953,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>1149</v>
+        <v>1181</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>653</v>
@@ -8863,7 +8962,7 @@
         <v>653</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>1150</v>
+        <v>1182</v>
       </c>
       <c r="F9" s="33" t="s">
         <v>258</v>
@@ -8881,16 +8980,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>1151</v>
+        <v>1183</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>1152</v>
+        <v>1184</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>1152</v>
+        <v>1184</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>1153</v>
+        <v>1185</v>
       </c>
       <c r="F10" s="33" t="s">
         <v>258</v>
@@ -8911,13 +9010,13 @@
         <v>18</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>1154</v>
+        <v>1186</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>1154</v>
+        <v>1186</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>1155</v>
+        <v>1187</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>258</v>
@@ -8935,7 +9034,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>1156</v>
+        <v>1188</v>
       </c>
       <c r="C12" s="62" t="s">
         <v>260</v>
@@ -8995,7 +9094,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1157</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="2">
@@ -9022,7 +9121,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>1158</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="5">
@@ -9031,7 +9130,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>1159</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="6">
@@ -9043,7 +9142,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1160</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="8">
@@ -9099,7 +9198,7 @@
         <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1161</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="16">
@@ -9117,7 +9216,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>1162</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="18">
@@ -9162,7 +9261,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>460</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="23">
@@ -9171,234 +9270,243 @@
         <v>7</v>
       </c>
       <c r="B23" s="35" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="35">
+        <f>ROW()-ROW(Table_Interaction[N])</f>
+        <v>8</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
+    <row r="26">
+      <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="35">
-        <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B26" s="35" t="s">
-        <v>546</v>
+      <c r="B26" s="1" t="s">
+        <v>1196</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>1164</v>
+        <v>553</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>543</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>1165</v>
+        <v>555</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>535</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>1166</v>
+        <v>535</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>540</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>567</v>
+        <v>540</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="35">
         <f>ROW()-ROW(Table_Unchain_Type[N])</f>
+        <v>10</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="35">
+        <f>ROW()-ROW(Table_Unchain_Type[N])</f>
         <v>11</v>
       </c>
-      <c r="B37" s="35" t="s">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
+      <c r="B38" s="35" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="B40" s="35" t="s">
-        <v>855</v>
+      <c r="B40" s="1" t="s">
+        <v>1201</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="35">
+        <v>0.0</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="35">
         <v>1.0</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B42" s="35" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
+    <row r="44">
+      <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="35">
-        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>259</v>
+      <c r="B44" s="1" t="s">
+        <v>1202</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="35">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>1</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>284</v>
+        <v>0</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="35">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="35">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="35">
         <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
+        <v>3</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="35">
+        <f>ROW()-ROW(Table_Item_Family_Type[N])</f>
         <v>4</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
+    <row r="51">
+      <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="35">
-        <f>ROW()-ROW(Table_Moment_Day[N])</f>
-        <v>0</v>
-      </c>
-      <c r="B51" s="35" t="s">
-        <v>453</v>
+      <c r="B51" s="1" t="s">
+        <v>1203</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="35">
         <f>ROW()-ROW(Table_Moment_Day[N])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="35">
         <f>ROW()-ROW(Table_Moment_Day[N])</f>
+        <v>1</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="35">
+        <f>ROW()-ROW(Table_Moment_Day[N])</f>
         <v>2</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B54" s="35" t="s">
         <v>388</v>
       </c>
     </row>
@@ -9443,7 +9551,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1171</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="2">
@@ -9470,7 +9578,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>1172</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="5">
@@ -9578,7 +9686,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>1173</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="17">
@@ -9587,7 +9695,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>1174</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="18">
@@ -9704,7 +9812,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>1175</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="31">
@@ -9731,7 +9839,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>1176</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="35">
@@ -9739,16 +9847,16 @@
         <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1177</v>
+        <v>1210</v>
       </c>
       <c r="C35" s="63" t="s">
         <v>250</v>
       </c>
       <c r="D35" s="63" t="s">
-        <v>1178</v>
+        <v>1211</v>
       </c>
       <c r="E35" s="63" t="s">
-        <v>1179</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="36">
@@ -9757,7 +9865,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>1180</v>
+        <v>1213</v>
       </c>
       <c r="C36" s="37" t="s">
         <v>258</v>
@@ -9776,7 +9884,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="35" t="s">
-        <v>1181</v>
+        <v>1214</v>
       </c>
       <c r="C37" s="37" t="s">
         <v>794</v>
@@ -9795,7 +9903,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>1182</v>
+        <v>1215</v>
       </c>
       <c r="C38" s="37" t="s">
         <v>825</v>
@@ -9833,7 +9941,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>1183</v>
+        <v>1216</v>
       </c>
       <c r="C40" s="37" t="s">
         <v>375</v>
@@ -9851,19 +9959,19 @@
         <v>46</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1184</v>
+        <v>1217</v>
       </c>
       <c r="C42" s="65" t="s">
-        <v>1185</v>
+        <v>1218</v>
       </c>
       <c r="D42" s="65" t="s">
         <v>755</v>
       </c>
       <c r="E42" s="63" t="s">
-        <v>1186</v>
+        <v>1219</v>
       </c>
       <c r="F42" s="65" t="s">
-        <v>1187</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="43">
@@ -9875,13 +9983,13 @@
         <v>537</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>1180</v>
+        <v>1213</v>
       </c>
       <c r="D43" s="43" t="s">
         <v>393</v>
       </c>
       <c r="E43" s="66" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="F43" s="46" t="b">
         <v>0</v>
@@ -9896,13 +10004,13 @@
         <v>541</v>
       </c>
       <c r="C44" s="43" t="s">
-        <v>1181</v>
+        <v>1214</v>
       </c>
       <c r="D44" s="43" t="s">
         <v>897</v>
       </c>
       <c r="E44" s="66" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="F44" s="46" t="b">
         <v>0</v>
@@ -9917,13 +10025,13 @@
         <v>563</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>1181</v>
+        <v>1214</v>
       </c>
       <c r="D45" s="43" t="s">
         <v>410</v>
       </c>
       <c r="E45" s="66" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="F45" s="46" t="b">
         <v>0</v>
@@ -9938,13 +10046,13 @@
         <v>577</v>
       </c>
       <c r="C46" s="43" t="s">
-        <v>1182</v>
+        <v>1215</v>
       </c>
       <c r="D46" s="43" t="s">
         <v>999</v>
       </c>
       <c r="E46" s="66" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="F46" s="46" t="b">
         <v>0</v>
@@ -9962,10 +10070,10 @@
         <v>41</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>1054</v>
+        <v>1072</v>
       </c>
       <c r="E47" s="66" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="F47" s="46" t="b">
         <v>0</v>
@@ -9977,16 +10085,16 @@
         <v>5</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>1189</v>
+        <v>1222</v>
       </c>
       <c r="C48" s="43" t="s">
         <v>41</v>
       </c>
       <c r="D48" s="43" t="s">
-        <v>1057</v>
+        <v>1075</v>
       </c>
       <c r="E48" s="66" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="F48" s="46" t="b">
         <v>0</v>
@@ -9998,16 +10106,16 @@
         <v>6</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>1190</v>
+        <v>1223</v>
       </c>
       <c r="C49" s="43" t="s">
         <v>41</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>1060</v>
+        <v>1078</v>
       </c>
       <c r="E49" s="66" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="F49" s="46" t="b">
         <v>1</v>
@@ -10019,16 +10127,16 @@
         <v>7</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>1191</v>
+        <v>1224</v>
       </c>
       <c r="C50" s="43" t="s">
-        <v>1183</v>
+        <v>1216</v>
       </c>
       <c r="D50" s="43" t="s">
         <v>393</v>
       </c>
       <c r="E50" s="66" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="F50" s="46" t="b">
         <v>0</v>
@@ -10039,10 +10147,10 @@
         <v>46</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1192</v>
+        <v>1225</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>1193</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="53">
@@ -10051,7 +10159,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>1188</v>
+        <v>1221</v>
       </c>
       <c r="C53" s="67" t="s">
         <v>387</v>
@@ -10062,7 +10170,7 @@
         <v>46</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1194</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="56">
@@ -11068,21 +11176,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1195</v>
+        <v>1228</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1196</v>
+        <v>1229</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1197</v>
+        <v>1230</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1198</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="35" t="s">
-        <v>1199</v>
+        <v>1232</v>
       </c>
       <c r="B2" s="69">
         <v>1.0</v>
@@ -11096,7 +11204,7 @@
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
-        <v>1200</v>
+        <v>1233</v>
       </c>
       <c r="B3" s="69">
         <v>1.0</v>
@@ -11110,7 +11218,7 @@
     </row>
     <row r="4">
       <c r="A4" s="35" t="s">
-        <v>1201</v>
+        <v>1234</v>
       </c>
       <c r="B4" s="69">
         <v>3.0</v>
@@ -11124,7 +11232,7 @@
     </row>
     <row r="5">
       <c r="A5" s="35" t="s">
-        <v>1202</v>
+        <v>1235</v>
       </c>
       <c r="B5" s="69">
         <v>1.0</v>
@@ -11138,7 +11246,7 @@
     </row>
     <row r="6">
       <c r="A6" s="35" t="s">
-        <v>1203</v>
+        <v>1236</v>
       </c>
       <c r="B6" s="69">
         <v>3.0</v>
@@ -11152,7 +11260,7 @@
     </row>
     <row r="7">
       <c r="A7" s="35" t="s">
-        <v>1204</v>
+        <v>1237</v>
       </c>
       <c r="B7" s="69">
         <v>3.0</v>
@@ -11166,7 +11274,7 @@
     </row>
     <row r="8">
       <c r="A8" s="35" t="s">
-        <v>1205</v>
+        <v>1238</v>
       </c>
       <c r="B8" s="69">
         <v>5.0</v>
@@ -11180,7 +11288,7 @@
     </row>
     <row r="9">
       <c r="A9" s="35" t="s">
-        <v>1206</v>
+        <v>1239</v>
       </c>
       <c r="B9" s="69">
         <v>4.0</v>
@@ -11194,7 +11302,7 @@
     </row>
     <row r="10">
       <c r="A10" s="35" t="s">
-        <v>1207</v>
+        <v>1240</v>
       </c>
       <c r="B10" s="69">
         <v>5.0</v>
@@ -11208,7 +11316,7 @@
     </row>
     <row r="11">
       <c r="A11" s="35" t="s">
-        <v>1208</v>
+        <v>1241</v>
       </c>
       <c r="B11" s="69">
         <v>4.0</v>
@@ -11222,7 +11330,7 @@
     </row>
     <row r="12">
       <c r="A12" s="35" t="s">
-        <v>1209</v>
+        <v>1242</v>
       </c>
       <c r="B12" s="69">
         <v>1.0</v>
@@ -11236,7 +11344,7 @@
     </row>
     <row r="13">
       <c r="A13" s="35" t="s">
-        <v>1210</v>
+        <v>1243</v>
       </c>
       <c r="B13" s="69">
         <v>4.0</v>
@@ -11250,7 +11358,7 @@
     </row>
     <row r="14">
       <c r="A14" s="35" t="s">
-        <v>1211</v>
+        <v>1244</v>
       </c>
       <c r="B14" s="69">
         <v>1.0</v>
@@ -11264,7 +11372,7 @@
     </row>
     <row r="15">
       <c r="A15" s="35" t="s">
-        <v>1212</v>
+        <v>1245</v>
       </c>
       <c r="B15" s="69">
         <v>2.0</v>
@@ -11278,7 +11386,7 @@
     </row>
     <row r="16">
       <c r="A16" s="35" t="s">
-        <v>1213</v>
+        <v>1246</v>
       </c>
       <c r="B16" s="69">
         <v>3.0</v>
@@ -11292,7 +11400,7 @@
     </row>
     <row r="17">
       <c r="A17" s="35" t="s">
-        <v>1214</v>
+        <v>1247</v>
       </c>
       <c r="B17" s="69">
         <v>2.0</v>
@@ -11306,7 +11414,7 @@
     </row>
     <row r="18">
       <c r="A18" s="35" t="s">
-        <v>1215</v>
+        <v>1248</v>
       </c>
       <c r="B18" s="69">
         <v>2.0</v>
@@ -11320,7 +11428,7 @@
     </row>
     <row r="19">
       <c r="A19" s="35" t="s">
-        <v>1216</v>
+        <v>1249</v>
       </c>
       <c r="B19" s="69">
         <v>2.0</v>
@@ -11334,7 +11442,7 @@
     </row>
     <row r="20">
       <c r="A20" s="35" t="s">
-        <v>1217</v>
+        <v>1250</v>
       </c>
       <c r="B20" s="69">
         <v>2.0</v>
@@ -11348,7 +11456,7 @@
     </row>
     <row r="21">
       <c r="A21" s="35" t="s">
-        <v>1218</v>
+        <v>1251</v>
       </c>
       <c r="B21" s="69">
         <v>3.0</v>
@@ -11362,7 +11470,7 @@
     </row>
     <row r="22">
       <c r="A22" s="35" t="s">
-        <v>1219</v>
+        <v>1252</v>
       </c>
       <c r="B22" s="69">
         <v>2.0</v>
@@ -11376,7 +11484,7 @@
     </row>
     <row r="23">
       <c r="A23" s="35" t="s">
-        <v>1220</v>
+        <v>1253</v>
       </c>
       <c r="B23" s="69">
         <v>2.0</v>
@@ -11390,7 +11498,7 @@
     </row>
     <row r="24">
       <c r="A24" s="35" t="s">
-        <v>1221</v>
+        <v>1254</v>
       </c>
       <c r="B24" s="69">
         <v>2.0</v>
@@ -11404,7 +11512,7 @@
     </row>
     <row r="25">
       <c r="A25" s="35" t="s">
-        <v>1222</v>
+        <v>1255</v>
       </c>
       <c r="B25" s="69">
         <v>2.0</v>
@@ -11418,7 +11526,7 @@
     </row>
     <row r="26">
       <c r="A26" s="35" t="s">
-        <v>1223</v>
+        <v>1256</v>
       </c>
       <c r="B26" s="69">
         <v>2.0</v>
@@ -11432,7 +11540,7 @@
     </row>
     <row r="27">
       <c r="A27" s="35" t="s">
-        <v>1224</v>
+        <v>1257</v>
       </c>
       <c r="B27" s="69">
         <v>2.0</v>
@@ -11446,7 +11554,7 @@
     </row>
     <row r="28">
       <c r="A28" s="35" t="s">
-        <v>1225</v>
+        <v>1258</v>
       </c>
       <c r="B28" s="69">
         <v>2.0</v>
@@ -11460,7 +11568,7 @@
     </row>
     <row r="29">
       <c r="A29" s="35" t="s">
-        <v>1226</v>
+        <v>1259</v>
       </c>
       <c r="B29" s="69">
         <v>4.0</v>
@@ -11474,7 +11582,7 @@
     </row>
     <row r="30">
       <c r="A30" s="35" t="s">
-        <v>1227</v>
+        <v>1260</v>
       </c>
       <c r="B30" s="69">
         <v>2.0</v>
@@ -14788,8 +14896,8 @@
       <c r="J25" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="K25" s="26" t="s">
-        <v>67</v>
+      <c r="K25" s="23" t="s">
+        <v>122</v>
       </c>
       <c r="L25" s="23" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Used GameMaster for detail resource management
</commit_message>
<xml_diff>
--- a/VARMAP_Generator/VARMAP.xlsx
+++ b/VARMAP_Generator/VARMAP.xlsx
@@ -3828,10 +3828,10 @@
     <t>NEEDED_PHRASES</t>
   </si>
   <si>
-    <t>string.Empty</t>
-  </si>
-  <si>
-    <t>"PREFAB_DETAIL_EXTRAPERLO"</t>
+    <t>PrefabEnum.PREFAB_NONE</t>
+  </si>
+  <si>
+    <t>PrefabEnum.PREFAB_DETAIL_EXTRAPERLO</t>
   </si>
   <si>
     <t>DETAIL_LAST</t>

</xml_diff>